<commit_message>
Blog Statistics - November 2016
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17531"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud Storage\OneDrive\GIT Hub\kunal-chowdhury.com\blog-stats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c93c05515dfe04a/GIT Hub/kunal-chowdhury.com/blog-stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>Jan</t>
   </si>
@@ -951,7 +951,7 @@
                   <c:v>1217957</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3142668</c:v>
+                  <c:v>3855748</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1987,8 +1987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2492,8 +2492,8 @@
       <c r="L13" s="11">
         <v>635500</v>
       </c>
-      <c r="M13" s="6" t="s">
-        <v>28</v>
+      <c r="M13" s="11">
+        <v>713080</v>
       </c>
       <c r="N13" s="6" t="s">
         <v>28</v>
@@ -2501,7 +2501,7 @@
       <c r="O13" s="7"/>
       <c r="P13" s="8">
         <f>SUM(C13:N13)</f>
-        <v>3142668</v>
+        <v>3855748</v>
       </c>
     </row>
     <row r="14" spans="2:16" ht="21" x14ac:dyDescent="0.35">
@@ -2521,7 +2521,7 @@
       <c r="O14" s="13"/>
       <c r="P14" s="9">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>8470602</v>
+        <v>9183682</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Blog Statistics - January 2017
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17668"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c93c05515dfe04a/GIT Hub/kunal-chowdhury.com/blog-stats/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud Storage\OneDrive\GIT Hub\kunal-chowdhury.com\blog-stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="8940"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>Jan</t>
   </si>
@@ -112,7 +112,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +138,17 @@
       <color rgb="FF002060"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="5">
@@ -258,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -281,6 +292,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -886,10 +903,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$13</c:f>
+              <c:f>Sheet1!$B$5:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>2008</c:v>
                 </c:pt>
@@ -917,15 +934,18 @@
                 <c:pt idx="8">
                   <c:v>2016</c:v>
                 </c:pt>
+                <c:pt idx="9">
+                  <c:v>2017</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$5:$P$13</c:f>
+              <c:f>Sheet1!$P$5:$P$14</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>326</c:v>
                 </c:pt>
@@ -951,7 +971,10 @@
                   <c:v>1217957</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3855748</c:v>
+                  <c:v>4530257</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>662423</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1603,13 +1626,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>9523</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>166686</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1639,8 +1662,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:P13" totalsRowShown="0" dataDxfId="15">
-  <autoFilter ref="B3:P13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:P14" totalsRowShown="0" dataDxfId="15">
+  <autoFilter ref="B3:P14"/>
   <tableColumns count="15">
     <tableColumn id="1" name="Column1" dataDxfId="14"/>
     <tableColumn id="2" name="Column2" dataDxfId="13"/>
@@ -1985,22 +2008,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:P14"/>
+  <dimension ref="B3:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" customWidth="1"/>
-    <col min="3" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.5703125" customWidth="1"/>
-    <col min="16" max="16" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" customWidth="1"/>
+    <col min="3" max="14" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.5546875" customWidth="1"/>
+    <col min="16" max="16" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>13</v>
       </c>
@@ -2047,7 +2068,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:16" ht="21" x14ac:dyDescent="0.4">
       <c r="B4" s="1"/>
       <c r="C4" s="2" t="s">
         <v>0</v>
@@ -2090,7 +2111,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:16" ht="21" x14ac:dyDescent="0.4">
       <c r="B5" s="5">
         <v>2008</v>
       </c>
@@ -2136,7 +2157,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="6" spans="2:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:16" ht="21" x14ac:dyDescent="0.4">
       <c r="B6" s="5">
         <v>2009</v>
       </c>
@@ -2182,7 +2203,7 @@
         <v>80379</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:16" ht="21" x14ac:dyDescent="0.4">
       <c r="B7" s="5">
         <v>2010</v>
       </c>
@@ -2228,7 +2249,7 @@
         <v>463113</v>
       </c>
     </row>
-    <row r="8" spans="2:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:16" ht="21" x14ac:dyDescent="0.4">
       <c r="B8" s="5">
         <v>2011</v>
       </c>
@@ -2274,7 +2295,7 @@
         <v>803010</v>
       </c>
     </row>
-    <row r="9" spans="2:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:16" ht="21" x14ac:dyDescent="0.4">
       <c r="B9" s="5">
         <v>2012</v>
       </c>
@@ -2320,7 +2341,7 @@
         <v>888853</v>
       </c>
     </row>
-    <row r="10" spans="2:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:16" ht="21" x14ac:dyDescent="0.4">
       <c r="B10" s="5">
         <v>2013</v>
       </c>
@@ -2366,7 +2387,7 @@
         <v>935657</v>
       </c>
     </row>
-    <row r="11" spans="2:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:16" ht="21" x14ac:dyDescent="0.4">
       <c r="B11" s="5">
         <v>2014</v>
       </c>
@@ -2412,7 +2433,7 @@
         <v>938639</v>
       </c>
     </row>
-    <row r="12" spans="2:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:16" ht="21" x14ac:dyDescent="0.4">
       <c r="B12" s="5">
         <v>2015</v>
       </c>
@@ -2458,7 +2479,7 @@
         <v>1217957</v>
       </c>
     </row>
-    <row r="13" spans="2:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:16" ht="21" x14ac:dyDescent="0.4">
       <c r="B13" s="5">
         <v>2016</v>
       </c>
@@ -2495,43 +2516,68 @@
       <c r="M13" s="11">
         <v>713080</v>
       </c>
-      <c r="N13" s="6" t="s">
-        <v>28</v>
+      <c r="N13" s="11">
+        <v>674509</v>
       </c>
       <c r="O13" s="7"/>
       <c r="P13" s="8">
         <f>SUM(C13:N13)</f>
-        <v>3855748</v>
+        <v>4530257</v>
       </c>
     </row>
-    <row r="14" spans="2:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="B14" s="12"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="9">
+    <row r="14" spans="2:16" ht="21" x14ac:dyDescent="0.4">
+      <c r="B14" s="14">
+        <v>2017</v>
+      </c>
+      <c r="C14" s="11">
+        <v>662423</v>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="17">
+        <f>SUM(C14:N14)</f>
+        <v>662423</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" ht="21" x14ac:dyDescent="0.4">
+      <c r="B15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="9">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>9183682</v>
+        <v>10520614</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B14:O14"/>
+    <mergeCell ref="B15:O15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="P5:P6 P7:P12" formulaRange="1"/>
+    <ignoredError sqref="P5:P14" formulaRange="1"/>
+    <ignoredError sqref="P4" calculatedColumn="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Updated the chart style
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Jan</t>
   </si>
@@ -105,7 +105,10 @@
     <t>Column15</t>
   </si>
   <si>
-    <t>-</t>
+    <t>Column16</t>
+  </si>
+  <si>
+    <t>Column152</t>
   </si>
 </sst>
 </file>
@@ -177,7 +180,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -206,30 +209,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -254,22 +237,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -277,32 +249,52 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="18">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -605,7 +597,9 @@
           <c:spPr>
             <a:ln w="31750" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent4">
+                  <a:shade val="65000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -659,13 +653,367 @@
               </a:effectLst>
             </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2017</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2017</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C6D6-4E14-869C-870F1EA86C0B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Series2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="3175" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="65000"/>
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="65000"/>
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:tint val="65000"/>
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="3175">
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="6"/>
+              <c:spPr>
+                <a:gradFill rotWithShape="1">
+                  <a:gsLst>
+                    <a:gs pos="0">
+                      <a:schemeClr val="accent4">
+                        <a:tint val="65000"/>
+                        <a:shade val="51000"/>
+                        <a:satMod val="130000"/>
+                      </a:schemeClr>
+                    </a:gs>
+                    <a:gs pos="80000">
+                      <a:schemeClr val="accent4">
+                        <a:tint val="65000"/>
+                        <a:shade val="93000"/>
+                        <a:satMod val="130000"/>
+                      </a:schemeClr>
+                    </a:gs>
+                    <a:gs pos="100000">
+                      <a:schemeClr val="accent4">
+                        <a:tint val="65000"/>
+                        <a:shade val="94000"/>
+                        <a:satMod val="135000"/>
+                      </a:schemeClr>
+                    </a:gs>
+                  </a:gsLst>
+                  <a:lin ang="16200000" scaled="0"/>
+                </a:gradFill>
+                <a:ln w="12700">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:prstDash val="lgDash"/>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="12700" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="lgDash"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000C-F234-47AE-98F4-23124B27C96C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2017</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$5:$R$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>326</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80379</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>463113</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>803010</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>888853</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>935657</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>938639</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1217957</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4530257</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7949076</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F234-47AE-98F4-23124B27C96C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Series3</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="12700">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.5238093409752852E-3"/>
-                  <c:y val="-4.4137911859717903E-2"/>
+                  <c:x val="-4.4444439259908068E-3"/>
+                  <c:y val="-0.1009218363128505"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -677,7 +1025,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000008-AF09-443A-86B6-D9B889E2406E}"/>
+                  <c16:uniqueId val="{00000002-F234-47AE-98F4-23124B27C96C}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -685,8 +1033,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.8285712091703085E-2"/>
-                  <c:y val="-8.0919505076149478E-2"/>
+                  <c:x val="-1.333333177797238E-2"/>
+                  <c:y val="-9.7040227223894576E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -698,7 +1046,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000007-AF09-443A-86B6-D9B889E2406E}"/>
+                  <c16:uniqueId val="{00000003-F234-47AE-98F4-23124B27C96C}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -706,8 +1054,8 @@
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="1.3714284068777314E-2"/>
-                  <c:y val="3.6781593216431582E-2"/>
+                  <c:x val="-8.8888878519815858E-3"/>
+                  <c:y val="-9.3158618134938795E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -719,7 +1067,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000006-AF09-443A-86B6-D9B889E2406E}"/>
+                  <c16:uniqueId val="{00000004-F234-47AE-98F4-23124B27C96C}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -727,8 +1075,8 @@
               <c:idx val="3"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.5238093409752572E-3"/>
-                  <c:y val="-6.2528708467933694E-2"/>
+                  <c:x val="0"/>
+                  <c:y val="-7.7632181779115655E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -740,7 +1088,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000000-AF09-443A-86B6-D9B889E2406E}"/>
+                  <c16:uniqueId val="{00000005-F234-47AE-98F4-23124B27C96C}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -748,8 +1096,8 @@
               <c:idx val="4"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="3.0476186819505145E-3"/>
-                  <c:y val="5.885054914629053E-2"/>
+                  <c:x val="0"/>
+                  <c:y val="-6.9868963601204093E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -761,7 +1109,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000001-AF09-443A-86B6-D9B889E2406E}"/>
+                  <c16:uniqueId val="{00000006-F234-47AE-98F4-23124B27C96C}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -769,8 +1117,8 @@
               <c:idx val="5"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="4.5714280229256594E-3"/>
-                  <c:y val="-6.9885027111220008E-2"/>
+                  <c:x val="1.4814813086634891E-3"/>
+                  <c:y val="-5.8224136334336887E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -782,7 +1130,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000002-AF09-443A-86B6-D9B889E2406E}"/>
+                  <c16:uniqueId val="{00000007-F234-47AE-98F4-23124B27C96C}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -790,8 +1138,8 @@
               <c:idx val="6"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="2.2857140114628857E-2"/>
-                  <c:y val="4.4137911859717903E-2"/>
+                  <c:x val="-4.4444439259907929E-3"/>
+                  <c:y val="-8.1513790868071437E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -803,7 +1151,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-AF09-443A-86B6-D9B889E2406E}"/>
+                  <c16:uniqueId val="{00000008-F234-47AE-98F4-23124B27C96C}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -811,8 +1159,8 @@
               <c:idx val="7"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="1.0666665386826689E-2"/>
-                  <c:y val="4.0459752538074607E-2"/>
+                  <c:x val="1.7777775703963172E-2"/>
+                  <c:y val="-1.5526436355823132E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -824,7 +1172,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000004-AF09-443A-86B6-D9B889E2406E}"/>
+                  <c16:uniqueId val="{00000009-F234-47AE-98F4-23124B27C96C}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -832,8 +1180,8 @@
               <c:idx val="8"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-8.2285704412664001E-2"/>
-                  <c:y val="-3.6781593216431582E-2"/>
+                  <c:x val="1.1851850469308782E-2"/>
+                  <c:y val="-7.1162011227896489E-17"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -845,7 +1193,48 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000005-AF09-443A-86B6-D9B889E2406E}"/>
+                  <c16:uniqueId val="{0000000A-F234-47AE-98F4-23124B27C96C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.1851850469308782E-2"/>
+                  <c:y val="-0.10480344540180614"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{528CCE5D-54F9-45A3-8AB0-78CA94A9AC10}" type="VALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[VALUE]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>  ^</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-F234-47AE-98F4-23124B27C96C}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -982,13 +1371,13 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C6D6-4E14-869C-870F1EA86C0B}"/>
+              <c16:uniqueId val="{00000000-F234-47AE-98F4-23124B27C96C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -1068,7 +1457,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1631,9 +2020,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1662,25 +2051,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:P14" totalsRowShown="0" dataDxfId="15">
-  <autoFilter ref="B3:P14"/>
-  <tableColumns count="15">
-    <tableColumn id="1" name="Column1" dataDxfId="14"/>
-    <tableColumn id="2" name="Column2" dataDxfId="13"/>
-    <tableColumn id="3" name="Column3" dataDxfId="12"/>
-    <tableColumn id="4" name="Column4" dataDxfId="11"/>
-    <tableColumn id="5" name="Column5" dataDxfId="10"/>
-    <tableColumn id="6" name="Column6" dataDxfId="9"/>
-    <tableColumn id="7" name="Column7" dataDxfId="8"/>
-    <tableColumn id="8" name="Column8" dataDxfId="7"/>
-    <tableColumn id="9" name="Column9" dataDxfId="6"/>
-    <tableColumn id="10" name="Column10" dataDxfId="5"/>
-    <tableColumn id="11" name="Column11" dataDxfId="4"/>
-    <tableColumn id="12" name="Column12" dataDxfId="3"/>
-    <tableColumn id="13" name="Column13" dataDxfId="2"/>
-    <tableColumn id="14" name="Column14" dataDxfId="1"/>
-    <tableColumn id="15" name="Column15" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:R14" totalsRowShown="0" dataDxfId="17">
+  <autoFilter ref="B3:R14"/>
+  <tableColumns count="17">
+    <tableColumn id="1" name="Column1" dataDxfId="16"/>
+    <tableColumn id="2" name="Column2" dataDxfId="15"/>
+    <tableColumn id="3" name="Column3" dataDxfId="14"/>
+    <tableColumn id="4" name="Column4" dataDxfId="13"/>
+    <tableColumn id="5" name="Column5" dataDxfId="12"/>
+    <tableColumn id="6" name="Column6" dataDxfId="11"/>
+    <tableColumn id="7" name="Column7" dataDxfId="10"/>
+    <tableColumn id="8" name="Column8" dataDxfId="9"/>
+    <tableColumn id="9" name="Column9" dataDxfId="8"/>
+    <tableColumn id="10" name="Column10" dataDxfId="7"/>
+    <tableColumn id="11" name="Column11" dataDxfId="6"/>
+    <tableColumn id="12" name="Column12" dataDxfId="5"/>
+    <tableColumn id="13" name="Column13" dataDxfId="4"/>
+    <tableColumn id="14" name="Column14" dataDxfId="3"/>
+    <tableColumn id="15" name="Column15" dataDxfId="2">
       <calculatedColumnFormula>SUM(C4:N4)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="17" name="Column152" dataDxfId="0" dataCellStyle="Normal"/>
+    <tableColumn id="16" name="Column16" dataDxfId="1">
+      <calculatedColumnFormula>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2008,9 +2401,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:P15"/>
+  <dimension ref="B2:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R24" sqref="R24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2018,10 +2413,14 @@
     <col min="2" max="2" width="9.5546875" customWidth="1"/>
     <col min="3" max="14" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5.5546875" customWidth="1"/>
-    <col min="16" max="16" width="18.33203125" customWidth="1"/>
+    <col min="16" max="17" width="18.33203125" customWidth="1"/>
+    <col min="18" max="18" width="25.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="Q2" s="16"/>
+    </row>
+    <row r="3" spans="2:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>13</v>
       </c>
@@ -2067,8 +2466,14 @@
       <c r="P3" t="s">
         <v>27</v>
       </c>
+      <c r="Q3" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="R3" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="4" spans="2:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:18" ht="21" x14ac:dyDescent="0.4">
       <c r="B4" s="1"/>
       <c r="C4" s="2" t="s">
         <v>0</v>
@@ -2107,449 +2512,486 @@
         <v>11</v>
       </c>
       <c r="O4" s="3"/>
-      <c r="P4" s="4" t="s">
+      <c r="P4" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="14" t="e">
+        <f>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
+        <v>#VALUE!</v>
+      </c>
     </row>
-    <row r="5" spans="2:16" ht="21" x14ac:dyDescent="0.4">
-      <c r="B5" s="5">
+    <row r="5" spans="2:18" ht="21" x14ac:dyDescent="0.4">
+      <c r="B5" s="4">
         <v>2008</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="L5" s="7">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="6">
         <v>105</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5" s="6">
         <v>112</v>
       </c>
-      <c r="N5" s="7">
+      <c r="N5" s="6">
         <v>109</v>
       </c>
-      <c r="O5" s="7"/>
-      <c r="P5" s="8">
+      <c r="O5" s="6"/>
+      <c r="P5" s="6">
         <f>SUM(C5:N5)</f>
         <v>326</v>
       </c>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="14">
+        <f>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
+        <v>326</v>
+      </c>
     </row>
-    <row r="6" spans="2:16" ht="21" x14ac:dyDescent="0.4">
-      <c r="B6" s="5">
+    <row r="6" spans="2:18" ht="21" x14ac:dyDescent="0.4">
+      <c r="B6" s="4">
         <v>2009</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>210</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <v>265</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>330</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <v>459</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="6">
         <v>2711</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="6">
         <v>4347</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="6">
         <v>7134</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="6">
         <v>7452</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="6">
         <v>10193</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6" s="6">
         <v>11773</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M6" s="6">
         <v>16989</v>
       </c>
-      <c r="N6" s="7">
+      <c r="N6" s="6">
         <v>18516</v>
       </c>
-      <c r="O6" s="7"/>
-      <c r="P6" s="8">
+      <c r="O6" s="6"/>
+      <c r="P6" s="6">
         <f t="shared" ref="P6:P12" si="0">SUM(C6:N6)</f>
         <v>80379</v>
       </c>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="14">
+        <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
+        <v>80379</v>
+      </c>
     </row>
-    <row r="7" spans="2:16" ht="21" x14ac:dyDescent="0.4">
-      <c r="B7" s="5">
+    <row r="7" spans="2:18" ht="21" x14ac:dyDescent="0.4">
+      <c r="B7" s="4">
         <v>2010</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>16660</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>23673</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>32985</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <v>35222</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <v>39909</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="6">
         <v>42087</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="6">
         <v>54395</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="6">
         <v>49067</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="6">
         <v>47658</v>
       </c>
-      <c r="L7" s="7">
+      <c r="L7" s="6">
         <v>38853</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M7" s="6">
         <v>39946</v>
       </c>
-      <c r="N7" s="7">
+      <c r="N7" s="6">
         <v>42658</v>
       </c>
-      <c r="O7" s="7"/>
-      <c r="P7" s="8">
+      <c r="O7" s="6"/>
+      <c r="P7" s="6">
         <f t="shared" si="0"/>
         <v>463113</v>
       </c>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="14">
+        <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
+        <v>463113</v>
+      </c>
     </row>
-    <row r="8" spans="2:16" ht="21" x14ac:dyDescent="0.4">
-      <c r="B8" s="5">
+    <row r="8" spans="2:18" ht="21" x14ac:dyDescent="0.4">
+      <c r="B8" s="4">
         <v>2011</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <v>45551</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="6">
         <v>69346</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <v>47856</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <v>64728</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <v>73308</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="6">
         <v>82846</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="6">
         <v>72286</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="6">
         <v>75867</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="6">
         <v>80961</v>
       </c>
-      <c r="L8" s="7">
+      <c r="L8" s="6">
         <v>62233</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="6">
         <v>63447</v>
       </c>
-      <c r="N8" s="7">
+      <c r="N8" s="6">
         <v>64581</v>
       </c>
-      <c r="O8" s="7"/>
-      <c r="P8" s="8">
+      <c r="O8" s="6"/>
+      <c r="P8" s="6">
         <f t="shared" si="0"/>
         <v>803010</v>
       </c>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="14">
+        <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
+        <v>803010</v>
+      </c>
     </row>
-    <row r="9" spans="2:16" ht="21" x14ac:dyDescent="0.4">
-      <c r="B9" s="5">
+    <row r="9" spans="2:18" ht="21" x14ac:dyDescent="0.4">
+      <c r="B9" s="4">
         <v>2012</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>76072</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>77385</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <v>70852</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <v>72356</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <v>78593</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="6">
         <v>70155</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="6">
         <v>72470</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="6">
         <v>70252</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="6">
         <v>79738</v>
       </c>
-      <c r="L9" s="7">
+      <c r="L9" s="6">
         <v>71284</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M9" s="6">
         <v>76524</v>
       </c>
-      <c r="N9" s="7">
+      <c r="N9" s="6">
         <v>73172</v>
       </c>
-      <c r="O9" s="7"/>
-      <c r="P9" s="8">
+      <c r="O9" s="6"/>
+      <c r="P9" s="6">
         <f t="shared" si="0"/>
         <v>888853</v>
       </c>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="14">
+        <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
+        <v>888853</v>
+      </c>
     </row>
-    <row r="10" spans="2:16" ht="21" x14ac:dyDescent="0.4">
-      <c r="B10" s="5">
+    <row r="10" spans="2:18" ht="21" x14ac:dyDescent="0.4">
+      <c r="B10" s="4">
         <v>2013</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>78648</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="6">
         <v>74894</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="6">
         <v>86029</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="6">
         <v>82489</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="6">
         <v>80316</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="6">
         <v>78764</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="6">
         <v>70746</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="6">
         <v>79324</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="6">
         <v>79148</v>
       </c>
-      <c r="L10" s="7">
+      <c r="L10" s="6">
         <v>76345</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M10" s="6">
         <v>75329</v>
       </c>
-      <c r="N10" s="7">
+      <c r="N10" s="6">
         <v>73625</v>
       </c>
-      <c r="O10" s="7"/>
-      <c r="P10" s="8">
+      <c r="O10" s="6"/>
+      <c r="P10" s="6">
         <f t="shared" si="0"/>
         <v>935657</v>
       </c>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="14">
+        <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
+        <v>935657</v>
+      </c>
     </row>
-    <row r="11" spans="2:16" ht="21" x14ac:dyDescent="0.4">
-      <c r="B11" s="5">
+    <row r="11" spans="2:18" ht="21" x14ac:dyDescent="0.4">
+      <c r="B11" s="4">
         <v>2014</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>67510</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="6">
         <v>67706</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="6">
         <v>73924</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <v>71449</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="6">
         <v>79877</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="6">
         <v>74705</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="6">
         <v>79936</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="6">
         <v>78746</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="6">
         <v>77891</v>
       </c>
-      <c r="L11" s="7">
+      <c r="L11" s="6">
         <v>77040</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M11" s="6">
         <v>87951</v>
       </c>
-      <c r="N11" s="10">
+      <c r="N11" s="7">
         <v>101904</v>
       </c>
-      <c r="O11" s="7"/>
-      <c r="P11" s="8">
+      <c r="O11" s="6"/>
+      <c r="P11" s="6">
         <f t="shared" si="0"/>
         <v>938639</v>
       </c>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="14">
+        <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
+        <v>938639</v>
+      </c>
     </row>
-    <row r="12" spans="2:16" ht="21" x14ac:dyDescent="0.4">
-      <c r="B12" s="5">
+    <row r="12" spans="2:18" ht="21" x14ac:dyDescent="0.4">
+      <c r="B12" s="4">
         <v>2015</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <v>90536</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <v>80976</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <v>95444</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <v>71951</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="6">
         <v>67019</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="6">
         <v>66244</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="6">
         <v>86294</v>
       </c>
-      <c r="J12" s="10">
+      <c r="J12" s="7">
         <v>128005</v>
       </c>
-      <c r="K12" s="10">
+      <c r="K12" s="7">
         <v>137300</v>
       </c>
-      <c r="L12" s="10">
+      <c r="L12" s="7">
         <v>138705</v>
       </c>
-      <c r="M12" s="10">
+      <c r="M12" s="7">
         <v>125538</v>
       </c>
-      <c r="N12" s="10">
+      <c r="N12" s="7">
         <v>129945</v>
       </c>
-      <c r="O12" s="7"/>
-      <c r="P12" s="8">
+      <c r="O12" s="6"/>
+      <c r="P12" s="6">
         <f t="shared" si="0"/>
         <v>1217957</v>
       </c>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="14">
+        <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
+        <v>1217957</v>
+      </c>
     </row>
-    <row r="13" spans="2:16" ht="21" x14ac:dyDescent="0.4">
-      <c r="B13" s="5">
+    <row r="13" spans="2:18" ht="21" x14ac:dyDescent="0.4">
+      <c r="B13" s="4">
         <v>2016</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="7">
         <v>142274</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="7">
         <v>123093</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="7">
         <v>147266</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="7">
         <v>152612</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="7">
         <v>134497</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13" s="7">
         <v>132768</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="8">
         <v>363723</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="8">
         <v>702130</v>
       </c>
-      <c r="K13" s="11">
+      <c r="K13" s="8">
         <v>608805</v>
       </c>
-      <c r="L13" s="11">
+      <c r="L13" s="8">
         <v>635500</v>
       </c>
-      <c r="M13" s="11">
+      <c r="M13" s="8">
         <v>713080</v>
       </c>
-      <c r="N13" s="11">
+      <c r="N13" s="8">
         <v>674509</v>
       </c>
-      <c r="O13" s="7"/>
-      <c r="P13" s="8">
+      <c r="O13" s="6"/>
+      <c r="P13" s="6">
         <f>SUM(C13:N13)</f>
         <v>4530257</v>
       </c>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="14">
+        <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
+        <v>4530257</v>
+      </c>
     </row>
-    <row r="14" spans="2:16" ht="21" x14ac:dyDescent="0.4">
-      <c r="B14" s="14">
+    <row r="14" spans="2:18" ht="21" x14ac:dyDescent="0.4">
+      <c r="B14" s="9">
         <v>2017</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="8">
         <v>662423</v>
       </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="17">
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11">
         <f>SUM(C14:N14)</f>
         <v>662423</v>
       </c>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="14">
+        <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
+        <v>7949076</v>
+      </c>
     </row>
-    <row r="15" spans="2:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:18" ht="21" x14ac:dyDescent="0.4">
       <c r="B15" s="12"/>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
@@ -2564,10 +3006,11 @@
       <c r="M15" s="13"/>
       <c r="N15" s="13"/>
       <c r="O15" s="13"/>
-      <c r="P15" s="9">
+      <c r="P15" s="15">
         <f>SUBTOTAL(109,Table1[Column15])</f>
         <v>10520614</v>
       </c>
+      <c r="Q15" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Updated Blog Statistics - February 2017
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -260,28 +260,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="18">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -294,6 +286,14 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -932,7 +932,7 @@
                   <c:v>4530257</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7949076</c:v>
+                  <c:v>7303590</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1363,7 +1363,7 @@
                   <c:v>4530257</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>662423</c:v>
+                  <c:v>1217265</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2013,16 +2013,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>9523</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>166686</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>485772</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>23811</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>62488</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2071,8 +2071,8 @@
     <tableColumn id="15" name="Column15" dataDxfId="2">
       <calculatedColumnFormula>SUM(C4:N4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Column152" dataDxfId="0" dataCellStyle="Normal"/>
-    <tableColumn id="16" name="Column16" dataDxfId="1">
+    <tableColumn id="17" name="Column152" dataDxfId="1" dataCellStyle="Normal"/>
+    <tableColumn id="16" name="Column16" dataDxfId="0">
       <calculatedColumnFormula>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2403,8 +2403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2418,7 +2418,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="Q2" s="16"/>
+      <c r="Q2" s="14"/>
     </row>
     <row r="3" spans="2:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
@@ -2466,7 +2466,7 @@
       <c r="P3" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="Q3" s="14" t="s">
         <v>29</v>
       </c>
       <c r="R3" t="s">
@@ -2515,8 +2515,8 @@
       <c r="P4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="14" t="e">
+      <c r="Q4" s="14"/>
+      <c r="R4" s="12" t="e">
         <f>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>#VALUE!</v>
       </c>
@@ -2548,8 +2548,8 @@
         <f>SUM(C5:N5)</f>
         <v>326</v>
       </c>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="14">
+      <c r="Q5" s="14"/>
+      <c r="R5" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>326</v>
       </c>
@@ -2599,8 +2599,8 @@
         <f t="shared" ref="P6:P12" si="0">SUM(C6:N6)</f>
         <v>80379</v>
       </c>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="14">
+      <c r="Q6" s="14"/>
+      <c r="R6" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>80379</v>
       </c>
@@ -2650,8 +2650,8 @@
         <f t="shared" si="0"/>
         <v>463113</v>
       </c>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="14">
+      <c r="Q7" s="14"/>
+      <c r="R7" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>463113</v>
       </c>
@@ -2701,8 +2701,8 @@
         <f t="shared" si="0"/>
         <v>803010</v>
       </c>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="14">
+      <c r="Q8" s="14"/>
+      <c r="R8" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>803010</v>
       </c>
@@ -2752,8 +2752,8 @@
         <f t="shared" si="0"/>
         <v>888853</v>
       </c>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="14">
+      <c r="Q9" s="14"/>
+      <c r="R9" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>888853</v>
       </c>
@@ -2803,8 +2803,8 @@
         <f t="shared" si="0"/>
         <v>935657</v>
       </c>
-      <c r="Q10" s="16"/>
-      <c r="R10" s="14">
+      <c r="Q10" s="14"/>
+      <c r="R10" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>935657</v>
       </c>
@@ -2854,8 +2854,8 @@
         <f t="shared" si="0"/>
         <v>938639</v>
       </c>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="14">
+      <c r="Q11" s="14"/>
+      <c r="R11" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>938639</v>
       </c>
@@ -2905,8 +2905,8 @@
         <f t="shared" si="0"/>
         <v>1217957</v>
       </c>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="14">
+      <c r="Q12" s="14"/>
+      <c r="R12" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>1217957</v>
       </c>
@@ -2956,8 +2956,8 @@
         <f>SUM(C13:N13)</f>
         <v>4530257</v>
       </c>
-      <c r="Q13" s="16"/>
-      <c r="R13" s="14">
+      <c r="Q13" s="14"/>
+      <c r="R13" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>4530257</v>
       </c>
@@ -2969,7 +2969,9 @@
       <c r="C14" s="8">
         <v>662423</v>
       </c>
-      <c r="D14" s="10"/>
+      <c r="D14" s="8">
+        <v>554842</v>
+      </c>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
@@ -2983,34 +2985,34 @@
       <c r="O14" s="11"/>
       <c r="P14" s="11">
         <f>SUM(C14:N14)</f>
-        <v>662423</v>
-      </c>
-      <c r="Q14" s="16"/>
-      <c r="R14" s="14">
+        <v>1217265</v>
+      </c>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>7949076</v>
+        <v>7303590</v>
       </c>
     </row>
     <row r="15" spans="2:18" ht="21" x14ac:dyDescent="0.4">
-      <c r="B15" s="12"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="15">
+      <c r="B15" s="15"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="13">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>10520614</v>
-      </c>
-      <c r="Q15" s="16"/>
+        <v>11075456</v>
+      </c>
+      <c r="Q15" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Blog Statistics (March 2017)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17668"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17766"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="8940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -932,7 +932,7 @@
                   <c:v>4530257</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7303590</c:v>
+                  <c:v>7500248</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1363,7 +1363,7 @@
                   <c:v>4530257</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1217265</c:v>
+                  <c:v>1875062</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2404,23 +2404,23 @@
   <dimension ref="B2:R15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+      <selection activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" customWidth="1"/>
-    <col min="3" max="14" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.5546875" customWidth="1"/>
-    <col min="16" max="17" width="18.33203125" customWidth="1"/>
-    <col min="18" max="18" width="25.44140625" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="3" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.5703125" customWidth="1"/>
+    <col min="16" max="17" width="18.28515625" customWidth="1"/>
+    <col min="18" max="18" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="Q2" s="14"/>
     </row>
-    <row r="3" spans="2:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>13</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:18" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:18" ht="21" x14ac:dyDescent="0.35">
       <c r="B4" s="1"/>
       <c r="C4" s="2" t="s">
         <v>0</v>
@@ -2521,7 +2521,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="5" spans="2:18" ht="21" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:18" ht="21" x14ac:dyDescent="0.35">
       <c r="B5" s="4">
         <v>2008</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="6" spans="2:18" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:18" ht="21" x14ac:dyDescent="0.35">
       <c r="B6" s="4">
         <v>2009</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>80379</v>
       </c>
     </row>
-    <row r="7" spans="2:18" ht="21" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:18" ht="21" x14ac:dyDescent="0.35">
       <c r="B7" s="4">
         <v>2010</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>463113</v>
       </c>
     </row>
-    <row r="8" spans="2:18" ht="21" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:18" ht="21" x14ac:dyDescent="0.35">
       <c r="B8" s="4">
         <v>2011</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>803010</v>
       </c>
     </row>
-    <row r="9" spans="2:18" ht="21" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:18" ht="21" x14ac:dyDescent="0.35">
       <c r="B9" s="4">
         <v>2012</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>888853</v>
       </c>
     </row>
-    <row r="10" spans="2:18" ht="21" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:18" ht="21" x14ac:dyDescent="0.35">
       <c r="B10" s="4">
         <v>2013</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>935657</v>
       </c>
     </row>
-    <row r="11" spans="2:18" ht="21" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:18" ht="21" x14ac:dyDescent="0.35">
       <c r="B11" s="4">
         <v>2014</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>938639</v>
       </c>
     </row>
-    <row r="12" spans="2:18" ht="21" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:18" ht="21" x14ac:dyDescent="0.35">
       <c r="B12" s="4">
         <v>2015</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>1217957</v>
       </c>
     </row>
-    <row r="13" spans="2:18" ht="21" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:18" ht="21" x14ac:dyDescent="0.35">
       <c r="B13" s="4">
         <v>2016</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>4530257</v>
       </c>
     </row>
-    <row r="14" spans="2:18" ht="21" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:18" ht="21" x14ac:dyDescent="0.35">
       <c r="B14" s="9">
         <v>2017</v>
       </c>
@@ -2972,7 +2972,9 @@
       <c r="D14" s="8">
         <v>554842</v>
       </c>
-      <c r="E14" s="10"/>
+      <c r="E14" s="8">
+        <v>657797</v>
+      </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
@@ -2985,15 +2987,15 @@
       <c r="O14" s="11"/>
       <c r="P14" s="11">
         <f>SUM(C14:N14)</f>
-        <v>1217265</v>
+        <v>1875062</v>
       </c>
       <c r="Q14" s="14"/>
       <c r="R14" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>7303590</v>
+        <v>7500248</v>
       </c>
     </row>
-    <row r="15" spans="2:18" ht="21" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:18" ht="21" x14ac:dyDescent="0.35">
       <c r="B15" s="15"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
@@ -3010,7 +3012,7 @@
       <c r="O15" s="16"/>
       <c r="P15" s="13">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>11075456</v>
+        <v>11733253</v>
       </c>
       <c r="Q15" s="14"/>
     </row>

</xml_diff>

<commit_message>
Updated Blog Statistics (March 2017)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Jan</t>
   </si>
@@ -110,12 +110,15 @@
   <si>
     <t>Column152</t>
   </si>
+  <si>
+    <t>Last 12 months 'Hit Count':</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,8 +156,15 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,8 +189,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -218,30 +234,19 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
-      </left>
-      <right/>
+      </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -261,19 +266,36 @@
     </xf>
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="18">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -288,14 +310,6 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -306,14 +320,6 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -543,7 +549,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx2"/>
                 </a:solidFill>
@@ -553,7 +559,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2000"/>
               <a:t>Blog Hit / Pageviews</a:t>
             </a:r>
           </a:p>
@@ -572,7 +578,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx2"/>
               </a:solidFill>
@@ -1054,8 +1060,8 @@
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-8.8888878519815858E-3"/>
-                  <c:y val="-9.3158618134938795E-2"/>
+                  <c:x val="-2.4335605818272096E-2"/>
+                  <c:y val="-0.14606230930457262"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1096,8 +1102,8 @@
               <c:idx val="4"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0"/>
-                  <c:y val="-6.9868963601204093E-2"/>
+                  <c:x val="-1.4042473063053691E-3"/>
+                  <c:y val="-0.13070815760385421"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1117,8 +1123,8 @@
               <c:idx val="5"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="1.4814813086634891E-3"/>
-                  <c:y val="-5.8224136334336887E-2"/>
+                  <c:x val="5.6942781123952907E-3"/>
+                  <c:y val="-0.11112775054950078"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1180,8 +1186,8 @@
               <c:idx val="8"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="1.1851850469308782E-2"/>
-                  <c:y val="-7.1162011227896489E-17"/>
+                  <c:x val="-0.15384933487881633"/>
+                  <c:y val="4.8494492840790837E-17"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1201,27 +1207,83 @@
               <c:idx val="9"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.1851850469308782E-2"/>
-                  <c:y val="-0.10480344540180614"/>
+                  <c:x val="-6.1786881477446528E-4"/>
+                  <c:y val="-0.36667675447083081"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
                 <c:rich>
-                  <a:bodyPr/>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:spAutoFit/>
+                  </a:bodyPr>
                   <a:lstStyle/>
                   <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx2"/>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="3200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:srgbClr val="00B050"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t>^</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:srgbClr val="00B050"/>
+                        </a:solidFill>
+                      </a:rPr>
+                      <a:t> </a:t>
+                    </a:r>
                     <a:fld id="{528CCE5D-54F9-45A3-8AB0-78CA94A9AC10}" type="VALUE">
-                      <a:rPr lang="en-US"/>
-                      <a:pPr/>
+                      <a:rPr lang="en-US" sz="1800" b="1"/>
+                      <a:pPr>
+                        <a:defRPr sz="1800" b="1"/>
+                      </a:pPr>
                       <a:t>[VALUE]</a:t>
                     </a:fld>
                     <a:r>
-                      <a:rPr lang="en-US"/>
-                      <a:t>  ^</a:t>
+                      <a:rPr lang="en-US" sz="1800" b="1"/>
+                      <a:t>  </a:t>
                     </a:r>
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -1252,7 +1314,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx2"/>
                     </a:solidFill>
@@ -1417,7 +1479,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx2"/>
                 </a:solidFill>
@@ -1457,7 +1519,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1473,7 +1535,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx2"/>
                 </a:solidFill>
@@ -1507,10 +1569,7 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx2">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="accent1"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -2014,14 +2073,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>485772</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:colOff>21429</xdr:colOff>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>23811</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:colOff>88107</xdr:colOff>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>62488</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2071,8 +2130,8 @@
     <tableColumn id="15" name="Column15" dataDxfId="2">
       <calculatedColumnFormula>SUM(C4:N4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Column152" dataDxfId="1" dataCellStyle="Normal"/>
-    <tableColumn id="16" name="Column16" dataDxfId="0">
+    <tableColumn id="17" name="Column152" dataDxfId="0" dataCellStyle="Normal"/>
+    <tableColumn id="16" name="Column16" dataDxfId="1">
       <calculatedColumnFormula>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2401,10 +2460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:R15"/>
+  <dimension ref="A1:T48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="T38" sqref="T38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2412,15 +2471,58 @@
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" customWidth="1"/>
     <col min="3" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.5703125" customWidth="1"/>
-    <col min="16" max="17" width="18.28515625" customWidth="1"/>
+    <col min="15" max="15" width="4" customWidth="1"/>
+    <col min="16" max="16" width="18.28515625" customWidth="1"/>
+    <col min="17" max="17" width="5.28515625" customWidth="1"/>
     <col min="18" max="18" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="Q2" s="14"/>
-    </row>
-    <row r="3" spans="2:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="19"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+    </row>
+    <row r="3" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
       <c r="B3" t="s">
         <v>13</v>
       </c>
@@ -2466,14 +2568,15 @@
       <c r="P3" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" s="14" t="s">
+      <c r="Q3" s="15" t="s">
         <v>29</v>
       </c>
       <c r="R3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:18" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+      <c r="A4" s="19"/>
       <c r="B4" s="1"/>
       <c r="C4" s="2" t="s">
         <v>0</v>
@@ -2515,13 +2618,16 @@
       <c r="P4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="Q4" s="14"/>
+      <c r="Q4" s="15"/>
       <c r="R4" s="12" t="e">
         <f>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="5" spans="2:18" ht="21" x14ac:dyDescent="0.35">
+      <c r="S4" s="19"/>
+      <c r="T4" s="19"/>
+    </row>
+    <row r="5" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="19"/>
       <c r="B5" s="4">
         <v>2008</v>
       </c>
@@ -2548,13 +2654,16 @@
         <f>SUM(C5:N5)</f>
         <v>326</v>
       </c>
-      <c r="Q5" s="14"/>
+      <c r="Q5" s="15"/>
       <c r="R5" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>326</v>
       </c>
-    </row>
-    <row r="6" spans="2:18" ht="21" x14ac:dyDescent="0.35">
+      <c r="S5" s="19"/>
+      <c r="T5" s="19"/>
+    </row>
+    <row r="6" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+      <c r="A6" s="19"/>
       <c r="B6" s="4">
         <v>2009</v>
       </c>
@@ -2599,13 +2708,16 @@
         <f t="shared" ref="P6:P12" si="0">SUM(C6:N6)</f>
         <v>80379</v>
       </c>
-      <c r="Q6" s="14"/>
+      <c r="Q6" s="15"/>
       <c r="R6" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>80379</v>
       </c>
-    </row>
-    <row r="7" spans="2:18" ht="21" x14ac:dyDescent="0.35">
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
+    </row>
+    <row r="7" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+      <c r="A7" s="19"/>
       <c r="B7" s="4">
         <v>2010</v>
       </c>
@@ -2650,13 +2762,16 @@
         <f t="shared" si="0"/>
         <v>463113</v>
       </c>
-      <c r="Q7" s="14"/>
+      <c r="Q7" s="15"/>
       <c r="R7" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>463113</v>
       </c>
-    </row>
-    <row r="8" spans="2:18" ht="21" x14ac:dyDescent="0.35">
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+    </row>
+    <row r="8" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+      <c r="A8" s="19"/>
       <c r="B8" s="4">
         <v>2011</v>
       </c>
@@ -2701,13 +2816,16 @@
         <f t="shared" si="0"/>
         <v>803010</v>
       </c>
-      <c r="Q8" s="14"/>
+      <c r="Q8" s="15"/>
       <c r="R8" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>803010</v>
       </c>
-    </row>
-    <row r="9" spans="2:18" ht="21" x14ac:dyDescent="0.35">
+      <c r="S8" s="19"/>
+      <c r="T8" s="19"/>
+    </row>
+    <row r="9" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+      <c r="A9" s="19"/>
       <c r="B9" s="4">
         <v>2012</v>
       </c>
@@ -2752,13 +2870,16 @@
         <f t="shared" si="0"/>
         <v>888853</v>
       </c>
-      <c r="Q9" s="14"/>
+      <c r="Q9" s="15"/>
       <c r="R9" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>888853</v>
       </c>
-    </row>
-    <row r="10" spans="2:18" ht="21" x14ac:dyDescent="0.35">
+      <c r="S9" s="19"/>
+      <c r="T9" s="19"/>
+    </row>
+    <row r="10" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+      <c r="A10" s="19"/>
       <c r="B10" s="4">
         <v>2013</v>
       </c>
@@ -2803,13 +2924,16 @@
         <f t="shared" si="0"/>
         <v>935657</v>
       </c>
-      <c r="Q10" s="14"/>
+      <c r="Q10" s="15"/>
       <c r="R10" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>935657</v>
       </c>
-    </row>
-    <row r="11" spans="2:18" ht="21" x14ac:dyDescent="0.35">
+      <c r="S10" s="19"/>
+      <c r="T10" s="19"/>
+    </row>
+    <row r="11" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+      <c r="A11" s="19"/>
       <c r="B11" s="4">
         <v>2014</v>
       </c>
@@ -2854,13 +2978,16 @@
         <f t="shared" si="0"/>
         <v>938639</v>
       </c>
-      <c r="Q11" s="14"/>
+      <c r="Q11" s="15"/>
       <c r="R11" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>938639</v>
       </c>
-    </row>
-    <row r="12" spans="2:18" ht="21" x14ac:dyDescent="0.35">
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
+    </row>
+    <row r="12" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+      <c r="A12" s="19"/>
       <c r="B12" s="4">
         <v>2015</v>
       </c>
@@ -2905,13 +3032,16 @@
         <f t="shared" si="0"/>
         <v>1217957</v>
       </c>
-      <c r="Q12" s="14"/>
+      <c r="Q12" s="15"/>
       <c r="R12" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>1217957</v>
       </c>
-    </row>
-    <row r="13" spans="2:18" ht="21" x14ac:dyDescent="0.35">
+      <c r="S12" s="19"/>
+      <c r="T12" s="19"/>
+    </row>
+    <row r="13" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+      <c r="A13" s="19"/>
       <c r="B13" s="4">
         <v>2016</v>
       </c>
@@ -2956,13 +3086,16 @@
         <f>SUM(C13:N13)</f>
         <v>4530257</v>
       </c>
-      <c r="Q13" s="14"/>
+      <c r="Q13" s="15"/>
       <c r="R13" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>4530257</v>
       </c>
-    </row>
-    <row r="14" spans="2:18" ht="21" x14ac:dyDescent="0.35">
+      <c r="S13" s="19"/>
+      <c r="T13" s="19"/>
+    </row>
+    <row r="14" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+      <c r="A14" s="19"/>
       <c r="B14" s="9">
         <v>2017</v>
       </c>
@@ -2989,41 +3122,779 @@
         <f>SUM(C14:N14)</f>
         <v>1875062</v>
       </c>
-      <c r="Q14" s="14"/>
+      <c r="Q14" s="15"/>
       <c r="R14" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>7500248</v>
       </c>
-    </row>
-    <row r="15" spans="2:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="B15" s="15"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="13">
+      <c r="S14" s="19"/>
+      <c r="T14" s="19"/>
+    </row>
+    <row r="15" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+      <c r="A15" s="19"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="20">
         <f>SUBTOTAL(109,Table1[Column15])</f>
         <v>11733253</v>
       </c>
-      <c r="Q15" s="14"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="19"/>
+      <c r="T15" s="19"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="19"/>
+      <c r="T16" s="19"/>
+    </row>
+    <row r="17" spans="1:20" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A17" s="19"/>
+      <c r="B17" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="18">
+        <f>SUM(C14:E14,F13:N13)</f>
+        <v>5992686</v>
+      </c>
+      <c r="G17" s="18"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
+      <c r="T17" s="19"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="19"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="19"/>
+      <c r="S18" s="19"/>
+      <c r="T18" s="19"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="19"/>
+      <c r="T19" s="19"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="19"/>
+      <c r="Q20" s="19"/>
+      <c r="R20" s="19"/>
+      <c r="S20" s="19"/>
+      <c r="T20" s="19"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="19"/>
+      <c r="S21" s="19"/>
+      <c r="T21" s="19"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="19"/>
+      <c r="Q22" s="19"/>
+      <c r="R22" s="19"/>
+      <c r="S22" s="19"/>
+      <c r="T22" s="19"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="19"/>
+      <c r="Q23" s="19"/>
+      <c r="R23" s="19"/>
+      <c r="S23" s="19"/>
+      <c r="T23" s="19"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="19"/>
+      <c r="P24" s="19"/>
+      <c r="Q24" s="19"/>
+      <c r="R24" s="19"/>
+      <c r="S24" s="19"/>
+      <c r="T24" s="19"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="19"/>
+      <c r="Q25" s="19"/>
+      <c r="R25" s="19"/>
+      <c r="S25" s="19"/>
+      <c r="T25" s="19"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="19"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="19"/>
+      <c r="T26" s="19"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="19"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="19"/>
+      <c r="T27" s="19"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="19"/>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="19"/>
+      <c r="S28" s="19"/>
+      <c r="T28" s="19"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="19"/>
+      <c r="Q29" s="19"/>
+      <c r="R29" s="19"/>
+      <c r="S29" s="19"/>
+      <c r="T29" s="19"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" s="19"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="19"/>
+      <c r="Q30" s="19"/>
+      <c r="R30" s="19"/>
+      <c r="S30" s="19"/>
+      <c r="T30" s="19"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" s="19"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="19"/>
+      <c r="Q31" s="19"/>
+      <c r="R31" s="19"/>
+      <c r="S31" s="19"/>
+      <c r="T31" s="19"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" s="19"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="19"/>
+      <c r="P32" s="19"/>
+      <c r="Q32" s="19"/>
+      <c r="R32" s="19"/>
+      <c r="S32" s="19"/>
+      <c r="T32" s="19"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A33" s="19"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="19"/>
+      <c r="O33" s="19"/>
+      <c r="P33" s="19"/>
+      <c r="Q33" s="19"/>
+      <c r="R33" s="19"/>
+      <c r="S33" s="19"/>
+      <c r="T33" s="19"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34" s="19"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+      <c r="O34" s="19"/>
+      <c r="P34" s="19"/>
+      <c r="Q34" s="19"/>
+      <c r="R34" s="19"/>
+      <c r="S34" s="19"/>
+      <c r="T34" s="19"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35" s="19"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="19"/>
+      <c r="O35" s="19"/>
+      <c r="P35" s="19"/>
+      <c r="Q35" s="19"/>
+      <c r="R35" s="19"/>
+      <c r="S35" s="19"/>
+      <c r="T35" s="19"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A36" s="19"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="19"/>
+      <c r="N36" s="19"/>
+      <c r="O36" s="19"/>
+      <c r="P36" s="19"/>
+      <c r="Q36" s="19"/>
+      <c r="R36" s="19"/>
+      <c r="S36" s="19"/>
+      <c r="T36" s="19"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A37" s="19"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
+      <c r="L37" s="19"/>
+      <c r="M37" s="19"/>
+      <c r="N37" s="19"/>
+      <c r="O37" s="19"/>
+      <c r="P37" s="19"/>
+      <c r="Q37" s="19"/>
+      <c r="R37" s="19"/>
+      <c r="S37" s="19"/>
+      <c r="T37" s="19"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A38" s="19"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="19"/>
+      <c r="L38" s="19"/>
+      <c r="M38" s="19"/>
+      <c r="N38" s="19"/>
+      <c r="O38" s="19"/>
+      <c r="P38" s="19"/>
+      <c r="Q38" s="19"/>
+      <c r="R38" s="19"/>
+      <c r="S38" s="19"/>
+      <c r="T38" s="19"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39" s="19"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="19"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="19"/>
+      <c r="O39" s="19"/>
+      <c r="P39" s="19"/>
+      <c r="Q39" s="19"/>
+      <c r="R39" s="19"/>
+      <c r="S39" s="19"/>
+      <c r="T39" s="19"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40" s="19"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
+      <c r="L40" s="19"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="19"/>
+      <c r="O40" s="19"/>
+      <c r="P40" s="19"/>
+      <c r="Q40" s="19"/>
+      <c r="R40" s="19"/>
+      <c r="S40" s="19"/>
+      <c r="T40" s="19"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41" s="19"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
+      <c r="L41" s="19"/>
+      <c r="M41" s="19"/>
+      <c r="N41" s="19"/>
+      <c r="O41" s="19"/>
+      <c r="P41" s="19"/>
+      <c r="Q41" s="19"/>
+      <c r="R41" s="19"/>
+      <c r="S41" s="19"/>
+      <c r="T41" s="19"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42" s="19"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="19"/>
+      <c r="M42" s="19"/>
+      <c r="N42" s="19"/>
+      <c r="O42" s="19"/>
+      <c r="P42" s="19"/>
+      <c r="Q42" s="19"/>
+      <c r="R42" s="19"/>
+      <c r="S42" s="19"/>
+      <c r="T42" s="19"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A43" s="19"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="19"/>
+      <c r="L43" s="19"/>
+      <c r="M43" s="19"/>
+      <c r="N43" s="19"/>
+      <c r="O43" s="19"/>
+      <c r="P43" s="19"/>
+      <c r="Q43" s="19"/>
+      <c r="R43" s="19"/>
+      <c r="S43" s="19"/>
+      <c r="T43" s="19"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A44" s="19"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="19"/>
+      <c r="K44" s="19"/>
+      <c r="L44" s="19"/>
+      <c r="M44" s="19"/>
+      <c r="N44" s="19"/>
+      <c r="O44" s="19"/>
+      <c r="P44" s="19"/>
+      <c r="Q44" s="19"/>
+      <c r="R44" s="19"/>
+      <c r="S44" s="19"/>
+      <c r="T44" s="19"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A45" s="19"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="19"/>
+      <c r="I45" s="19"/>
+      <c r="J45" s="19"/>
+      <c r="K45" s="19"/>
+      <c r="L45" s="19"/>
+      <c r="M45" s="19"/>
+      <c r="N45" s="19"/>
+      <c r="O45" s="19"/>
+      <c r="P45" s="19"/>
+      <c r="Q45" s="19"/>
+      <c r="R45" s="19"/>
+      <c r="S45" s="19"/>
+      <c r="T45" s="19"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A46" s="19"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="19"/>
+      <c r="I46" s="19"/>
+      <c r="J46" s="19"/>
+      <c r="K46" s="19"/>
+      <c r="L46" s="21"/>
+      <c r="M46" s="19"/>
+      <c r="N46" s="19"/>
+      <c r="O46" s="19"/>
+      <c r="P46" s="19"/>
+      <c r="Q46" s="19"/>
+      <c r="R46" s="19"/>
+      <c r="S46" s="19"/>
+      <c r="T46" s="19"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A47" s="19"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="19"/>
+      <c r="I47" s="19"/>
+      <c r="J47" s="19"/>
+      <c r="K47" s="19"/>
+      <c r="L47" s="19"/>
+      <c r="M47" s="19"/>
+      <c r="N47" s="19"/>
+      <c r="O47" s="19"/>
+      <c r="P47" s="19"/>
+      <c r="Q47" s="19"/>
+      <c r="R47" s="19"/>
+      <c r="S47" s="19"/>
+      <c r="T47" s="19"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A48" s="19"/>
+      <c r="B48" s="19"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="19"/>
+      <c r="I48" s="19"/>
+      <c r="J48" s="19"/>
+      <c r="K48" s="19"/>
+      <c r="L48" s="19"/>
+      <c r="M48" s="19"/>
+      <c r="N48" s="19"/>
+      <c r="O48" s="19"/>
+      <c r="P48" s="19"/>
+      <c r="Q48" s="19"/>
+      <c r="R48" s="19"/>
+      <c r="S48" s="19"/>
+      <c r="T48" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="B15:O15"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="B17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="P5:P14" formulaRange="1"/>
+    <ignoredError sqref="P5:P14 F17" formulaRange="1"/>
     <ignoredError sqref="P4" calculatedColumn="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Blog Statistics (April 2017)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20487" windowHeight="8941"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -266,36 +266,28 @@
     </xf>
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="18">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -308,6 +300,14 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -938,7 +938,7 @@
                   <c:v>4530257</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7500248</c:v>
+                  <c:v>7644813</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1207,8 +1207,8 @@
               <c:idx val="9"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-6.1786881477446528E-4"/>
-                  <c:y val="-0.36667675447083081"/>
+                  <c:x val="-6.1783031451233283E-4"/>
+                  <c:y val="-0.17811295029660074"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -1425,7 +1425,7 @@
                   <c:v>4530257</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1875062</c:v>
+                  <c:v>2548271</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2130,8 +2130,8 @@
     <tableColumn id="15" name="Column15" dataDxfId="2">
       <calculatedColumnFormula>SUM(C4:N4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Column152" dataDxfId="0" dataCellStyle="Normal"/>
-    <tableColumn id="16" name="Column16" dataDxfId="1">
+    <tableColumn id="17" name="Column152" dataDxfId="1" dataCellStyle="Normal"/>
+    <tableColumn id="16" name="Column16" dataDxfId="0">
       <calculatedColumnFormula>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2463,66 +2463,66 @@
   <dimension ref="A1:T48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="T38" sqref="T38"/>
+      <selection activeCell="U25" sqref="U25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" customWidth="1"/>
-    <col min="3" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" customWidth="1"/>
+    <col min="3" max="14" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="4" customWidth="1"/>
-    <col min="16" max="16" width="18.28515625" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" customWidth="1"/>
-    <col min="18" max="18" width="25.42578125" customWidth="1"/>
+    <col min="16" max="16" width="18.33203125" customWidth="1"/>
+    <col min="17" max="17" width="5.33203125" customWidth="1"/>
+    <col min="18" max="18" width="25.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="19"/>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-    </row>
-    <row r="3" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A1" s="15"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+    </row>
+    <row r="3" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="15"/>
       <c r="B3" t="s">
         <v>13</v>
       </c>
@@ -2568,15 +2568,15 @@
       <c r="P3" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" s="15" t="s">
+      <c r="Q3" s="13" t="s">
         <v>29</v>
       </c>
       <c r="R3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="19"/>
+    <row r="4" spans="1:20" ht="20.3" x14ac:dyDescent="0.35">
+      <c r="A4" s="15"/>
       <c r="B4" s="1"/>
       <c r="C4" s="2" t="s">
         <v>0</v>
@@ -2618,16 +2618,16 @@
       <c r="P4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="Q4" s="15"/>
+      <c r="Q4" s="13"/>
       <c r="R4" s="12" t="e">
         <f>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="S4" s="19"/>
-      <c r="T4" s="19"/>
-    </row>
-    <row r="5" spans="1:20" ht="21" x14ac:dyDescent="0.35">
-      <c r="A5" s="19"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+    </row>
+    <row r="5" spans="1:20" ht="20.3" x14ac:dyDescent="0.35">
+      <c r="A5" s="15"/>
       <c r="B5" s="4">
         <v>2008</v>
       </c>
@@ -2654,16 +2654,16 @@
         <f>SUM(C5:N5)</f>
         <v>326</v>
       </c>
-      <c r="Q5" s="15"/>
+      <c r="Q5" s="13"/>
       <c r="R5" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>326</v>
       </c>
-      <c r="S5" s="19"/>
-      <c r="T5" s="19"/>
-    </row>
-    <row r="6" spans="1:20" ht="21" x14ac:dyDescent="0.35">
-      <c r="A6" s="19"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
+    </row>
+    <row r="6" spans="1:20" ht="20.3" x14ac:dyDescent="0.35">
+      <c r="A6" s="15"/>
       <c r="B6" s="4">
         <v>2009</v>
       </c>
@@ -2708,16 +2708,16 @@
         <f t="shared" ref="P6:P12" si="0">SUM(C6:N6)</f>
         <v>80379</v>
       </c>
-      <c r="Q6" s="15"/>
+      <c r="Q6" s="13"/>
       <c r="R6" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>80379</v>
       </c>
-      <c r="S6" s="19"/>
-      <c r="T6" s="19"/>
-    </row>
-    <row r="7" spans="1:20" ht="21" x14ac:dyDescent="0.35">
-      <c r="A7" s="19"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+    </row>
+    <row r="7" spans="1:20" ht="20.3" x14ac:dyDescent="0.35">
+      <c r="A7" s="15"/>
       <c r="B7" s="4">
         <v>2010</v>
       </c>
@@ -2762,16 +2762,16 @@
         <f t="shared" si="0"/>
         <v>463113</v>
       </c>
-      <c r="Q7" s="15"/>
+      <c r="Q7" s="13"/>
       <c r="R7" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>463113</v>
       </c>
-      <c r="S7" s="19"/>
-      <c r="T7" s="19"/>
-    </row>
-    <row r="8" spans="1:20" ht="21" x14ac:dyDescent="0.35">
-      <c r="A8" s="19"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
+    </row>
+    <row r="8" spans="1:20" ht="20.3" x14ac:dyDescent="0.35">
+      <c r="A8" s="15"/>
       <c r="B8" s="4">
         <v>2011</v>
       </c>
@@ -2816,16 +2816,16 @@
         <f t="shared" si="0"/>
         <v>803010</v>
       </c>
-      <c r="Q8" s="15"/>
+      <c r="Q8" s="13"/>
       <c r="R8" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>803010</v>
       </c>
-      <c r="S8" s="19"/>
-      <c r="T8" s="19"/>
-    </row>
-    <row r="9" spans="1:20" ht="21" x14ac:dyDescent="0.35">
-      <c r="A9" s="19"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="15"/>
+    </row>
+    <row r="9" spans="1:20" ht="20.3" x14ac:dyDescent="0.35">
+      <c r="A9" s="15"/>
       <c r="B9" s="4">
         <v>2012</v>
       </c>
@@ -2870,16 +2870,16 @@
         <f t="shared" si="0"/>
         <v>888853</v>
       </c>
-      <c r="Q9" s="15"/>
+      <c r="Q9" s="13"/>
       <c r="R9" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>888853</v>
       </c>
-      <c r="S9" s="19"/>
-      <c r="T9" s="19"/>
-    </row>
-    <row r="10" spans="1:20" ht="21" x14ac:dyDescent="0.35">
-      <c r="A10" s="19"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+    </row>
+    <row r="10" spans="1:20" ht="20.3" x14ac:dyDescent="0.35">
+      <c r="A10" s="15"/>
       <c r="B10" s="4">
         <v>2013</v>
       </c>
@@ -2924,16 +2924,16 @@
         <f t="shared" si="0"/>
         <v>935657</v>
       </c>
-      <c r="Q10" s="15"/>
+      <c r="Q10" s="13"/>
       <c r="R10" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>935657</v>
       </c>
-      <c r="S10" s="19"/>
-      <c r="T10" s="19"/>
-    </row>
-    <row r="11" spans="1:20" ht="21" x14ac:dyDescent="0.35">
-      <c r="A11" s="19"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+    </row>
+    <row r="11" spans="1:20" ht="20.3" x14ac:dyDescent="0.35">
+      <c r="A11" s="15"/>
       <c r="B11" s="4">
         <v>2014</v>
       </c>
@@ -2978,16 +2978,16 @@
         <f t="shared" si="0"/>
         <v>938639</v>
       </c>
-      <c r="Q11" s="15"/>
+      <c r="Q11" s="13"/>
       <c r="R11" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>938639</v>
       </c>
-      <c r="S11" s="19"/>
-      <c r="T11" s="19"/>
-    </row>
-    <row r="12" spans="1:20" ht="21" x14ac:dyDescent="0.35">
-      <c r="A12" s="19"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+    </row>
+    <row r="12" spans="1:20" ht="20.3" x14ac:dyDescent="0.35">
+      <c r="A12" s="15"/>
       <c r="B12" s="4">
         <v>2015</v>
       </c>
@@ -3032,16 +3032,16 @@
         <f t="shared" si="0"/>
         <v>1217957</v>
       </c>
-      <c r="Q12" s="15"/>
+      <c r="Q12" s="13"/>
       <c r="R12" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>1217957</v>
       </c>
-      <c r="S12" s="19"/>
-      <c r="T12" s="19"/>
-    </row>
-    <row r="13" spans="1:20" ht="21" x14ac:dyDescent="0.35">
-      <c r="A13" s="19"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
+    </row>
+    <row r="13" spans="1:20" ht="20.3" x14ac:dyDescent="0.35">
+      <c r="A13" s="15"/>
       <c r="B13" s="4">
         <v>2016</v>
       </c>
@@ -3086,16 +3086,16 @@
         <f>SUM(C13:N13)</f>
         <v>4530257</v>
       </c>
-      <c r="Q13" s="15"/>
+      <c r="Q13" s="13"/>
       <c r="R13" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>4530257</v>
       </c>
-      <c r="S13" s="19"/>
-      <c r="T13" s="19"/>
-    </row>
-    <row r="14" spans="1:20" ht="21" x14ac:dyDescent="0.35">
-      <c r="A14" s="19"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
+    </row>
+    <row r="14" spans="1:20" ht="20.3" x14ac:dyDescent="0.35">
+      <c r="A14" s="15"/>
       <c r="B14" s="9">
         <v>2017</v>
       </c>
@@ -3108,7 +3108,9 @@
       <c r="E14" s="8">
         <v>657797</v>
       </c>
-      <c r="F14" s="10"/>
+      <c r="F14" s="8">
+        <v>673209</v>
+      </c>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
@@ -3120,770 +3122,770 @@
       <c r="O14" s="11"/>
       <c r="P14" s="11">
         <f>SUM(C14:N14)</f>
-        <v>1875062</v>
-      </c>
-      <c r="Q14" s="15"/>
+        <v>2548271</v>
+      </c>
+      <c r="Q14" s="13"/>
       <c r="R14" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>7500248</v>
-      </c>
-      <c r="S14" s="19"/>
-      <c r="T14" s="19"/>
-    </row>
-    <row r="15" spans="1:20" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="19"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="20">
+        <v>7644813</v>
+      </c>
+      <c r="S14" s="15"/>
+      <c r="T14" s="15"/>
+    </row>
+    <row r="15" spans="1:20" ht="20.3" x14ac:dyDescent="0.35">
+      <c r="A15" s="15"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="16">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>11733253</v>
-      </c>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="19"/>
-      <c r="S15" s="19"/>
-      <c r="T15" s="19"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
-      <c r="N16" s="16"/>
-      <c r="O16" s="16"/>
-      <c r="P16" s="16"/>
-      <c r="Q16" s="19"/>
-      <c r="R16" s="19"/>
-      <c r="S16" s="19"/>
-      <c r="T16" s="19"/>
-    </row>
-    <row r="17" spans="1:20" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A17" s="19"/>
-      <c r="B17" s="17" t="s">
+        <v>12406462</v>
+      </c>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="15"/>
+      <c r="T15" s="15"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
+    </row>
+    <row r="17" spans="1:20" ht="24.25" x14ac:dyDescent="0.45">
+      <c r="A17" s="15"/>
+      <c r="B17" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="18">
-        <f>SUM(C14:E14,F13:N13)</f>
-        <v>5992686</v>
-      </c>
-      <c r="G17" s="18"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="19"/>
-      <c r="R17" s="19"/>
-      <c r="S17" s="19"/>
-      <c r="T17" s="19"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="19"/>
-      <c r="R18" s="19"/>
-      <c r="S18" s="19"/>
-      <c r="T18" s="19"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19"/>
-      <c r="O19" s="19"/>
-      <c r="P19" s="19"/>
-      <c r="Q19" s="19"/>
-      <c r="R19" s="19"/>
-      <c r="S19" s="19"/>
-      <c r="T19" s="19"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
-      <c r="N20" s="19"/>
-      <c r="O20" s="19"/>
-      <c r="P20" s="19"/>
-      <c r="Q20" s="19"/>
-      <c r="R20" s="19"/>
-      <c r="S20" s="19"/>
-      <c r="T20" s="19"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="19"/>
-      <c r="O21" s="19"/>
-      <c r="P21" s="19"/>
-      <c r="Q21" s="19"/>
-      <c r="R21" s="19"/>
-      <c r="S21" s="19"/>
-      <c r="T21" s="19"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="19"/>
-      <c r="O22" s="19"/>
-      <c r="P22" s="19"/>
-      <c r="Q22" s="19"/>
-      <c r="R22" s="19"/>
-      <c r="S22" s="19"/>
-      <c r="T22" s="19"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="19"/>
-      <c r="O23" s="19"/>
-      <c r="P23" s="19"/>
-      <c r="Q23" s="19"/>
-      <c r="R23" s="19"/>
-      <c r="S23" s="19"/>
-      <c r="T23" s="19"/>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19"/>
-      <c r="M24" s="19"/>
-      <c r="N24" s="19"/>
-      <c r="O24" s="19"/>
-      <c r="P24" s="19"/>
-      <c r="Q24" s="19"/>
-      <c r="R24" s="19"/>
-      <c r="S24" s="19"/>
-      <c r="T24" s="19"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="19"/>
-      <c r="N25" s="19"/>
-      <c r="O25" s="19"/>
-      <c r="P25" s="19"/>
-      <c r="Q25" s="19"/>
-      <c r="R25" s="19"/>
-      <c r="S25" s="19"/>
-      <c r="T25" s="19"/>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19"/>
-      <c r="M26" s="19"/>
-      <c r="N26" s="19"/>
-      <c r="O26" s="19"/>
-      <c r="P26" s="19"/>
-      <c r="Q26" s="19"/>
-      <c r="R26" s="19"/>
-      <c r="S26" s="19"/>
-      <c r="T26" s="19"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="19"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19"/>
-      <c r="K27" s="19"/>
-      <c r="L27" s="19"/>
-      <c r="M27" s="19"/>
-      <c r="N27" s="19"/>
-      <c r="O27" s="19"/>
-      <c r="P27" s="19"/>
-      <c r="Q27" s="19"/>
-      <c r="R27" s="19"/>
-      <c r="S27" s="19"/>
-      <c r="T27" s="19"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="19"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
-      <c r="L28" s="19"/>
-      <c r="M28" s="19"/>
-      <c r="N28" s="19"/>
-      <c r="O28" s="19"/>
-      <c r="P28" s="19"/>
-      <c r="Q28" s="19"/>
-      <c r="R28" s="19"/>
-      <c r="S28" s="19"/>
-      <c r="T28" s="19"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="19"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="19"/>
-      <c r="L29" s="19"/>
-      <c r="M29" s="19"/>
-      <c r="N29" s="19"/>
-      <c r="O29" s="19"/>
-      <c r="P29" s="19"/>
-      <c r="Q29" s="19"/>
-      <c r="R29" s="19"/>
-      <c r="S29" s="19"/>
-      <c r="T29" s="19"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="19"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19"/>
-      <c r="M30" s="19"/>
-      <c r="N30" s="19"/>
-      <c r="O30" s="19"/>
-      <c r="P30" s="19"/>
-      <c r="Q30" s="19"/>
-      <c r="R30" s="19"/>
-      <c r="S30" s="19"/>
-      <c r="T30" s="19"/>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" s="19"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="19"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="19"/>
-      <c r="O31" s="19"/>
-      <c r="P31" s="19"/>
-      <c r="Q31" s="19"/>
-      <c r="R31" s="19"/>
-      <c r="S31" s="19"/>
-      <c r="T31" s="19"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A32" s="19"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="19"/>
-      <c r="O32" s="19"/>
-      <c r="P32" s="19"/>
-      <c r="Q32" s="19"/>
-      <c r="R32" s="19"/>
-      <c r="S32" s="19"/>
-      <c r="T32" s="19"/>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
-      <c r="L33" s="19"/>
-      <c r="M33" s="19"/>
-      <c r="N33" s="19"/>
-      <c r="O33" s="19"/>
-      <c r="P33" s="19"/>
-      <c r="Q33" s="19"/>
-      <c r="R33" s="19"/>
-      <c r="S33" s="19"/>
-      <c r="T33" s="19"/>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A34" s="19"/>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="19"/>
-      <c r="N34" s="19"/>
-      <c r="O34" s="19"/>
-      <c r="P34" s="19"/>
-      <c r="Q34" s="19"/>
-      <c r="R34" s="19"/>
-      <c r="S34" s="19"/>
-      <c r="T34" s="19"/>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A35" s="19"/>
-      <c r="B35" s="19"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="19"/>
-      <c r="L35" s="19"/>
-      <c r="M35" s="19"/>
-      <c r="N35" s="19"/>
-      <c r="O35" s="19"/>
-      <c r="P35" s="19"/>
-      <c r="Q35" s="19"/>
-      <c r="R35" s="19"/>
-      <c r="S35" s="19"/>
-      <c r="T35" s="19"/>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A36" s="19"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
-      <c r="L36" s="19"/>
-      <c r="M36" s="19"/>
-      <c r="N36" s="19"/>
-      <c r="O36" s="19"/>
-      <c r="P36" s="19"/>
-      <c r="Q36" s="19"/>
-      <c r="R36" s="19"/>
-      <c r="S36" s="19"/>
-      <c r="T36" s="19"/>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A37" s="19"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="19"/>
-      <c r="I37" s="19"/>
-      <c r="J37" s="19"/>
-      <c r="K37" s="19"/>
-      <c r="L37" s="19"/>
-      <c r="M37" s="19"/>
-      <c r="N37" s="19"/>
-      <c r="O37" s="19"/>
-      <c r="P37" s="19"/>
-      <c r="Q37" s="19"/>
-      <c r="R37" s="19"/>
-      <c r="S37" s="19"/>
-      <c r="T37" s="19"/>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A38" s="19"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="19"/>
-      <c r="J38" s="19"/>
-      <c r="K38" s="19"/>
-      <c r="L38" s="19"/>
-      <c r="M38" s="19"/>
-      <c r="N38" s="19"/>
-      <c r="O38" s="19"/>
-      <c r="P38" s="19"/>
-      <c r="Q38" s="19"/>
-      <c r="R38" s="19"/>
-      <c r="S38" s="19"/>
-      <c r="T38" s="19"/>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="19"/>
-      <c r="I39" s="19"/>
-      <c r="J39" s="19"/>
-      <c r="K39" s="19"/>
-      <c r="L39" s="19"/>
-      <c r="M39" s="19"/>
-      <c r="N39" s="19"/>
-      <c r="O39" s="19"/>
-      <c r="P39" s="19"/>
-      <c r="Q39" s="19"/>
-      <c r="R39" s="19"/>
-      <c r="S39" s="19"/>
-      <c r="T39" s="19"/>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A40" s="19"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="19"/>
-      <c r="H40" s="19"/>
-      <c r="I40" s="19"/>
-      <c r="J40" s="19"/>
-      <c r="K40" s="19"/>
-      <c r="L40" s="19"/>
-      <c r="M40" s="19"/>
-      <c r="N40" s="19"/>
-      <c r="O40" s="19"/>
-      <c r="P40" s="19"/>
-      <c r="Q40" s="19"/>
-      <c r="R40" s="19"/>
-      <c r="S40" s="19"/>
-      <c r="T40" s="19"/>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A41" s="19"/>
-      <c r="B41" s="19"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="19"/>
-      <c r="H41" s="19"/>
-      <c r="I41" s="19"/>
-      <c r="J41" s="19"/>
-      <c r="K41" s="19"/>
-      <c r="L41" s="19"/>
-      <c r="M41" s="19"/>
-      <c r="N41" s="19"/>
-      <c r="O41" s="19"/>
-      <c r="P41" s="19"/>
-      <c r="Q41" s="19"/>
-      <c r="R41" s="19"/>
-      <c r="S41" s="19"/>
-      <c r="T41" s="19"/>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A42" s="19"/>
-      <c r="B42" s="19"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="19"/>
-      <c r="J42" s="19"/>
-      <c r="K42" s="19"/>
-      <c r="L42" s="19"/>
-      <c r="M42" s="19"/>
-      <c r="N42" s="19"/>
-      <c r="O42" s="19"/>
-      <c r="P42" s="19"/>
-      <c r="Q42" s="19"/>
-      <c r="R42" s="19"/>
-      <c r="S42" s="19"/>
-      <c r="T42" s="19"/>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A43" s="19"/>
-      <c r="B43" s="19"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="19"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="19"/>
-      <c r="J43" s="19"/>
-      <c r="K43" s="19"/>
-      <c r="L43" s="19"/>
-      <c r="M43" s="19"/>
-      <c r="N43" s="19"/>
-      <c r="O43" s="19"/>
-      <c r="P43" s="19"/>
-      <c r="Q43" s="19"/>
-      <c r="R43" s="19"/>
-      <c r="S43" s="19"/>
-      <c r="T43" s="19"/>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A44" s="19"/>
-      <c r="B44" s="19"/>
-      <c r="C44" s="19"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="19"/>
-      <c r="G44" s="19"/>
-      <c r="H44" s="19"/>
-      <c r="I44" s="19"/>
-      <c r="J44" s="19"/>
-      <c r="K44" s="19"/>
-      <c r="L44" s="19"/>
-      <c r="M44" s="19"/>
-      <c r="N44" s="19"/>
-      <c r="O44" s="19"/>
-      <c r="P44" s="19"/>
-      <c r="Q44" s="19"/>
-      <c r="R44" s="19"/>
-      <c r="S44" s="19"/>
-      <c r="T44" s="19"/>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A45" s="19"/>
-      <c r="B45" s="19"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="19"/>
-      <c r="H45" s="19"/>
-      <c r="I45" s="19"/>
-      <c r="J45" s="19"/>
-      <c r="K45" s="19"/>
-      <c r="L45" s="19"/>
-      <c r="M45" s="19"/>
-      <c r="N45" s="19"/>
-      <c r="O45" s="19"/>
-      <c r="P45" s="19"/>
-      <c r="Q45" s="19"/>
-      <c r="R45" s="19"/>
-      <c r="S45" s="19"/>
-      <c r="T45" s="19"/>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A46" s="19"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="19"/>
-      <c r="G46" s="19"/>
-      <c r="H46" s="19"/>
-      <c r="I46" s="19"/>
-      <c r="J46" s="19"/>
-      <c r="K46" s="19"/>
-      <c r="L46" s="21"/>
-      <c r="M46" s="19"/>
-      <c r="N46" s="19"/>
-      <c r="O46" s="19"/>
-      <c r="P46" s="19"/>
-      <c r="Q46" s="19"/>
-      <c r="R46" s="19"/>
-      <c r="S46" s="19"/>
-      <c r="T46" s="19"/>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A47" s="19"/>
-      <c r="B47" s="19"/>
-      <c r="C47" s="19"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="19"/>
-      <c r="G47" s="19"/>
-      <c r="H47" s="19"/>
-      <c r="I47" s="19"/>
-      <c r="J47" s="19"/>
-      <c r="K47" s="19"/>
-      <c r="L47" s="19"/>
-      <c r="M47" s="19"/>
-      <c r="N47" s="19"/>
-      <c r="O47" s="19"/>
-      <c r="P47" s="19"/>
-      <c r="Q47" s="19"/>
-      <c r="R47" s="19"/>
-      <c r="S47" s="19"/>
-      <c r="T47" s="19"/>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A48" s="19"/>
-      <c r="B48" s="19"/>
-      <c r="C48" s="19"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="19"/>
-      <c r="G48" s="19"/>
-      <c r="H48" s="19"/>
-      <c r="I48" s="19"/>
-      <c r="J48" s="19"/>
-      <c r="K48" s="19"/>
-      <c r="L48" s="19"/>
-      <c r="M48" s="19"/>
-      <c r="N48" s="19"/>
-      <c r="O48" s="19"/>
-      <c r="P48" s="19"/>
-      <c r="Q48" s="19"/>
-      <c r="R48" s="19"/>
-      <c r="S48" s="19"/>
-      <c r="T48" s="19"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="20">
+        <f>SUM(G13:N13,C14:F14)</f>
+        <v>6513283</v>
+      </c>
+      <c r="G17" s="20"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="15"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A18" s="15"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15"/>
+      <c r="S18" s="15"/>
+      <c r="T18" s="15"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="15"/>
+      <c r="S19" s="15"/>
+      <c r="T19" s="15"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
+      <c r="S20" s="15"/>
+      <c r="T20" s="15"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
+      <c r="S21" s="15"/>
+      <c r="T21" s="15"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15"/>
+      <c r="S22" s="15"/>
+      <c r="T22" s="15"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+      <c r="S23" s="15"/>
+      <c r="T23" s="15"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="15"/>
+      <c r="S24" s="15"/>
+      <c r="T24" s="15"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="15"/>
+      <c r="S25" s="15"/>
+      <c r="T25" s="15"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15"/>
+      <c r="R26" s="15"/>
+      <c r="S26" s="15"/>
+      <c r="T26" s="15"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="15"/>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="15"/>
+      <c r="R27" s="15"/>
+      <c r="S27" s="15"/>
+      <c r="T27" s="15"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="15"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="15"/>
+      <c r="R28" s="15"/>
+      <c r="S28" s="15"/>
+      <c r="T28" s="15"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="15"/>
+      <c r="P29" s="15"/>
+      <c r="Q29" s="15"/>
+      <c r="R29" s="15"/>
+      <c r="S29" s="15"/>
+      <c r="T29" s="15"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="15"/>
+      <c r="R30" s="15"/>
+      <c r="S30" s="15"/>
+      <c r="T30" s="15"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="15"/>
+      <c r="R31" s="15"/>
+      <c r="S31" s="15"/>
+      <c r="T31" s="15"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A32" s="15"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
+      <c r="P32" s="15"/>
+      <c r="Q32" s="15"/>
+      <c r="R32" s="15"/>
+      <c r="S32" s="15"/>
+      <c r="T32" s="15"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="15"/>
+      <c r="Q33" s="15"/>
+      <c r="R33" s="15"/>
+      <c r="S33" s="15"/>
+      <c r="T33" s="15"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A34" s="15"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="15"/>
+      <c r="P34" s="15"/>
+      <c r="Q34" s="15"/>
+      <c r="R34" s="15"/>
+      <c r="S34" s="15"/>
+      <c r="T34" s="15"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A35" s="15"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="15"/>
+      <c r="R35" s="15"/>
+      <c r="S35" s="15"/>
+      <c r="T35" s="15"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A36" s="15"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="15"/>
+      <c r="P36" s="15"/>
+      <c r="Q36" s="15"/>
+      <c r="R36" s="15"/>
+      <c r="S36" s="15"/>
+      <c r="T36" s="15"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A37" s="15"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="15"/>
+      <c r="O37" s="15"/>
+      <c r="P37" s="15"/>
+      <c r="Q37" s="15"/>
+      <c r="R37" s="15"/>
+      <c r="S37" s="15"/>
+      <c r="T37" s="15"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A38" s="15"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="15"/>
+      <c r="O38" s="15"/>
+      <c r="P38" s="15"/>
+      <c r="Q38" s="15"/>
+      <c r="R38" s="15"/>
+      <c r="S38" s="15"/>
+      <c r="T38" s="15"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A39" s="15"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="15"/>
+      <c r="K39" s="15"/>
+      <c r="L39" s="15"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="15"/>
+      <c r="O39" s="15"/>
+      <c r="P39" s="15"/>
+      <c r="Q39" s="15"/>
+      <c r="R39" s="15"/>
+      <c r="S39" s="15"/>
+      <c r="T39" s="15"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A40" s="15"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="15"/>
+      <c r="K40" s="15"/>
+      <c r="L40" s="15"/>
+      <c r="M40" s="15"/>
+      <c r="N40" s="15"/>
+      <c r="O40" s="15"/>
+      <c r="P40" s="15"/>
+      <c r="Q40" s="15"/>
+      <c r="R40" s="15"/>
+      <c r="S40" s="15"/>
+      <c r="T40" s="15"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A41" s="15"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="15"/>
+      <c r="K41" s="15"/>
+      <c r="L41" s="15"/>
+      <c r="M41" s="15"/>
+      <c r="N41" s="15"/>
+      <c r="O41" s="15"/>
+      <c r="P41" s="15"/>
+      <c r="Q41" s="15"/>
+      <c r="R41" s="15"/>
+      <c r="S41" s="15"/>
+      <c r="T41" s="15"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A42" s="15"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="15"/>
+      <c r="K42" s="15"/>
+      <c r="L42" s="15"/>
+      <c r="M42" s="15"/>
+      <c r="N42" s="15"/>
+      <c r="O42" s="15"/>
+      <c r="P42" s="15"/>
+      <c r="Q42" s="15"/>
+      <c r="R42" s="15"/>
+      <c r="S42" s="15"/>
+      <c r="T42" s="15"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A43" s="15"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="15"/>
+      <c r="K43" s="15"/>
+      <c r="L43" s="15"/>
+      <c r="M43" s="15"/>
+      <c r="N43" s="15"/>
+      <c r="O43" s="15"/>
+      <c r="P43" s="15"/>
+      <c r="Q43" s="15"/>
+      <c r="R43" s="15"/>
+      <c r="S43" s="15"/>
+      <c r="T43" s="15"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A44" s="15"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="15"/>
+      <c r="K44" s="15"/>
+      <c r="L44" s="15"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="15"/>
+      <c r="O44" s="15"/>
+      <c r="P44" s="15"/>
+      <c r="Q44" s="15"/>
+      <c r="R44" s="15"/>
+      <c r="S44" s="15"/>
+      <c r="T44" s="15"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A45" s="15"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="15"/>
+      <c r="J45" s="15"/>
+      <c r="K45" s="15"/>
+      <c r="L45" s="15"/>
+      <c r="M45" s="15"/>
+      <c r="N45" s="15"/>
+      <c r="O45" s="15"/>
+      <c r="P45" s="15"/>
+      <c r="Q45" s="15"/>
+      <c r="R45" s="15"/>
+      <c r="S45" s="15"/>
+      <c r="T45" s="15"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A46" s="15"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="15"/>
+      <c r="J46" s="15"/>
+      <c r="K46" s="15"/>
+      <c r="L46" s="17"/>
+      <c r="M46" s="15"/>
+      <c r="N46" s="15"/>
+      <c r="O46" s="15"/>
+      <c r="P46" s="15"/>
+      <c r="Q46" s="15"/>
+      <c r="R46" s="15"/>
+      <c r="S46" s="15"/>
+      <c r="T46" s="15"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A47" s="15"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="15"/>
+      <c r="K47" s="15"/>
+      <c r="L47" s="15"/>
+      <c r="M47" s="15"/>
+      <c r="N47" s="15"/>
+      <c r="O47" s="15"/>
+      <c r="P47" s="15"/>
+      <c r="Q47" s="15"/>
+      <c r="R47" s="15"/>
+      <c r="S47" s="15"/>
+      <c r="T47" s="15"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A48" s="15"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="15"/>
+      <c r="H48" s="15"/>
+      <c r="I48" s="15"/>
+      <c r="J48" s="15"/>
+      <c r="K48" s="15"/>
+      <c r="L48" s="15"/>
+      <c r="M48" s="15"/>
+      <c r="N48" s="15"/>
+      <c r="O48" s="15"/>
+      <c r="P48" s="15"/>
+      <c r="Q48" s="15"/>
+      <c r="R48" s="15"/>
+      <c r="S48" s="15"/>
+      <c r="T48" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Blog Statistics (May 2017)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20487" windowHeight="8941"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20486" windowHeight="8939"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -938,7 +938,7 @@
                   <c:v>4530257</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7644813</c:v>
+                  <c:v>7905146.4000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1425,7 +1425,7 @@
                   <c:v>4530257</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2548271</c:v>
+                  <c:v>3293811</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2462,22 +2462,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="U25" sqref="U25"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" customWidth="1"/>
-    <col min="3" max="14" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="14" width="12.5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="4" customWidth="1"/>
-    <col min="16" max="16" width="18.33203125" customWidth="1"/>
-    <col min="17" max="17" width="5.33203125" customWidth="1"/>
-    <col min="18" max="18" width="25.44140625" customWidth="1"/>
+    <col min="16" max="16" width="18.375" customWidth="1"/>
+    <col min="17" max="17" width="5.375" customWidth="1"/>
+    <col min="18" max="18" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="15"/>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -2499,7 +2499,7 @@
       <c r="S1" s="15"/>
       <c r="T1" s="15"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -2521,7 +2521,7 @@
       <c r="S2" s="15"/>
       <c r="T2" s="15"/>
     </row>
-    <row r="3" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15"/>
       <c r="B3" t="s">
         <v>13</v>
@@ -2575,7 +2575,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="20.3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
       <c r="A4" s="15"/>
       <c r="B4" s="1"/>
       <c r="C4" s="2" t="s">
@@ -2626,7 +2626,7 @@
       <c r="S4" s="15"/>
       <c r="T4" s="15"/>
     </row>
-    <row r="5" spans="1:20" ht="20.3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
       <c r="A5" s="15"/>
       <c r="B5" s="4">
         <v>2008</v>
@@ -2662,7 +2662,7 @@
       <c r="S5" s="15"/>
       <c r="T5" s="15"/>
     </row>
-    <row r="6" spans="1:20" ht="20.3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
       <c r="A6" s="15"/>
       <c r="B6" s="4">
         <v>2009</v>
@@ -2716,7 +2716,7 @@
       <c r="S6" s="15"/>
       <c r="T6" s="15"/>
     </row>
-    <row r="7" spans="1:20" ht="20.3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
       <c r="A7" s="15"/>
       <c r="B7" s="4">
         <v>2010</v>
@@ -2770,7 +2770,7 @@
       <c r="S7" s="15"/>
       <c r="T7" s="15"/>
     </row>
-    <row r="8" spans="1:20" ht="20.3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
       <c r="A8" s="15"/>
       <c r="B8" s="4">
         <v>2011</v>
@@ -2824,7 +2824,7 @@
       <c r="S8" s="15"/>
       <c r="T8" s="15"/>
     </row>
-    <row r="9" spans="1:20" ht="20.3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
       <c r="A9" s="15"/>
       <c r="B9" s="4">
         <v>2012</v>
@@ -2878,7 +2878,7 @@
       <c r="S9" s="15"/>
       <c r="T9" s="15"/>
     </row>
-    <row r="10" spans="1:20" ht="20.3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
       <c r="A10" s="15"/>
       <c r="B10" s="4">
         <v>2013</v>
@@ -2932,7 +2932,7 @@
       <c r="S10" s="15"/>
       <c r="T10" s="15"/>
     </row>
-    <row r="11" spans="1:20" ht="20.3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
       <c r="A11" s="15"/>
       <c r="B11" s="4">
         <v>2014</v>
@@ -2986,7 +2986,7 @@
       <c r="S11" s="15"/>
       <c r="T11" s="15"/>
     </row>
-    <row r="12" spans="1:20" ht="20.3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
       <c r="A12" s="15"/>
       <c r="B12" s="4">
         <v>2015</v>
@@ -3040,7 +3040,7 @@
       <c r="S12" s="15"/>
       <c r="T12" s="15"/>
     </row>
-    <row r="13" spans="1:20" ht="20.3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
       <c r="A13" s="15"/>
       <c r="B13" s="4">
         <v>2016</v>
@@ -3094,7 +3094,7 @@
       <c r="S13" s="15"/>
       <c r="T13" s="15"/>
     </row>
-    <row r="14" spans="1:20" ht="20.3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
       <c r="A14" s="15"/>
       <c r="B14" s="9">
         <v>2017</v>
@@ -3111,7 +3111,9 @@
       <c r="F14" s="8">
         <v>673209</v>
       </c>
-      <c r="G14" s="10"/>
+      <c r="G14" s="8">
+        <v>745540</v>
+      </c>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
@@ -3122,17 +3124,17 @@
       <c r="O14" s="11"/>
       <c r="P14" s="11">
         <f>SUM(C14:N14)</f>
-        <v>2548271</v>
+        <v>3293811</v>
       </c>
       <c r="Q14" s="13"/>
       <c r="R14" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>7644813</v>
+        <v>7905146.4000000004</v>
       </c>
       <c r="S14" s="15"/>
       <c r="T14" s="15"/>
     </row>
-    <row r="15" spans="1:20" ht="20.3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
       <c r="A15" s="15"/>
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
@@ -3150,14 +3152,14 @@
       <c r="O15" s="19"/>
       <c r="P15" s="16">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>12406462</v>
+        <v>13152002</v>
       </c>
       <c r="Q15" s="13"/>
       <c r="R15" s="15"/>
       <c r="S15" s="15"/>
       <c r="T15" s="15"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
@@ -3178,7 +3180,7 @@
       <c r="S16" s="15"/>
       <c r="T16" s="15"/>
     </row>
-    <row r="17" spans="1:20" ht="24.25" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:20" ht="23.8" x14ac:dyDescent="0.4">
       <c r="A17" s="15"/>
       <c r="B17" s="21" t="s">
         <v>30</v>
@@ -3187,8 +3189,7 @@
       <c r="D17" s="21"/>
       <c r="E17" s="21"/>
       <c r="F17" s="20">
-        <f>SUM(G13:N13,C14:F14)</f>
-        <v>6513283</v>
+        <v>7124326</v>
       </c>
       <c r="G17" s="20"/>
       <c r="H17" s="13"/>
@@ -3205,7 +3206,7 @@
       <c r="S17" s="15"/>
       <c r="T17" s="15"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
@@ -3227,7 +3228,7 @@
       <c r="S18" s="15"/>
       <c r="T18" s="15"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
@@ -3249,7 +3250,7 @@
       <c r="S19" s="15"/>
       <c r="T19" s="15"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
@@ -3271,7 +3272,7 @@
       <c r="S20" s="15"/>
       <c r="T20" s="15"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
@@ -3293,7 +3294,7 @@
       <c r="S21" s="15"/>
       <c r="T21" s="15"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
@@ -3315,7 +3316,7 @@
       <c r="S22" s="15"/>
       <c r="T22" s="15"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
@@ -3337,7 +3338,7 @@
       <c r="S23" s="15"/>
       <c r="T23" s="15"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
@@ -3359,7 +3360,7 @@
       <c r="S24" s="15"/>
       <c r="T24" s="15"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
@@ -3381,7 +3382,7 @@
       <c r="S25" s="15"/>
       <c r="T25" s="15"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
@@ -3403,7 +3404,7 @@
       <c r="S26" s="15"/>
       <c r="T26" s="15"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
@@ -3425,7 +3426,7 @@
       <c r="S27" s="15"/>
       <c r="T27" s="15"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -3447,7 +3448,7 @@
       <c r="S28" s="15"/>
       <c r="T28" s="15"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -3469,7 +3470,7 @@
       <c r="S29" s="15"/>
       <c r="T29" s="15"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="15"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -3491,7 +3492,7 @@
       <c r="S30" s="15"/>
       <c r="T30" s="15"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="15"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -3513,7 +3514,7 @@
       <c r="S31" s="15"/>
       <c r="T31" s="15"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
@@ -3535,7 +3536,7 @@
       <c r="S32" s="15"/>
       <c r="T32" s="15"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="15"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
@@ -3557,7 +3558,7 @@
       <c r="S33" s="15"/>
       <c r="T33" s="15"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="15"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
@@ -3579,7 +3580,7 @@
       <c r="S34" s="15"/>
       <c r="T34" s="15"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="15"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
@@ -3601,7 +3602,7 @@
       <c r="S35" s="15"/>
       <c r="T35" s="15"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
@@ -3623,7 +3624,7 @@
       <c r="S36" s="15"/>
       <c r="T36" s="15"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="15"/>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
@@ -3645,7 +3646,7 @@
       <c r="S37" s="15"/>
       <c r="T37" s="15"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="15"/>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
@@ -3667,7 +3668,7 @@
       <c r="S38" s="15"/>
       <c r="T38" s="15"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
@@ -3689,7 +3690,7 @@
       <c r="S39" s="15"/>
       <c r="T39" s="15"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="15"/>
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
@@ -3711,7 +3712,7 @@
       <c r="S40" s="15"/>
       <c r="T40" s="15"/>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="15"/>
       <c r="B41" s="15"/>
       <c r="C41" s="15"/>
@@ -3733,7 +3734,7 @@
       <c r="S41" s="15"/>
       <c r="T41" s="15"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="15"/>
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
@@ -3755,7 +3756,7 @@
       <c r="S42" s="15"/>
       <c r="T42" s="15"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="15"/>
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
@@ -3777,7 +3778,7 @@
       <c r="S43" s="15"/>
       <c r="T43" s="15"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="15"/>
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
@@ -3799,7 +3800,7 @@
       <c r="S44" s="15"/>
       <c r="T44" s="15"/>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="15"/>
       <c r="B45" s="15"/>
       <c r="C45" s="15"/>
@@ -3821,7 +3822,7 @@
       <c r="S45" s="15"/>
       <c r="T45" s="15"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="15"/>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
@@ -3843,7 +3844,7 @@
       <c r="S46" s="15"/>
       <c r="T46" s="15"/>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="15"/>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>
@@ -3865,7 +3866,7 @@
       <c r="S47" s="15"/>
       <c r="T47" s="15"/>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="15"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
@@ -3896,7 +3897,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="P5:P14 F17" formulaRange="1"/>
+    <ignoredError sqref="P5:P14" formulaRange="1"/>
     <ignoredError sqref="P4" calculatedColumn="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Blog Statistics (June 2017)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -938,7 +938,7 @@
                   <c:v>4530257</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7905146.4000000004</c:v>
+                  <c:v>7907738</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1425,7 +1425,7 @@
                   <c:v>4530257</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3293811</c:v>
+                  <c:v>3953869</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2463,7 +2463,7 @@
   <dimension ref="A1:T48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="U22" sqref="U22"/>
+      <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -3114,7 +3114,9 @@
       <c r="G14" s="8">
         <v>745540</v>
       </c>
-      <c r="H14" s="10"/>
+      <c r="H14" s="8">
+        <v>660058</v>
+      </c>
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
@@ -3124,12 +3126,12 @@
       <c r="O14" s="11"/>
       <c r="P14" s="11">
         <f>SUM(C14:N14)</f>
-        <v>3293811</v>
+        <v>3953869</v>
       </c>
       <c r="Q14" s="13"/>
       <c r="R14" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>7905146.4000000004</v>
+        <v>7907738</v>
       </c>
       <c r="S14" s="15"/>
       <c r="T14" s="15"/>
@@ -3152,7 +3154,7 @@
       <c r="O15" s="19"/>
       <c r="P15" s="16">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>13152002</v>
+        <v>13812060</v>
       </c>
       <c r="Q15" s="13"/>
       <c r="R15" s="15"/>
@@ -3189,7 +3191,7 @@
       <c r="D17" s="21"/>
       <c r="E17" s="21"/>
       <c r="F17" s="20">
-        <v>7124326</v>
+        <v>7651616</v>
       </c>
       <c r="G17" s="20"/>
       <c r="H17" s="13"/>

</xml_diff>

<commit_message>
Blog Statistics (July 2017)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -938,7 +938,7 @@
                   <c:v>4530257</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7907738</c:v>
+                  <c:v>7961797.7142857146</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1425,7 +1425,7 @@
                   <c:v>4530257</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3953869</c:v>
+                  <c:v>4644382</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2462,8 +2462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="W13" sqref="W13"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -3117,7 +3117,9 @@
       <c r="H14" s="8">
         <v>660058</v>
       </c>
-      <c r="I14" s="10"/>
+      <c r="I14" s="8">
+        <v>690513</v>
+      </c>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
@@ -3126,12 +3128,12 @@
       <c r="O14" s="11"/>
       <c r="P14" s="11">
         <f>SUM(C14:N14)</f>
-        <v>3953869</v>
+        <v>4644382</v>
       </c>
       <c r="Q14" s="13"/>
       <c r="R14" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>7907738</v>
+        <v>7961797.7142857146</v>
       </c>
       <c r="S14" s="15"/>
       <c r="T14" s="15"/>
@@ -3154,7 +3156,7 @@
       <c r="O15" s="19"/>
       <c r="P15" s="16">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>13812060</v>
+        <v>14502573</v>
       </c>
       <c r="Q15" s="13"/>
       <c r="R15" s="15"/>

</xml_diff>

<commit_message>
Blog Statistics (August 2017)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20486" windowHeight="8939"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20486" windowHeight="8939" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -117,7 +117,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -938,7 +938,7 @@
                   <c:v>4530257</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7961797.7142857146</c:v>
+                  <c:v>7972317</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1425,7 +1425,7 @@
                   <c:v>4530257</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4644382</c:v>
+                  <c:v>5314878</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2110,28 +2110,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:R14" totalsRowShown="0" dataDxfId="17">
-  <autoFilter ref="B3:R14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B3:R14" totalsRowShown="0" dataDxfId="17">
+  <autoFilter ref="B3:R14" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Column1" dataDxfId="16"/>
-    <tableColumn id="2" name="Column2" dataDxfId="15"/>
-    <tableColumn id="3" name="Column3" dataDxfId="14"/>
-    <tableColumn id="4" name="Column4" dataDxfId="13"/>
-    <tableColumn id="5" name="Column5" dataDxfId="12"/>
-    <tableColumn id="6" name="Column6" dataDxfId="11"/>
-    <tableColumn id="7" name="Column7" dataDxfId="10"/>
-    <tableColumn id="8" name="Column8" dataDxfId="9"/>
-    <tableColumn id="9" name="Column9" dataDxfId="8"/>
-    <tableColumn id="10" name="Column10" dataDxfId="7"/>
-    <tableColumn id="11" name="Column11" dataDxfId="6"/>
-    <tableColumn id="12" name="Column12" dataDxfId="5"/>
-    <tableColumn id="13" name="Column13" dataDxfId="4"/>
-    <tableColumn id="14" name="Column14" dataDxfId="3"/>
-    <tableColumn id="15" name="Column15" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Column3" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Column4" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Column5" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column6" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Column7" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Column8" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Column9" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Column10" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Column11" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Column12" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Column13" dataDxfId="4"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Column14" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Column15" dataDxfId="2">
       <calculatedColumnFormula>SUM(C4:N4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Column152" dataDxfId="1" dataCellStyle="Normal"/>
-    <tableColumn id="16" name="Column16" dataDxfId="0">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Column152" dataDxfId="1" dataCellStyle="Normal"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Column16" dataDxfId="0">
       <calculatedColumnFormula>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2459,11 +2459,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:O15"/>
+      <selection activeCell="W24" sqref="W24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -3120,7 +3120,9 @@
       <c r="I14" s="8">
         <v>690513</v>
       </c>
-      <c r="J14" s="10"/>
+      <c r="J14" s="8">
+        <v>670496</v>
+      </c>
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
@@ -3128,12 +3130,12 @@
       <c r="O14" s="11"/>
       <c r="P14" s="11">
         <f>SUM(C14:N14)</f>
-        <v>4644382</v>
+        <v>5314878</v>
       </c>
       <c r="Q14" s="13"/>
       <c r="R14" s="12">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>7961797.7142857146</v>
+        <v>7972317</v>
       </c>
       <c r="S14" s="15"/>
       <c r="T14" s="15"/>
@@ -3156,7 +3158,7 @@
       <c r="O15" s="19"/>
       <c r="P15" s="16">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>14502573</v>
+        <v>15173069</v>
       </c>
       <c r="Q15" s="13"/>
       <c r="R15" s="15"/>
@@ -3193,7 +3195,8 @@
       <c r="D17" s="21"/>
       <c r="E17" s="21"/>
       <c r="F17" s="20">
-        <v>7651616</v>
+        <f>SUM(C14:J14,K13:N13)</f>
+        <v>7946772</v>
       </c>
       <c r="G17" s="20"/>
       <c r="H17" s="13"/>

</xml_diff>

<commit_message>
Blog Statistics (September 2017)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud Storage\OneDrive\GIT Hub\kunal-chowdhury.com\blog-stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="6" documentId="40FDE6E5555299D8B362937CCDD5C9106F5153E0" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{2013FE1B-69C0-4151-89AF-69552898E9B4}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20486" windowHeight="8939" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -118,7 +119,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,6 +138,11 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="16"/>
@@ -149,11 +161,6 @@
       <b/>
       <sz val="16"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -246,43 +253,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -938,7 +946,7 @@
                   <c:v>4530257</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7972317</c:v>
+                  <c:v>7856630.666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1425,7 +1433,7 @@
                   <c:v>4530257</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5314878</c:v>
+                  <c:v>5892473</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2462,1438 +2470,1440 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="W24" sqref="W24"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="14" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4" customWidth="1"/>
-    <col min="16" max="16" width="18.375" customWidth="1"/>
-    <col min="17" max="17" width="5.375" customWidth="1"/>
-    <col min="18" max="18" width="25.5" customWidth="1"/>
+    <col min="1" max="1" width="5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.5" style="2" customWidth="1"/>
+    <col min="3" max="14" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4" style="2" customWidth="1"/>
+    <col min="16" max="16" width="18.375" style="2" customWidth="1"/>
+    <col min="17" max="17" width="5.375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="25.5" style="2" customWidth="1"/>
+    <col min="19" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15"/>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
     </row>
     <row r="3" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" t="s">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" s="13" t="s">
+      <c r="Q3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="R3" t="s">
+      <c r="R3" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
-      <c r="A4" s="15"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="2" t="s">
+      <c r="A4" s="1"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="N4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3" t="s">
+      <c r="O4" s="6"/>
+      <c r="P4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="12" t="e">
+      <c r="Q4" s="3"/>
+      <c r="R4" s="7" t="e">
         <f>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
     </row>
     <row r="5" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
-      <c r="A5" s="15"/>
-      <c r="B5" s="4">
+      <c r="A5" s="1"/>
+      <c r="B5" s="8">
         <v>2008</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="6">
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="10">
         <v>105</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="10">
         <v>112</v>
       </c>
-      <c r="N5" s="6">
+      <c r="N5" s="10">
         <v>109</v>
       </c>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6">
+      <c r="O5" s="10"/>
+      <c r="P5" s="10">
         <f>SUM(C5:N5)</f>
         <v>326</v>
       </c>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="12">
+      <c r="Q5" s="3"/>
+      <c r="R5" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>326</v>
       </c>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
     </row>
     <row r="6" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
-      <c r="A6" s="15"/>
-      <c r="B6" s="4">
+      <c r="A6" s="1"/>
+      <c r="B6" s="8">
         <v>2009</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="10">
         <v>210</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="10">
         <v>265</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="10">
         <v>330</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="10">
         <v>459</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="10">
         <v>2711</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="10">
         <v>4347</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="10">
         <v>7134</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="10">
         <v>7452</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="10">
         <v>10193</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="10">
         <v>11773</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="10">
         <v>16989</v>
       </c>
-      <c r="N6" s="6">
+      <c r="N6" s="10">
         <v>18516</v>
       </c>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6">
+      <c r="O6" s="10"/>
+      <c r="P6" s="10">
         <f t="shared" ref="P6:P12" si="0">SUM(C6:N6)</f>
         <v>80379</v>
       </c>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="12">
+      <c r="Q6" s="3"/>
+      <c r="R6" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>80379</v>
       </c>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
     </row>
     <row r="7" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
-      <c r="A7" s="15"/>
-      <c r="B7" s="4">
+      <c r="A7" s="1"/>
+      <c r="B7" s="8">
         <v>2010</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="10">
         <v>16660</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="10">
         <v>23673</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="10">
         <v>32985</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="10">
         <v>35222</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="10">
         <v>39909</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="10">
         <v>42087</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="10">
         <v>54395</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="10">
         <v>49067</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="10">
         <v>47658</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="10">
         <v>38853</v>
       </c>
-      <c r="M7" s="6">
+      <c r="M7" s="10">
         <v>39946</v>
       </c>
-      <c r="N7" s="6">
+      <c r="N7" s="10">
         <v>42658</v>
       </c>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6">
+      <c r="O7" s="10"/>
+      <c r="P7" s="10">
         <f t="shared" si="0"/>
         <v>463113</v>
       </c>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="12">
+      <c r="Q7" s="3"/>
+      <c r="R7" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>463113</v>
       </c>
-      <c r="S7" s="15"/>
-      <c r="T7" s="15"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
     </row>
     <row r="8" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
-      <c r="A8" s="15"/>
-      <c r="B8" s="4">
+      <c r="A8" s="1"/>
+      <c r="B8" s="8">
         <v>2011</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="10">
         <v>45551</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="10">
         <v>69346</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="10">
         <v>47856</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="10">
         <v>64728</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="10">
         <v>73308</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="10">
         <v>82846</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="10">
         <v>72286</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="10">
         <v>75867</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="10">
         <v>80961</v>
       </c>
-      <c r="L8" s="6">
+      <c r="L8" s="10">
         <v>62233</v>
       </c>
-      <c r="M8" s="6">
+      <c r="M8" s="10">
         <v>63447</v>
       </c>
-      <c r="N8" s="6">
+      <c r="N8" s="10">
         <v>64581</v>
       </c>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6">
+      <c r="O8" s="10"/>
+      <c r="P8" s="10">
         <f t="shared" si="0"/>
         <v>803010</v>
       </c>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="12">
+      <c r="Q8" s="3"/>
+      <c r="R8" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>803010</v>
       </c>
-      <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
     </row>
     <row r="9" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
-      <c r="A9" s="15"/>
-      <c r="B9" s="4">
+      <c r="A9" s="1"/>
+      <c r="B9" s="8">
         <v>2012</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="10">
         <v>76072</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="10">
         <v>77385</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="10">
         <v>70852</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="10">
         <v>72356</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="10">
         <v>78593</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="10">
         <v>70155</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="10">
         <v>72470</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="10">
         <v>70252</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="10">
         <v>79738</v>
       </c>
-      <c r="L9" s="6">
+      <c r="L9" s="10">
         <v>71284</v>
       </c>
-      <c r="M9" s="6">
+      <c r="M9" s="10">
         <v>76524</v>
       </c>
-      <c r="N9" s="6">
+      <c r="N9" s="10">
         <v>73172</v>
       </c>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6">
+      <c r="O9" s="10"/>
+      <c r="P9" s="10">
         <f t="shared" si="0"/>
         <v>888853</v>
       </c>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="12">
+      <c r="Q9" s="3"/>
+      <c r="R9" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>888853</v>
       </c>
-      <c r="S9" s="15"/>
-      <c r="T9" s="15"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
     </row>
     <row r="10" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
-      <c r="A10" s="15"/>
-      <c r="B10" s="4">
+      <c r="A10" s="1"/>
+      <c r="B10" s="8">
         <v>2013</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="10">
         <v>78648</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="10">
         <v>74894</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="10">
         <v>86029</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="10">
         <v>82489</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="10">
         <v>80316</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="10">
         <v>78764</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="10">
         <v>70746</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="10">
         <v>79324</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="10">
         <v>79148</v>
       </c>
-      <c r="L10" s="6">
+      <c r="L10" s="10">
         <v>76345</v>
       </c>
-      <c r="M10" s="6">
+      <c r="M10" s="10">
         <v>75329</v>
       </c>
-      <c r="N10" s="6">
+      <c r="N10" s="10">
         <v>73625</v>
       </c>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6">
+      <c r="O10" s="10"/>
+      <c r="P10" s="10">
         <f t="shared" si="0"/>
         <v>935657</v>
       </c>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="12">
+      <c r="Q10" s="3"/>
+      <c r="R10" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>935657</v>
       </c>
-      <c r="S10" s="15"/>
-      <c r="T10" s="15"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
     </row>
     <row r="11" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
-      <c r="A11" s="15"/>
-      <c r="B11" s="4">
+      <c r="A11" s="1"/>
+      <c r="B11" s="8">
         <v>2014</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="10">
         <v>67510</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="10">
         <v>67706</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="10">
         <v>73924</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="10">
         <v>71449</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="10">
         <v>79877</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="10">
         <v>74705</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="10">
         <v>79936</v>
       </c>
-      <c r="J11" s="6">
+      <c r="J11" s="10">
         <v>78746</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K11" s="10">
         <v>77891</v>
       </c>
-      <c r="L11" s="6">
+      <c r="L11" s="10">
         <v>77040</v>
       </c>
-      <c r="M11" s="6">
+      <c r="M11" s="10">
         <v>87951</v>
       </c>
-      <c r="N11" s="7">
+      <c r="N11" s="11">
         <v>101904</v>
       </c>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6">
+      <c r="O11" s="10"/>
+      <c r="P11" s="10">
         <f t="shared" si="0"/>
         <v>938639</v>
       </c>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="12">
+      <c r="Q11" s="3"/>
+      <c r="R11" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>938639</v>
       </c>
-      <c r="S11" s="15"/>
-      <c r="T11" s="15"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
     </row>
     <row r="12" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
-      <c r="A12" s="15"/>
-      <c r="B12" s="4">
+      <c r="A12" s="1"/>
+      <c r="B12" s="8">
         <v>2015</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="10">
         <v>90536</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="10">
         <v>80976</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="10">
         <v>95444</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="10">
         <v>71951</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="10">
         <v>67019</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="10">
         <v>66244</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="10">
         <v>86294</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="11">
         <v>128005</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="11">
         <v>137300</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12" s="11">
         <v>138705</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12" s="11">
         <v>125538</v>
       </c>
-      <c r="N12" s="7">
+      <c r="N12" s="11">
         <v>129945</v>
       </c>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6">
+      <c r="O12" s="10"/>
+      <c r="P12" s="10">
         <f t="shared" si="0"/>
         <v>1217957</v>
       </c>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="12">
+      <c r="Q12" s="3"/>
+      <c r="R12" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>1217957</v>
       </c>
-      <c r="S12" s="15"/>
-      <c r="T12" s="15"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
     </row>
     <row r="13" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
-      <c r="A13" s="15"/>
-      <c r="B13" s="4">
+      <c r="A13" s="1"/>
+      <c r="B13" s="8">
         <v>2016</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="11">
         <v>142274</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="11">
         <v>123093</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="11">
         <v>147266</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="11">
         <v>152612</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="11">
         <v>134497</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="11">
         <v>132768</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="12">
         <v>363723</v>
       </c>
-      <c r="J13" s="8">
+      <c r="J13" s="12">
         <v>702130</v>
       </c>
-      <c r="K13" s="8">
+      <c r="K13" s="12">
         <v>608805</v>
       </c>
-      <c r="L13" s="8">
+      <c r="L13" s="12">
         <v>635500</v>
       </c>
-      <c r="M13" s="8">
+      <c r="M13" s="12">
         <v>713080</v>
       </c>
-      <c r="N13" s="8">
+      <c r="N13" s="12">
         <v>674509</v>
       </c>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6">
+      <c r="O13" s="10"/>
+      <c r="P13" s="10">
         <f>SUM(C13:N13)</f>
         <v>4530257</v>
       </c>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="12">
+      <c r="Q13" s="3"/>
+      <c r="R13" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>4530257</v>
       </c>
-      <c r="S13" s="15"/>
-      <c r="T13" s="15"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
     </row>
     <row r="14" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
-      <c r="A14" s="15"/>
-      <c r="B14" s="9">
+      <c r="A14" s="1"/>
+      <c r="B14" s="13">
         <v>2017</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="12">
         <v>662423</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="12">
         <v>554842</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="12">
         <v>657797</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="12">
         <v>673209</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="12">
         <v>745540</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="12">
         <v>660058</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="12">
         <v>690513</v>
       </c>
-      <c r="J14" s="8">
+      <c r="J14" s="12">
         <v>670496</v>
       </c>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="11"/>
-      <c r="P14" s="11">
+      <c r="K14" s="12">
+        <v>577595</v>
+      </c>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15">
         <f>SUM(C14:N14)</f>
-        <v>5314878</v>
-      </c>
-      <c r="Q14" s="13"/>
-      <c r="R14" s="12">
+        <v>5892473</v>
+      </c>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>7972317</v>
-      </c>
-      <c r="S14" s="15"/>
-      <c r="T14" s="15"/>
+        <v>7856630.666666667</v>
+      </c>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
     </row>
     <row r="15" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
-      <c r="A15" s="15"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19"/>
-      <c r="N15" s="19"/>
-      <c r="O15" s="19"/>
-      <c r="P15" s="16">
+      <c r="A15" s="1"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="18">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>15173069</v>
-      </c>
-      <c r="Q15" s="13"/>
-      <c r="R15" s="15"/>
-      <c r="S15" s="15"/>
-      <c r="T15" s="15"/>
+        <v>15750664</v>
+      </c>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
-      <c r="S16" s="15"/>
-      <c r="T16" s="15"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
     </row>
     <row r="17" spans="1:20" ht="23.8" x14ac:dyDescent="0.4">
-      <c r="A17" s="15"/>
-      <c r="B17" s="21" t="s">
+      <c r="A17" s="1"/>
+      <c r="B17" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="20">
-        <f>SUM(C14:J14,K13:N13)</f>
-        <v>7946772</v>
-      </c>
-      <c r="G17" s="20"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="15"/>
-      <c r="S17" s="15"/>
-      <c r="T17" s="15"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="21">
+        <v>7915562</v>
+      </c>
+      <c r="G17" s="21"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="15"/>
-      <c r="S18" s="15"/>
-      <c r="T18" s="15"/>
+      <c r="A18" s="1"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="15"/>
-      <c r="P19" s="15"/>
-      <c r="Q19" s="15"/>
-      <c r="R19" s="15"/>
-      <c r="S19" s="15"/>
-      <c r="T19" s="15"/>
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="15"/>
-      <c r="S20" s="15"/>
-      <c r="T20" s="15"/>
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="15"/>
-      <c r="S21" s="15"/>
-      <c r="T21" s="15"/>
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="15"/>
-      <c r="S22" s="15"/>
-      <c r="T22" s="15"/>
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="15"/>
-      <c r="S23" s="15"/>
-      <c r="T23" s="15"/>
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="15"/>
-      <c r="S24" s="15"/>
-      <c r="T24" s="15"/>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
-      <c r="P25" s="15"/>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="15"/>
-      <c r="S25" s="15"/>
-      <c r="T25" s="15"/>
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
-      <c r="S26" s="15"/>
-      <c r="T26" s="15"/>
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
-      <c r="Q27" s="15"/>
-      <c r="R27" s="15"/>
-      <c r="S27" s="15"/>
-      <c r="T27" s="15"/>
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="15"/>
-      <c r="S28" s="15"/>
-      <c r="T28" s="15"/>
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
-      <c r="O29" s="15"/>
-      <c r="P29" s="15"/>
-      <c r="Q29" s="15"/>
-      <c r="R29" s="15"/>
-      <c r="S29" s="15"/>
-      <c r="T29" s="15"/>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="15"/>
-      <c r="O30" s="15"/>
-      <c r="P30" s="15"/>
-      <c r="Q30" s="15"/>
-      <c r="R30" s="15"/>
-      <c r="S30" s="15"/>
-      <c r="T30" s="15"/>
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
-      <c r="O31" s="15"/>
-      <c r="P31" s="15"/>
-      <c r="Q31" s="15"/>
-      <c r="R31" s="15"/>
-      <c r="S31" s="15"/>
-      <c r="T31" s="15"/>
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="15"/>
-      <c r="O32" s="15"/>
-      <c r="P32" s="15"/>
-      <c r="Q32" s="15"/>
-      <c r="R32" s="15"/>
-      <c r="S32" s="15"/>
-      <c r="T32" s="15"/>
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="15"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="15"/>
-      <c r="N33" s="15"/>
-      <c r="O33" s="15"/>
-      <c r="P33" s="15"/>
-      <c r="Q33" s="15"/>
-      <c r="R33" s="15"/>
-      <c r="S33" s="15"/>
-      <c r="T33" s="15"/>
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
-      <c r="M34" s="15"/>
-      <c r="N34" s="15"/>
-      <c r="O34" s="15"/>
-      <c r="P34" s="15"/>
-      <c r="Q34" s="15"/>
-      <c r="R34" s="15"/>
-      <c r="S34" s="15"/>
-      <c r="T34" s="15"/>
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="1"/>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="15"/>
-      <c r="N35" s="15"/>
-      <c r="O35" s="15"/>
-      <c r="P35" s="15"/>
-      <c r="Q35" s="15"/>
-      <c r="R35" s="15"/>
-      <c r="S35" s="15"/>
-      <c r="T35" s="15"/>
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+      <c r="S35" s="1"/>
+      <c r="T35" s="1"/>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
-      <c r="M36" s="15"/>
-      <c r="N36" s="15"/>
-      <c r="O36" s="15"/>
-      <c r="P36" s="15"/>
-      <c r="Q36" s="15"/>
-      <c r="R36" s="15"/>
-      <c r="S36" s="15"/>
-      <c r="T36" s="15"/>
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
+      <c r="S36" s="1"/>
+      <c r="T36" s="1"/>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
-      <c r="J37" s="15"/>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
-      <c r="M37" s="15"/>
-      <c r="N37" s="15"/>
-      <c r="O37" s="15"/>
-      <c r="P37" s="15"/>
-      <c r="Q37" s="15"/>
-      <c r="R37" s="15"/>
-      <c r="S37" s="15"/>
-      <c r="T37" s="15"/>
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+      <c r="S37" s="1"/>
+      <c r="T37" s="1"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="15"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
-      <c r="L38" s="15"/>
-      <c r="M38" s="15"/>
-      <c r="N38" s="15"/>
-      <c r="O38" s="15"/>
-      <c r="P38" s="15"/>
-      <c r="Q38" s="15"/>
-      <c r="R38" s="15"/>
-      <c r="S38" s="15"/>
-      <c r="T38" s="15"/>
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
+      <c r="T38" s="1"/>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="15"/>
-      <c r="G39" s="15"/>
-      <c r="H39" s="15"/>
-      <c r="I39" s="15"/>
-      <c r="J39" s="15"/>
-      <c r="K39" s="15"/>
-      <c r="L39" s="15"/>
-      <c r="M39" s="15"/>
-      <c r="N39" s="15"/>
-      <c r="O39" s="15"/>
-      <c r="P39" s="15"/>
-      <c r="Q39" s="15"/>
-      <c r="R39" s="15"/>
-      <c r="S39" s="15"/>
-      <c r="T39" s="15"/>
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1"/>
+      <c r="T39" s="1"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A40" s="15"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="15"/>
-      <c r="I40" s="15"/>
-      <c r="J40" s="15"/>
-      <c r="K40" s="15"/>
-      <c r="L40" s="15"/>
-      <c r="M40" s="15"/>
-      <c r="N40" s="15"/>
-      <c r="O40" s="15"/>
-      <c r="P40" s="15"/>
-      <c r="Q40" s="15"/>
-      <c r="R40" s="15"/>
-      <c r="S40" s="15"/>
-      <c r="T40" s="15"/>
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
+      <c r="R40" s="1"/>
+      <c r="S40" s="1"/>
+      <c r="T40" s="1"/>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A41" s="15"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
-      <c r="H41" s="15"/>
-      <c r="I41" s="15"/>
-      <c r="J41" s="15"/>
-      <c r="K41" s="15"/>
-      <c r="L41" s="15"/>
-      <c r="M41" s="15"/>
-      <c r="N41" s="15"/>
-      <c r="O41" s="15"/>
-      <c r="P41" s="15"/>
-      <c r="Q41" s="15"/>
-      <c r="R41" s="15"/>
-      <c r="S41" s="15"/>
-      <c r="T41" s="15"/>
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="1"/>
+      <c r="S41" s="1"/>
+      <c r="T41" s="1"/>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A42" s="15"/>
-      <c r="B42" s="15"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
-      <c r="G42" s="15"/>
-      <c r="H42" s="15"/>
-      <c r="I42" s="15"/>
-      <c r="J42" s="15"/>
-      <c r="K42" s="15"/>
-      <c r="L42" s="15"/>
-      <c r="M42" s="15"/>
-      <c r="N42" s="15"/>
-      <c r="O42" s="15"/>
-      <c r="P42" s="15"/>
-      <c r="Q42" s="15"/>
-      <c r="R42" s="15"/>
-      <c r="S42" s="15"/>
-      <c r="T42" s="15"/>
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="1"/>
+      <c r="R42" s="1"/>
+      <c r="S42" s="1"/>
+      <c r="T42" s="1"/>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A43" s="15"/>
-      <c r="B43" s="15"/>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15"/>
-      <c r="G43" s="15"/>
-      <c r="H43" s="15"/>
-      <c r="I43" s="15"/>
-      <c r="J43" s="15"/>
-      <c r="K43" s="15"/>
-      <c r="L43" s="15"/>
-      <c r="M43" s="15"/>
-      <c r="N43" s="15"/>
-      <c r="O43" s="15"/>
-      <c r="P43" s="15"/>
-      <c r="Q43" s="15"/>
-      <c r="R43" s="15"/>
-      <c r="S43" s="15"/>
-      <c r="T43" s="15"/>
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="1"/>
+      <c r="P43" s="1"/>
+      <c r="Q43" s="1"/>
+      <c r="R43" s="1"/>
+      <c r="S43" s="1"/>
+      <c r="T43" s="1"/>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A44" s="15"/>
-      <c r="B44" s="15"/>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
-      <c r="G44" s="15"/>
-      <c r="H44" s="15"/>
-      <c r="I44" s="15"/>
-      <c r="J44" s="15"/>
-      <c r="K44" s="15"/>
-      <c r="L44" s="15"/>
-      <c r="M44" s="15"/>
-      <c r="N44" s="15"/>
-      <c r="O44" s="15"/>
-      <c r="P44" s="15"/>
-      <c r="Q44" s="15"/>
-      <c r="R44" s="15"/>
-      <c r="S44" s="15"/>
-      <c r="T44" s="15"/>
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+      <c r="R44" s="1"/>
+      <c r="S44" s="1"/>
+      <c r="T44" s="1"/>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A45" s="15"/>
-      <c r="B45" s="15"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="15"/>
-      <c r="J45" s="15"/>
-      <c r="K45" s="15"/>
-      <c r="L45" s="15"/>
-      <c r="M45" s="15"/>
-      <c r="N45" s="15"/>
-      <c r="O45" s="15"/>
-      <c r="P45" s="15"/>
-      <c r="Q45" s="15"/>
-      <c r="R45" s="15"/>
-      <c r="S45" s="15"/>
-      <c r="T45" s="15"/>
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="1"/>
+      <c r="R45" s="1"/>
+      <c r="S45" s="1"/>
+      <c r="T45" s="1"/>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A46" s="15"/>
-      <c r="B46" s="15"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="15"/>
-      <c r="F46" s="15"/>
-      <c r="G46" s="15"/>
-      <c r="H46" s="15"/>
-      <c r="I46" s="15"/>
-      <c r="J46" s="15"/>
-      <c r="K46" s="15"/>
-      <c r="L46" s="17"/>
-      <c r="M46" s="15"/>
-      <c r="N46" s="15"/>
-      <c r="O46" s="15"/>
-      <c r="P46" s="15"/>
-      <c r="Q46" s="15"/>
-      <c r="R46" s="15"/>
-      <c r="S46" s="15"/>
-      <c r="T46" s="15"/>
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="22"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
+      <c r="Q46" s="1"/>
+      <c r="R46" s="1"/>
+      <c r="S46" s="1"/>
+      <c r="T46" s="1"/>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A47" s="15"/>
-      <c r="B47" s="15"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="15"/>
-      <c r="F47" s="15"/>
-      <c r="G47" s="15"/>
-      <c r="H47" s="15"/>
-      <c r="I47" s="15"/>
-      <c r="J47" s="15"/>
-      <c r="K47" s="15"/>
-      <c r="L47" s="15"/>
-      <c r="M47" s="15"/>
-      <c r="N47" s="15"/>
-      <c r="O47" s="15"/>
-      <c r="P47" s="15"/>
-      <c r="Q47" s="15"/>
-      <c r="R47" s="15"/>
-      <c r="S47" s="15"/>
-      <c r="T47" s="15"/>
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="1"/>
+      <c r="R47" s="1"/>
+      <c r="S47" s="1"/>
+      <c r="T47" s="1"/>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A48" s="15"/>
-      <c r="B48" s="15"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="15"/>
-      <c r="H48" s="15"/>
-      <c r="I48" s="15"/>
-      <c r="J48" s="15"/>
-      <c r="K48" s="15"/>
-      <c r="L48" s="15"/>
-      <c r="M48" s="15"/>
-      <c r="N48" s="15"/>
-      <c r="O48" s="15"/>
-      <c r="P48" s="15"/>
-      <c r="Q48" s="15"/>
-      <c r="R48" s="15"/>
-      <c r="S48" s="15"/>
-      <c r="T48" s="15"/>
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="1"/>
+      <c r="S48" s="1"/>
+      <c r="T48" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Blog Statistics (October 2017)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud Storage\OneDrive\GIT Hub\kunal-chowdhury.com\blog-stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="40FDE6E5555299D8B362937CCDD5C9106F5153E0" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{2013FE1B-69C0-4151-89AF-69552898E9B4}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="40FDE6E5555299D8B362937CCDD5C9106F5153E0" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{532D8758-6E8E-4CDB-8AD3-E57DFE6C86F2}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20486" windowHeight="8939" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -276,21 +276,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -946,7 +946,7 @@
                   <c:v>4530257</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7856630.666666667</c:v>
+                  <c:v>7870134</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1433,7 +1433,7 @@
                   <c:v>4530257</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5892473</c:v>
+                  <c:v>6558445</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2471,7 +2471,7 @@
   <dimension ref="A1:T48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="W8" sqref="W8"/>
+      <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -3135,41 +3135,43 @@
       <c r="K14" s="12">
         <v>577595</v>
       </c>
-      <c r="L14" s="14"/>
+      <c r="L14" s="12">
+        <v>665972</v>
+      </c>
       <c r="M14" s="14"/>
       <c r="N14" s="14"/>
       <c r="O14" s="15"/>
       <c r="P14" s="15">
         <f>SUM(C14:N14)</f>
-        <v>5892473</v>
+        <v>6558445</v>
       </c>
       <c r="Q14" s="3"/>
       <c r="R14" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>7856630.666666667</v>
+        <v>7870134</v>
       </c>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
     </row>
     <row r="15" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="18">
+      <c r="B15" s="19"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="16">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>15750664</v>
+        <v>16416636</v>
       </c>
       <c r="Q15" s="3"/>
       <c r="R15" s="1"/>
@@ -3177,21 +3179,21 @@
       <c r="T15" s="1"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="19"/>
-      <c r="O16" s="19"/>
-      <c r="P16" s="19"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
@@ -3199,14 +3201,14 @@
     </row>
     <row r="17" spans="1:20" ht="23.8" x14ac:dyDescent="0.4">
       <c r="A17" s="1"/>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
       <c r="F17" s="21">
-        <v>7915562</v>
+        <v>7946034</v>
       </c>
       <c r="G17" s="21"/>
       <c r="H17" s="3"/>
@@ -3851,7 +3853,7 @@
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
-      <c r="L46" s="22"/>
+      <c r="L46" s="18"/>
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>

</xml_diff>

<commit_message>
Blog Statistics (November 2017)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud Storage\OneDrive\GIT Hub\kunal-chowdhury.com\blog-stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="40FDE6E5555299D8B362937CCDD5C9106F5153E0" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{532D8758-6E8E-4CDB-8AD3-E57DFE6C86F2}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="40FDE6E5555299D8B362937CCDD5C9106F5153E0" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{E7732DBE-B534-4DB0-A20A-EAC323779822}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20486" windowHeight="8939" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -946,7 +946,7 @@
                   <c:v>4530257</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7870134</c:v>
+                  <c:v>7775882.1818181816</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1433,7 +1433,7 @@
                   <c:v>4530257</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6558445</c:v>
+                  <c:v>7127892</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2471,18 +2471,18 @@
   <dimension ref="A1:T48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="W18" sqref="W18"/>
+      <selection activeCell="X17" sqref="X17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.5" style="2" customWidth="1"/>
-    <col min="3" max="14" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="2" customWidth="1"/>
+    <col min="3" max="14" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="4" style="2" customWidth="1"/>
-    <col min="16" max="16" width="18.375" style="2" customWidth="1"/>
-    <col min="17" max="17" width="5.375" style="2" customWidth="1"/>
-    <col min="18" max="18" width="25.5" style="2" customWidth="1"/>
+    <col min="16" max="16" width="18.42578125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="5.42578125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="25.42578125" style="2" customWidth="1"/>
     <col min="19" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
@@ -2584,7 +2584,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
@@ -2635,7 +2635,7 @@
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
     </row>
-    <row r="5" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="8">
         <v>2008</v>
@@ -2671,7 +2671,7 @@
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="8">
         <v>2009</v>
@@ -2725,7 +2725,7 @@
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
     </row>
-    <row r="7" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="8">
         <v>2010</v>
@@ -2779,7 +2779,7 @@
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
     </row>
-    <row r="8" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="8">
         <v>2011</v>
@@ -2833,7 +2833,7 @@
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
     </row>
-    <row r="9" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="8">
         <v>2012</v>
@@ -2887,7 +2887,7 @@
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
     </row>
-    <row r="10" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="8">
         <v>2013</v>
@@ -2941,7 +2941,7 @@
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
     </row>
-    <row r="11" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="8">
         <v>2014</v>
@@ -2995,7 +2995,7 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
     </row>
-    <row r="12" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="8">
         <v>2015</v>
@@ -3049,7 +3049,7 @@
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
     </row>
-    <row r="13" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="8">
         <v>2016</v>
@@ -3103,7 +3103,7 @@
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
     </row>
-    <row r="14" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="13">
         <v>2017</v>
@@ -3138,22 +3138,24 @@
       <c r="L14" s="12">
         <v>665972</v>
       </c>
-      <c r="M14" s="14"/>
+      <c r="M14" s="12">
+        <v>569447</v>
+      </c>
       <c r="N14" s="14"/>
       <c r="O14" s="15"/>
       <c r="P14" s="15">
         <f>SUM(C14:N14)</f>
-        <v>6558445</v>
+        <v>7127892</v>
       </c>
       <c r="Q14" s="3"/>
       <c r="R14" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>7870134</v>
+        <v>7775882.1818181816</v>
       </c>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
     </row>
-    <row r="15" spans="1:20" ht="21.1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="19"/>
       <c r="C15" s="20"/>
@@ -3171,7 +3173,7 @@
       <c r="O15" s="20"/>
       <c r="P15" s="16">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>16416636</v>
+        <v>16986083</v>
       </c>
       <c r="Q15" s="3"/>
       <c r="R15" s="1"/>
@@ -3199,7 +3201,7 @@
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
     </row>
-    <row r="17" spans="1:20" ht="23.8" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:20" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="22" t="s">
         <v>30</v>
@@ -3208,7 +3210,8 @@
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
       <c r="F17" s="21">
-        <v>7946034</v>
+        <f>SUM(N13,C14:M14)</f>
+        <v>7802401</v>
       </c>
       <c r="G17" s="21"/>
       <c r="H17" s="3"/>

</xml_diff>

<commit_message>
Blog Statistics (December 2017)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18911"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud Storage\OneDrive\GIT Hub\kunal-chowdhury.com\blog-stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="40FDE6E5555299D8B362937CCDD5C9106F5153E0" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{E7732DBE-B534-4DB0-A20A-EAC323779822}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="40FDE6E5555299D8B362937CCDD5C9106F5153E0" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{F5C7720E-3861-4995-8067-56BFF11CA95B}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -272,9 +272,6 @@
     <xf numFmtId="3" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -291,6 +288,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -669,10 +667,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$14</c:f>
+              <c:f>Sheet1!$B$5:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>2008</c:v>
                 </c:pt>
@@ -702,16 +700,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2018</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$14</c:f>
+              <c:f>Sheet1!$B$5:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>2008</c:v>
                 </c:pt>
@@ -741,6 +742,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2018</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -875,10 +879,10 @@
           </c:dPt>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$14</c:f>
+              <c:f>Sheet1!$B$5:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>2008</c:v>
                 </c:pt>
@@ -908,16 +912,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2018</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$5:$R$14</c:f>
+              <c:f>Sheet1!$R$5:$R$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>326</c:v>
                 </c:pt>
@@ -946,7 +953,10 @@
                   <c:v>4530257</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7775882.1818181816</c:v>
+                  <c:v>7693253</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1215,8 +1225,8 @@
               <c:idx val="9"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-6.1783031451233283E-4"/>
-                  <c:y val="-0.17811295029660074"/>
+                  <c:x val="-0.16794352222587833"/>
+                  <c:y val="-1.940190915685883E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -1236,14 +1246,6 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="3200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                        <a:solidFill>
-                          <a:srgbClr val="00B050"/>
-                        </a:solidFill>
-                      </a:rPr>
-                      <a:t>^</a:t>
-                    </a:r>
                     <a:r>
                       <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                         <a:solidFill>
@@ -1362,10 +1364,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$14</c:f>
+              <c:f>Sheet1!$B$5:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>2008</c:v>
                 </c:pt>
@@ -1395,16 +1397,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2018</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$5:$P$14</c:f>
+              <c:f>Sheet1!$P$5:$P$15</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>326</c:v>
                 </c:pt>
@@ -1433,7 +1438,10 @@
                   <c:v>4530257</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7127892</c:v>
+                  <c:v>7693253</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2082,13 +2090,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>21429</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>23811</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>88107</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>62488</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2118,8 +2126,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B3:R14" totalsRowShown="0" dataDxfId="17">
-  <autoFilter ref="B3:R14" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B3:R15" totalsRowShown="0" dataDxfId="17">
+  <autoFilter ref="B3:R15" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1" dataDxfId="16"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2" dataDxfId="15"/>
@@ -2468,10 +2476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T48"/>
+  <dimension ref="A1:T49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="X17" sqref="X17"/>
+      <selection activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3141,101 +3149,111 @@
       <c r="M14" s="12">
         <v>569447</v>
       </c>
-      <c r="N14" s="14"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15">
+      <c r="N14" s="12">
+        <v>565361</v>
+      </c>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14">
         <f>SUM(C14:N14)</f>
-        <v>7127892</v>
+        <v>7693253</v>
       </c>
       <c r="Q14" s="3"/>
       <c r="R14" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>7775882.1818181816</v>
+        <v>7693253</v>
       </c>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
     </row>
     <row r="15" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="16">
-        <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>16986083</v>
-      </c>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="1"/>
+      <c r="B15" s="13">
+        <v>2018</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14">
+        <f>SUM(C15:N15)</f>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="22"/>
+      <c r="R15" s="7" t="e">
+        <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17"/>
-      <c r="Q16" s="1"/>
+    <row r="16" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+      <c r="A16" s="1"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="15">
+        <f>SUBTOTAL(109,Table1[Column15])</f>
+        <v>17551444</v>
+      </c>
+      <c r="Q16" s="3"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
     </row>
-    <row r="17" spans="1:20" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A17" s="1"/>
-      <c r="B17" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="21">
-        <f>SUM(N13,C14:M14)</f>
-        <v>7802401</v>
-      </c>
-      <c r="G17" s="21"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
+      <c r="B18" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="20">
+        <f>SUM(P14)</f>
+        <v>7693253</v>
+      </c>
+      <c r="G18" s="20"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
@@ -3252,21 +3270,21 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
@@ -3856,7 +3874,7 @@
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
-      <c r="L46" s="18"/>
+      <c r="L46" s="1"/>
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
@@ -3878,7 +3896,7 @@
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
-      <c r="L47" s="1"/>
+      <c r="L47" s="17"/>
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
@@ -3910,11 +3928,33 @@
       <c r="S48" s="1"/>
       <c r="T48" s="1"/>
     </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
+      <c r="P49" s="1"/>
+      <c r="Q49" s="1"/>
+      <c r="R49" s="1"/>
+      <c r="S49" s="1"/>
+      <c r="T49" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B15:O15"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B16:O16"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="B18:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Blog Statistics (January 2018)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19020"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud Storage\OneDrive\GIT Hub\kunal-chowdhury.com\blog-stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="40FDE6E5555299D8B362937CCDD5C9106F5153E0" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{F5C7720E-3861-4995-8067-56BFF11CA95B}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="40FDE6E5555299D8B362937CCDD5C9106F5153E0" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{3C50D6C9-A861-4D1C-A717-246172F55FF3}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -253,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -276,24 +276,34 @@
     <xf numFmtId="3" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="18">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -306,14 +316,6 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -877,6 +879,181 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000C-094D-4ED5-9227-CC4EE8D01624}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-094D-4ED5-9227-CC4EE8D01624}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-094D-4ED5-9227-CC4EE8D01624}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-094D-4ED5-9227-CC4EE8D01624}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-094D-4ED5-9227-CC4EE8D01624}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-094D-4ED5-9227-CC4EE8D01624}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-094D-4ED5-9227-CC4EE8D01624}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-094D-4ED5-9227-CC4EE8D01624}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-094D-4ED5-9227-CC4EE8D01624}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000C-F234-47AE-98F4-23124B27C96C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.9685379365382342E-2"/>
+                  <c:y val="-0.1640014521439222"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-094D-4ED5-9227-CC4EE8D01624}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$5:$B$15</c:f>
@@ -956,7 +1133,7 @@
                   <c:v>7693253</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>7536336</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1183,8 +1360,8 @@
               <c:idx val="7"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="1.7777775703963172E-2"/>
-                  <c:y val="-1.5526436355823132E-2"/>
+                  <c:x val="3.8869213350983006E-2"/>
+                  <c:y val="-2.6107139978384469E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1225,8 +1402,8 @@
               <c:idx val="9"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.16794352222587833"/>
-                  <c:y val="-1.940190915685883E-2"/>
+                  <c:x val="-0.20590818243054426"/>
+                  <c:y val="5.9953632203103534E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -1255,7 +1432,7 @@
                       <a:t> </a:t>
                     </a:r>
                     <a:fld id="{528CCE5D-54F9-45A3-8AB0-78CA94A9AC10}" type="VALUE">
-                      <a:rPr lang="en-US" sz="1800" b="1"/>
+                      <a:rPr lang="en-US" sz="1400" b="0"/>
                       <a:pPr>
                         <a:defRPr sz="1800" b="1"/>
                       </a:pPr>
@@ -1307,6 +1484,84 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000B-F234-47AE-98F4-23124B27C96C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-0.47877843287177291"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:spAutoFit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="2800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx2"/>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:fld id="{D7A76F95-4772-4256-A17D-4758AD75F025}" type="VALUE">
+                      <a:rPr lang="en-US" sz="1800" b="1"/>
+                      <a:pPr>
+                        <a:defRPr sz="2800" b="1"/>
+                      </a:pPr>
+                      <a:t>[VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="2800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-094D-4ED5-9227-CC4EE8D01624}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1441,7 +1696,7 @@
                   <c:v>7693253</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>628028</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1584,9 +1839,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="accent1"/>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -2122,6 +2375,64 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>773905</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>59530</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1893093" cy="342786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E07368B-A589-4B45-B521-F28735D4E821}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6738936" y="4714874"/>
+          <a:ext cx="1893093" cy="342786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>Projected (2018): </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2146,8 +2457,8 @@
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Column15" dataDxfId="2">
       <calculatedColumnFormula>SUM(C4:N4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Column152" dataDxfId="1" dataCellStyle="Normal"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Column16" dataDxfId="0">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Column152" dataDxfId="0" dataCellStyle="Normal"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Column16" dataDxfId="1">
       <calculatedColumnFormula>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2478,8 +2789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="W4" sqref="W4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="X13" sqref="X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2533,7 +2844,7 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
-      <c r="Q2" s="3"/>
+      <c r="Q2" s="22"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -2585,7 +2896,7 @@
       <c r="P3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="Q3" s="22" t="s">
         <v>29</v>
       </c>
       <c r="R3" s="2" t="s">
@@ -2635,7 +2946,7 @@
       <c r="P4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="Q4" s="3"/>
+      <c r="Q4" s="22"/>
       <c r="R4" s="7" t="e">
         <f>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>#VALUE!</v>
@@ -2671,7 +2982,7 @@
         <f>SUM(C5:N5)</f>
         <v>326</v>
       </c>
-      <c r="Q5" s="3"/>
+      <c r="Q5" s="22"/>
       <c r="R5" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>326</v>
@@ -2725,7 +3036,7 @@
         <f t="shared" ref="P6:P12" si="0">SUM(C6:N6)</f>
         <v>80379</v>
       </c>
-      <c r="Q6" s="3"/>
+      <c r="Q6" s="22"/>
       <c r="R6" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>80379</v>
@@ -2779,7 +3090,7 @@
         <f t="shared" si="0"/>
         <v>463113</v>
       </c>
-      <c r="Q7" s="3"/>
+      <c r="Q7" s="22"/>
       <c r="R7" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>463113</v>
@@ -2833,7 +3144,7 @@
         <f t="shared" si="0"/>
         <v>803010</v>
       </c>
-      <c r="Q8" s="3"/>
+      <c r="Q8" s="22"/>
       <c r="R8" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>803010</v>
@@ -2887,7 +3198,7 @@
         <f t="shared" si="0"/>
         <v>888853</v>
       </c>
-      <c r="Q9" s="3"/>
+      <c r="Q9" s="22"/>
       <c r="R9" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>888853</v>
@@ -2941,7 +3252,7 @@
         <f t="shared" si="0"/>
         <v>935657</v>
       </c>
-      <c r="Q10" s="3"/>
+      <c r="Q10" s="22"/>
       <c r="R10" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>935657</v>
@@ -2995,7 +3306,7 @@
         <f t="shared" si="0"/>
         <v>938639</v>
       </c>
-      <c r="Q11" s="3"/>
+      <c r="Q11" s="22"/>
       <c r="R11" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>938639</v>
@@ -3049,7 +3360,7 @@
         <f t="shared" si="0"/>
         <v>1217957</v>
       </c>
-      <c r="Q12" s="3"/>
+      <c r="Q12" s="22"/>
       <c r="R12" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>1217957</v>
@@ -3103,7 +3414,7 @@
         <f>SUM(C13:N13)</f>
         <v>4530257</v>
       </c>
-      <c r="Q13" s="3"/>
+      <c r="Q13" s="22"/>
       <c r="R13" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>4530257</v>
@@ -3157,7 +3468,7 @@
         <f>SUM(C14:N14)</f>
         <v>7693253</v>
       </c>
-      <c r="Q14" s="3"/>
+      <c r="Q14" s="22"/>
       <c r="R14" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>7693253</v>
@@ -3170,7 +3481,9 @@
       <c r="B15" s="13">
         <v>2018</v>
       </c>
-      <c r="C15" s="10"/>
+      <c r="C15" s="12">
+        <v>628028</v>
+      </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -3185,37 +3498,37 @@
       <c r="O15" s="14"/>
       <c r="P15" s="14">
         <f>SUM(C15:N15)</f>
-        <v>0</v>
-      </c>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="7" t="e">
+        <v>628028</v>
+      </c>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>#DIV/0!</v>
+        <v>7536336</v>
       </c>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
     </row>
     <row r="16" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="19"/>
-      <c r="O16" s="19"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="21"/>
       <c r="P16" s="15">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>17551444</v>
-      </c>
-      <c r="Q16" s="3"/>
+        <v>18179472</v>
+      </c>
+      <c r="Q16" s="22"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
@@ -3236,24 +3549,24 @@
       <c r="N17" s="16"/>
       <c r="O17" s="16"/>
       <c r="P17" s="16"/>
-      <c r="Q17" s="1"/>
+      <c r="Q17" s="24"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
     </row>
     <row r="18" spans="1:20" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="20">
-        <f>SUM(P14)</f>
-        <v>7693253</v>
-      </c>
-      <c r="G18" s="20"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="18">
+        <f>SUM(D14:N14,C15)</f>
+        <v>7658858</v>
+      </c>
+      <c r="G18" s="18"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
@@ -3959,7 +4272,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="P5:P14" formulaRange="1"/>
+    <ignoredError sqref="P5:P14 F18" formulaRange="1"/>
     <ignoredError sqref="P4" calculatedColumn="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Blog Statistics (March 2018)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,21 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19020"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud Storage\OneDrive\GIT Hub\kunal-chowdhury.com\blog-stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="40FDE6E5555299D8B362937CCDD5C9106F5153E0" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{3C50D6C9-A861-4D1C-A717-246172F55FF3}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="40FDE6E5555299D8B362937CCDD5C9106F5153E0" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{1E56DB3E-D690-4E1A-BFFE-B3E87DFF7B18}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -276,34 +283,26 @@
     <xf numFmtId="3" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="3" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="18">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -316,6 +315,14 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1133,7 +1140,7 @@
                   <c:v>7693253</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7536336</c:v>
+                  <c:v>8214448</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1696,7 +1703,7 @@
                   <c:v>7693253</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>628028</c:v>
+                  <c:v>2053612</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2457,8 +2464,8 @@
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Column15" dataDxfId="2">
       <calculatedColumnFormula>SUM(C4:N4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Column152" dataDxfId="0" dataCellStyle="Normal"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Column16" dataDxfId="1">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Column152" dataDxfId="1" dataCellStyle="Normal"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Column16" dataDxfId="0">
       <calculatedColumnFormula>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2789,8 +2796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="X13" sqref="X13"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AB4" sqref="AB4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2844,7 +2851,7 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
-      <c r="Q2" s="22"/>
+      <c r="Q2" s="18"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -2896,7 +2903,7 @@
       <c r="P3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" s="22" t="s">
+      <c r="Q3" s="18" t="s">
         <v>29</v>
       </c>
       <c r="R3" s="2" t="s">
@@ -2946,7 +2953,7 @@
       <c r="P4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="Q4" s="22"/>
+      <c r="Q4" s="18"/>
       <c r="R4" s="7" t="e">
         <f>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>#VALUE!</v>
@@ -2982,7 +2989,7 @@
         <f>SUM(C5:N5)</f>
         <v>326</v>
       </c>
-      <c r="Q5" s="22"/>
+      <c r="Q5" s="18"/>
       <c r="R5" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>326</v>
@@ -3036,7 +3043,7 @@
         <f t="shared" ref="P6:P12" si="0">SUM(C6:N6)</f>
         <v>80379</v>
       </c>
-      <c r="Q6" s="22"/>
+      <c r="Q6" s="18"/>
       <c r="R6" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>80379</v>
@@ -3090,7 +3097,7 @@
         <f t="shared" si="0"/>
         <v>463113</v>
       </c>
-      <c r="Q7" s="22"/>
+      <c r="Q7" s="18"/>
       <c r="R7" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>463113</v>
@@ -3144,7 +3151,7 @@
         <f t="shared" si="0"/>
         <v>803010</v>
       </c>
-      <c r="Q8" s="22"/>
+      <c r="Q8" s="18"/>
       <c r="R8" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>803010</v>
@@ -3198,7 +3205,7 @@
         <f t="shared" si="0"/>
         <v>888853</v>
       </c>
-      <c r="Q9" s="22"/>
+      <c r="Q9" s="18"/>
       <c r="R9" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>888853</v>
@@ -3252,7 +3259,7 @@
         <f t="shared" si="0"/>
         <v>935657</v>
       </c>
-      <c r="Q10" s="22"/>
+      <c r="Q10" s="18"/>
       <c r="R10" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>935657</v>
@@ -3306,7 +3313,7 @@
         <f t="shared" si="0"/>
         <v>938639</v>
       </c>
-      <c r="Q11" s="22"/>
+      <c r="Q11" s="18"/>
       <c r="R11" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>938639</v>
@@ -3360,7 +3367,7 @@
         <f t="shared" si="0"/>
         <v>1217957</v>
       </c>
-      <c r="Q12" s="22"/>
+      <c r="Q12" s="18"/>
       <c r="R12" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>1217957</v>
@@ -3414,7 +3421,7 @@
         <f>SUM(C13:N13)</f>
         <v>4530257</v>
       </c>
-      <c r="Q13" s="22"/>
+      <c r="Q13" s="18"/>
       <c r="R13" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>4530257</v>
@@ -3468,7 +3475,7 @@
         <f>SUM(C14:N14)</f>
         <v>7693253</v>
       </c>
-      <c r="Q14" s="22"/>
+      <c r="Q14" s="18"/>
       <c r="R14" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>7693253</v>
@@ -3484,8 +3491,12 @@
       <c r="C15" s="12">
         <v>628028</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
+      <c r="D15" s="12">
+        <v>728208</v>
+      </c>
+      <c r="E15" s="12">
+        <v>697376</v>
+      </c>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
@@ -3498,37 +3509,37 @@
       <c r="O15" s="14"/>
       <c r="P15" s="14">
         <f>SUM(C15:N15)</f>
-        <v>628028</v>
-      </c>
-      <c r="Q15" s="23"/>
+        <v>2053612</v>
+      </c>
+      <c r="Q15" s="19"/>
       <c r="R15" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>7536336</v>
+        <v>8214448</v>
       </c>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
     </row>
     <row r="16" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21"/>
-      <c r="O16" s="21"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="22"/>
+      <c r="N16" s="22"/>
+      <c r="O16" s="22"/>
       <c r="P16" s="15">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>18179472</v>
-      </c>
-      <c r="Q16" s="22"/>
+        <v>19605056</v>
+      </c>
+      <c r="Q16" s="18"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
@@ -3549,24 +3560,23 @@
       <c r="N17" s="16"/>
       <c r="O17" s="16"/>
       <c r="P17" s="16"/>
-      <c r="Q17" s="24"/>
+      <c r="Q17" s="20"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
     </row>
     <row r="18" spans="1:20" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="18">
-        <f>SUM(D14:N14,C15)</f>
-        <v>7658858</v>
-      </c>
-      <c r="G18" s="18"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="23">
+        <v>7871803</v>
+      </c>
+      <c r="G18" s="23"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
@@ -4272,7 +4282,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="P5:P14 F18" formulaRange="1"/>
+    <ignoredError sqref="P5:P14" formulaRange="1"/>
     <ignoredError sqref="P4" calculatedColumn="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Blog Statistics (May 2018) Updated
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud Storage\OneDrive\GIT Hub\kunal-chowdhury.com\blog-stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="40FDE6E5555299D8B362937CCDD5C9106F5153E0" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{1E56DB3E-D690-4E1A-BFFE-B3E87DFF7B18}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="40FDE6E5555299D8B362937CCDD5C9106F5153E0" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{4131B706-8E8B-4C2D-8AF3-48F6D4667410}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,6 +20,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -619,7 +620,7 @@
             <a:ln w="31750" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4">
-                  <a:shade val="65000"/>
+                  <a:shade val="76000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -766,395 +767,8 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>Series2</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="3175" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="6"/>
-            <c:spPr>
-              <a:gradFill rotWithShape="1">
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent4">
-                      <a:tint val="65000"/>
-                      <a:shade val="51000"/>
-                      <a:satMod val="130000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="80000">
-                    <a:schemeClr val="accent4">
-                      <a:tint val="65000"/>
-                      <a:shade val="93000"/>
-                      <a:satMod val="130000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent4">
-                      <a:tint val="65000"/>
-                      <a:shade val="94000"/>
-                      <a:satMod val="135000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="16200000" scaled="0"/>
-              </a:gradFill>
-              <a:ln w="3175">
-                <a:solidFill>
-                  <a:schemeClr val="bg1">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="9"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="6"/>
-              <c:spPr>
-                <a:gradFill rotWithShape="1">
-                  <a:gsLst>
-                    <a:gs pos="0">
-                      <a:schemeClr val="accent4">
-                        <a:tint val="65000"/>
-                        <a:shade val="51000"/>
-                        <a:satMod val="130000"/>
-                      </a:schemeClr>
-                    </a:gs>
-                    <a:gs pos="80000">
-                      <a:schemeClr val="accent4">
-                        <a:tint val="65000"/>
-                        <a:shade val="93000"/>
-                        <a:satMod val="130000"/>
-                      </a:schemeClr>
-                    </a:gs>
-                    <a:gs pos="100000">
-                      <a:schemeClr val="accent4">
-                        <a:tint val="65000"/>
-                        <a:shade val="94000"/>
-                        <a:satMod val="135000"/>
-                      </a:schemeClr>
-                    </a:gs>
-                  </a:gsLst>
-                  <a:lin ang="16200000" scaled="0"/>
-                </a:gradFill>
-                <a:ln w="12700">
-                  <a:solidFill>
-                    <a:schemeClr val="bg1">
-                      <a:lumMod val="75000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:prstDash val="lgDash"/>
-                  <a:round/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:ln w="12700" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="bg1">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:prstDash val="lgDash"/>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000C-F234-47AE-98F4-23124B27C96C}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000C-094D-4ED5-9227-CC4EE8D01624}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000B-094D-4ED5-9227-CC4EE8D01624}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000A-094D-4ED5-9227-CC4EE8D01624}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000009-094D-4ED5-9227-CC4EE8D01624}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000008-094D-4ED5-9227-CC4EE8D01624}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000007-094D-4ED5-9227-CC4EE8D01624}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="6"/>
-              <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000006-094D-4ED5-9227-CC4EE8D01624}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="7"/>
-              <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000005-094D-4ED5-9227-CC4EE8D01624}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="8"/>
-              <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000004-094D-4ED5-9227-CC4EE8D01624}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="9"/>
-              <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000C-F234-47AE-98F4-23124B27C96C}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="10"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-1.9685379365382342E-2"/>
-                  <c:y val="-0.1640014521439222"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-094D-4ED5-9227-CC4EE8D01624}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx2"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="tx2">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$5:$B$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>2008</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2009</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2010</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2011</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2012</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2013</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2014</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2016</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2017</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2018</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$R$5:$R$15</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>326</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>80379</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>463113</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>803010</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>888853</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>935657</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>938639</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1217957</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4530257</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7693253</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>8214448</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F234-47AE-98F4-23124B27C96C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="2"/>
           <c:tx>
             <c:v>Series3</c:v>
           </c:tx>
@@ -1498,8 +1112,8 @@
               <c:idx val="10"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0"/>
-                  <c:y val="-0.47877843287177291"/>
+                  <c:x val="-2.0622540149437904E-16"/>
+                  <c:y val="-0.27509921004786952"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -1703,7 +1317,7 @@
                   <c:v>7693253</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2053612</c:v>
+                  <c:v>3520552</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2382,64 +1996,6 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>773905</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>59530</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1893093" cy="342786"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E07368B-A589-4B45-B521-F28735D4E821}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6738936" y="4714874"/>
-          <a:ext cx="1893093" cy="342786"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600"/>
-            <a:t>Projected (2018): </a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2796,8 +2352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AB4" sqref="AB4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3497,8 +3053,12 @@
       <c r="E15" s="12">
         <v>697376</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
+      <c r="F15" s="12">
+        <v>707376</v>
+      </c>
+      <c r="G15" s="12">
+        <v>759564</v>
+      </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
@@ -3509,12 +3069,12 @@
       <c r="O15" s="14"/>
       <c r="P15" s="14">
         <f>SUM(C15:N15)</f>
-        <v>2053612</v>
+        <v>3520552</v>
       </c>
       <c r="Q15" s="19"/>
       <c r="R15" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>8214448</v>
+        <v>8449324.8000000007</v>
       </c>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
@@ -3537,7 +3097,7 @@
       <c r="O16" s="22"/>
       <c r="P16" s="15">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>19605056</v>
+        <v>21071996</v>
       </c>
       <c r="Q16" s="18"/>
       <c r="R16" s="1"/>
@@ -3574,7 +3134,7 @@
       <c r="D18" s="24"/>
       <c r="E18" s="24"/>
       <c r="F18" s="23">
-        <v>7871803</v>
+        <v>7919994</v>
       </c>
       <c r="G18" s="23"/>
       <c r="H18" s="3"/>

</xml_diff>

<commit_message>
Blog Statistics (August 2018)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud Storage\OneDrive\GIT Hub\kunal-chowdhury.com\blog-stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="40FDE6E5555299D8B362937CCDD5C9106F5153E0" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{4131B706-8E8B-4C2D-8AF3-48F6D4667410}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="40FDE6E5555299D8B362937CCDD5C9106F5153E0" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{46E61B2A-06FE-402E-9BF8-C34E0D28A6F7}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1317,7 +1316,7 @@
                   <c:v>7693253</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3520552</c:v>
+                  <c:v>5353193</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2352,8 +2351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AA14" sqref="AA14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3059,9 +3058,15 @@
       <c r="G15" s="12">
         <v>759564</v>
       </c>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
+      <c r="H15" s="12">
+        <v>592381</v>
+      </c>
+      <c r="I15" s="12">
+        <v>545423</v>
+      </c>
+      <c r="J15" s="12">
+        <v>694837</v>
+      </c>
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
@@ -3069,12 +3074,12 @@
       <c r="O15" s="14"/>
       <c r="P15" s="14">
         <f>SUM(C15:N15)</f>
-        <v>3520552</v>
+        <v>5353193</v>
       </c>
       <c r="Q15" s="19"/>
       <c r="R15" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>8449324.8000000007</v>
+        <v>8029789.5</v>
       </c>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
@@ -3097,7 +3102,7 @@
       <c r="O16" s="22"/>
       <c r="P16" s="15">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>21071996</v>
+        <v>22904637</v>
       </c>
       <c r="Q16" s="18"/>
       <c r="R16" s="1"/>
@@ -3134,7 +3139,7 @@
       <c r="D18" s="24"/>
       <c r="E18" s="24"/>
       <c r="F18" s="23">
-        <v>7919994</v>
+        <v>7731568</v>
       </c>
       <c r="G18" s="23"/>
       <c r="H18" s="3"/>

</xml_diff>

<commit_message>
Blog Statistics (October 2018)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud Storage\OneDrive\GIT Hub\kunal-chowdhury.com\blog-stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="40FDE6E5555299D8B362937CCDD5C9106F5153E0" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{46E61B2A-06FE-402E-9BF8-C34E0D28A6F7}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="40FDE6E5555299D8B362937CCDD5C9106F5153E0" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{7C0E6AF3-04FC-41D6-B3DE-90179F57629E}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,6 +20,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1316,7 +1319,7 @@
                   <c:v>7693253</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5353193</c:v>
+                  <c:v>6116926</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2352,7 +2355,7 @@
   <dimension ref="A1:T49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AA14" sqref="AA14"/>
+      <selection activeCell="Z30" sqref="Z30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3067,19 +3070,21 @@
       <c r="J15" s="12">
         <v>694837</v>
       </c>
-      <c r="K15" s="10"/>
+      <c r="K15" s="12">
+        <v>763733</v>
+      </c>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
       <c r="O15" s="14"/>
       <c r="P15" s="14">
         <f>SUM(C15:N15)</f>
-        <v>5353193</v>
+        <v>6116926</v>
       </c>
       <c r="Q15" s="19"/>
       <c r="R15" s="7">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>8029789.5</v>
+        <v>8155901.333333333</v>
       </c>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
@@ -3102,7 +3107,7 @@
       <c r="O16" s="22"/>
       <c r="P16" s="15">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>22904637</v>
+        <v>23668370</v>
       </c>
       <c r="Q16" s="18"/>
       <c r="R16" s="1"/>
@@ -3139,7 +3144,7 @@
       <c r="D18" s="24"/>
       <c r="E18" s="24"/>
       <c r="F18" s="23">
-        <v>7731568</v>
+        <v>7917706</v>
       </c>
       <c r="G18" s="23"/>
       <c r="H18" s="3"/>

</xml_diff>

<commit_message>
Blog Statistics (November 2018)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud Storage\OneDrive\GIT Hub\kunal-chowdhury.com\blog-stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="112" documentId="40FDE6E5555299D8B362937CCDD5C9106F5153E0" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{914B064E-770D-4295-9DC0-7DC3848D10D9}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="114_{74F32795-CFBC-4D92-BE50-BF4880A80A36}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{7A06BCE4-DC1C-4BD5-8F31-BCFAAC6F4511}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -283,12 +283,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -310,14 +304,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="3" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1337,7 +1337,7 @@
                   <c:v>7693253</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6856582</c:v>
+                  <c:v>7555544</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2373,7 +2373,7 @@
   <dimension ref="A1:T49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Y25" sqref="Y25"/>
+      <selection activeCell="AA13" sqref="AA13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2486,56 +2486,56 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:20" s="25" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="21" t="s">
+    <row r="4" spans="1:20" s="23" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="I4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="J4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="21" t="s">
+      <c r="K4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="21" t="s">
+      <c r="L4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="21" t="s">
+      <c r="M4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="21" t="s">
+      <c r="N4" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22" t="s">
+      <c r="O4" s="20"/>
+      <c r="P4" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="24" t="e">
+      <c r="Q4" s="21"/>
+      <c r="R4" s="22" t="e">
         <f>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="S4" s="19"/>
-      <c r="T4" s="19"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
     </row>
     <row r="5" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
@@ -3094,45 +3094,47 @@
       <c r="L15" s="9">
         <v>763733</v>
       </c>
-      <c r="M15" s="7"/>
+      <c r="M15" s="9">
+        <v>698962</v>
+      </c>
       <c r="N15" s="7"/>
       <c r="O15" s="11"/>
       <c r="P15" s="11">
         <f>SUM(C15:N15)</f>
-        <v>6856582</v>
+        <v>7555544</v>
       </c>
       <c r="Q15" s="15"/>
       <c r="R15" s="4">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>8227898.4000000004</v>
+        <v>8242411.6363636367</v>
       </c>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
     </row>
-    <row r="16" spans="1:20" s="25" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="27"/>
-      <c r="N16" s="27"/>
-      <c r="O16" s="27"/>
-      <c r="P16" s="28">
+    <row r="16" spans="1:20" s="23" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="17"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="26"/>
+      <c r="O16" s="26"/>
+      <c r="P16" s="24">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>24408026</v>
-      </c>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="19"/>
-      <c r="S16" s="19"/>
-      <c r="T16" s="19"/>
+        <v>25106988</v>
+      </c>
+      <c r="Q16" s="21"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="17"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B17" s="12"/>
@@ -3157,16 +3159,16 @@
     </row>
     <row r="18" spans="1:20" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="17">
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="27">
         <v>7991390</v>
       </c>
-      <c r="G18" s="17"/>
+      <c r="G18" s="27"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>

</xml_diff>

<commit_message>
Blog Statistics (December 2018)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21220"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud Storage\OneDrive\GIT Hub\kunal-chowdhury.com\blog-stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="114_{74F32795-CFBC-4D92-BE50-BF4880A80A36}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{7A06BCE4-DC1C-4BD5-8F31-BCFAAC6F4511}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="114_{74F32795-CFBC-4D92-BE50-BF4880A80A36}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{DD3472A5-26BD-45A0-B459-193CCE0F1198}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -129,7 +129,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,6 +180,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -213,7 +219,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -259,6 +265,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -267,22 +286,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -295,7 +312,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -310,15 +327,17 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,10 +590,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="106"/>
+      <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="6"/>
+      <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -636,12 +655,13 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Year</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="31750" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:shade val="76000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -660,19 +680,19 @@
               <a:gradFill rotWithShape="1">
                 <a:gsLst>
                   <a:gs pos="0">
-                    <a:schemeClr val="accent4">
+                    <a:schemeClr val="accent1">
                       <a:shade val="51000"/>
                       <a:satMod val="130000"/>
                     </a:schemeClr>
                   </a:gs>
                   <a:gs pos="80000">
-                    <a:schemeClr val="accent4">
+                    <a:schemeClr val="accent1">
                       <a:shade val="93000"/>
                       <a:satMod val="130000"/>
                     </a:schemeClr>
                   </a:gs>
                   <a:gs pos="100000">
-                    <a:schemeClr val="accent4">
+                    <a:schemeClr val="accent1">
                       <a:shade val="94000"/>
                       <a:satMod val="135000"/>
                     </a:schemeClr>
@@ -697,10 +717,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$15</c:f>
+              <c:f>Sheet1!$B$5:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>2008</c:v>
                 </c:pt>
@@ -733,16 +753,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2019</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$15</c:f>
+              <c:f>Sheet1!$B$5:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>2008</c:v>
                 </c:pt>
@@ -775,6 +798,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2019</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -790,12 +816,12 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Series3</c:v>
+            <c:v>Blog Hit / Pageviews</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="31750" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -814,19 +840,19 @@
               <a:gradFill rotWithShape="1">
                 <a:gsLst>
                   <a:gs pos="0">
-                    <a:schemeClr val="accent4">
+                    <a:schemeClr val="accent2">
                       <a:shade val="51000"/>
                       <a:satMod val="130000"/>
                     </a:schemeClr>
                   </a:gs>
                   <a:gs pos="80000">
-                    <a:schemeClr val="accent4">
+                    <a:schemeClr val="accent2">
                       <a:shade val="93000"/>
                       <a:satMod val="130000"/>
                     </a:schemeClr>
                   </a:gs>
                   <a:gs pos="100000">
-                    <a:schemeClr val="accent4">
+                    <a:schemeClr val="accent2">
                       <a:shade val="94000"/>
                       <a:satMod val="135000"/>
                     </a:schemeClr>
@@ -836,7 +862,7 @@
               </a:gradFill>
               <a:ln w="12700">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="lt2"/>
                 </a:solidFill>
                 <a:round/>
               </a:ln>
@@ -1144,7 +1170,7 @@
                   <a:lstStyle/>
                   <a:p>
                     <a:pPr>
-                      <a:defRPr sz="2800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                         <a:solidFill>
                           <a:schemeClr val="tx2"/>
                         </a:solidFill>
@@ -1154,9 +1180,9 @@
                       </a:defRPr>
                     </a:pPr>
                     <a:fld id="{D7A76F95-4772-4256-A17D-4758AD75F025}" type="VALUE">
-                      <a:rPr lang="en-US" sz="1800" b="1"/>
+                      <a:rPr lang="en-US" sz="1400" b="0"/>
                       <a:pPr>
-                        <a:defRPr sz="2800" b="1"/>
+                        <a:defRPr sz="1400" b="0"/>
                       </a:pPr>
                       <a:t>[VALUE]</a:t>
                     </a:fld>
@@ -1178,7 +1204,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="2800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx2"/>
                       </a:solidFill>
@@ -1203,6 +1229,53 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-094D-4ED5-9227-CC4EE8D01624}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.4060985260985325E-3"/>
+                  <c:y val="-7.4065171935964971E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-4E3A-49ED-AF1F-326603D91C04}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1260,10 +1333,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$15</c:f>
+              <c:f>Sheet1!$B$5:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>2008</c:v>
                 </c:pt>
@@ -1296,16 +1369,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2019</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$5:$P$15</c:f>
+              <c:f>Sheet1!$P$5:$P$16</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>326</c:v>
                 </c:pt>
@@ -1337,7 +1413,10 @@
                   <c:v>7693253</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7555544</c:v>
+                  <c:v>8287717</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1357,6 +1436,20 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:dropLines>
+          <c:spPr>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:dropLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="84979784"/>
@@ -1504,8 +1597,42 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="17">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
   <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
 </cs:colorStyle>
 </file>
 
@@ -1984,13 +2111,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>21429</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>23811</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>88107</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>62488</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2020,8 +2147,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B3:R15" totalsRowShown="0" dataDxfId="17">
-  <autoFilter ref="B3:R15" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B3:R16" totalsRowShown="0" dataDxfId="17">
+  <autoFilter ref="B3:R16" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1" dataDxfId="16"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2" dataDxfId="15"/>
@@ -2370,10 +2497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T49"/>
+  <dimension ref="A1:T50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AA13" sqref="AA13"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="X36" sqref="X36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2427,7 +2554,7 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
-      <c r="Q2" s="14"/>
+      <c r="Q2" s="13"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -2479,94 +2606,94 @@
       <c r="P3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" s="14" t="s">
+      <c r="Q3" s="13" t="s">
         <v>29</v>
       </c>
       <c r="R3" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:20" s="23" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="19" t="s">
+    <row r="4" spans="1:20" s="21" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="19" t="s">
+      <c r="K4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="19" t="s">
+      <c r="L4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="19" t="s">
+      <c r="M4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="19" t="s">
+      <c r="N4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20" t="s">
+      <c r="O4" s="18"/>
+      <c r="P4" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="22" t="e">
+      <c r="Q4" s="19"/>
+      <c r="R4" s="20" t="e">
         <f>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="S4" s="17"/>
-      <c r="T4" s="17"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>2008</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="7">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="6">
         <v>105</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5" s="6">
         <v>112</v>
       </c>
-      <c r="N5" s="7">
+      <c r="N5" s="6">
         <v>109</v>
       </c>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7">
+      <c r="O5" s="6"/>
+      <c r="P5" s="6">
         <f>SUM(C5:N5)</f>
         <v>326</v>
       </c>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="4">
+      <c r="Q5" s="13"/>
+      <c r="R5" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>326</v>
       </c>
@@ -2575,52 +2702,52 @@
     </row>
     <row r="6" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>2009</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>210</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <v>265</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>330</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <v>459</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="6">
         <v>2711</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="6">
         <v>4347</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="6">
         <v>7134</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="6">
         <v>7452</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="6">
         <v>10193</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6" s="6">
         <v>11773</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M6" s="6">
         <v>16989</v>
       </c>
-      <c r="N6" s="7">
+      <c r="N6" s="6">
         <v>18516</v>
       </c>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7">
+      <c r="O6" s="6"/>
+      <c r="P6" s="6">
         <f t="shared" ref="P6:P12" si="0">SUM(C6:N6)</f>
         <v>80379</v>
       </c>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="4">
+      <c r="Q6" s="13"/>
+      <c r="R6" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>80379</v>
       </c>
@@ -2629,52 +2756,52 @@
     </row>
     <row r="7" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>2010</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>16660</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>23673</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>32985</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <v>35222</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <v>39909</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="6">
         <v>42087</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="6">
         <v>54395</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="6">
         <v>49067</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="6">
         <v>47658</v>
       </c>
-      <c r="L7" s="7">
+      <c r="L7" s="6">
         <v>38853</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M7" s="6">
         <v>39946</v>
       </c>
-      <c r="N7" s="7">
+      <c r="N7" s="6">
         <v>42658</v>
       </c>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7">
+      <c r="O7" s="6"/>
+      <c r="P7" s="6">
         <f t="shared" si="0"/>
         <v>463113</v>
       </c>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="4">
+      <c r="Q7" s="13"/>
+      <c r="R7" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>463113</v>
       </c>
@@ -2683,52 +2810,52 @@
     </row>
     <row r="8" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>2011</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <v>45551</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="6">
         <v>69346</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <v>47856</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <v>64728</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <v>73308</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="6">
         <v>82846</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="6">
         <v>72286</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="6">
         <v>75867</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="6">
         <v>80961</v>
       </c>
-      <c r="L8" s="7">
+      <c r="L8" s="6">
         <v>62233</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="6">
         <v>63447</v>
       </c>
-      <c r="N8" s="7">
+      <c r="N8" s="6">
         <v>64581</v>
       </c>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7">
+      <c r="O8" s="6"/>
+      <c r="P8" s="6">
         <f t="shared" si="0"/>
         <v>803010</v>
       </c>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="4">
+      <c r="Q8" s="13"/>
+      <c r="R8" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>803010</v>
       </c>
@@ -2737,52 +2864,52 @@
     </row>
     <row r="9" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>2012</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>76072</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>77385</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <v>70852</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <v>72356</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <v>78593</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="6">
         <v>70155</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="6">
         <v>72470</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="6">
         <v>70252</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="6">
         <v>79738</v>
       </c>
-      <c r="L9" s="7">
+      <c r="L9" s="6">
         <v>71284</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M9" s="6">
         <v>76524</v>
       </c>
-      <c r="N9" s="7">
+      <c r="N9" s="6">
         <v>73172</v>
       </c>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7">
+      <c r="O9" s="6"/>
+      <c r="P9" s="6">
         <f t="shared" si="0"/>
         <v>888853</v>
       </c>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="4">
+      <c r="Q9" s="13"/>
+      <c r="R9" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>888853</v>
       </c>
@@ -2791,52 +2918,52 @@
     </row>
     <row r="10" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>2013</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>78648</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="6">
         <v>74894</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="6">
         <v>86029</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="6">
         <v>82489</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="6">
         <v>80316</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="6">
         <v>78764</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="6">
         <v>70746</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="6">
         <v>79324</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="6">
         <v>79148</v>
       </c>
-      <c r="L10" s="7">
+      <c r="L10" s="6">
         <v>76345</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M10" s="6">
         <v>75329</v>
       </c>
-      <c r="N10" s="7">
+      <c r="N10" s="6">
         <v>73625</v>
       </c>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7">
+      <c r="O10" s="6"/>
+      <c r="P10" s="6">
         <f t="shared" si="0"/>
         <v>935657</v>
       </c>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="4">
+      <c r="Q10" s="13"/>
+      <c r="R10" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>935657</v>
       </c>
@@ -2845,52 +2972,52 @@
     </row>
     <row r="11" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>2014</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>67510</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="6">
         <v>67706</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="6">
         <v>73924</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <v>71449</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="6">
         <v>79877</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="6">
         <v>74705</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="6">
         <v>79936</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="6">
         <v>78746</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="6">
         <v>77891</v>
       </c>
-      <c r="L11" s="7">
+      <c r="L11" s="6">
         <v>77040</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M11" s="6">
         <v>87951</v>
       </c>
-      <c r="N11" s="8">
+      <c r="N11" s="7">
         <v>101904</v>
       </c>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7">
+      <c r="O11" s="6"/>
+      <c r="P11" s="6">
         <f t="shared" si="0"/>
         <v>938639</v>
       </c>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="4">
+      <c r="Q11" s="13"/>
+      <c r="R11" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>938639</v>
       </c>
@@ -2899,52 +3026,52 @@
     </row>
     <row r="12" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <v>2015</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <v>90536</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <v>80976</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <v>95444</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <v>71951</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="6">
         <v>67019</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="6">
         <v>66244</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="6">
         <v>86294</v>
       </c>
-      <c r="J12" s="8">
+      <c r="J12" s="7">
         <v>128005</v>
       </c>
-      <c r="K12" s="8">
+      <c r="K12" s="7">
         <v>137300</v>
       </c>
-      <c r="L12" s="8">
+      <c r="L12" s="7">
         <v>138705</v>
       </c>
-      <c r="M12" s="8">
+      <c r="M12" s="7">
         <v>125538</v>
       </c>
-      <c r="N12" s="8">
+      <c r="N12" s="7">
         <v>129945</v>
       </c>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7">
+      <c r="O12" s="6"/>
+      <c r="P12" s="6">
         <f t="shared" si="0"/>
         <v>1217957</v>
       </c>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="4">
+      <c r="Q12" s="13"/>
+      <c r="R12" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>1217957</v>
       </c>
@@ -2953,52 +3080,52 @@
     </row>
     <row r="13" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <v>2016</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="7">
         <v>142274</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="7">
         <v>123093</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="7">
         <v>147266</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="7">
         <v>152612</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="7">
         <v>134497</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="7">
         <v>132768</v>
       </c>
-      <c r="I13" s="9">
+      <c r="I13" s="8">
         <v>363723</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J13" s="8">
         <v>702130</v>
       </c>
-      <c r="K13" s="9">
+      <c r="K13" s="8">
         <v>608805</v>
       </c>
-      <c r="L13" s="9">
+      <c r="L13" s="8">
         <v>635500</v>
       </c>
-      <c r="M13" s="9">
+      <c r="M13" s="8">
         <v>713080</v>
       </c>
-      <c r="N13" s="9">
+      <c r="N13" s="8">
         <v>674509</v>
       </c>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7">
+      <c r="O13" s="6"/>
+      <c r="P13" s="6">
         <f>SUM(C13:N13)</f>
         <v>4530257</v>
       </c>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="4">
+      <c r="Q13" s="13"/>
+      <c r="R13" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>4530257</v>
       </c>
@@ -3007,52 +3134,52 @@
     </row>
     <row r="14" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
-      <c r="B14" s="10">
+      <c r="B14" s="9">
         <v>2017</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="8">
         <v>662423</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="8">
         <v>554842</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="8">
         <v>657797</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="8">
         <v>673209</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="8">
         <v>745540</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="8">
         <v>660058</v>
       </c>
-      <c r="I14" s="9">
+      <c r="I14" s="8">
         <v>690513</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J14" s="8">
         <v>670496</v>
       </c>
-      <c r="K14" s="9">
+      <c r="K14" s="8">
         <v>577595</v>
       </c>
-      <c r="L14" s="9">
+      <c r="L14" s="8">
         <v>665972</v>
       </c>
-      <c r="M14" s="9">
+      <c r="M14" s="8">
         <v>569447</v>
       </c>
-      <c r="N14" s="9">
+      <c r="N14" s="8">
         <v>565361</v>
       </c>
-      <c r="O14" s="11"/>
-      <c r="P14" s="11">
+      <c r="O14" s="10"/>
+      <c r="P14" s="10">
         <f>SUM(C14:N14)</f>
         <v>7693253</v>
       </c>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="4">
+      <c r="Q14" s="13"/>
+      <c r="R14" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>7693253</v>
       </c>
@@ -3061,145 +3188,155 @@
     </row>
     <row r="15" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
-      <c r="B15" s="10">
+      <c r="B15" s="9">
         <v>2018</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="8">
         <v>628028</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="8">
         <v>728208</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="8">
         <v>697376</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="8">
         <v>707376</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="8">
         <v>759564</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="8">
         <v>592381</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I15" s="8">
         <v>545423</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J15" s="8">
         <v>694837</v>
       </c>
-      <c r="K15" s="9">
+      <c r="K15" s="8">
         <v>739656</v>
       </c>
-      <c r="L15" s="9">
+      <c r="L15" s="8">
         <v>763733</v>
       </c>
-      <c r="M15" s="9">
+      <c r="M15" s="8">
         <v>698962</v>
       </c>
-      <c r="N15" s="7"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11">
+      <c r="N15" s="8">
+        <v>732173</v>
+      </c>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10">
         <f>SUM(C15:N15)</f>
-        <v>7555544</v>
-      </c>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="4">
+        <v>8287717</v>
+      </c>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>8242411.6363636367</v>
+        <v>8287717</v>
       </c>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
     </row>
-    <row r="16" spans="1:20" s="23" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26"/>
-      <c r="O16" s="26"/>
-      <c r="P16" s="24">
+    <row r="16" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+      <c r="A16" s="1"/>
+      <c r="B16" s="9">
+        <v>2019</v>
+      </c>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="28">
+        <f>SUM(C16:N16)</f>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="3" t="e">
+        <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+    </row>
+    <row r="17" spans="1:20" s="21" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="22">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>25106988</v>
-      </c>
-      <c r="Q16" s="21"/>
-      <c r="R16" s="17"/>
-      <c r="S16" s="17"/>
-      <c r="T16" s="17"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="16"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
-    </row>
-    <row r="18" spans="1:20" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A18" s="1"/>
-      <c r="B18" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="27">
-        <v>7991390</v>
-      </c>
-      <c r="G18" s="27"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="1"/>
+        <v>25839161</v>
+      </c>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="15"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="15"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="13"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
+      <c r="B19" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="25">
+        <v>8287717</v>
+      </c>
+      <c r="G19" s="25"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
@@ -3811,7 +3948,7 @@
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
-      <c r="L47" s="13"/>
+      <c r="L47" s="1"/>
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
@@ -3833,7 +3970,7 @@
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
-      <c r="L48" s="1"/>
+      <c r="L48" s="12"/>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
@@ -3865,11 +4002,33 @@
       <c r="S49" s="1"/>
       <c r="T49" s="1"/>
     </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1"/>
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
+      <c r="Q50" s="1"/>
+      <c r="R50" s="1"/>
+      <c r="S50" s="1"/>
+      <c r="T50" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B16:O16"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B17:O17"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="B19:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Blog Statistics (March 2019)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21220"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21514"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud Storage\OneDrive\GIT Hub\kunal-chowdhury.com\blog-stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="114_{74F32795-CFBC-4D92-BE50-BF4880A80A36}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{DD3472A5-26BD-45A0-B459-193CCE0F1198}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="114_{74F32795-CFBC-4D92-BE50-BF4880A80A36}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{E849284F-6537-4CD2-9941-FE0FF1DFF459}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -129,7 +129,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,6 +185,12 @@
       <sz val="16"/>
       <color rgb="FF002060"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -282,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -324,6 +330,8 @@
     <xf numFmtId="3" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -336,8 +344,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,7 +575,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF66FF33"/>
       <color rgb="FF99FF66"/>
+      <color rgb="FFCCFF99"/>
       <color rgb="FFFFFF99"/>
     </mruColors>
   </colors>
@@ -1164,58 +1173,18 @@
               </c:layout>
               <c:tx>
                 <c:rich>
-                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                    <a:spAutoFit/>
-                  </a:bodyPr>
+                  <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:pPr>
-                      <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx2"/>
-                        </a:solidFill>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:defRPr>
-                    </a:pPr>
                     <a:fld id="{D7A76F95-4772-4256-A17D-4758AD75F025}" type="VALUE">
                       <a:rPr lang="en-US" sz="1400" b="0"/>
-                      <a:pPr>
-                        <a:defRPr sz="1400" b="0"/>
-                      </a:pPr>
+                      <a:pPr/>
                       <a:t>[VALUE]</a:t>
                     </a:fld>
                     <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                  <a:spAutoFit/>
-                </a:bodyPr>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx2"/>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -1236,8 +1205,8 @@
               <c:idx val="11"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="1.4060985260985325E-3"/>
-                  <c:y val="-7.4065171935964971E-2"/>
+                  <c:x val="-8.4365911565924323E-2"/>
+                  <c:y val="-6.3484433087969985E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:spPr>
@@ -1416,7 +1385,7 @@
                   <c:v>8287717</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>2532277</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2499,8 +2468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="X36" sqref="X36"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Y39" sqref="Y39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3101,22 +3070,22 @@
       <c r="H13" s="7">
         <v>132768</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="29">
         <v>363723</v>
       </c>
-      <c r="J13" s="8">
+      <c r="J13" s="29">
         <v>702130</v>
       </c>
-      <c r="K13" s="8">
+      <c r="K13" s="29">
         <v>608805</v>
       </c>
-      <c r="L13" s="8">
+      <c r="L13" s="29">
         <v>635500</v>
       </c>
-      <c r="M13" s="8">
+      <c r="M13" s="29">
         <v>713080</v>
       </c>
-      <c r="N13" s="8">
+      <c r="N13" s="29">
         <v>674509</v>
       </c>
       <c r="O13" s="6"/>
@@ -3137,40 +3106,40 @@
       <c r="B14" s="9">
         <v>2017</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="29">
         <v>662423</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="29">
         <v>554842</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="29">
         <v>657797</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="29">
         <v>673209</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="29">
         <v>745540</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="29">
         <v>660058</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="29">
         <v>690513</v>
       </c>
-      <c r="J14" s="8">
+      <c r="J14" s="29">
         <v>670496</v>
       </c>
-      <c r="K14" s="8">
+      <c r="K14" s="29">
         <v>577595</v>
       </c>
-      <c r="L14" s="8">
+      <c r="L14" s="29">
         <v>665972</v>
       </c>
-      <c r="M14" s="8">
+      <c r="M14" s="29">
         <v>569447</v>
       </c>
-      <c r="N14" s="8">
+      <c r="N14" s="29">
         <v>565361</v>
       </c>
       <c r="O14" s="10"/>
@@ -3191,40 +3160,40 @@
       <c r="B15" s="9">
         <v>2018</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="29">
         <v>628028</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="29">
         <v>728208</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="29">
         <v>697376</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="29">
         <v>707376</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="29">
         <v>759564</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="29">
         <v>592381</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15" s="29">
         <v>545423</v>
       </c>
-      <c r="J15" s="8">
+      <c r="J15" s="29">
         <v>694837</v>
       </c>
-      <c r="K15" s="8">
+      <c r="K15" s="29">
         <v>739656</v>
       </c>
-      <c r="L15" s="8">
+      <c r="L15" s="29">
         <v>763733</v>
       </c>
-      <c r="M15" s="8">
+      <c r="M15" s="29">
         <v>698962</v>
       </c>
-      <c r="N15" s="8">
+      <c r="N15" s="29">
         <v>732173</v>
       </c>
       <c r="O15" s="10"/>
@@ -3245,50 +3214,56 @@
       <c r="B16" s="9">
         <v>2019</v>
       </c>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="27"/>
-      <c r="N16" s="27"/>
-      <c r="O16" s="28"/>
-      <c r="P16" s="28">
+      <c r="C16" s="29">
+        <v>816792</v>
+      </c>
+      <c r="D16" s="29">
+        <v>811807</v>
+      </c>
+      <c r="E16" s="8">
+        <v>903678</v>
+      </c>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="24">
         <f>SUM(C16:N16)</f>
-        <v>0</v>
+        <v>2532277</v>
       </c>
       <c r="Q16" s="14"/>
-      <c r="R16" s="3" t="e">
+      <c r="R16" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>#DIV/0!</v>
+        <v>10129108</v>
       </c>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
     </row>
     <row r="17" spans="1:20" s="21" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="24"/>
-      <c r="M17" s="24"/>
-      <c r="N17" s="24"/>
-      <c r="O17" s="24"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="26"/>
       <c r="P17" s="22">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>25839161</v>
+        <v>28371438</v>
       </c>
       <c r="Q17" s="19"/>
       <c r="R17" s="15"/>
@@ -3318,16 +3293,16 @@
     </row>
     <row r="19" spans="1:20" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="25">
-        <v>8287717</v>
-      </c>
-      <c r="G19" s="25"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="27">
+        <v>8766382</v>
+      </c>
+      <c r="G19" s="27"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>

</xml_diff>

<commit_message>
Blog Statistics (April 2019)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21624"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud Storage\OneDrive\GIT Hub\kunal-chowdhury.com\blog-stats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c93c05515dfe04a/GIT Hub/kunal-chowdhury.com/blog-stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="114_{74F32795-CFBC-4D92-BE50-BF4880A80A36}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{E849284F-6537-4CD2-9941-FE0FF1DFF459}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="114_{74F32795-CFBC-4D92-BE50-BF4880A80A36}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{C732A0A7-1F23-43D3-92BB-3E9ED2D2B31A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -193,7 +193,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,13 +214,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF99FF66"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FFCCFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FF33"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -288,9 +294,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -299,14 +305,13 @@
     </xf>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -338,13 +343,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="8" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -576,8 +583,8 @@
   <colors>
     <mruColors>
       <color rgb="FF66FF33"/>
+      <color rgb="FFCCFF99"/>
       <color rgb="FF99FF66"/>
-      <color rgb="FFCCFF99"/>
       <color rgb="FFFFFF99"/>
     </mruColors>
   </colors>
@@ -1385,7 +1392,7 @@
                   <c:v>8287717</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2532277</c:v>
+                  <c:v>3706549</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2469,14 +2476,16 @@
   <dimension ref="A1:T50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Y39" sqref="Y39"/>
+      <selection activeCell="AB33" sqref="AB33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="2" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" style="2" customWidth="1"/>
-    <col min="3" max="14" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="14" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="4" style="2" customWidth="1"/>
     <col min="16" max="16" width="18.42578125" style="2" customWidth="1"/>
     <col min="17" max="17" width="5.42578125" style="2" customWidth="1"/>
@@ -2523,7 +2532,7 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
-      <c r="Q2" s="13"/>
+      <c r="Q2" s="12"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -2575,63 +2584,63 @@
       <c r="P3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" s="13" t="s">
+      <c r="Q3" s="12" t="s">
         <v>29</v>
       </c>
       <c r="R3" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:20" s="21" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17" t="s">
+    <row r="4" spans="1:20" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="I4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="17" t="s">
+      <c r="J4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="17" t="s">
+      <c r="K4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="17" t="s">
+      <c r="L4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="17" t="s">
+      <c r="M4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="17" t="s">
+      <c r="N4" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="18"/>
-      <c r="P4" s="18" t="s">
+      <c r="O4" s="17"/>
+      <c r="P4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="20" t="e">
+      <c r="Q4" s="18"/>
+      <c r="R4" s="19" t="e">
         <f>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
     </row>
     <row r="5" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
@@ -2661,7 +2670,7 @@
         <f>SUM(C5:N5)</f>
         <v>326</v>
       </c>
-      <c r="Q5" s="13"/>
+      <c r="Q5" s="12"/>
       <c r="R5" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>326</v>
@@ -2715,7 +2724,7 @@
         <f t="shared" ref="P6:P12" si="0">SUM(C6:N6)</f>
         <v>80379</v>
       </c>
-      <c r="Q6" s="13"/>
+      <c r="Q6" s="12"/>
       <c r="R6" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>80379</v>
@@ -2769,7 +2778,7 @@
         <f t="shared" si="0"/>
         <v>463113</v>
       </c>
-      <c r="Q7" s="13"/>
+      <c r="Q7" s="12"/>
       <c r="R7" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>463113</v>
@@ -2823,7 +2832,7 @@
         <f t="shared" si="0"/>
         <v>803010</v>
       </c>
-      <c r="Q8" s="13"/>
+      <c r="Q8" s="12"/>
       <c r="R8" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>803010</v>
@@ -2877,7 +2886,7 @@
         <f t="shared" si="0"/>
         <v>888853</v>
       </c>
-      <c r="Q9" s="13"/>
+      <c r="Q9" s="12"/>
       <c r="R9" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>888853</v>
@@ -2931,7 +2940,7 @@
         <f t="shared" si="0"/>
         <v>935657</v>
       </c>
-      <c r="Q10" s="13"/>
+      <c r="Q10" s="12"/>
       <c r="R10" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>935657</v>
@@ -2985,7 +2994,7 @@
         <f t="shared" si="0"/>
         <v>938639</v>
       </c>
-      <c r="Q11" s="13"/>
+      <c r="Q11" s="12"/>
       <c r="R11" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>938639</v>
@@ -3039,7 +3048,7 @@
         <f t="shared" si="0"/>
         <v>1217957</v>
       </c>
-      <c r="Q12" s="13"/>
+      <c r="Q12" s="12"/>
       <c r="R12" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>1217957</v>
@@ -3070,22 +3079,22 @@
       <c r="H13" s="7">
         <v>132768</v>
       </c>
-      <c r="I13" s="29">
+      <c r="I13" s="28">
         <v>363723</v>
       </c>
-      <c r="J13" s="29">
+      <c r="J13" s="28">
         <v>702130</v>
       </c>
-      <c r="K13" s="29">
+      <c r="K13" s="28">
         <v>608805</v>
       </c>
-      <c r="L13" s="29">
+      <c r="L13" s="28">
         <v>635500</v>
       </c>
-      <c r="M13" s="29">
+      <c r="M13" s="28">
         <v>713080</v>
       </c>
-      <c r="N13" s="29">
+      <c r="N13" s="28">
         <v>674509</v>
       </c>
       <c r="O13" s="6"/>
@@ -3093,7 +3102,7 @@
         <f>SUM(C13:N13)</f>
         <v>4530257</v>
       </c>
-      <c r="Q13" s="13"/>
+      <c r="Q13" s="12"/>
       <c r="R13" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>4530257</v>
@@ -3103,51 +3112,51 @@
     </row>
     <row r="14" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
-      <c r="B14" s="9">
+      <c r="B14" s="8">
         <v>2017</v>
       </c>
-      <c r="C14" s="29">
+      <c r="C14" s="28">
         <v>662423</v>
       </c>
-      <c r="D14" s="29">
+      <c r="D14" s="28">
         <v>554842</v>
       </c>
-      <c r="E14" s="29">
+      <c r="E14" s="28">
         <v>657797</v>
       </c>
-      <c r="F14" s="29">
+      <c r="F14" s="28">
         <v>673209</v>
       </c>
-      <c r="G14" s="29">
+      <c r="G14" s="28">
         <v>745540</v>
       </c>
-      <c r="H14" s="29">
+      <c r="H14" s="28">
         <v>660058</v>
       </c>
-      <c r="I14" s="29">
+      <c r="I14" s="28">
         <v>690513</v>
       </c>
-      <c r="J14" s="29">
+      <c r="J14" s="28">
         <v>670496</v>
       </c>
-      <c r="K14" s="29">
+      <c r="K14" s="28">
         <v>577595</v>
       </c>
-      <c r="L14" s="29">
+      <c r="L14" s="28">
         <v>665972</v>
       </c>
-      <c r="M14" s="29">
+      <c r="M14" s="28">
         <v>569447</v>
       </c>
-      <c r="N14" s="29">
+      <c r="N14" s="28">
         <v>565361</v>
       </c>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10">
+      <c r="O14" s="9"/>
+      <c r="P14" s="9">
         <f>SUM(C14:N14)</f>
         <v>7693253</v>
       </c>
-      <c r="Q14" s="13"/>
+      <c r="Q14" s="12"/>
       <c r="R14" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>7693253</v>
@@ -3157,51 +3166,51 @@
     </row>
     <row r="15" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
-      <c r="B15" s="9">
+      <c r="B15" s="8">
         <v>2018</v>
       </c>
-      <c r="C15" s="29">
+      <c r="C15" s="28">
         <v>628028</v>
       </c>
-      <c r="D15" s="29">
+      <c r="D15" s="28">
         <v>728208</v>
       </c>
-      <c r="E15" s="29">
+      <c r="E15" s="28">
         <v>697376</v>
       </c>
-      <c r="F15" s="29">
+      <c r="F15" s="28">
         <v>707376</v>
       </c>
-      <c r="G15" s="29">
+      <c r="G15" s="28">
         <v>759564</v>
       </c>
-      <c r="H15" s="29">
+      <c r="H15" s="28">
         <v>592381</v>
       </c>
-      <c r="I15" s="29">
+      <c r="I15" s="28">
         <v>545423</v>
       </c>
-      <c r="J15" s="29">
+      <c r="J15" s="28">
         <v>694837</v>
       </c>
-      <c r="K15" s="29">
+      <c r="K15" s="28">
         <v>739656</v>
       </c>
-      <c r="L15" s="29">
+      <c r="L15" s="28">
         <v>763733</v>
       </c>
-      <c r="M15" s="29">
+      <c r="M15" s="28">
         <v>698962</v>
       </c>
-      <c r="N15" s="29">
+      <c r="N15" s="28">
         <v>732173</v>
       </c>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10">
+      <c r="O15" s="9"/>
+      <c r="P15" s="9">
         <f>SUM(C15:N15)</f>
         <v>8287717</v>
       </c>
-      <c r="Q15" s="14"/>
+      <c r="Q15" s="13"/>
       <c r="R15" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>8287717</v>
@@ -3211,98 +3220,100 @@
     </row>
     <row r="16" spans="1:20" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
-      <c r="B16" s="9">
+      <c r="B16" s="8">
         <v>2019</v>
       </c>
-      <c r="C16" s="29">
+      <c r="C16" s="28">
         <v>816792</v>
       </c>
-      <c r="D16" s="29">
+      <c r="D16" s="28">
         <v>811807</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="29">
         <v>903678</v>
       </c>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="23"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="24">
+      <c r="F16" s="30">
+        <v>1174272</v>
+      </c>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="22"/>
+      <c r="N16" s="22"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23">
         <f>SUM(C16:N16)</f>
-        <v>2532277</v>
-      </c>
-      <c r="Q16" s="14"/>
+        <v>3706549</v>
+      </c>
+      <c r="Q16" s="13"/>
       <c r="R16" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>10129108</v>
+        <v>11119647</v>
       </c>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
     </row>
-    <row r="17" spans="1:20" s="21" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="22">
+    <row r="17" spans="1:20" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="21">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>28371438</v>
-      </c>
-      <c r="Q17" s="19"/>
-      <c r="R17" s="15"/>
-      <c r="S17" s="15"/>
-      <c r="T17" s="15"/>
+        <v>29545710</v>
+      </c>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="14"/>
+      <c r="S17" s="14"/>
+      <c r="T17" s="14"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="11"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="13"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="12"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
     </row>
     <row r="19" spans="1:20" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="27">
-        <v>8766382</v>
-      </c>
-      <c r="G19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="26">
+        <v>9233278</v>
+      </c>
+      <c r="G19" s="26"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -3945,7 +3956,7 @@
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
-      <c r="L48" s="12"/>
+      <c r="L48" s="11"/>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>

</xml_diff>

<commit_message>
Blog Statistics (May 2019)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c93c05515dfe04a/GIT Hub/kunal-chowdhury.com/blog-stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="114_{74F32795-CFBC-4D92-BE50-BF4880A80A36}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{C732A0A7-1F23-43D3-92BB-3E9ED2D2B31A}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="114_{74F32795-CFBC-4D92-BE50-BF4880A80A36}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{3C356D4E-1466-4012-878D-F5D94D005257}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -337,6 +337,9 @@
     </xf>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="8" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -349,9 +352,6 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="8" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1392,7 +1392,7 @@
                   <c:v>8287717</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3706549</c:v>
+                  <c:v>5106430</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2476,7 +2476,7 @@
   <dimension ref="A1:T50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AB33" sqref="AB33"/>
+      <selection activeCell="Y20" sqref="Y20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2484,8 +2484,8 @@
     <col min="1" max="1" width="5" style="2" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" style="2" customWidth="1"/>
     <col min="3" max="5" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="14" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="14" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="4" style="2" customWidth="1"/>
     <col min="16" max="16" width="18.42578125" style="2" customWidth="1"/>
     <col min="17" max="17" width="5.42578125" style="2" customWidth="1"/>
@@ -3079,22 +3079,22 @@
       <c r="H13" s="7">
         <v>132768</v>
       </c>
-      <c r="I13" s="28">
+      <c r="I13" s="24">
         <v>363723</v>
       </c>
-      <c r="J13" s="28">
+      <c r="J13" s="24">
         <v>702130</v>
       </c>
-      <c r="K13" s="28">
+      <c r="K13" s="24">
         <v>608805</v>
       </c>
-      <c r="L13" s="28">
+      <c r="L13" s="24">
         <v>635500</v>
       </c>
-      <c r="M13" s="28">
+      <c r="M13" s="24">
         <v>713080</v>
       </c>
-      <c r="N13" s="28">
+      <c r="N13" s="24">
         <v>674509</v>
       </c>
       <c r="O13" s="6"/>
@@ -3115,40 +3115,40 @@
       <c r="B14" s="8">
         <v>2017</v>
       </c>
-      <c r="C14" s="28">
+      <c r="C14" s="24">
         <v>662423</v>
       </c>
-      <c r="D14" s="28">
+      <c r="D14" s="24">
         <v>554842</v>
       </c>
-      <c r="E14" s="28">
+      <c r="E14" s="24">
         <v>657797</v>
       </c>
-      <c r="F14" s="28">
+      <c r="F14" s="24">
         <v>673209</v>
       </c>
-      <c r="G14" s="28">
+      <c r="G14" s="24">
         <v>745540</v>
       </c>
-      <c r="H14" s="28">
+      <c r="H14" s="24">
         <v>660058</v>
       </c>
-      <c r="I14" s="28">
+      <c r="I14" s="24">
         <v>690513</v>
       </c>
-      <c r="J14" s="28">
+      <c r="J14" s="24">
         <v>670496</v>
       </c>
-      <c r="K14" s="28">
+      <c r="K14" s="24">
         <v>577595</v>
       </c>
-      <c r="L14" s="28">
+      <c r="L14" s="24">
         <v>665972</v>
       </c>
-      <c r="M14" s="28">
+      <c r="M14" s="24">
         <v>569447</v>
       </c>
-      <c r="N14" s="28">
+      <c r="N14" s="24">
         <v>565361</v>
       </c>
       <c r="O14" s="9"/>
@@ -3169,40 +3169,40 @@
       <c r="B15" s="8">
         <v>2018</v>
       </c>
-      <c r="C15" s="28">
+      <c r="C15" s="24">
         <v>628028</v>
       </c>
-      <c r="D15" s="28">
+      <c r="D15" s="24">
         <v>728208</v>
       </c>
-      <c r="E15" s="28">
+      <c r="E15" s="24">
         <v>697376</v>
       </c>
-      <c r="F15" s="28">
+      <c r="F15" s="24">
         <v>707376</v>
       </c>
-      <c r="G15" s="28">
+      <c r="G15" s="24">
         <v>759564</v>
       </c>
-      <c r="H15" s="28">
+      <c r="H15" s="24">
         <v>592381</v>
       </c>
-      <c r="I15" s="28">
+      <c r="I15" s="24">
         <v>545423</v>
       </c>
-      <c r="J15" s="28">
+      <c r="J15" s="24">
         <v>694837</v>
       </c>
-      <c r="K15" s="28">
+      <c r="K15" s="24">
         <v>739656</v>
       </c>
-      <c r="L15" s="28">
+      <c r="L15" s="24">
         <v>763733</v>
       </c>
-      <c r="M15" s="28">
+      <c r="M15" s="24">
         <v>698962</v>
       </c>
-      <c r="N15" s="28">
+      <c r="N15" s="24">
         <v>732173</v>
       </c>
       <c r="O15" s="9"/>
@@ -3223,19 +3223,21 @@
       <c r="B16" s="8">
         <v>2019</v>
       </c>
-      <c r="C16" s="28">
+      <c r="C16" s="24">
         <v>816792</v>
       </c>
-      <c r="D16" s="28">
+      <c r="D16" s="24">
         <v>811807</v>
       </c>
-      <c r="E16" s="29">
+      <c r="E16" s="25">
         <v>903678</v>
       </c>
-      <c r="F16" s="30">
+      <c r="F16" s="26">
         <v>1174272</v>
       </c>
-      <c r="G16" s="22"/>
+      <c r="G16" s="26">
+        <v>1399881</v>
+      </c>
       <c r="H16" s="22"/>
       <c r="I16" s="22"/>
       <c r="J16" s="22"/>
@@ -3246,35 +3248,35 @@
       <c r="O16" s="23"/>
       <c r="P16" s="23">
         <f>SUM(C16:N16)</f>
-        <v>3706549</v>
+        <v>5106430</v>
       </c>
       <c r="Q16" s="13"/>
       <c r="R16" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>11119647</v>
+        <v>12255432</v>
       </c>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
     </row>
     <row r="17" spans="1:20" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="25"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="28"/>
       <c r="P17" s="21">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>29545710</v>
+        <v>30945591</v>
       </c>
       <c r="Q17" s="18"/>
       <c r="R17" s="14"/>
@@ -3304,16 +3306,16 @@
     </row>
     <row r="19" spans="1:20" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="26">
-        <v>9233278</v>
-      </c>
-      <c r="G19" s="26"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="29">
+        <v>9873595</v>
+      </c>
+      <c r="G19" s="29"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>

</xml_diff>

<commit_message>
Blog Statistics (July 2019)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21916"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c93c05515dfe04a/GIT Hub/kunal-chowdhury.com/blog-stats/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud Storage\OneDrive\GIT Hub\kunal-chowdhury.com\blog-stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="114_{74F32795-CFBC-4D92-BE50-BF4880A80A36}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{3C356D4E-1466-4012-878D-F5D94D005257}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="114_{74F32795-CFBC-4D92-BE50-BF4880A80A36}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{271B8A1A-4FBE-4143-B8A3-453CC462AB79}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1392,7 +1392,7 @@
                   <c:v>8287717</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5106430</c:v>
+                  <c:v>7665530</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2476,7 +2476,7 @@
   <dimension ref="A1:T50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Y20" sqref="Y20"/>
+      <selection activeCell="W20" sqref="W20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2484,8 +2484,8 @@
     <col min="1" max="1" width="5" style="2" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" style="2" customWidth="1"/>
     <col min="3" max="5" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="14" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="4" style="2" customWidth="1"/>
     <col min="16" max="16" width="18.42578125" style="2" customWidth="1"/>
     <col min="17" max="17" width="5.42578125" style="2" customWidth="1"/>
@@ -3238,8 +3238,12 @@
       <c r="G16" s="26">
         <v>1399881</v>
       </c>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
+      <c r="H16" s="26">
+        <v>1179014</v>
+      </c>
+      <c r="I16" s="26">
+        <v>1380086</v>
+      </c>
       <c r="J16" s="22"/>
       <c r="K16" s="22"/>
       <c r="L16" s="22"/>
@@ -3248,12 +3252,12 @@
       <c r="O16" s="23"/>
       <c r="P16" s="23">
         <f>SUM(C16:N16)</f>
-        <v>5106430</v>
+        <v>7665530</v>
       </c>
       <c r="Q16" s="13"/>
       <c r="R16" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>12255432</v>
+        <v>13140908.571428571</v>
       </c>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
@@ -3276,7 +3280,7 @@
       <c r="O17" s="28"/>
       <c r="P17" s="21">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>30945591</v>
+        <v>33504691</v>
       </c>
       <c r="Q17" s="18"/>
       <c r="R17" s="14"/>
@@ -3313,7 +3317,8 @@
       <c r="D19" s="30"/>
       <c r="E19" s="30"/>
       <c r="F19" s="29">
-        <v>9873595</v>
+        <f>SUM(J15:N15,C16:I16)</f>
+        <v>11294891</v>
       </c>
       <c r="G19" s="29"/>
       <c r="H19" s="1"/>
@@ -4021,7 +4026,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="P5:P14" formulaRange="1"/>
+    <ignoredError sqref="P5:P14 F19" formulaRange="1"/>
     <ignoredError sqref="P4" calculatedColumn="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Blog Statistics (August 2019)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22008"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud Storage\OneDrive\GIT Hub\kunal-chowdhury.com\blog-stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="114_{74F32795-CFBC-4D92-BE50-BF4880A80A36}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{271B8A1A-4FBE-4143-B8A3-453CC462AB79}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="14_{5AA5FF64-5DC9-4691-B4E0-3E88BB220E46}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{BB103818-9A6C-4515-9AFE-1C9A2A7F1841}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1392,7 +1392,7 @@
                   <c:v>8287717</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7665530</c:v>
+                  <c:v>9114416</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2475,8 +2475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="W20" sqref="W20"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="X19" sqref="X19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2484,8 +2484,8 @@
     <col min="1" max="1" width="5" style="2" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" style="2" customWidth="1"/>
     <col min="3" max="5" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="14" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="4" style="2" customWidth="1"/>
     <col min="16" max="16" width="18.42578125" style="2" customWidth="1"/>
     <col min="17" max="17" width="5.42578125" style="2" customWidth="1"/>
@@ -3244,7 +3244,9 @@
       <c r="I16" s="26">
         <v>1380086</v>
       </c>
-      <c r="J16" s="22"/>
+      <c r="J16" s="26">
+        <v>1448886</v>
+      </c>
       <c r="K16" s="22"/>
       <c r="L16" s="22"/>
       <c r="M16" s="22"/>
@@ -3252,12 +3254,12 @@
       <c r="O16" s="23"/>
       <c r="P16" s="23">
         <f>SUM(C16:N16)</f>
-        <v>7665530</v>
+        <v>9114416</v>
       </c>
       <c r="Q16" s="13"/>
       <c r="R16" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>13140908.571428571</v>
+        <v>13671624</v>
       </c>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
@@ -3280,7 +3282,7 @@
       <c r="O17" s="28"/>
       <c r="P17" s="21">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>33504691</v>
+        <v>34953577</v>
       </c>
       <c r="Q17" s="18"/>
       <c r="R17" s="14"/>
@@ -3317,8 +3319,7 @@
       <c r="D19" s="30"/>
       <c r="E19" s="30"/>
       <c r="F19" s="29">
-        <f>SUM(J15:N15,C16:I16)</f>
-        <v>11294891</v>
+        <v>12048940</v>
       </c>
       <c r="G19" s="29"/>
       <c r="H19" s="1"/>
@@ -4026,7 +4027,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="P5:P14 F19" formulaRange="1"/>
+    <ignoredError sqref="P5:P14" formulaRange="1"/>
     <ignoredError sqref="P4" calculatedColumn="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Blog Statistics (September 2019)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22119"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud Storage\OneDrive\GIT Hub\kunal-chowdhury.com\blog-stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="14_{5AA5FF64-5DC9-4691-B4E0-3E88BB220E46}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{BB103818-9A6C-4515-9AFE-1C9A2A7F1841}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B31C5007-284E-4E0B-B58D-FB23AD227A09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1174,8 +1174,8 @@
               <c:idx val="10"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-2.0622540149437904E-16"/>
-                  <c:y val="-0.27509921004786952"/>
+                  <c:x val="-0.18112219012053507"/>
+                  <c:y val="-6.3484433087969888E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -1392,7 +1392,7 @@
                   <c:v>8287717</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9114416</c:v>
+                  <c:v>10621284</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2475,8 +2475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="X19" sqref="X19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2484,8 +2484,8 @@
     <col min="1" max="1" width="5" style="2" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" style="2" customWidth="1"/>
     <col min="3" max="5" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="11" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="4" style="2" customWidth="1"/>
     <col min="16" max="16" width="18.42578125" style="2" customWidth="1"/>
     <col min="17" max="17" width="5.42578125" style="2" customWidth="1"/>
@@ -3247,19 +3247,21 @@
       <c r="J16" s="26">
         <v>1448886</v>
       </c>
-      <c r="K16" s="22"/>
+      <c r="K16" s="26">
+        <v>1506868</v>
+      </c>
       <c r="L16" s="22"/>
       <c r="M16" s="22"/>
       <c r="N16" s="22"/>
       <c r="O16" s="23"/>
       <c r="P16" s="23">
         <f>SUM(C16:N16)</f>
-        <v>9114416</v>
+        <v>10621284</v>
       </c>
       <c r="Q16" s="13"/>
       <c r="R16" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>13671624</v>
+        <v>14161712</v>
       </c>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
@@ -3282,7 +3284,7 @@
       <c r="O17" s="28"/>
       <c r="P17" s="21">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>34953577</v>
+        <v>36460445</v>
       </c>
       <c r="Q17" s="18"/>
       <c r="R17" s="14"/>
@@ -3319,7 +3321,7 @@
       <c r="D19" s="30"/>
       <c r="E19" s="30"/>
       <c r="F19" s="29">
-        <v>12048940</v>
+        <v>12816152</v>
       </c>
       <c r="G19" s="29"/>
       <c r="H19" s="1"/>

</xml_diff>

<commit_message>
Blog Statistics (October 2019)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud Storage\OneDrive\GIT Hub\kunal-chowdhury.com\blog-stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B31C5007-284E-4E0B-B58D-FB23AD227A09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F230394E-DE7A-4CA0-BDF3-B9DC656BF654}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1392,7 +1392,7 @@
                   <c:v>8287717</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10621284</c:v>
+                  <c:v>12383175</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2475,17 +2475,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="S28" sqref="S28"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="2" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" style="2" customWidth="1"/>
     <col min="3" max="5" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="11" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="4" style="2" customWidth="1"/>
     <col min="16" max="16" width="18.42578125" style="2" customWidth="1"/>
     <col min="17" max="17" width="5.42578125" style="2" customWidth="1"/>
@@ -3250,18 +3248,20 @@
       <c r="K16" s="26">
         <v>1506868</v>
       </c>
-      <c r="L16" s="22"/>
+      <c r="L16" s="26">
+        <v>1761891</v>
+      </c>
       <c r="M16" s="22"/>
       <c r="N16" s="22"/>
       <c r="O16" s="23"/>
       <c r="P16" s="23">
         <f>SUM(C16:N16)</f>
-        <v>10621284</v>
+        <v>12383175</v>
       </c>
       <c r="Q16" s="13"/>
       <c r="R16" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>14161712</v>
+        <v>14859810</v>
       </c>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
@@ -3284,7 +3284,7 @@
       <c r="O17" s="28"/>
       <c r="P17" s="21">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>36460445</v>
+        <v>38222336</v>
       </c>
       <c r="Q17" s="18"/>
       <c r="R17" s="14"/>
@@ -3321,7 +3321,7 @@
       <c r="D19" s="30"/>
       <c r="E19" s="30"/>
       <c r="F19" s="29">
-        <v>12816152</v>
+        <v>13814380</v>
       </c>
       <c r="G19" s="29"/>
       <c r="H19" s="1"/>

</xml_diff>

<commit_message>
Blog Statistics (November 2019)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud Storage\OneDrive\GIT Hub\kunal-chowdhury.com\blog-stats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c93c05515dfe04a/GIT Hub/kunal-chowdhury.com/blog-stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F230394E-DE7A-4CA0-BDF3-B9DC656BF654}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="114_{B49989D9-13EE-4EB4-8B18-ED25DB6F8102}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6FFD386F-0F83-4063-9849-78E7FD8FC46C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -129,7 +129,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,8 +192,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -227,6 +232,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF66FF33"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99FF66"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -294,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -352,6 +363,13 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="3" fontId="8" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,9 +600,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF99FF66"/>
       <color rgb="FF66FF33"/>
       <color rgb="FFCCFF99"/>
-      <color rgb="FF99FF66"/>
       <color rgb="FFFFFF99"/>
     </mruColors>
   </colors>
@@ -1392,7 +1410,7 @@
                   <c:v>8287717</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12383175</c:v>
+                  <c:v>14443031</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2087,13 +2105,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>21429</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>23811</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>88107</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>62488</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2123,8 +2141,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B3:R16" totalsRowShown="0" dataDxfId="17">
-  <autoFilter ref="B3:R16" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B3:R17" totalsRowShown="0" dataDxfId="17">
+  <autoFilter ref="B3:R17" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1" dataDxfId="16"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2" dataDxfId="15"/>
@@ -2473,17 +2491,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T50"/>
+  <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="X29" sqref="X29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="2" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" style="2" customWidth="1"/>
     <col min="3" max="5" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="13" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="4" style="2" customWidth="1"/>
     <col min="16" max="16" width="18.42578125" style="2" customWidth="1"/>
     <col min="17" max="17" width="5.42578125" style="2" customWidth="1"/>
@@ -3230,122 +3250,132 @@
       <c r="E16" s="25">
         <v>903678</v>
       </c>
-      <c r="F16" s="26">
+      <c r="F16" s="31">
         <v>1174272</v>
       </c>
-      <c r="G16" s="26">
+      <c r="G16" s="31">
         <v>1399881</v>
       </c>
-      <c r="H16" s="26">
+      <c r="H16" s="31">
         <v>1179014</v>
       </c>
-      <c r="I16" s="26">
+      <c r="I16" s="31">
         <v>1380086</v>
       </c>
-      <c r="J16" s="26">
+      <c r="J16" s="31">
         <v>1448886</v>
       </c>
-      <c r="K16" s="26">
+      <c r="K16" s="31">
         <v>1506868</v>
       </c>
-      <c r="L16" s="26">
+      <c r="L16" s="31">
         <v>1761891</v>
       </c>
-      <c r="M16" s="22"/>
+      <c r="M16" s="26">
+        <v>2059856</v>
+      </c>
       <c r="N16" s="22"/>
       <c r="O16" s="23"/>
       <c r="P16" s="23">
         <f>SUM(C16:N16)</f>
-        <v>12383175</v>
+        <v>14443031</v>
       </c>
       <c r="Q16" s="13"/>
       <c r="R16" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>14859810</v>
+        <v>15756033.818181818</v>
       </c>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
     </row>
-    <row r="17" spans="1:20" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
-      <c r="N17" s="28"/>
-      <c r="O17" s="28"/>
-      <c r="P17" s="21">
+    <row r="17" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+      <c r="A17" s="1"/>
+      <c r="B17" s="8">
+        <v>2020</v>
+      </c>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="35"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="35"/>
+      <c r="N17" s="32"/>
+      <c r="O17" s="33"/>
+      <c r="P17" s="34">
+        <f>SUM(C17:N17)</f>
+        <v>0</v>
+      </c>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="3" t="e">
+        <f>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+    </row>
+    <row r="18" spans="1:20" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="21">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>38222336</v>
-      </c>
-      <c r="Q17" s="18"/>
-      <c r="R17" s="14"/>
-      <c r="S17" s="14"/>
-      <c r="T17" s="14"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="12"/>
-      <c r="R18" s="1"/>
-      <c r="S18" s="1"/>
-      <c r="T18" s="1"/>
-    </row>
-    <row r="19" spans="1:20" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
-      <c r="B19" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="29">
-        <v>13814380</v>
-      </c>
-      <c r="G19" s="29"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
+        <v>40282192</v>
+      </c>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="12"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+      <c r="B20" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="29">
+        <v>15175204</v>
+      </c>
+      <c r="G20" s="29"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -3966,7 +3996,7 @@
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
-      <c r="L48" s="11"/>
+      <c r="L48" s="1"/>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
@@ -3988,7 +4018,7 @@
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
+      <c r="L49" s="11"/>
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
@@ -4020,11 +4050,33 @@
       <c r="S50" s="1"/>
       <c r="T50" s="1"/>
     </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+      <c r="O51" s="1"/>
+      <c r="P51" s="1"/>
+      <c r="Q51" s="1"/>
+      <c r="R51" s="1"/>
+      <c r="S51" s="1"/>
+      <c r="T51" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B17:O17"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B18:O18"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="B20:E20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Blog Statistics (December 2019)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c93c05515dfe04a/GIT Hub/kunal-chowdhury.com/blog-stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="114_{B49989D9-13EE-4EB4-8B18-ED25DB6F8102}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6FFD386F-0F83-4063-9849-78E7FD8FC46C}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="114_{B49989D9-13EE-4EB4-8B18-ED25DB6F8102}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2FA90DE0-A8A2-4F98-800C-429C0F388299}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Jan</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>Last 12 months 'Hit Count':</t>
+  </si>
+  <si>
+    <t>Last updated: 1st January 2020</t>
   </si>
 </sst>
 </file>
@@ -346,11 +349,17 @@
     <xf numFmtId="3" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="8" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="8" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -363,13 +372,9 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="8" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -751,10 +756,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$16</c:f>
+              <c:f>Sheet1!$B$5:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>2008</c:v>
                 </c:pt>
@@ -790,16 +795,19 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2020</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$16</c:f>
+              <c:f>Sheet1!$B$5:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>2008</c:v>
                 </c:pt>
@@ -835,6 +843,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2020</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1327,10 +1338,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$16</c:f>
+              <c:f>Sheet1!$B$5:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>2008</c:v>
                 </c:pt>
@@ -1366,16 +1377,19 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2020</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$5:$P$16</c:f>
+              <c:f>Sheet1!$P$5:$P$17</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>326</c:v>
                 </c:pt>
@@ -1410,7 +1424,10 @@
                   <c:v>8287717</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>14443031</c:v>
+                  <c:v>16768940</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2493,8 +2510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="X29" sqref="X29"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="V20" sqref="V20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2502,8 +2519,7 @@
     <col min="1" max="1" width="5" style="2" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" style="2" customWidth="1"/>
     <col min="3" max="5" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="13" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="14" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="4" style="2" customWidth="1"/>
     <col min="16" max="16" width="18.42578125" style="2" customWidth="1"/>
     <col min="17" max="17" width="5.42578125" style="2" customWidth="1"/>
@@ -3097,22 +3113,22 @@
       <c r="H13" s="7">
         <v>132768</v>
       </c>
-      <c r="I13" s="24">
+      <c r="I13" s="23">
         <v>363723</v>
       </c>
-      <c r="J13" s="24">
+      <c r="J13" s="23">
         <v>702130</v>
       </c>
-      <c r="K13" s="24">
+      <c r="K13" s="23">
         <v>608805</v>
       </c>
-      <c r="L13" s="24">
+      <c r="L13" s="23">
         <v>635500</v>
       </c>
-      <c r="M13" s="24">
+      <c r="M13" s="23">
         <v>713080</v>
       </c>
-      <c r="N13" s="24">
+      <c r="N13" s="23">
         <v>674509</v>
       </c>
       <c r="O13" s="6"/>
@@ -3133,40 +3149,40 @@
       <c r="B14" s="8">
         <v>2017</v>
       </c>
-      <c r="C14" s="24">
+      <c r="C14" s="23">
         <v>662423</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="23">
         <v>554842</v>
       </c>
-      <c r="E14" s="24">
+      <c r="E14" s="23">
         <v>657797</v>
       </c>
-      <c r="F14" s="24">
+      <c r="F14" s="23">
         <v>673209</v>
       </c>
-      <c r="G14" s="24">
+      <c r="G14" s="23">
         <v>745540</v>
       </c>
-      <c r="H14" s="24">
+      <c r="H14" s="23">
         <v>660058</v>
       </c>
-      <c r="I14" s="24">
+      <c r="I14" s="23">
         <v>690513</v>
       </c>
-      <c r="J14" s="24">
+      <c r="J14" s="23">
         <v>670496</v>
       </c>
-      <c r="K14" s="24">
+      <c r="K14" s="23">
         <v>577595</v>
       </c>
-      <c r="L14" s="24">
+      <c r="L14" s="23">
         <v>665972</v>
       </c>
-      <c r="M14" s="24">
+      <c r="M14" s="23">
         <v>569447</v>
       </c>
-      <c r="N14" s="24">
+      <c r="N14" s="23">
         <v>565361</v>
       </c>
       <c r="O14" s="9"/>
@@ -3187,40 +3203,40 @@
       <c r="B15" s="8">
         <v>2018</v>
       </c>
-      <c r="C15" s="24">
+      <c r="C15" s="23">
         <v>628028</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="23">
         <v>728208</v>
       </c>
-      <c r="E15" s="24">
+      <c r="E15" s="23">
         <v>697376</v>
       </c>
-      <c r="F15" s="24">
+      <c r="F15" s="23">
         <v>707376</v>
       </c>
-      <c r="G15" s="24">
+      <c r="G15" s="23">
         <v>759564</v>
       </c>
-      <c r="H15" s="24">
+      <c r="H15" s="23">
         <v>592381</v>
       </c>
-      <c r="I15" s="24">
+      <c r="I15" s="23">
         <v>545423</v>
       </c>
-      <c r="J15" s="24">
+      <c r="J15" s="23">
         <v>694837</v>
       </c>
-      <c r="K15" s="24">
+      <c r="K15" s="23">
         <v>739656</v>
       </c>
-      <c r="L15" s="24">
+      <c r="L15" s="23">
         <v>763733</v>
       </c>
-      <c r="M15" s="24">
+      <c r="M15" s="23">
         <v>698962</v>
       </c>
-      <c r="N15" s="24">
+      <c r="N15" s="23">
         <v>732173</v>
       </c>
       <c r="O15" s="9"/>
@@ -3241,49 +3257,51 @@
       <c r="B16" s="8">
         <v>2019</v>
       </c>
-      <c r="C16" s="24">
+      <c r="C16" s="23">
         <v>816792</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="23">
         <v>811807</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="24">
         <v>903678</v>
       </c>
-      <c r="F16" s="31">
+      <c r="F16" s="26">
         <v>1174272</v>
       </c>
-      <c r="G16" s="31">
+      <c r="G16" s="26">
         <v>1399881</v>
       </c>
-      <c r="H16" s="31">
+      <c r="H16" s="26">
         <v>1179014</v>
       </c>
-      <c r="I16" s="31">
+      <c r="I16" s="26">
         <v>1380086</v>
       </c>
-      <c r="J16" s="31">
+      <c r="J16" s="26">
         <v>1448886</v>
       </c>
-      <c r="K16" s="31">
+      <c r="K16" s="26">
         <v>1506868</v>
       </c>
-      <c r="L16" s="31">
+      <c r="L16" s="26">
         <v>1761891</v>
       </c>
-      <c r="M16" s="26">
+      <c r="M16" s="25">
         <v>2059856</v>
       </c>
-      <c r="N16" s="22"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="23">
+      <c r="N16" s="25">
+        <v>2325909</v>
+      </c>
+      <c r="O16" s="22"/>
+      <c r="P16" s="22">
         <f>SUM(C16:N16)</f>
-        <v>14443031</v>
+        <v>16768940</v>
       </c>
       <c r="Q16" s="13"/>
       <c r="R16" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>15756033.818181818</v>
+        <v>16768940</v>
       </c>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
@@ -3293,20 +3311,20 @@
       <c r="B17" s="8">
         <v>2020</v>
       </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="32"/>
-      <c r="O17" s="33"/>
-      <c r="P17" s="34">
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="27"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="29">
         <f>SUM(C17:N17)</f>
         <v>0</v>
       </c>
@@ -3320,23 +3338,23 @@
     </row>
     <row r="18" spans="1:20" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
-      <c r="O18" s="28"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="34"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="34"/>
+      <c r="O18" s="34"/>
       <c r="P18" s="21">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>40282192</v>
+        <v>42608101</v>
       </c>
       <c r="Q18" s="18"/>
       <c r="R18" s="14"/>
@@ -3366,16 +3384,17 @@
     </row>
     <row r="20" spans="1:20" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="29">
-        <v>15175204</v>
-      </c>
-      <c r="G20" s="29"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="35">
+        <f>SUM(C16:N16)</f>
+        <v>16768940</v>
+      </c>
+      <c r="G20" s="35"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -3994,9 +4013,11 @@
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="1"/>
-      <c r="L48" s="1"/>
+      <c r="J48" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="K48" s="37"/>
+      <c r="L48" s="37"/>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
@@ -4073,10 +4094,11 @@
       <c r="T51" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B18:O18"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="B20:E20"/>
+    <mergeCell ref="J48:L48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
Blog Statistics (February 2020)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22703"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c93c05515dfe04a/GIT Hub/kunal-chowdhury.com/blog-stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="114_{B49989D9-13EE-4EB4-8B18-ED25DB6F8102}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2FA90DE0-A8A2-4F98-800C-429C0F388299}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="114_{B49989D9-13EE-4EB4-8B18-ED25DB6F8102}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F00B048F-1872-4F0B-8B14-9D85E956054C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -125,14 +125,14 @@
     <t>Last 12 months 'Hit Count':</t>
   </si>
   <si>
-    <t>Last updated: 1st January 2020</t>
+    <t>Last updated: 29th February 2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,11 +194,6 @@
       <sz val="16"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="8">
@@ -308,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -358,7 +353,6 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1427,7 +1421,7 @@
                   <c:v>16768940</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>4898472</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2511,14 +2505,15 @@
   <dimension ref="A1:T51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="V20" sqref="V20"/>
+      <selection activeCell="W28" sqref="W28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="2" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" style="2" customWidth="1"/>
-    <col min="3" max="5" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="14" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="4" style="2" customWidth="1"/>
     <col min="16" max="16" width="18.42578125" style="2" customWidth="1"/>
@@ -3311,9 +3306,13 @@
       <c r="B17" s="8">
         <v>2020</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="32"/>
+      <c r="C17" s="26">
+        <v>1694534</v>
+      </c>
+      <c r="D17" s="25">
+        <v>3203938</v>
+      </c>
+      <c r="E17" s="31"/>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
       <c r="H17" s="30"/>
@@ -3326,35 +3325,35 @@
       <c r="O17" s="28"/>
       <c r="P17" s="29">
         <f>SUM(C17:N17)</f>
-        <v>0</v>
+        <v>4898472</v>
       </c>
       <c r="Q17" s="13"/>
-      <c r="R17" s="3" t="e">
+      <c r="R17" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>#DIV/0!</v>
+        <v>7347708</v>
       </c>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
     </row>
     <row r="18" spans="1:20" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="34"/>
-      <c r="L18" s="34"/>
-      <c r="M18" s="34"/>
-      <c r="N18" s="34"/>
-      <c r="O18" s="34"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
+      <c r="M18" s="33"/>
+      <c r="N18" s="33"/>
+      <c r="O18" s="33"/>
       <c r="P18" s="21">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>42608101</v>
+        <v>47506573</v>
       </c>
       <c r="Q18" s="18"/>
       <c r="R18" s="14"/>
@@ -3384,17 +3383,16 @@
     </row>
     <row r="20" spans="1:20" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="35">
-        <f>SUM(C16:N16)</f>
-        <v>16768940</v>
-      </c>
-      <c r="G20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="34">
+        <v>20038113</v>
+      </c>
+      <c r="G20" s="34"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -4013,11 +4011,11 @@
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
-      <c r="J48" s="37" t="s">
+      <c r="J48" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="K48" s="37"/>
-      <c r="L48" s="37"/>
+      <c r="K48" s="36"/>
+      <c r="L48" s="36"/>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>

</xml_diff>

<commit_message>
Blog Statistics (April 2020)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22703"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c93c05515dfe04a/GIT Hub/kunal-chowdhury.com/blog-stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="114_{B49989D9-13EE-4EB4-8B18-ED25DB6F8102}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F00B048F-1872-4F0B-8B14-9D85E956054C}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="114_{B49989D9-13EE-4EB4-8B18-ED25DB6F8102}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7E829401-38B4-43A3-AD8E-14A10A37254E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -125,7 +125,7 @@
     <t>Last 12 months 'Hit Count':</t>
   </si>
   <si>
-    <t>Last updated: 29th February 2020</t>
+    <t>Last updated: 1st May 2020</t>
   </si>
 </sst>
 </file>
@@ -303,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -353,7 +353,6 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1421,7 +1420,7 @@
                   <c:v>16768940</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4898472</c:v>
+                  <c:v>10889371</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2504,25 +2503,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="W28" sqref="W28"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q47" sqref="Q47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="2" customWidth="1"/>
-    <col min="3" max="4" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="14" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="14" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="4" style="2" customWidth="1"/>
-    <col min="16" max="16" width="18.42578125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="5.42578125" style="2" customWidth="1"/>
-    <col min="18" max="18" width="25.42578125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="18.44140625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="5.44140625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="25.44140625" style="2" customWidth="1"/>
     <col min="19" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2544,7 +2543,7 @@
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2566,7 +2565,7 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>13</v>
@@ -2620,7 +2619,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:20" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14"/>
       <c r="B4" s="15"/>
       <c r="C4" s="16" t="s">
@@ -2671,7 +2670,7 @@
       <c r="S4" s="14"/>
       <c r="T4" s="14"/>
     </row>
-    <row r="5" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" ht="21" x14ac:dyDescent="0.4">
       <c r="A5" s="1"/>
       <c r="B5" s="4">
         <v>2008</v>
@@ -2707,7 +2706,7 @@
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" ht="21" x14ac:dyDescent="0.4">
       <c r="A6" s="1"/>
       <c r="B6" s="4">
         <v>2009</v>
@@ -2761,7 +2760,7 @@
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
     </row>
-    <row r="7" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" ht="21" x14ac:dyDescent="0.4">
       <c r="A7" s="1"/>
       <c r="B7" s="4">
         <v>2010</v>
@@ -2815,7 +2814,7 @@
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
     </row>
-    <row r="8" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" ht="21" x14ac:dyDescent="0.4">
       <c r="A8" s="1"/>
       <c r="B8" s="4">
         <v>2011</v>
@@ -2869,7 +2868,7 @@
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
     </row>
-    <row r="9" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" ht="21" x14ac:dyDescent="0.4">
       <c r="A9" s="1"/>
       <c r="B9" s="4">
         <v>2012</v>
@@ -2923,7 +2922,7 @@
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
     </row>
-    <row r="10" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" ht="21" x14ac:dyDescent="0.4">
       <c r="A10" s="1"/>
       <c r="B10" s="4">
         <v>2013</v>
@@ -2977,7 +2976,7 @@
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
     </row>
-    <row r="11" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" ht="21" x14ac:dyDescent="0.4">
       <c r="A11" s="1"/>
       <c r="B11" s="4">
         <v>2014</v>
@@ -3031,7 +3030,7 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
     </row>
-    <row r="12" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" ht="21" x14ac:dyDescent="0.4">
       <c r="A12" s="1"/>
       <c r="B12" s="4">
         <v>2015</v>
@@ -3085,7 +3084,7 @@
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
     </row>
-    <row r="13" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" ht="21" x14ac:dyDescent="0.4">
       <c r="A13" s="1"/>
       <c r="B13" s="4">
         <v>2016</v>
@@ -3139,7 +3138,7 @@
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
     </row>
-    <row r="14" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" ht="21" x14ac:dyDescent="0.4">
       <c r="A14" s="1"/>
       <c r="B14" s="8">
         <v>2017</v>
@@ -3193,7 +3192,7 @@
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
     </row>
-    <row r="15" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" ht="21" x14ac:dyDescent="0.4">
       <c r="A15" s="1"/>
       <c r="B15" s="8">
         <v>2018</v>
@@ -3247,7 +3246,7 @@
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
     </row>
-    <row r="16" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" ht="21" x14ac:dyDescent="0.4">
       <c r="A16" s="1"/>
       <c r="B16" s="8">
         <v>2019</v>
@@ -3301,7 +3300,7 @@
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
     </row>
-    <row r="17" spans="1:20" ht="21" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" ht="21" x14ac:dyDescent="0.4">
       <c r="A17" s="1"/>
       <c r="B17" s="8">
         <v>2020</v>
@@ -3312,8 +3311,12 @@
       <c r="D17" s="25">
         <v>3203938</v>
       </c>
-      <c r="E17" s="31"/>
-      <c r="F17" s="30"/>
+      <c r="E17" s="25">
+        <v>3296329</v>
+      </c>
+      <c r="F17" s="25">
+        <v>2694570</v>
+      </c>
       <c r="G17" s="30"/>
       <c r="H17" s="30"/>
       <c r="I17" s="30"/>
@@ -3325,42 +3328,42 @@
       <c r="O17" s="28"/>
       <c r="P17" s="29">
         <f>SUM(C17:N17)</f>
-        <v>4898472</v>
+        <v>10889371</v>
       </c>
       <c r="Q17" s="13"/>
       <c r="R17" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>7347708</v>
+        <v>8167028.25</v>
       </c>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
     </row>
-    <row r="18" spans="1:20" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="33"/>
-      <c r="L18" s="33"/>
-      <c r="M18" s="33"/>
-      <c r="N18" s="33"/>
-      <c r="O18" s="33"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="32"/>
+      <c r="N18" s="32"/>
+      <c r="O18" s="32"/>
       <c r="P18" s="21">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>47506573</v>
+        <v>53497472</v>
       </c>
       <c r="Q18" s="18"/>
       <c r="R18" s="14"/>
       <c r="S18" s="14"/>
       <c r="T18" s="14"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -3381,18 +3384,19 @@
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
     </row>
-    <row r="20" spans="1:20" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="34">
-        <v>20038113</v>
-      </c>
-      <c r="G20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="33">
+        <f>SUM(G16:N16,C17,D17,E17,F17)</f>
+        <v>23951762</v>
+      </c>
+      <c r="G20" s="33"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -3407,7 +3411,7 @@
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -3429,7 +3433,7 @@
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -3451,7 +3455,7 @@
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -3473,7 +3477,7 @@
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -3495,7 +3499,7 @@
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -3517,7 +3521,7 @@
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -3539,7 +3543,7 @@
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -3561,7 +3565,7 @@
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -3583,7 +3587,7 @@
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -3605,7 +3609,7 @@
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -3627,7 +3631,7 @@
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -3649,7 +3653,7 @@
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -3671,7 +3675,7 @@
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -3693,7 +3697,7 @@
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -3715,7 +3719,7 @@
       <c r="S34" s="1"/>
       <c r="T34" s="1"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -3737,7 +3741,7 @@
       <c r="S35" s="1"/>
       <c r="T35" s="1"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -3759,7 +3763,7 @@
       <c r="S36" s="1"/>
       <c r="T36" s="1"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -3781,7 +3785,7 @@
       <c r="S37" s="1"/>
       <c r="T37" s="1"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -3803,7 +3807,7 @@
       <c r="S38" s="1"/>
       <c r="T38" s="1"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -3825,7 +3829,7 @@
       <c r="S39" s="1"/>
       <c r="T39" s="1"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -3847,7 +3851,7 @@
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -3869,7 +3873,7 @@
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -3891,7 +3895,7 @@
       <c r="S42" s="1"/>
       <c r="T42" s="1"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -3913,7 +3917,7 @@
       <c r="S43" s="1"/>
       <c r="T43" s="1"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -3935,7 +3939,7 @@
       <c r="S44" s="1"/>
       <c r="T44" s="1"/>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -3957,7 +3961,7 @@
       <c r="S45" s="1"/>
       <c r="T45" s="1"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -3979,7 +3983,7 @@
       <c r="S46" s="1"/>
       <c r="T46" s="1"/>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -4001,7 +4005,7 @@
       <c r="S47" s="1"/>
       <c r="T47" s="1"/>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -4011,11 +4015,11 @@
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
-      <c r="J48" s="36" t="s">
+      <c r="J48" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="K48" s="36"/>
-      <c r="L48" s="36"/>
+      <c r="K48" s="35"/>
+      <c r="L48" s="35"/>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
@@ -4025,7 +4029,7 @@
       <c r="S48" s="1"/>
       <c r="T48" s="1"/>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -4047,7 +4051,7 @@
       <c r="S49" s="1"/>
       <c r="T49" s="1"/>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -4069,7 +4073,7 @@
       <c r="S50" s="1"/>
       <c r="T50" s="1"/>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -4101,7 +4105,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="P5:P14" formulaRange="1"/>
+    <ignoredError sqref="P5:P14 F20" formulaRange="1"/>
     <ignoredError sqref="P4" calculatedColumn="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Blog Statistics (June 2020)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c93c05515dfe04a/GIT Hub/kunal-chowdhury.com/blog-stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="114_{B49989D9-13EE-4EB4-8B18-ED25DB6F8102}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7E829401-38B4-43A3-AD8E-14A10A37254E}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="114_{B49989D9-13EE-4EB4-8B18-ED25DB6F8102}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B1D9D889-0126-4FA2-853C-1E9176F9562E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -125,7 +125,7 @@
     <t>Last 12 months 'Hit Count':</t>
   </si>
   <si>
-    <t>Last updated: 1st May 2020</t>
+    <t>Last updated: 1st July 2020</t>
   </si>
 </sst>
 </file>
@@ -1210,7 +1210,7 @@
                       <a:pPr/>
                       <a:t>[VALUE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-IN"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1420,7 +1420,7 @@
                   <c:v>16768940</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10889371</c:v>
+                  <c:v>15665564</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2503,8 +2503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q47" sqref="Q47"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S39" sqref="S39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3317,8 +3317,12 @@
       <c r="F17" s="25">
         <v>2694570</v>
       </c>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
+      <c r="G17" s="25">
+        <v>2511957</v>
+      </c>
+      <c r="H17" s="25">
+        <v>2264236</v>
+      </c>
       <c r="I17" s="30"/>
       <c r="J17" s="30"/>
       <c r="K17" s="30"/>
@@ -3328,12 +3332,12 @@
       <c r="O17" s="28"/>
       <c r="P17" s="29">
         <f>SUM(C17:N17)</f>
-        <v>10889371</v>
+        <v>15665564</v>
       </c>
       <c r="Q17" s="13"/>
       <c r="R17" s="3">
-        <f>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>8167028.25</v>
+        <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
+        <v>31331128</v>
       </c>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
@@ -3356,7 +3360,7 @@
       <c r="O18" s="32"/>
       <c r="P18" s="21">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>53497472</v>
+        <v>58273665</v>
       </c>
       <c r="Q18" s="18"/>
       <c r="R18" s="14"/>
@@ -3393,8 +3397,8 @@
       <c r="D20" s="34"/>
       <c r="E20" s="34"/>
       <c r="F20" s="33">
-        <f>SUM(G16:N16,C17,D17,E17,F17)</f>
-        <v>23951762</v>
+        <f>SUM(I16:N16,C17:H17)</f>
+        <v>26149060</v>
       </c>
       <c r="G20" s="33"/>
       <c r="H20" s="1"/>

</xml_diff>

<commit_message>
Blog Statistics (July 2020)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c93c05515dfe04a/GIT Hub/kunal-chowdhury.com/blog-stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="114_{B49989D9-13EE-4EB4-8B18-ED25DB6F8102}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B1D9D889-0126-4FA2-853C-1E9176F9562E}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="114_{B49989D9-13EE-4EB4-8B18-ED25DB6F8102}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{99844B87-EFE3-491D-825F-9652D9079D09}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -125,7 +125,7 @@
     <t>Last 12 months 'Hit Count':</t>
   </si>
   <si>
-    <t>Last updated: 1st July 2020</t>
+    <t>Last updated: 1st August 2020</t>
   </si>
 </sst>
 </file>
@@ -857,11 +857,26 @@
             <c:v>Blog Hit / Pageviews</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="31750" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
+            <a:ln w="50800" cap="rnd" cmpd="sng">
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:srgbClr val="FF0000"/>
+                  </a:gs>
+                  <a:gs pos="46000">
+                    <a:srgbClr val="FFC000"/>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:srgbClr val="C00000"/>
+                  </a:gs>
+                </a:gsLst>
+                <a:path path="circle">
+                  <a:fillToRect l="50000" t="130000" r="50000" b="-30000"/>
+                </a:path>
+                <a:tileRect/>
+              </a:gradFill>
               <a:round/>
+              <a:tailEnd type="arrow"/>
             </a:ln>
             <a:effectLst>
               <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
@@ -981,8 +996,8 @@
               <c:idx val="3"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0"/>
-                  <c:y val="-7.7632181779115655E-2"/>
+                  <c:x val="-2.9064478515743449E-2"/>
+                  <c:y val="-0.26967477030724174"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1002,8 +1017,8 @@
               <c:idx val="4"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.4042473063053691E-3"/>
-                  <c:y val="-0.13070815760385421"/>
+                  <c:x val="-4.9845008519096116E-2"/>
+                  <c:y val="-0.11400878184162716"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1023,8 +1038,8 @@
               <c:idx val="5"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="5.6942781123952907E-3"/>
-                  <c:y val="-0.11112775054950078"/>
+                  <c:x val="-3.4269384996397451E-2"/>
+                  <c:y val="-0.21410713706527998"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1044,8 +1059,8 @@
               <c:idx val="6"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-4.4444439259907929E-3"/>
-                  <c:y val="-8.1513790868071437E-2"/>
+                  <c:x val="-3.5930961565087932E-2"/>
+                  <c:y val="-0.10099643834871934"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1086,8 +1101,8 @@
               <c:idx val="8"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.15384933487881633"/>
-                  <c:y val="4.8494492840790837E-17"/>
+                  <c:x val="-0.11994074965757696"/>
+                  <c:y val="-4.1748373676215055E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1107,8 +1122,8 @@
               <c:idx val="9"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.20590818243054426"/>
-                  <c:y val="5.9953632203103534E-2"/>
+                  <c:x val="-0.19379799500869083"/>
+                  <c:y val="-5.1375263748911909E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -1196,8 +1211,8 @@
               <c:idx val="10"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.18112219012053507"/>
-                  <c:y val="-6.3484433087969888E-2"/>
+                  <c:x val="-0.17627806467189761"/>
+                  <c:y val="-0.13028188151263678"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -1234,8 +1249,55 @@
               <c:idx val="11"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-8.4365911565924323E-2"/>
-                  <c:y val="-6.3484433087969985E-2"/>
+                  <c:x val="-0.18972467700095785"/>
+                  <c:y val="1.7229038809989456E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-4E3A-49ED-AF1F-326603D91C04}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.12836811344453358"/>
+                  <c:y val="-0.10854577155815888"/>
                 </c:manualLayout>
               </c:layout>
               <c:spPr>
@@ -1273,7 +1335,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000000-4E3A-49ED-AF1F-326603D91C04}"/>
+                  <c16:uniqueId val="{00000001-F5FD-4EEB-9B05-96C7834AADBD}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1420,7 +1482,7 @@
                   <c:v>16768940</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>15665564</c:v>
+                  <c:v>16920917</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1442,13 +1504,27 @@
         </c:dLbls>
         <c:dropLines>
           <c:spPr>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
+            <a:ln w="12700">
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="48000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="97000"/>
+                      <a:lumOff val="3000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="bg1"/>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="13500000" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
               <a:prstDash val="dash"/>
             </a:ln>
             <a:effectLst/>
@@ -1473,12 +1549,7 @@
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx2">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
+            <a:noFill/>
             <a:round/>
           </a:ln>
           <a:effectLst/>
@@ -2504,7 +2575,7 @@
   <dimension ref="A1:T51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="S39" sqref="S39"/>
+      <selection activeCell="P46" sqref="P46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3323,7 +3394,9 @@
       <c r="H17" s="25">
         <v>2264236</v>
       </c>
-      <c r="I17" s="30"/>
+      <c r="I17" s="26">
+        <v>1255353</v>
+      </c>
       <c r="J17" s="30"/>
       <c r="K17" s="30"/>
       <c r="L17" s="30"/>
@@ -3332,12 +3405,12 @@
       <c r="O17" s="28"/>
       <c r="P17" s="29">
         <f>SUM(C17:N17)</f>
-        <v>15665564</v>
+        <v>16920917</v>
       </c>
       <c r="Q17" s="13"/>
       <c r="R17" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>31331128</v>
+        <v>29007286.285714287</v>
       </c>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
@@ -3360,7 +3433,7 @@
       <c r="O18" s="32"/>
       <c r="P18" s="21">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>58273665</v>
+        <v>59529018</v>
       </c>
       <c r="Q18" s="18"/>
       <c r="R18" s="14"/>
@@ -3397,8 +3470,8 @@
       <c r="D20" s="34"/>
       <c r="E20" s="34"/>
       <c r="F20" s="33">
-        <f>SUM(I16:N16,C17:H17)</f>
-        <v>26149060</v>
+        <f>SUM(J16:N16,C17:I17)</f>
+        <v>26024327</v>
       </c>
       <c r="G20" s="33"/>
       <c r="H20" s="1"/>
@@ -4109,7 +4182,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="P5:P14 F20" formulaRange="1"/>
+    <ignoredError sqref="P5:P17 F20" formulaRange="1"/>
     <ignoredError sqref="P4" calculatedColumn="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Blog Statistics (September 2020)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c93c05515dfe04a/GIT Hub/kunal-chowdhury.com/blog-stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="114_{B49989D9-13EE-4EB4-8B18-ED25DB6F8102}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{99844B87-EFE3-491D-825F-9652D9079D09}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="114_{B49989D9-13EE-4EB4-8B18-ED25DB6F8102}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B115FC35-6E87-42D0-87D5-8FD0C19940B8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -125,7 +125,7 @@
     <t>Last 12 months 'Hit Count':</t>
   </si>
   <si>
-    <t>Last updated: 1st August 2020</t>
+    <t>Last updated: 1st October 2020</t>
   </si>
 </sst>
 </file>
@@ -1253,32 +1253,6 @@
                   <c:y val="1.7229038809989456E-2"/>
                 </c:manualLayout>
               </c:layout>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                  <a:spAutoFit/>
-                </a:bodyPr>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx2"/>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -1482,7 +1456,7 @@
                   <c:v>16768940</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16920917</c:v>
+                  <c:v>19748578</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2575,7 +2549,7 @@
   <dimension ref="A1:T51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P46" sqref="P46"/>
+      <selection activeCell="S44" sqref="S44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3397,20 +3371,24 @@
       <c r="I17" s="26">
         <v>1255353</v>
       </c>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
+      <c r="J17" s="26">
+        <v>1205188</v>
+      </c>
+      <c r="K17" s="26">
+        <v>1622473</v>
+      </c>
       <c r="L17" s="30"/>
       <c r="M17" s="30"/>
       <c r="N17" s="27"/>
       <c r="O17" s="28"/>
       <c r="P17" s="29">
         <f>SUM(C17:N17)</f>
-        <v>16920917</v>
+        <v>19748578</v>
       </c>
       <c r="Q17" s="13"/>
       <c r="R17" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>29007286.285714287</v>
+        <v>26331437.333333332</v>
       </c>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
@@ -3433,7 +3411,7 @@
       <c r="O18" s="32"/>
       <c r="P18" s="21">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>59529018</v>
+        <v>62356679</v>
       </c>
       <c r="Q18" s="18"/>
       <c r="R18" s="14"/>
@@ -3470,8 +3448,7 @@
       <c r="D20" s="34"/>
       <c r="E20" s="34"/>
       <c r="F20" s="33">
-        <f>SUM(J16:N16,C17:I17)</f>
-        <v>26024327</v>
+        <v>25896234</v>
       </c>
       <c r="G20" s="33"/>
       <c r="H20" s="1"/>
@@ -4182,7 +4159,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="P5:P17 F20" formulaRange="1"/>
+    <ignoredError sqref="P5:P17" formulaRange="1"/>
     <ignoredError sqref="P4" calculatedColumn="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Blog Statistics (December 2020)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23624"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c93c05515dfe04a/GIT Hub/kunal-chowdhury.com/blog-stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="114_{B49989D9-13EE-4EB4-8B18-ED25DB6F8102}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B115FC35-6E87-42D0-87D5-8FD0C19940B8}"/>
+  <xr:revisionPtr revIDLastSave="101" documentId="114_{B49989D9-13EE-4EB4-8B18-ED25DB6F8102}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B043ADAC-2FA4-46BC-8EB0-15BCFD3C2C0C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -125,7 +125,7 @@
     <t>Last 12 months 'Hit Count':</t>
   </si>
   <si>
-    <t>Last updated: 1st October 2020</t>
+    <t>Last updated: 1st January 2021</t>
   </si>
 </sst>
 </file>
@@ -303,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -349,10 +349,8 @@
     <xf numFmtId="3" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="8" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="8" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1456,7 +1454,7 @@
                   <c:v>16768940</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>19748578</c:v>
+                  <c:v>26204397</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2548,8 +2546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="S44" sqref="S44"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q40" sqref="Q40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3377,41 +3375,47 @@
       <c r="K17" s="26">
         <v>1622473</v>
       </c>
-      <c r="L17" s="30"/>
-      <c r="M17" s="30"/>
-      <c r="N17" s="27"/>
-      <c r="O17" s="28"/>
-      <c r="P17" s="29">
+      <c r="L17" s="26">
+        <v>1912285</v>
+      </c>
+      <c r="M17" s="25">
+        <v>2366693</v>
+      </c>
+      <c r="N17" s="25">
+        <v>2176841</v>
+      </c>
+      <c r="O17" s="27"/>
+      <c r="P17" s="28">
         <f>SUM(C17:N17)</f>
-        <v>19748578</v>
+        <v>26204397</v>
       </c>
       <c r="Q17" s="13"/>
       <c r="R17" s="3">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>26331437.333333332</v>
+        <v>26204397</v>
       </c>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
     </row>
     <row r="18" spans="1:20" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="32"/>
-      <c r="M18" s="32"/>
-      <c r="N18" s="32"/>
-      <c r="O18" s="32"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="30"/>
       <c r="P18" s="21">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>62356679</v>
+        <v>68812498</v>
       </c>
       <c r="Q18" s="18"/>
       <c r="R18" s="14"/>
@@ -3441,16 +3445,17 @@
     </row>
     <row r="20" spans="1:20" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="33">
-        <v>25896234</v>
-      </c>
-      <c r="G20" s="33"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="31">
+        <f>SUM(C17:N17)</f>
+        <v>26204397</v>
+      </c>
+      <c r="G20" s="31"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -4069,11 +4074,11 @@
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
-      <c r="J48" s="35" t="s">
+      <c r="J48" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="K48" s="35"/>
-      <c r="L48" s="35"/>
+      <c r="K48" s="33"/>
+      <c r="L48" s="33"/>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>

</xml_diff>

<commit_message>
Blog Statistics (February 2021)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c93c05515dfe04a/GIT Hub/kunal-chowdhury.com/blog-stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="101" documentId="114_{B49989D9-13EE-4EB4-8B18-ED25DB6F8102}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B043ADAC-2FA4-46BC-8EB0-15BCFD3C2C0C}"/>
+  <xr:revisionPtr revIDLastSave="176" documentId="114_{B49989D9-13EE-4EB4-8B18-ED25DB6F8102}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AFEE2193-6E0C-493A-8329-5EB9B8BABC3B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Jan</t>
   </si>
@@ -110,9 +110,6 @@
     <t>Column13</t>
   </si>
   <si>
-    <t>Column14</t>
-  </si>
-  <si>
     <t>Column15</t>
   </si>
   <si>
@@ -122,9 +119,6 @@
     <t>Column152</t>
   </si>
   <si>
-    <t>Last 12 months 'Hit Count':</t>
-  </si>
-  <si>
     <t>Last updated: 1st January 2021</t>
   </si>
 </sst>
@@ -132,7 +126,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,38 +159,44 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="16"/>
       <color rgb="FF002060"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="16"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="16"/>
-      <color rgb="FF002060"/>
+      <sz val="18"/>
+      <color theme="0"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="16"/>
+      <sz val="20"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,31 +211,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFF99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF66FF33"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF99FF66"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -303,33 +279,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -341,36 +300,48 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="8" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="8" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="10" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="10" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="17">
     <dxf>
       <font>
         <strike val="0"/>
@@ -391,18 +362,6 @@
           <bgColor theme="1"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -747,10 +706,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$17</c:f>
+              <c:f>Sheet1!$B$5:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>2008</c:v>
                 </c:pt>
@@ -789,16 +748,19 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$17</c:f>
+              <c:f>Sheet1!$B$5:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>2008</c:v>
                 </c:pt>
@@ -837,6 +799,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1268,8 +1233,86 @@
               <c:idx val="12"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.12836811344453358"/>
-                  <c:y val="-0.10854577155815888"/>
+                  <c:x val="-0.19517644581043192"/>
+                  <c:y val="-2.6403329231788997E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:spAutoFit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx2"/>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:fld id="{2675B164-AE68-4D10-B325-288EC93F69C9}" type="VALUE">
+                      <a:rPr lang="en-US" sz="1400" b="0"/>
+                      <a:pPr>
+                        <a:defRPr sz="1400" b="1"/>
+                      </a:pPr>
+                      <a:t>[VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-IN"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-F5FD-4EEB-9B05-96C7834AADBD}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.1174258296810501E-2"/>
+                  <c:y val="-0.1254428804447888"/>
                 </c:manualLayout>
               </c:layout>
               <c:spPr>
@@ -1286,7 +1329,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx2"/>
                       </a:solidFill>
@@ -1307,7 +1350,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000001-F5FD-4EEB-9B05-96C7834AADBD}"/>
+                  <c16:uniqueId val="{00000012-98B3-4A13-AF08-2983E2EA9C03}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1365,10 +1408,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$17</c:f>
+              <c:f>Sheet1!$B$5:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>2008</c:v>
                 </c:pt>
@@ -1407,16 +1450,19 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$5:$P$17</c:f>
+              <c:f>Sheet1!$O$5:$O$18</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>326</c:v>
                 </c:pt>
@@ -1455,6 +1501,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>26204397</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2159486</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2157,15 +2206,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>21429</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:colOff>21428</xdr:colOff>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>23811</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>88107</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>62488</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>355599</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2194,23 +2243,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B3:R17" totalsRowShown="0" dataDxfId="17">
-  <autoFilter ref="B3:R17" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Column3" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Column4" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Column5" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column6" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Column7" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Column8" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Column9" dataDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Column10" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Column11" dataDxfId="6"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Column12" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Column13" dataDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Column14" dataDxfId="3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B3:Q18" totalsRowShown="0" dataDxfId="16">
+  <autoFilter ref="B3:Q18" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="16">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Column3" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Column4" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Column5" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column6" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Column7" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Column8" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Column9" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Column10" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Column11" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Column12" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Column13" dataDxfId="3"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Column15" dataDxfId="2">
       <calculatedColumnFormula>SUM(C4:N4)</calculatedColumnFormula>
     </tableColumn>
@@ -2544,27 +2592,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T51"/>
+  <dimension ref="A1:S64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q40" sqref="Q40"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="T37" sqref="T37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" style="2" customWidth="1"/>
     <col min="3" max="4" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="14" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4" style="2" customWidth="1"/>
-    <col min="16" max="16" width="18.44140625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="5.44140625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="25.44140625" style="2" customWidth="1"/>
-    <col min="19" max="16384" width="9" style="2"/>
+    <col min="15" max="15" width="22" style="2" customWidth="1"/>
+    <col min="16" max="16" width="5.44140625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="25.44140625" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2584,9 +2631,8 @@
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2602,13 +2648,12 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="12"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>13</v>
@@ -2652,854 +2697,850 @@
       <c r="O3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="P3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="16" t="s">
+    </row>
+    <row r="4" spans="1:19" s="9" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="J4" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="16" t="s">
+      <c r="K4" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="16" t="s">
+      <c r="L4" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="16" t="s">
+      <c r="M4" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="16" t="s">
+      <c r="N4" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17" t="s">
+      <c r="O4" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="19" t="e">
-        <f>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14"/>
-    </row>
-    <row r="5" spans="1:20" ht="21" x14ac:dyDescent="0.4">
+      <c r="P4" s="7"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+    </row>
+    <row r="5" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A5" s="1"/>
-      <c r="B5" s="4">
+      <c r="B5" s="25">
         <v>2008</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="6">
+      <c r="C5" s="15">
+        <v>0</v>
+      </c>
+      <c r="D5" s="15">
+        <v>0</v>
+      </c>
+      <c r="E5" s="15">
+        <v>0</v>
+      </c>
+      <c r="F5" s="15">
+        <v>0</v>
+      </c>
+      <c r="G5" s="15">
+        <v>0</v>
+      </c>
+      <c r="H5" s="15">
+        <v>0</v>
+      </c>
+      <c r="I5" s="15">
+        <v>0</v>
+      </c>
+      <c r="J5" s="15">
+        <v>0</v>
+      </c>
+      <c r="K5" s="15">
+        <v>0</v>
+      </c>
+      <c r="L5" s="10">
         <v>105</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="10">
         <v>112</v>
       </c>
-      <c r="N5" s="6">
+      <c r="N5" s="10">
         <v>109</v>
       </c>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6">
+      <c r="O5" s="27">
         <f>SUM(C5:N5)</f>
         <v>326</v>
       </c>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="3">
-        <f>SUM((Table1[[#This Row],[Column15]]*3)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="16">
+        <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>326</v>
       </c>
+      <c r="R5" s="1"/>
       <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-    </row>
-    <row r="6" spans="1:20" ht="21" x14ac:dyDescent="0.4">
+    </row>
+    <row r="6" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A6" s="1"/>
-      <c r="B6" s="4">
+      <c r="B6" s="25">
         <v>2009</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="10">
         <v>210</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="10">
         <v>265</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="10">
         <v>330</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="10">
         <v>459</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="10">
         <v>2711</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="10">
         <v>4347</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="10">
         <v>7134</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="10">
         <v>7452</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="10">
         <v>10193</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="10">
         <v>11773</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="10">
         <v>16989</v>
       </c>
-      <c r="N6" s="6">
+      <c r="N6" s="10">
         <v>18516</v>
       </c>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6">
-        <f t="shared" ref="P6:P12" si="0">SUM(C6:N6)</f>
+      <c r="O6" s="27">
+        <f t="shared" ref="O6:O12" si="0">SUM(C6:N6)</f>
         <v>80379</v>
       </c>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="3">
+      <c r="P6" s="3"/>
+      <c r="Q6" s="16">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>80379</v>
       </c>
+      <c r="R6" s="1"/>
       <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-    </row>
-    <row r="7" spans="1:20" ht="21" x14ac:dyDescent="0.4">
+    </row>
+    <row r="7" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A7" s="1"/>
-      <c r="B7" s="4">
+      <c r="B7" s="25">
         <v>2010</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="10">
         <v>16660</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="10">
         <v>23673</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="10">
         <v>32985</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="10">
         <v>35222</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="10">
         <v>39909</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="10">
         <v>42087</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="10">
         <v>54395</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="10">
         <v>49067</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="10">
         <v>47658</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="10">
         <v>38853</v>
       </c>
-      <c r="M7" s="6">
+      <c r="M7" s="10">
         <v>39946</v>
       </c>
-      <c r="N7" s="6">
+      <c r="N7" s="10">
         <v>42658</v>
       </c>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6">
+      <c r="O7" s="27">
         <f t="shared" si="0"/>
         <v>463113</v>
       </c>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="3">
+      <c r="P7" s="3"/>
+      <c r="Q7" s="16">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>463113</v>
       </c>
+      <c r="R7" s="1"/>
       <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-    </row>
-    <row r="8" spans="1:20" ht="21" x14ac:dyDescent="0.4">
+    </row>
+    <row r="8" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A8" s="1"/>
-      <c r="B8" s="4">
+      <c r="B8" s="25">
         <v>2011</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="10">
         <v>45551</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="10">
         <v>69346</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="10">
         <v>47856</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="10">
         <v>64728</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="10">
         <v>73308</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="10">
         <v>82846</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="10">
         <v>72286</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="10">
         <v>75867</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="10">
         <v>80961</v>
       </c>
-      <c r="L8" s="6">
+      <c r="L8" s="10">
         <v>62233</v>
       </c>
-      <c r="M8" s="6">
+      <c r="M8" s="10">
         <v>63447</v>
       </c>
-      <c r="N8" s="6">
+      <c r="N8" s="10">
         <v>64581</v>
       </c>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6">
+      <c r="O8" s="27">
         <f t="shared" si="0"/>
         <v>803010</v>
       </c>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="3">
+      <c r="P8" s="3"/>
+      <c r="Q8" s="16">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>803010</v>
       </c>
+      <c r="R8" s="1"/>
       <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-    </row>
-    <row r="9" spans="1:20" ht="21" x14ac:dyDescent="0.4">
+    </row>
+    <row r="9" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A9" s="1"/>
-      <c r="B9" s="4">
+      <c r="B9" s="25">
         <v>2012</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="10">
         <v>76072</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="10">
         <v>77385</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="10">
         <v>70852</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="10">
         <v>72356</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="10">
         <v>78593</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="10">
         <v>70155</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="10">
         <v>72470</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="10">
         <v>70252</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="10">
         <v>79738</v>
       </c>
-      <c r="L9" s="6">
+      <c r="L9" s="10">
         <v>71284</v>
       </c>
-      <c r="M9" s="6">
+      <c r="M9" s="10">
         <v>76524</v>
       </c>
-      <c r="N9" s="6">
+      <c r="N9" s="10">
         <v>73172</v>
       </c>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6">
+      <c r="O9" s="27">
         <f t="shared" si="0"/>
         <v>888853</v>
       </c>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="3">
+      <c r="P9" s="3"/>
+      <c r="Q9" s="16">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>888853</v>
       </c>
+      <c r="R9" s="1"/>
       <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-    </row>
-    <row r="10" spans="1:20" ht="21" x14ac:dyDescent="0.4">
+    </row>
+    <row r="10" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A10" s="1"/>
-      <c r="B10" s="4">
+      <c r="B10" s="25">
         <v>2013</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="10">
         <v>78648</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="10">
         <v>74894</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="10">
         <v>86029</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="10">
         <v>82489</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="10">
         <v>80316</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="10">
         <v>78764</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="10">
         <v>70746</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="10">
         <v>79324</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="10">
         <v>79148</v>
       </c>
-      <c r="L10" s="6">
+      <c r="L10" s="10">
         <v>76345</v>
       </c>
-      <c r="M10" s="6">
+      <c r="M10" s="10">
         <v>75329</v>
       </c>
-      <c r="N10" s="6">
+      <c r="N10" s="10">
         <v>73625</v>
       </c>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6">
+      <c r="O10" s="27">
         <f t="shared" si="0"/>
         <v>935657</v>
       </c>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="3">
+      <c r="P10" s="3"/>
+      <c r="Q10" s="16">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>935657</v>
       </c>
+      <c r="R10" s="1"/>
       <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-    </row>
-    <row r="11" spans="1:20" ht="21" x14ac:dyDescent="0.4">
+    </row>
+    <row r="11" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A11" s="1"/>
-      <c r="B11" s="4">
+      <c r="B11" s="25">
         <v>2014</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="10">
         <v>67510</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="10">
         <v>67706</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="10">
         <v>73924</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="10">
         <v>71449</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="10">
         <v>79877</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="10">
         <v>74705</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="10">
         <v>79936</v>
       </c>
-      <c r="J11" s="6">
+      <c r="J11" s="10">
         <v>78746</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K11" s="10">
         <v>77891</v>
       </c>
-      <c r="L11" s="6">
+      <c r="L11" s="10">
         <v>77040</v>
       </c>
-      <c r="M11" s="6">
+      <c r="M11" s="10">
         <v>87951</v>
       </c>
-      <c r="N11" s="7">
+      <c r="N11" s="11">
         <v>101904</v>
       </c>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6">
+      <c r="O11" s="27">
         <f t="shared" si="0"/>
         <v>938639</v>
       </c>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="3">
+      <c r="P11" s="3"/>
+      <c r="Q11" s="16">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>938639</v>
       </c>
+      <c r="R11" s="1"/>
       <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
-    </row>
-    <row r="12" spans="1:20" ht="21" x14ac:dyDescent="0.4">
+    </row>
+    <row r="12" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A12" s="1"/>
-      <c r="B12" s="4">
+      <c r="B12" s="25">
         <v>2015</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="10">
         <v>90536</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="10">
         <v>80976</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="10">
         <v>95444</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="10">
         <v>71951</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="10">
         <v>67019</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="10">
         <v>66244</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="10">
         <v>86294</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="11">
         <v>128005</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="11">
         <v>137300</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12" s="11">
         <v>138705</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12" s="11">
         <v>125538</v>
       </c>
-      <c r="N12" s="7">
+      <c r="N12" s="11">
         <v>129945</v>
       </c>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6">
+      <c r="O12" s="27">
         <f t="shared" si="0"/>
         <v>1217957</v>
       </c>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="3">
+      <c r="P12" s="3"/>
+      <c r="Q12" s="16">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>1217957</v>
       </c>
+      <c r="R12" s="1"/>
       <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
-    </row>
-    <row r="13" spans="1:20" ht="21" x14ac:dyDescent="0.4">
+    </row>
+    <row r="13" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A13" s="1"/>
-      <c r="B13" s="4">
+      <c r="B13" s="25">
         <v>2016</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="11">
         <v>142274</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="11">
         <v>123093</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="11">
         <v>147266</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="11">
         <v>152612</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="11">
         <v>134497</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="11">
         <v>132768</v>
       </c>
-      <c r="I13" s="23">
+      <c r="I13" s="12">
         <v>363723</v>
       </c>
-      <c r="J13" s="23">
+      <c r="J13" s="12">
         <v>702130</v>
       </c>
-      <c r="K13" s="23">
+      <c r="K13" s="12">
         <v>608805</v>
       </c>
-      <c r="L13" s="23">
+      <c r="L13" s="12">
         <v>635500</v>
       </c>
-      <c r="M13" s="23">
+      <c r="M13" s="12">
         <v>713080</v>
       </c>
-      <c r="N13" s="23">
+      <c r="N13" s="12">
         <v>674509</v>
       </c>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6">
-        <f>SUM(C13:N13)</f>
+      <c r="O13" s="27">
+        <f t="shared" ref="O13:O18" si="1">SUM(C13:N13)</f>
         <v>4530257</v>
       </c>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="3">
+      <c r="P13" s="3"/>
+      <c r="Q13" s="16">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>4530257</v>
       </c>
+      <c r="R13" s="1"/>
       <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-    </row>
-    <row r="14" spans="1:20" ht="21" x14ac:dyDescent="0.4">
+    </row>
+    <row r="14" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A14" s="1"/>
-      <c r="B14" s="8">
+      <c r="B14" s="25">
         <v>2017</v>
       </c>
-      <c r="C14" s="23">
+      <c r="C14" s="12">
         <v>662423</v>
       </c>
-      <c r="D14" s="23">
+      <c r="D14" s="12">
         <v>554842</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E14" s="12">
         <v>657797</v>
       </c>
-      <c r="F14" s="23">
+      <c r="F14" s="12">
         <v>673209</v>
       </c>
-      <c r="G14" s="23">
+      <c r="G14" s="12">
         <v>745540</v>
       </c>
-      <c r="H14" s="23">
+      <c r="H14" s="12">
         <v>660058</v>
       </c>
-      <c r="I14" s="23">
+      <c r="I14" s="12">
         <v>690513</v>
       </c>
-      <c r="J14" s="23">
+      <c r="J14" s="12">
         <v>670496</v>
       </c>
-      <c r="K14" s="23">
+      <c r="K14" s="12">
         <v>577595</v>
       </c>
-      <c r="L14" s="23">
+      <c r="L14" s="12">
         <v>665972</v>
       </c>
-      <c r="M14" s="23">
+      <c r="M14" s="12">
         <v>569447</v>
       </c>
-      <c r="N14" s="23">
+      <c r="N14" s="12">
         <v>565361</v>
       </c>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9">
-        <f>SUM(C14:N14)</f>
+      <c r="O14" s="27">
+        <f t="shared" si="1"/>
         <v>7693253</v>
       </c>
-      <c r="Q14" s="12"/>
-      <c r="R14" s="3">
+      <c r="P14" s="3"/>
+      <c r="Q14" s="16">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>7693253</v>
       </c>
+      <c r="R14" s="1"/>
       <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-    </row>
-    <row r="15" spans="1:20" ht="21" x14ac:dyDescent="0.4">
+    </row>
+    <row r="15" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A15" s="1"/>
-      <c r="B15" s="8">
+      <c r="B15" s="25">
         <v>2018</v>
       </c>
-      <c r="C15" s="23">
+      <c r="C15" s="12">
         <v>628028</v>
       </c>
-      <c r="D15" s="23">
+      <c r="D15" s="12">
         <v>728208</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="12">
         <v>697376</v>
       </c>
-      <c r="F15" s="23">
+      <c r="F15" s="12">
         <v>707376</v>
       </c>
-      <c r="G15" s="23">
+      <c r="G15" s="12">
         <v>759564</v>
       </c>
-      <c r="H15" s="23">
+      <c r="H15" s="12">
         <v>592381</v>
       </c>
-      <c r="I15" s="23">
+      <c r="I15" s="12">
         <v>545423</v>
       </c>
-      <c r="J15" s="23">
+      <c r="J15" s="12">
         <v>694837</v>
       </c>
-      <c r="K15" s="23">
+      <c r="K15" s="12">
         <v>739656</v>
       </c>
-      <c r="L15" s="23">
+      <c r="L15" s="12">
         <v>763733</v>
       </c>
-      <c r="M15" s="23">
+      <c r="M15" s="12">
         <v>698962</v>
       </c>
-      <c r="N15" s="23">
+      <c r="N15" s="12">
         <v>732173</v>
       </c>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9">
-        <f>SUM(C15:N15)</f>
+      <c r="O15" s="27">
+        <f t="shared" si="1"/>
         <v>8287717</v>
       </c>
-      <c r="Q15" s="13"/>
-      <c r="R15" s="3">
+      <c r="P15" s="4"/>
+      <c r="Q15" s="16">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>8287717</v>
       </c>
+      <c r="R15" s="1"/>
       <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
-    </row>
-    <row r="16" spans="1:20" ht="21" x14ac:dyDescent="0.4">
+    </row>
+    <row r="16" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A16" s="1"/>
-      <c r="B16" s="8">
+      <c r="B16" s="25">
         <v>2019</v>
       </c>
-      <c r="C16" s="23">
+      <c r="C16" s="12">
         <v>816792</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="12">
         <v>811807</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16" s="11">
         <v>903678</v>
       </c>
-      <c r="F16" s="26">
+      <c r="F16" s="13">
         <v>1174272</v>
       </c>
-      <c r="G16" s="26">
+      <c r="G16" s="13">
         <v>1399881</v>
       </c>
-      <c r="H16" s="26">
+      <c r="H16" s="13">
         <v>1179014</v>
       </c>
-      <c r="I16" s="26">
+      <c r="I16" s="13">
         <v>1380086</v>
       </c>
-      <c r="J16" s="26">
+      <c r="J16" s="13">
         <v>1448886</v>
       </c>
-      <c r="K16" s="26">
+      <c r="K16" s="13">
         <v>1506868</v>
       </c>
-      <c r="L16" s="26">
+      <c r="L16" s="13">
         <v>1761891</v>
       </c>
-      <c r="M16" s="25">
+      <c r="M16" s="13">
         <v>2059856</v>
       </c>
-      <c r="N16" s="25">
+      <c r="N16" s="13">
         <v>2325909</v>
       </c>
-      <c r="O16" s="22"/>
-      <c r="P16" s="22">
-        <f>SUM(C16:N16)</f>
+      <c r="O16" s="28">
+        <f t="shared" si="1"/>
         <v>16768940</v>
       </c>
-      <c r="Q16" s="13"/>
-      <c r="R16" s="3">
+      <c r="P16" s="4"/>
+      <c r="Q16" s="16">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>16768940</v>
       </c>
+      <c r="R16" s="1"/>
       <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
-    </row>
-    <row r="17" spans="1:20" ht="21" x14ac:dyDescent="0.4">
+    </row>
+    <row r="17" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A17" s="1"/>
-      <c r="B17" s="8">
+      <c r="B17" s="25">
         <v>2020</v>
       </c>
-      <c r="C17" s="26">
+      <c r="C17" s="13">
         <v>1694534</v>
       </c>
-      <c r="D17" s="25">
+      <c r="D17" s="13">
         <v>3203938</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="13">
         <v>3296329</v>
       </c>
-      <c r="F17" s="25">
+      <c r="F17" s="13">
         <v>2694570</v>
       </c>
-      <c r="G17" s="25">
+      <c r="G17" s="13">
         <v>2511957</v>
       </c>
-      <c r="H17" s="25">
+      <c r="H17" s="13">
         <v>2264236</v>
       </c>
-      <c r="I17" s="26">
+      <c r="I17" s="13">
         <v>1255353</v>
       </c>
-      <c r="J17" s="26">
+      <c r="J17" s="13">
         <v>1205188</v>
       </c>
-      <c r="K17" s="26">
+      <c r="K17" s="13">
         <v>1622473</v>
       </c>
-      <c r="L17" s="26">
+      <c r="L17" s="13">
         <v>1912285</v>
       </c>
-      <c r="M17" s="25">
+      <c r="M17" s="13">
         <v>2366693</v>
       </c>
-      <c r="N17" s="25">
+      <c r="N17" s="13">
         <v>2176841</v>
       </c>
-      <c r="O17" s="27"/>
-      <c r="P17" s="28">
-        <f>SUM(C17:N17)</f>
+      <c r="O17" s="29">
+        <f t="shared" si="1"/>
         <v>26204397</v>
       </c>
-      <c r="Q17" s="13"/>
-      <c r="R17" s="3">
+      <c r="P17" s="4"/>
+      <c r="Q17" s="16">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
         <v>26204397</v>
       </c>
+      <c r="R17" s="1"/>
       <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
-    </row>
-    <row r="18" spans="1:20" s="20" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="14"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="30"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="30"/>
-      <c r="P18" s="21">
+    </row>
+    <row r="18" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A18" s="1"/>
+      <c r="B18" s="25">
+        <v>2021</v>
+      </c>
+      <c r="C18" s="14">
+        <v>924261</v>
+      </c>
+      <c r="D18" s="14">
+        <v>1235225</v>
+      </c>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="29">
+        <f t="shared" si="1"/>
+        <v>2159486</v>
+      </c>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="16">
+        <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
+        <v>12956916</v>
+      </c>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+    </row>
+    <row r="19" spans="1:19" s="9" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="5"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="26">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>68812498</v>
-      </c>
-      <c r="Q18" s="18"/>
-      <c r="R18" s="14"/>
-      <c r="S18" s="14"/>
-      <c r="T18" s="14"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="12"/>
-      <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
-    </row>
-    <row r="20" spans="1:20" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A20" s="1"/>
-      <c r="B20" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="31">
-        <f>SUM(C17:N17)</f>
-        <v>26204397</v>
-      </c>
-      <c r="G20" s="31"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
+        <v>70971984</v>
+      </c>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="30"/>
+      <c r="P20" s="3"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
-      <c r="T20" s="1"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
-      <c r="T21" s="1"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
+      <c r="O21" s="22"/>
+    </row>
+    <row r="22" spans="1:19" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -3512,9 +3553,8 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
-      <c r="T22" s="1"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -3534,9 +3574,8 @@
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
-      <c r="T23" s="1"/>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -3556,9 +3595,8 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
-      <c r="T24" s="1"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -3578,9 +3616,8 @@
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
-      <c r="T25" s="1"/>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -3600,9 +3637,8 @@
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
-      <c r="T26" s="1"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -3622,9 +3658,8 @@
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
-      <c r="T27" s="1"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -3644,9 +3679,8 @@
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
-      <c r="T28" s="1"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -3666,9 +3700,8 @@
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
-      <c r="T29" s="1"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -3688,9 +3721,8 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
-      <c r="T30" s="1"/>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -3710,9 +3742,8 @@
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
-      <c r="T31" s="1"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -3732,9 +3763,8 @@
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
-      <c r="T32" s="1"/>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -3754,9 +3784,8 @@
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
-      <c r="T33" s="1"/>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -3776,9 +3805,8 @@
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
-      <c r="T34" s="1"/>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -3798,9 +3826,8 @@
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
-      <c r="T35" s="1"/>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -3820,9 +3847,8 @@
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
-      <c r="T36" s="1"/>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -3842,9 +3868,8 @@
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
-      <c r="T37" s="1"/>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -3864,9 +3889,8 @@
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
-      <c r="T38" s="1"/>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -3886,9 +3910,8 @@
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
-      <c r="T39" s="1"/>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -3908,9 +3931,8 @@
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
-      <c r="T40" s="1"/>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -3930,9 +3952,8 @@
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
       <c r="S41" s="1"/>
-      <c r="T41" s="1"/>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -3952,9 +3973,8 @@
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
       <c r="S42" s="1"/>
-      <c r="T42" s="1"/>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -3974,9 +3994,8 @@
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
       <c r="S43" s="1"/>
-      <c r="T43" s="1"/>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -3996,9 +4015,8 @@
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
       <c r="S44" s="1"/>
-      <c r="T44" s="1"/>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -4018,9 +4036,8 @@
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
       <c r="S45" s="1"/>
-      <c r="T45" s="1"/>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -4040,9 +4057,8 @@
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
       <c r="S46" s="1"/>
-      <c r="T46" s="1"/>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -4062,9 +4078,8 @@
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
       <c r="S47" s="1"/>
-      <c r="T47" s="1"/>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -4074,11 +4089,9 @@
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
-      <c r="J48" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="K48" s="33"/>
-      <c r="L48" s="33"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
@@ -4086,9 +4099,8 @@
       <c r="Q48" s="1"/>
       <c r="R48" s="1"/>
       <c r="S48" s="1"/>
-      <c r="T48" s="1"/>
-    </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -4100,7 +4112,7 @@
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
-      <c r="L49" s="11"/>
+      <c r="L49" s="1"/>
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
@@ -4108,9 +4120,8 @@
       <c r="Q49" s="1"/>
       <c r="R49" s="1"/>
       <c r="S49" s="1"/>
-      <c r="T49" s="1"/>
-    </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -4120,9 +4131,11 @@
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
-      <c r="K50" s="1"/>
-      <c r="L50" s="1"/>
+      <c r="J50" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="K50" s="21"/>
+      <c r="L50" s="21"/>
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
       <c r="O50" s="1"/>
@@ -4130,42 +4143,325 @@
       <c r="Q50" s="1"/>
       <c r="R50" s="1"/>
       <c r="S50" s="1"/>
-      <c r="T50" s="1"/>
-    </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
-      <c r="J51" s="1"/>
-      <c r="K51" s="1"/>
-      <c r="L51" s="1"/>
-      <c r="M51" s="1"/>
-      <c r="N51" s="1"/>
-      <c r="O51" s="1"/>
-      <c r="P51" s="1"/>
-      <c r="Q51" s="1"/>
-      <c r="R51" s="1"/>
-      <c r="S51" s="1"/>
-      <c r="T51" s="1"/>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A51" s="22"/>
+      <c r="B51" s="22"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="22"/>
+      <c r="F51" s="22"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="22"/>
+      <c r="I51" s="22"/>
+      <c r="J51" s="22"/>
+      <c r="K51" s="22"/>
+      <c r="L51" s="23"/>
+      <c r="M51" s="22"/>
+      <c r="N51" s="22"/>
+      <c r="O51" s="22"/>
+      <c r="P51" s="22"/>
+      <c r="Q51" s="22"/>
+      <c r="R51" s="22"/>
+      <c r="S51" s="22"/>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A52" s="22"/>
+      <c r="B52" s="22"/>
+      <c r="C52" s="22"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="22"/>
+      <c r="G52" s="22"/>
+      <c r="H52" s="22"/>
+      <c r="I52" s="22"/>
+      <c r="J52" s="22"/>
+      <c r="K52" s="22"/>
+      <c r="L52" s="22"/>
+      <c r="M52" s="22"/>
+      <c r="N52" s="22"/>
+      <c r="O52" s="22"/>
+      <c r="P52" s="22"/>
+      <c r="Q52" s="22"/>
+      <c r="R52" s="22"/>
+      <c r="S52" s="22"/>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A53" s="22"/>
+      <c r="B53" s="22"/>
+      <c r="C53" s="22"/>
+      <c r="D53" s="22"/>
+      <c r="E53" s="22"/>
+      <c r="F53" s="22"/>
+      <c r="G53" s="22"/>
+      <c r="H53" s="22"/>
+      <c r="I53" s="22"/>
+      <c r="J53" s="22"/>
+      <c r="K53" s="22"/>
+      <c r="L53" s="22"/>
+      <c r="M53" s="22"/>
+      <c r="N53" s="22"/>
+      <c r="O53" s="22"/>
+      <c r="P53" s="22"/>
+      <c r="Q53" s="22"/>
+      <c r="R53" s="22"/>
+      <c r="S53" s="22"/>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A54" s="22"/>
+      <c r="B54" s="22"/>
+      <c r="C54" s="22"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="22"/>
+      <c r="F54" s="22"/>
+      <c r="G54" s="22"/>
+      <c r="H54" s="22"/>
+      <c r="I54" s="22"/>
+      <c r="J54" s="22"/>
+      <c r="K54" s="22"/>
+      <c r="L54" s="22"/>
+      <c r="M54" s="22"/>
+      <c r="N54" s="22"/>
+      <c r="O54" s="22"/>
+      <c r="P54" s="22"/>
+      <c r="Q54" s="22"/>
+      <c r="R54" s="22"/>
+      <c r="S54" s="22"/>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A55" s="22"/>
+      <c r="B55" s="22"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="22"/>
+      <c r="G55" s="22"/>
+      <c r="H55" s="22"/>
+      <c r="I55" s="22"/>
+      <c r="J55" s="22"/>
+      <c r="K55" s="22"/>
+      <c r="L55" s="22"/>
+      <c r="M55" s="22"/>
+      <c r="N55" s="22"/>
+      <c r="O55" s="22"/>
+      <c r="P55" s="22"/>
+      <c r="Q55" s="22"/>
+      <c r="R55" s="22"/>
+      <c r="S55" s="22"/>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A56" s="22"/>
+      <c r="B56" s="22"/>
+      <c r="C56" s="22"/>
+      <c r="D56" s="22"/>
+      <c r="E56" s="22"/>
+      <c r="F56" s="22"/>
+      <c r="G56" s="22"/>
+      <c r="H56" s="22"/>
+      <c r="I56" s="22"/>
+      <c r="J56" s="22"/>
+      <c r="K56" s="22"/>
+      <c r="L56" s="22"/>
+      <c r="M56" s="22"/>
+      <c r="N56" s="22"/>
+      <c r="O56" s="22"/>
+      <c r="P56" s="22"/>
+      <c r="Q56" s="22"/>
+      <c r="R56" s="22"/>
+      <c r="S56" s="22"/>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A57" s="22"/>
+      <c r="B57" s="22"/>
+      <c r="C57" s="22"/>
+      <c r="D57" s="22"/>
+      <c r="E57" s="22"/>
+      <c r="F57" s="22"/>
+      <c r="G57" s="22"/>
+      <c r="H57" s="22"/>
+      <c r="I57" s="22"/>
+      <c r="J57" s="22"/>
+      <c r="K57" s="22"/>
+      <c r="L57" s="22"/>
+      <c r="M57" s="22"/>
+      <c r="N57" s="22"/>
+      <c r="O57" s="22"/>
+      <c r="P57" s="22"/>
+      <c r="Q57" s="22"/>
+      <c r="R57" s="22"/>
+      <c r="S57" s="22"/>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A58" s="22"/>
+      <c r="B58" s="22"/>
+      <c r="C58" s="22"/>
+      <c r="D58" s="22"/>
+      <c r="E58" s="22"/>
+      <c r="F58" s="22"/>
+      <c r="G58" s="22"/>
+      <c r="H58" s="22"/>
+      <c r="I58" s="22"/>
+      <c r="J58" s="22"/>
+      <c r="K58" s="22"/>
+      <c r="L58" s="22"/>
+      <c r="M58" s="22"/>
+      <c r="N58" s="22"/>
+      <c r="O58" s="22"/>
+      <c r="P58" s="22"/>
+      <c r="Q58" s="22"/>
+      <c r="R58" s="22"/>
+      <c r="S58" s="22"/>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A59" s="22"/>
+      <c r="B59" s="22"/>
+      <c r="C59" s="22"/>
+      <c r="D59" s="22"/>
+      <c r="E59" s="22"/>
+      <c r="F59" s="22"/>
+      <c r="G59" s="22"/>
+      <c r="H59" s="22"/>
+      <c r="I59" s="22"/>
+      <c r="J59" s="22"/>
+      <c r="K59" s="22"/>
+      <c r="L59" s="22"/>
+      <c r="M59" s="22"/>
+      <c r="N59" s="22"/>
+      <c r="O59" s="22"/>
+      <c r="P59" s="22"/>
+      <c r="Q59" s="22"/>
+      <c r="R59" s="22"/>
+      <c r="S59" s="22"/>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A60" s="22"/>
+      <c r="B60" s="22"/>
+      <c r="C60" s="22"/>
+      <c r="D60" s="22"/>
+      <c r="E60" s="22"/>
+      <c r="F60" s="22"/>
+      <c r="G60" s="22"/>
+      <c r="H60" s="22"/>
+      <c r="I60" s="22"/>
+      <c r="J60" s="22"/>
+      <c r="K60" s="22"/>
+      <c r="L60" s="22"/>
+      <c r="M60" s="22"/>
+      <c r="N60" s="22"/>
+      <c r="O60" s="22"/>
+      <c r="P60" s="22"/>
+      <c r="Q60" s="22"/>
+      <c r="R60" s="22"/>
+      <c r="S60" s="22"/>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A61" s="22"/>
+      <c r="B61" s="22"/>
+      <c r="C61" s="22"/>
+      <c r="D61" s="22"/>
+      <c r="E61" s="22"/>
+      <c r="F61" s="22"/>
+      <c r="G61" s="22"/>
+      <c r="H61" s="22"/>
+      <c r="I61" s="22"/>
+      <c r="J61" s="22"/>
+      <c r="K61" s="22"/>
+      <c r="L61" s="22"/>
+      <c r="M61" s="22"/>
+      <c r="N61" s="22"/>
+      <c r="O61" s="22"/>
+      <c r="P61" s="22"/>
+      <c r="Q61" s="22"/>
+      <c r="R61" s="22"/>
+      <c r="S61" s="22"/>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A62" s="22"/>
+      <c r="B62" s="22"/>
+      <c r="C62" s="22"/>
+      <c r="D62" s="22"/>
+      <c r="E62" s="22"/>
+      <c r="F62" s="22"/>
+      <c r="G62" s="22"/>
+      <c r="H62" s="22"/>
+      <c r="I62" s="22"/>
+      <c r="J62" s="22"/>
+      <c r="K62" s="22"/>
+      <c r="L62" s="22"/>
+      <c r="M62" s="22"/>
+      <c r="N62" s="22"/>
+      <c r="O62" s="22"/>
+      <c r="P62" s="22"/>
+      <c r="Q62" s="22"/>
+      <c r="R62" s="22"/>
+      <c r="S62" s="22"/>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A63" s="22"/>
+      <c r="B63" s="22"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="22"/>
+      <c r="F63" s="22"/>
+      <c r="G63" s="22"/>
+      <c r="H63" s="22"/>
+      <c r="I63" s="22"/>
+      <c r="J63" s="22"/>
+      <c r="K63" s="22"/>
+      <c r="L63" s="22"/>
+      <c r="M63" s="22"/>
+      <c r="N63" s="22"/>
+      <c r="O63" s="22"/>
+      <c r="P63" s="22"/>
+      <c r="Q63" s="22"/>
+      <c r="R63" s="22"/>
+      <c r="S63" s="22"/>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A64" s="22"/>
+      <c r="B64" s="22"/>
+      <c r="C64" s="22"/>
+      <c r="D64" s="22"/>
+      <c r="E64" s="22"/>
+      <c r="F64" s="22"/>
+      <c r="G64" s="22"/>
+      <c r="H64" s="22"/>
+      <c r="I64" s="22"/>
+      <c r="J64" s="22"/>
+      <c r="K64" s="22"/>
+      <c r="L64" s="22"/>
+      <c r="M64" s="22"/>
+      <c r="N64" s="22"/>
+      <c r="O64" s="22"/>
+      <c r="P64" s="22"/>
+      <c r="Q64" s="22"/>
+      <c r="R64" s="22"/>
+      <c r="S64" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B18:O18"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="J48:L48"/>
+    <mergeCell ref="B19:N19"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="J50:L50"/>
   </mergeCells>
+  <conditionalFormatting sqref="C5:N18">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="P5:P17" formulaRange="1"/>
-    <ignoredError sqref="P4" calculatedColumn="1"/>
+    <ignoredError sqref="O5:O18" formulaRange="1"/>
+    <ignoredError sqref="O4" calculatedColumn="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Blog Statistics (March 2021)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c93c05515dfe04a/GIT Hub/kunal-chowdhury.com/blog-stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="176" documentId="114_{B49989D9-13EE-4EB4-8B18-ED25DB6F8102}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AFEE2193-6E0C-493A-8329-5EB9B8BABC3B}"/>
+  <xr:revisionPtr revIDLastSave="179" documentId="114_{B49989D9-13EE-4EB4-8B18-ED25DB6F8102}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{66AF4201-C5EF-4A7D-8D6B-6F122ED4AC77}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -307,6 +307,21 @@
     <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="10" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="10" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -322,21 +337,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="10" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="10" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,10 +555,13 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFA9496"/>
+      <color rgb="FF66FF33"/>
+      <color rgb="FF33CC33"/>
+      <color rgb="FFF8696B"/>
+      <color rgb="FFFFFF99"/>
       <color rgb="FF99FF66"/>
-      <color rgb="FF66FF33"/>
       <color rgb="FFCCFF99"/>
-      <color rgb="FFFFFF99"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1503,7 +1506,7 @@
                   <c:v>26204397</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2159486</c:v>
+                  <c:v>4206692</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2594,9 +2597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="T37" sqref="T37"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2707,43 +2708,43 @@
     <row r="4" spans="1:19" s="9" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="6"/>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="J4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="24" t="s">
+      <c r="L4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="24" t="s">
+      <c r="M4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="24" t="s">
+      <c r="N4" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="19" t="s">
         <v>12</v>
       </c>
       <c r="P4" s="7"/>
@@ -2753,7 +2754,7 @@
     </row>
     <row r="5" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A5" s="1"/>
-      <c r="B5" s="25">
+      <c r="B5" s="20">
         <v>2008</v>
       </c>
       <c r="C5" s="15">
@@ -2792,7 +2793,7 @@
       <c r="N5" s="10">
         <v>109</v>
       </c>
-      <c r="O5" s="27">
+      <c r="O5" s="22">
         <f>SUM(C5:N5)</f>
         <v>326</v>
       </c>
@@ -2806,7 +2807,7 @@
     </row>
     <row r="6" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A6" s="1"/>
-      <c r="B6" s="25">
+      <c r="B6" s="20">
         <v>2009</v>
       </c>
       <c r="C6" s="10">
@@ -2845,7 +2846,7 @@
       <c r="N6" s="10">
         <v>18516</v>
       </c>
-      <c r="O6" s="27">
+      <c r="O6" s="22">
         <f t="shared" ref="O6:O12" si="0">SUM(C6:N6)</f>
         <v>80379</v>
       </c>
@@ -2859,7 +2860,7 @@
     </row>
     <row r="7" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A7" s="1"/>
-      <c r="B7" s="25">
+      <c r="B7" s="20">
         <v>2010</v>
       </c>
       <c r="C7" s="10">
@@ -2898,7 +2899,7 @@
       <c r="N7" s="10">
         <v>42658</v>
       </c>
-      <c r="O7" s="27">
+      <c r="O7" s="22">
         <f t="shared" si="0"/>
         <v>463113</v>
       </c>
@@ -2912,7 +2913,7 @@
     </row>
     <row r="8" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A8" s="1"/>
-      <c r="B8" s="25">
+      <c r="B8" s="20">
         <v>2011</v>
       </c>
       <c r="C8" s="10">
@@ -2951,7 +2952,7 @@
       <c r="N8" s="10">
         <v>64581</v>
       </c>
-      <c r="O8" s="27">
+      <c r="O8" s="22">
         <f t="shared" si="0"/>
         <v>803010</v>
       </c>
@@ -2965,7 +2966,7 @@
     </row>
     <row r="9" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A9" s="1"/>
-      <c r="B9" s="25">
+      <c r="B9" s="20">
         <v>2012</v>
       </c>
       <c r="C9" s="10">
@@ -3004,7 +3005,7 @@
       <c r="N9" s="10">
         <v>73172</v>
       </c>
-      <c r="O9" s="27">
+      <c r="O9" s="22">
         <f t="shared" si="0"/>
         <v>888853</v>
       </c>
@@ -3018,7 +3019,7 @@
     </row>
     <row r="10" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A10" s="1"/>
-      <c r="B10" s="25">
+      <c r="B10" s="20">
         <v>2013</v>
       </c>
       <c r="C10" s="10">
@@ -3057,7 +3058,7 @@
       <c r="N10" s="10">
         <v>73625</v>
       </c>
-      <c r="O10" s="27">
+      <c r="O10" s="22">
         <f t="shared" si="0"/>
         <v>935657</v>
       </c>
@@ -3071,7 +3072,7 @@
     </row>
     <row r="11" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A11" s="1"/>
-      <c r="B11" s="25">
+      <c r="B11" s="20">
         <v>2014</v>
       </c>
       <c r="C11" s="10">
@@ -3110,7 +3111,7 @@
       <c r="N11" s="11">
         <v>101904</v>
       </c>
-      <c r="O11" s="27">
+      <c r="O11" s="22">
         <f t="shared" si="0"/>
         <v>938639</v>
       </c>
@@ -3124,7 +3125,7 @@
     </row>
     <row r="12" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A12" s="1"/>
-      <c r="B12" s="25">
+      <c r="B12" s="20">
         <v>2015</v>
       </c>
       <c r="C12" s="10">
@@ -3163,7 +3164,7 @@
       <c r="N12" s="11">
         <v>129945</v>
       </c>
-      <c r="O12" s="27">
+      <c r="O12" s="22">
         <f t="shared" si="0"/>
         <v>1217957</v>
       </c>
@@ -3177,7 +3178,7 @@
     </row>
     <row r="13" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A13" s="1"/>
-      <c r="B13" s="25">
+      <c r="B13" s="20">
         <v>2016</v>
       </c>
       <c r="C13" s="11">
@@ -3216,7 +3217,7 @@
       <c r="N13" s="12">
         <v>674509</v>
       </c>
-      <c r="O13" s="27">
+      <c r="O13" s="22">
         <f t="shared" ref="O13:O18" si="1">SUM(C13:N13)</f>
         <v>4530257</v>
       </c>
@@ -3230,7 +3231,7 @@
     </row>
     <row r="14" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A14" s="1"/>
-      <c r="B14" s="25">
+      <c r="B14" s="20">
         <v>2017</v>
       </c>
       <c r="C14" s="12">
@@ -3269,7 +3270,7 @@
       <c r="N14" s="12">
         <v>565361</v>
       </c>
-      <c r="O14" s="27">
+      <c r="O14" s="22">
         <f t="shared" si="1"/>
         <v>7693253</v>
       </c>
@@ -3283,7 +3284,7 @@
     </row>
     <row r="15" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A15" s="1"/>
-      <c r="B15" s="25">
+      <c r="B15" s="20">
         <v>2018</v>
       </c>
       <c r="C15" s="12">
@@ -3322,7 +3323,7 @@
       <c r="N15" s="12">
         <v>732173</v>
       </c>
-      <c r="O15" s="27">
+      <c r="O15" s="22">
         <f t="shared" si="1"/>
         <v>8287717</v>
       </c>
@@ -3336,7 +3337,7 @@
     </row>
     <row r="16" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A16" s="1"/>
-      <c r="B16" s="25">
+      <c r="B16" s="20">
         <v>2019</v>
       </c>
       <c r="C16" s="12">
@@ -3375,7 +3376,7 @@
       <c r="N16" s="13">
         <v>2325909</v>
       </c>
-      <c r="O16" s="28">
+      <c r="O16" s="23">
         <f t="shared" si="1"/>
         <v>16768940</v>
       </c>
@@ -3389,7 +3390,7 @@
     </row>
     <row r="17" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A17" s="1"/>
-      <c r="B17" s="25">
+      <c r="B17" s="20">
         <v>2020</v>
       </c>
       <c r="C17" s="13">
@@ -3428,7 +3429,7 @@
       <c r="N17" s="13">
         <v>2176841</v>
       </c>
-      <c r="O17" s="29">
+      <c r="O17" s="24">
         <f t="shared" si="1"/>
         <v>26204397</v>
       </c>
@@ -3442,7 +3443,7 @@
     </row>
     <row r="18" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A18" s="1"/>
-      <c r="B18" s="25">
+      <c r="B18" s="20">
         <v>2021</v>
       </c>
       <c r="C18" s="14">
@@ -3451,7 +3452,9 @@
       <c r="D18" s="14">
         <v>1235225</v>
       </c>
-      <c r="E18" s="14"/>
+      <c r="E18" s="14">
+        <v>2047206</v>
+      </c>
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
@@ -3461,36 +3464,36 @@
       <c r="L18" s="14"/>
       <c r="M18" s="14"/>
       <c r="N18" s="14"/>
-      <c r="O18" s="29">
+      <c r="O18" s="24">
         <f t="shared" si="1"/>
-        <v>2159486</v>
+        <v>4206692</v>
       </c>
       <c r="P18" s="4"/>
       <c r="Q18" s="16">
         <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>12956916</v>
+        <v>16826768</v>
       </c>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
     </row>
     <row r="19" spans="1:19" s="9" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="26">
+      <c r="B19" s="26"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="27"/>
+      <c r="O19" s="21">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>70971984</v>
+        <v>73019190</v>
       </c>
       <c r="P19" s="7"/>
       <c r="Q19" s="5"/>
@@ -3498,49 +3501,49 @@
       <c r="S19" s="5"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B20" s="30"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
-      <c r="K20" s="30"/>
-      <c r="L20" s="30"/>
-      <c r="M20" s="30"/>
-      <c r="N20" s="30"/>
-      <c r="O20" s="30"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="25"/>
+      <c r="N20" s="25"/>
+      <c r="O20" s="25"/>
       <c r="P20" s="3"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
     </row>
     <row r="21" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="22"/>
-      <c r="O21" s="22"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17"/>
     </row>
     <row r="22" spans="1:19" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -4131,11 +4134,11 @@
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
-      <c r="J50" s="21" t="s">
+      <c r="J50" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="K50" s="21"/>
-      <c r="L50" s="21"/>
+      <c r="K50" s="30"/>
+      <c r="L50" s="30"/>
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
       <c r="O50" s="1"/>
@@ -4145,298 +4148,298 @@
       <c r="S50" s="1"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A51" s="22"/>
-      <c r="B51" s="22"/>
-      <c r="C51" s="22"/>
-      <c r="D51" s="22"/>
-      <c r="E51" s="22"/>
-      <c r="F51" s="22"/>
-      <c r="G51" s="22"/>
-      <c r="H51" s="22"/>
-      <c r="I51" s="22"/>
-      <c r="J51" s="22"/>
-      <c r="K51" s="22"/>
-      <c r="L51" s="23"/>
-      <c r="M51" s="22"/>
-      <c r="N51" s="22"/>
-      <c r="O51" s="22"/>
-      <c r="P51" s="22"/>
-      <c r="Q51" s="22"/>
-      <c r="R51" s="22"/>
-      <c r="S51" s="22"/>
+      <c r="A51" s="17"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="17"/>
+      <c r="H51" s="17"/>
+      <c r="I51" s="17"/>
+      <c r="J51" s="17"/>
+      <c r="K51" s="17"/>
+      <c r="L51" s="18"/>
+      <c r="M51" s="17"/>
+      <c r="N51" s="17"/>
+      <c r="O51" s="17"/>
+      <c r="P51" s="17"/>
+      <c r="Q51" s="17"/>
+      <c r="R51" s="17"/>
+      <c r="S51" s="17"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A52" s="22"/>
-      <c r="B52" s="22"/>
-      <c r="C52" s="22"/>
-      <c r="D52" s="22"/>
-      <c r="E52" s="22"/>
-      <c r="F52" s="22"/>
-      <c r="G52" s="22"/>
-      <c r="H52" s="22"/>
-      <c r="I52" s="22"/>
-      <c r="J52" s="22"/>
-      <c r="K52" s="22"/>
-      <c r="L52" s="22"/>
-      <c r="M52" s="22"/>
-      <c r="N52" s="22"/>
-      <c r="O52" s="22"/>
-      <c r="P52" s="22"/>
-      <c r="Q52" s="22"/>
-      <c r="R52" s="22"/>
-      <c r="S52" s="22"/>
+      <c r="A52" s="17"/>
+      <c r="B52" s="17"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="17"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="17"/>
+      <c r="H52" s="17"/>
+      <c r="I52" s="17"/>
+      <c r="J52" s="17"/>
+      <c r="K52" s="17"/>
+      <c r="L52" s="17"/>
+      <c r="M52" s="17"/>
+      <c r="N52" s="17"/>
+      <c r="O52" s="17"/>
+      <c r="P52" s="17"/>
+      <c r="Q52" s="17"/>
+      <c r="R52" s="17"/>
+      <c r="S52" s="17"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A53" s="22"/>
-      <c r="B53" s="22"/>
-      <c r="C53" s="22"/>
-      <c r="D53" s="22"/>
-      <c r="E53" s="22"/>
-      <c r="F53" s="22"/>
-      <c r="G53" s="22"/>
-      <c r="H53" s="22"/>
-      <c r="I53" s="22"/>
-      <c r="J53" s="22"/>
-      <c r="K53" s="22"/>
-      <c r="L53" s="22"/>
-      <c r="M53" s="22"/>
-      <c r="N53" s="22"/>
-      <c r="O53" s="22"/>
-      <c r="P53" s="22"/>
-      <c r="Q53" s="22"/>
-      <c r="R53" s="22"/>
-      <c r="S53" s="22"/>
+      <c r="A53" s="17"/>
+      <c r="B53" s="17"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="17"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="17"/>
+      <c r="I53" s="17"/>
+      <c r="J53" s="17"/>
+      <c r="K53" s="17"/>
+      <c r="L53" s="17"/>
+      <c r="M53" s="17"/>
+      <c r="N53" s="17"/>
+      <c r="O53" s="17"/>
+      <c r="P53" s="17"/>
+      <c r="Q53" s="17"/>
+      <c r="R53" s="17"/>
+      <c r="S53" s="17"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A54" s="22"/>
-      <c r="B54" s="22"/>
-      <c r="C54" s="22"/>
-      <c r="D54" s="22"/>
-      <c r="E54" s="22"/>
-      <c r="F54" s="22"/>
-      <c r="G54" s="22"/>
-      <c r="H54" s="22"/>
-      <c r="I54" s="22"/>
-      <c r="J54" s="22"/>
-      <c r="K54" s="22"/>
-      <c r="L54" s="22"/>
-      <c r="M54" s="22"/>
-      <c r="N54" s="22"/>
-      <c r="O54" s="22"/>
-      <c r="P54" s="22"/>
-      <c r="Q54" s="22"/>
-      <c r="R54" s="22"/>
-      <c r="S54" s="22"/>
+      <c r="A54" s="17"/>
+      <c r="B54" s="17"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="17"/>
+      <c r="F54" s="17"/>
+      <c r="G54" s="17"/>
+      <c r="H54" s="17"/>
+      <c r="I54" s="17"/>
+      <c r="J54" s="17"/>
+      <c r="K54" s="17"/>
+      <c r="L54" s="17"/>
+      <c r="M54" s="17"/>
+      <c r="N54" s="17"/>
+      <c r="O54" s="17"/>
+      <c r="P54" s="17"/>
+      <c r="Q54" s="17"/>
+      <c r="R54" s="17"/>
+      <c r="S54" s="17"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A55" s="22"/>
-      <c r="B55" s="22"/>
-      <c r="C55" s="22"/>
-      <c r="D55" s="22"/>
-      <c r="E55" s="22"/>
-      <c r="F55" s="22"/>
-      <c r="G55" s="22"/>
-      <c r="H55" s="22"/>
-      <c r="I55" s="22"/>
-      <c r="J55" s="22"/>
-      <c r="K55" s="22"/>
-      <c r="L55" s="22"/>
-      <c r="M55" s="22"/>
-      <c r="N55" s="22"/>
-      <c r="O55" s="22"/>
-      <c r="P55" s="22"/>
-      <c r="Q55" s="22"/>
-      <c r="R55" s="22"/>
-      <c r="S55" s="22"/>
+      <c r="A55" s="17"/>
+      <c r="B55" s="17"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="17"/>
+      <c r="H55" s="17"/>
+      <c r="I55" s="17"/>
+      <c r="J55" s="17"/>
+      <c r="K55" s="17"/>
+      <c r="L55" s="17"/>
+      <c r="M55" s="17"/>
+      <c r="N55" s="17"/>
+      <c r="O55" s="17"/>
+      <c r="P55" s="17"/>
+      <c r="Q55" s="17"/>
+      <c r="R55" s="17"/>
+      <c r="S55" s="17"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A56" s="22"/>
-      <c r="B56" s="22"/>
-      <c r="C56" s="22"/>
-      <c r="D56" s="22"/>
-      <c r="E56" s="22"/>
-      <c r="F56" s="22"/>
-      <c r="G56" s="22"/>
-      <c r="H56" s="22"/>
-      <c r="I56" s="22"/>
-      <c r="J56" s="22"/>
-      <c r="K56" s="22"/>
-      <c r="L56" s="22"/>
-      <c r="M56" s="22"/>
-      <c r="N56" s="22"/>
-      <c r="O56" s="22"/>
-      <c r="P56" s="22"/>
-      <c r="Q56" s="22"/>
-      <c r="R56" s="22"/>
-      <c r="S56" s="22"/>
+      <c r="A56" s="17"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="17"/>
+      <c r="I56" s="17"/>
+      <c r="J56" s="17"/>
+      <c r="K56" s="17"/>
+      <c r="L56" s="17"/>
+      <c r="M56" s="17"/>
+      <c r="N56" s="17"/>
+      <c r="O56" s="17"/>
+      <c r="P56" s="17"/>
+      <c r="Q56" s="17"/>
+      <c r="R56" s="17"/>
+      <c r="S56" s="17"/>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A57" s="22"/>
-      <c r="B57" s="22"/>
-      <c r="C57" s="22"/>
-      <c r="D57" s="22"/>
-      <c r="E57" s="22"/>
-      <c r="F57" s="22"/>
-      <c r="G57" s="22"/>
-      <c r="H57" s="22"/>
-      <c r="I57" s="22"/>
-      <c r="J57" s="22"/>
-      <c r="K57" s="22"/>
-      <c r="L57" s="22"/>
-      <c r="M57" s="22"/>
-      <c r="N57" s="22"/>
-      <c r="O57" s="22"/>
-      <c r="P57" s="22"/>
-      <c r="Q57" s="22"/>
-      <c r="R57" s="22"/>
-      <c r="S57" s="22"/>
+      <c r="A57" s="17"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="17"/>
+      <c r="H57" s="17"/>
+      <c r="I57" s="17"/>
+      <c r="J57" s="17"/>
+      <c r="K57" s="17"/>
+      <c r="L57" s="17"/>
+      <c r="M57" s="17"/>
+      <c r="N57" s="17"/>
+      <c r="O57" s="17"/>
+      <c r="P57" s="17"/>
+      <c r="Q57" s="17"/>
+      <c r="R57" s="17"/>
+      <c r="S57" s="17"/>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A58" s="22"/>
-      <c r="B58" s="22"/>
-      <c r="C58" s="22"/>
-      <c r="D58" s="22"/>
-      <c r="E58" s="22"/>
-      <c r="F58" s="22"/>
-      <c r="G58" s="22"/>
-      <c r="H58" s="22"/>
-      <c r="I58" s="22"/>
-      <c r="J58" s="22"/>
-      <c r="K58" s="22"/>
-      <c r="L58" s="22"/>
-      <c r="M58" s="22"/>
-      <c r="N58" s="22"/>
-      <c r="O58" s="22"/>
-      <c r="P58" s="22"/>
-      <c r="Q58" s="22"/>
-      <c r="R58" s="22"/>
-      <c r="S58" s="22"/>
+      <c r="A58" s="17"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="17"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="17"/>
+      <c r="H58" s="17"/>
+      <c r="I58" s="17"/>
+      <c r="J58" s="17"/>
+      <c r="K58" s="17"/>
+      <c r="L58" s="17"/>
+      <c r="M58" s="17"/>
+      <c r="N58" s="17"/>
+      <c r="O58" s="17"/>
+      <c r="P58" s="17"/>
+      <c r="Q58" s="17"/>
+      <c r="R58" s="17"/>
+      <c r="S58" s="17"/>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A59" s="22"/>
-      <c r="B59" s="22"/>
-      <c r="C59" s="22"/>
-      <c r="D59" s="22"/>
-      <c r="E59" s="22"/>
-      <c r="F59" s="22"/>
-      <c r="G59" s="22"/>
-      <c r="H59" s="22"/>
-      <c r="I59" s="22"/>
-      <c r="J59" s="22"/>
-      <c r="K59" s="22"/>
-      <c r="L59" s="22"/>
-      <c r="M59" s="22"/>
-      <c r="N59" s="22"/>
-      <c r="O59" s="22"/>
-      <c r="P59" s="22"/>
-      <c r="Q59" s="22"/>
-      <c r="R59" s="22"/>
-      <c r="S59" s="22"/>
+      <c r="A59" s="17"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="17"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="17"/>
+      <c r="H59" s="17"/>
+      <c r="I59" s="17"/>
+      <c r="J59" s="17"/>
+      <c r="K59" s="17"/>
+      <c r="L59" s="17"/>
+      <c r="M59" s="17"/>
+      <c r="N59" s="17"/>
+      <c r="O59" s="17"/>
+      <c r="P59" s="17"/>
+      <c r="Q59" s="17"/>
+      <c r="R59" s="17"/>
+      <c r="S59" s="17"/>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A60" s="22"/>
-      <c r="B60" s="22"/>
-      <c r="C60" s="22"/>
-      <c r="D60" s="22"/>
-      <c r="E60" s="22"/>
-      <c r="F60" s="22"/>
-      <c r="G60" s="22"/>
-      <c r="H60" s="22"/>
-      <c r="I60" s="22"/>
-      <c r="J60" s="22"/>
-      <c r="K60" s="22"/>
-      <c r="L60" s="22"/>
-      <c r="M60" s="22"/>
-      <c r="N60" s="22"/>
-      <c r="O60" s="22"/>
-      <c r="P60" s="22"/>
-      <c r="Q60" s="22"/>
-      <c r="R60" s="22"/>
-      <c r="S60" s="22"/>
+      <c r="A60" s="17"/>
+      <c r="B60" s="17"/>
+      <c r="C60" s="17"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="17"/>
+      <c r="F60" s="17"/>
+      <c r="G60" s="17"/>
+      <c r="H60" s="17"/>
+      <c r="I60" s="17"/>
+      <c r="J60" s="17"/>
+      <c r="K60" s="17"/>
+      <c r="L60" s="17"/>
+      <c r="M60" s="17"/>
+      <c r="N60" s="17"/>
+      <c r="O60" s="17"/>
+      <c r="P60" s="17"/>
+      <c r="Q60" s="17"/>
+      <c r="R60" s="17"/>
+      <c r="S60" s="17"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A61" s="22"/>
-      <c r="B61" s="22"/>
-      <c r="C61" s="22"/>
-      <c r="D61" s="22"/>
-      <c r="E61" s="22"/>
-      <c r="F61" s="22"/>
-      <c r="G61" s="22"/>
-      <c r="H61" s="22"/>
-      <c r="I61" s="22"/>
-      <c r="J61" s="22"/>
-      <c r="K61" s="22"/>
-      <c r="L61" s="22"/>
-      <c r="M61" s="22"/>
-      <c r="N61" s="22"/>
-      <c r="O61" s="22"/>
-      <c r="P61" s="22"/>
-      <c r="Q61" s="22"/>
-      <c r="R61" s="22"/>
-      <c r="S61" s="22"/>
+      <c r="A61" s="17"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="17"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="17"/>
+      <c r="F61" s="17"/>
+      <c r="G61" s="17"/>
+      <c r="H61" s="17"/>
+      <c r="I61" s="17"/>
+      <c r="J61" s="17"/>
+      <c r="K61" s="17"/>
+      <c r="L61" s="17"/>
+      <c r="M61" s="17"/>
+      <c r="N61" s="17"/>
+      <c r="O61" s="17"/>
+      <c r="P61" s="17"/>
+      <c r="Q61" s="17"/>
+      <c r="R61" s="17"/>
+      <c r="S61" s="17"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A62" s="22"/>
-      <c r="B62" s="22"/>
-      <c r="C62" s="22"/>
-      <c r="D62" s="22"/>
-      <c r="E62" s="22"/>
-      <c r="F62" s="22"/>
-      <c r="G62" s="22"/>
-      <c r="H62" s="22"/>
-      <c r="I62" s="22"/>
-      <c r="J62" s="22"/>
-      <c r="K62" s="22"/>
-      <c r="L62" s="22"/>
-      <c r="M62" s="22"/>
-      <c r="N62" s="22"/>
-      <c r="O62" s="22"/>
-      <c r="P62" s="22"/>
-      <c r="Q62" s="22"/>
-      <c r="R62" s="22"/>
-      <c r="S62" s="22"/>
+      <c r="A62" s="17"/>
+      <c r="B62" s="17"/>
+      <c r="C62" s="17"/>
+      <c r="D62" s="17"/>
+      <c r="E62" s="17"/>
+      <c r="F62" s="17"/>
+      <c r="G62" s="17"/>
+      <c r="H62" s="17"/>
+      <c r="I62" s="17"/>
+      <c r="J62" s="17"/>
+      <c r="K62" s="17"/>
+      <c r="L62" s="17"/>
+      <c r="M62" s="17"/>
+      <c r="N62" s="17"/>
+      <c r="O62" s="17"/>
+      <c r="P62" s="17"/>
+      <c r="Q62" s="17"/>
+      <c r="R62" s="17"/>
+      <c r="S62" s="17"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A63" s="22"/>
-      <c r="B63" s="22"/>
-      <c r="C63" s="22"/>
-      <c r="D63" s="22"/>
-      <c r="E63" s="22"/>
-      <c r="F63" s="22"/>
-      <c r="G63" s="22"/>
-      <c r="H63" s="22"/>
-      <c r="I63" s="22"/>
-      <c r="J63" s="22"/>
-      <c r="K63" s="22"/>
-      <c r="L63" s="22"/>
-      <c r="M63" s="22"/>
-      <c r="N63" s="22"/>
-      <c r="O63" s="22"/>
-      <c r="P63" s="22"/>
-      <c r="Q63" s="22"/>
-      <c r="R63" s="22"/>
-      <c r="S63" s="22"/>
+      <c r="A63" s="17"/>
+      <c r="B63" s="17"/>
+      <c r="C63" s="17"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="17"/>
+      <c r="F63" s="17"/>
+      <c r="G63" s="17"/>
+      <c r="H63" s="17"/>
+      <c r="I63" s="17"/>
+      <c r="J63" s="17"/>
+      <c r="K63" s="17"/>
+      <c r="L63" s="17"/>
+      <c r="M63" s="17"/>
+      <c r="N63" s="17"/>
+      <c r="O63" s="17"/>
+      <c r="P63" s="17"/>
+      <c r="Q63" s="17"/>
+      <c r="R63" s="17"/>
+      <c r="S63" s="17"/>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A64" s="22"/>
-      <c r="B64" s="22"/>
-      <c r="C64" s="22"/>
-      <c r="D64" s="22"/>
-      <c r="E64" s="22"/>
-      <c r="F64" s="22"/>
-      <c r="G64" s="22"/>
-      <c r="H64" s="22"/>
-      <c r="I64" s="22"/>
-      <c r="J64" s="22"/>
-      <c r="K64" s="22"/>
-      <c r="L64" s="22"/>
-      <c r="M64" s="22"/>
-      <c r="N64" s="22"/>
-      <c r="O64" s="22"/>
-      <c r="P64" s="22"/>
-      <c r="Q64" s="22"/>
-      <c r="R64" s="22"/>
-      <c r="S64" s="22"/>
+      <c r="A64" s="17"/>
+      <c r="B64" s="17"/>
+      <c r="C64" s="17"/>
+      <c r="D64" s="17"/>
+      <c r="E64" s="17"/>
+      <c r="F64" s="17"/>
+      <c r="G64" s="17"/>
+      <c r="H64" s="17"/>
+      <c r="I64" s="17"/>
+      <c r="J64" s="17"/>
+      <c r="K64" s="17"/>
+      <c r="L64" s="17"/>
+      <c r="M64" s="17"/>
+      <c r="N64" s="17"/>
+      <c r="O64" s="17"/>
+      <c r="P64" s="17"/>
+      <c r="Q64" s="17"/>
+      <c r="R64" s="17"/>
+      <c r="S64" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4451,9 +4454,9 @@
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFA9496"/>
+        <color theme="0"/>
+        <color rgb="FF66FF33"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Blog Statistics (May 2021)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24204"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c93c05515dfe04a/GIT Hub/kunal-chowdhury.com/blog-stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="179" documentId="114_{B49989D9-13EE-4EB4-8B18-ED25DB6F8102}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{66AF4201-C5EF-4A7D-8D6B-6F122ED4AC77}"/>
+  <xr:revisionPtr revIDLastSave="253" documentId="114_{B49989D9-13EE-4EB4-8B18-ED25DB6F8102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75943531-B19F-4C28-BD2D-3CDEC0015002}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Jan</t>
   </si>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t>Column152</t>
-  </si>
-  <si>
-    <t>Last updated: 1st January 2021</t>
   </si>
 </sst>
 </file>
@@ -306,7 +303,6 @@
     <xf numFmtId="3" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -322,6 +318,7 @@
     <xf numFmtId="3" fontId="10" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="10" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -812,7 +809,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C6D6-4E14-869C-870F1EA86C0B}"/>
+              <c16:uniqueId val="{00000000-29C2-49FF-B5B6-D24038307561}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -912,7 +909,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000002-F234-47AE-98F4-23124B27C96C}"/>
+                  <c16:uniqueId val="{00000001-29C2-49FF-B5B6-D24038307561}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -933,7 +930,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-F234-47AE-98F4-23124B27C96C}"/>
+                  <c16:uniqueId val="{00000002-29C2-49FF-B5B6-D24038307561}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -954,7 +951,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000004-F234-47AE-98F4-23124B27C96C}"/>
+                  <c16:uniqueId val="{00000003-29C2-49FF-B5B6-D24038307561}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -975,7 +972,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000005-F234-47AE-98F4-23124B27C96C}"/>
+                  <c16:uniqueId val="{00000004-29C2-49FF-B5B6-D24038307561}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -996,7 +993,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000006-F234-47AE-98F4-23124B27C96C}"/>
+                  <c16:uniqueId val="{00000005-29C2-49FF-B5B6-D24038307561}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1017,7 +1014,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000007-F234-47AE-98F4-23124B27C96C}"/>
+                  <c16:uniqueId val="{00000006-29C2-49FF-B5B6-D24038307561}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1038,7 +1035,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000008-F234-47AE-98F4-23124B27C96C}"/>
+                  <c16:uniqueId val="{00000007-29C2-49FF-B5B6-D24038307561}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1059,7 +1056,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000009-F234-47AE-98F4-23124B27C96C}"/>
+                  <c16:uniqueId val="{00000008-29C2-49FF-B5B6-D24038307561}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1080,7 +1077,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000A-F234-47AE-98F4-23124B27C96C}"/>
+                  <c16:uniqueId val="{00000009-29C2-49FF-B5B6-D24038307561}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1169,7 +1166,7 @@
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000B-F234-47AE-98F4-23124B27C96C}"/>
+                  <c16:uniqueId val="{0000000A-29C2-49FF-B5B6-D24038307561}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1207,7 +1204,7 @@
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000002-094D-4ED5-9227-CC4EE8D01624}"/>
+                  <c16:uniqueId val="{0000000B-29C2-49FF-B5B6-D24038307561}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1228,7 +1225,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000000-4E3A-49ED-AF1F-326603D91C04}"/>
+                  <c16:uniqueId val="{0000000C-29C2-49FF-B5B6-D24038307561}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1306,7 +1303,7 @@
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000001-F5FD-4EEB-9B05-96C7834AADBD}"/>
+                  <c16:uniqueId val="{0000000D-29C2-49FF-B5B6-D24038307561}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1353,7 +1350,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000012-98B3-4A13-AF08-2983E2EA9C03}"/>
+                  <c16:uniqueId val="{0000000E-29C2-49FF-B5B6-D24038307561}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1506,7 +1503,7 @@
                   <c:v>26204397</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4206692</c:v>
+                  <c:v>8984698</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1514,7 +1511,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F234-47AE-98F4-23124B27C96C}"/>
+              <c16:uniqueId val="{0000000F-29C2-49FF-B5B6-D24038307561}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1657,7 +1654,7 @@
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="25400">
           <a:noFill/>
         </a:ln>
         <a:effectLst/>
@@ -1668,9 +1665,7 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
+    <a:noFill/>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:noFill/>
       <a:round/>
@@ -2208,27 +2203,29 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>21428</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>422275</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>23811</xdr:rowOff>
+      <xdr:rowOff>146050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>355599</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>502446</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>109539</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79CC319E-0D5D-439B-82BD-CF05CB30E9F0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2597,22 +2594,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="X34" sqref="X34"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" style="2" customWidth="1"/>
-    <col min="3" max="4" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="14" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="2" customWidth="1"/>
+    <col min="3" max="4" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" style="2" customWidth="1"/>
+    <col min="6" max="10" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="22" style="2" customWidth="1"/>
-    <col min="16" max="16" width="5.44140625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="25.44140625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="5.42578125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="25.42578125" style="2" customWidth="1"/>
     <col min="18" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2633,7 +2635,7 @@
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2654,7 +2656,7 @@
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>13</v>
@@ -2705,46 +2707,46 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="9" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" s="9" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="6"/>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="19" t="s">
+      <c r="K4" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="19" t="s">
+      <c r="L4" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="19" t="s">
+      <c r="M4" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="19" t="s">
+      <c r="N4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="19" t="s">
+      <c r="O4" s="18" t="s">
         <v>12</v>
       </c>
       <c r="P4" s="7"/>
@@ -2752,9 +2754,9 @@
       <c r="R4" s="5"/>
       <c r="S4" s="5"/>
     </row>
-    <row r="5" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:19" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A5" s="1"/>
-      <c r="B5" s="20">
+      <c r="B5" s="19">
         <v>2008</v>
       </c>
       <c r="C5" s="15">
@@ -2793,21 +2795,21 @@
       <c r="N5" s="10">
         <v>109</v>
       </c>
-      <c r="O5" s="22">
+      <c r="O5" s="21">
         <f>SUM(C5:N5)</f>
         <v>326</v>
       </c>
       <c r="P5" s="3"/>
-      <c r="Q5" s="16">
-        <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
+      <c r="Q5" s="25">
+        <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>326</v>
       </c>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
     </row>
-    <row r="6" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:19" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A6" s="1"/>
-      <c r="B6" s="20">
+      <c r="B6" s="19">
         <v>2009</v>
       </c>
       <c r="C6" s="10">
@@ -2846,21 +2848,21 @@
       <c r="N6" s="10">
         <v>18516</v>
       </c>
-      <c r="O6" s="22">
+      <c r="O6" s="21">
         <f t="shared" ref="O6:O12" si="0">SUM(C6:N6)</f>
         <v>80379</v>
       </c>
       <c r="P6" s="3"/>
-      <c r="Q6" s="16">
-        <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
+      <c r="Q6" s="25">
+        <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>80379</v>
       </c>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
     </row>
-    <row r="7" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:19" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A7" s="1"/>
-      <c r="B7" s="20">
+      <c r="B7" s="19">
         <v>2010</v>
       </c>
       <c r="C7" s="10">
@@ -2899,21 +2901,21 @@
       <c r="N7" s="10">
         <v>42658</v>
       </c>
-      <c r="O7" s="22">
+      <c r="O7" s="21">
         <f t="shared" si="0"/>
         <v>463113</v>
       </c>
       <c r="P7" s="3"/>
-      <c r="Q7" s="16">
-        <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
+      <c r="Q7" s="25">
+        <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>463113</v>
       </c>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
     </row>
-    <row r="8" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:19" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A8" s="1"/>
-      <c r="B8" s="20">
+      <c r="B8" s="19">
         <v>2011</v>
       </c>
       <c r="C8" s="10">
@@ -2952,21 +2954,21 @@
       <c r="N8" s="10">
         <v>64581</v>
       </c>
-      <c r="O8" s="22">
+      <c r="O8" s="21">
         <f t="shared" si="0"/>
         <v>803010</v>
       </c>
       <c r="P8" s="3"/>
-      <c r="Q8" s="16">
-        <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
+      <c r="Q8" s="25">
+        <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>803010</v>
       </c>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
     </row>
-    <row r="9" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:19" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A9" s="1"/>
-      <c r="B9" s="20">
+      <c r="B9" s="19">
         <v>2012</v>
       </c>
       <c r="C9" s="10">
@@ -3005,21 +3007,21 @@
       <c r="N9" s="10">
         <v>73172</v>
       </c>
-      <c r="O9" s="22">
+      <c r="O9" s="21">
         <f t="shared" si="0"/>
         <v>888853</v>
       </c>
       <c r="P9" s="3"/>
-      <c r="Q9" s="16">
-        <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
+      <c r="Q9" s="25">
+        <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>888853</v>
       </c>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
     </row>
-    <row r="10" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:19" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A10" s="1"/>
-      <c r="B10" s="20">
+      <c r="B10" s="19">
         <v>2013</v>
       </c>
       <c r="C10" s="10">
@@ -3058,21 +3060,21 @@
       <c r="N10" s="10">
         <v>73625</v>
       </c>
-      <c r="O10" s="22">
+      <c r="O10" s="21">
         <f t="shared" si="0"/>
         <v>935657</v>
       </c>
       <c r="P10" s="3"/>
-      <c r="Q10" s="16">
-        <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
+      <c r="Q10" s="25">
+        <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>935657</v>
       </c>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
     </row>
-    <row r="11" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:19" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A11" s="1"/>
-      <c r="B11" s="20">
+      <c r="B11" s="19">
         <v>2014</v>
       </c>
       <c r="C11" s="10">
@@ -3111,21 +3113,21 @@
       <c r="N11" s="11">
         <v>101904</v>
       </c>
-      <c r="O11" s="22">
+      <c r="O11" s="21">
         <f t="shared" si="0"/>
         <v>938639</v>
       </c>
       <c r="P11" s="3"/>
-      <c r="Q11" s="16">
-        <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
+      <c r="Q11" s="25">
+        <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>938639</v>
       </c>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
     </row>
-    <row r="12" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:19" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A12" s="1"/>
-      <c r="B12" s="20">
+      <c r="B12" s="19">
         <v>2015</v>
       </c>
       <c r="C12" s="10">
@@ -3164,21 +3166,21 @@
       <c r="N12" s="11">
         <v>129945</v>
       </c>
-      <c r="O12" s="22">
+      <c r="O12" s="21">
         <f t="shared" si="0"/>
         <v>1217957</v>
       </c>
       <c r="P12" s="3"/>
-      <c r="Q12" s="16">
-        <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
+      <c r="Q12" s="25">
+        <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>1217957</v>
       </c>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
     </row>
-    <row r="13" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:19" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A13" s="1"/>
-      <c r="B13" s="20">
+      <c r="B13" s="19">
         <v>2016</v>
       </c>
       <c r="C13" s="11">
@@ -3217,21 +3219,21 @@
       <c r="N13" s="12">
         <v>674509</v>
       </c>
-      <c r="O13" s="22">
+      <c r="O13" s="21">
         <f t="shared" ref="O13:O18" si="1">SUM(C13:N13)</f>
         <v>4530257</v>
       </c>
       <c r="P13" s="3"/>
-      <c r="Q13" s="16">
-        <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
+      <c r="Q13" s="25">
+        <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>4530257</v>
       </c>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
     </row>
-    <row r="14" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:19" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A14" s="1"/>
-      <c r="B14" s="20">
+      <c r="B14" s="19">
         <v>2017</v>
       </c>
       <c r="C14" s="12">
@@ -3270,21 +3272,21 @@
       <c r="N14" s="12">
         <v>565361</v>
       </c>
-      <c r="O14" s="22">
+      <c r="O14" s="21">
         <f t="shared" si="1"/>
         <v>7693253</v>
       </c>
       <c r="P14" s="3"/>
-      <c r="Q14" s="16">
-        <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
+      <c r="Q14" s="25">
+        <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>7693253</v>
       </c>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
     </row>
-    <row r="15" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:19" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A15" s="1"/>
-      <c r="B15" s="20">
+      <c r="B15" s="19">
         <v>2018</v>
       </c>
       <c r="C15" s="12">
@@ -3323,21 +3325,21 @@
       <c r="N15" s="12">
         <v>732173</v>
       </c>
-      <c r="O15" s="22">
+      <c r="O15" s="21">
         <f t="shared" si="1"/>
         <v>8287717</v>
       </c>
       <c r="P15" s="4"/>
-      <c r="Q15" s="16">
-        <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
+      <c r="Q15" s="25">
+        <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>8287717</v>
       </c>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
     </row>
-    <row r="16" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:19" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A16" s="1"/>
-      <c r="B16" s="20">
+      <c r="B16" s="19">
         <v>2019</v>
       </c>
       <c r="C16" s="12">
@@ -3376,21 +3378,21 @@
       <c r="N16" s="13">
         <v>2325909</v>
       </c>
-      <c r="O16" s="23">
+      <c r="O16" s="22">
         <f t="shared" si="1"/>
         <v>16768940</v>
       </c>
       <c r="P16" s="4"/>
-      <c r="Q16" s="16">
-        <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
+      <c r="Q16" s="25">
+        <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>16768940</v>
       </c>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
     </row>
-    <row r="17" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:19" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A17" s="1"/>
-      <c r="B17" s="20">
+      <c r="B17" s="19">
         <v>2020</v>
       </c>
       <c r="C17" s="13">
@@ -3429,21 +3431,21 @@
       <c r="N17" s="13">
         <v>2176841</v>
       </c>
-      <c r="O17" s="24">
+      <c r="O17" s="23">
         <f t="shared" si="1"/>
         <v>26204397</v>
       </c>
       <c r="P17" s="4"/>
-      <c r="Q17" s="16">
-        <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
+      <c r="Q17" s="25">
+        <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>26204397</v>
       </c>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
     </row>
-    <row r="18" spans="1:19" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:19" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A18" s="1"/>
-      <c r="B18" s="20">
+      <c r="B18" s="19">
         <v>2021</v>
       </c>
       <c r="C18" s="14">
@@ -3455,8 +3457,12 @@
       <c r="E18" s="14">
         <v>2047206</v>
       </c>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
+      <c r="F18" s="14">
+        <v>2337103</v>
+      </c>
+      <c r="G18" s="14">
+        <v>2440903</v>
+      </c>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
@@ -3464,19 +3470,19 @@
       <c r="L18" s="14"/>
       <c r="M18" s="14"/>
       <c r="N18" s="14"/>
-      <c r="O18" s="24">
+      <c r="O18" s="23">
         <f t="shared" si="1"/>
-        <v>4206692</v>
+        <v>8984698</v>
       </c>
       <c r="P18" s="4"/>
-      <c r="Q18" s="16">
-        <f>SUM((Table1[[#This Row],[Column15]]*12)/COUNT(Table1[[#This Row],[Column2]:[Column13]]))</f>
-        <v>16826768</v>
+      <c r="Q18" s="25">
+        <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
+        <v>21563275.200000003</v>
       </c>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
     </row>
-    <row r="19" spans="1:19" s="9" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" s="9" customFormat="1" ht="44.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="26"/>
       <c r="C19" s="27"/>
@@ -3491,52 +3497,52 @@
       <c r="L19" s="27"/>
       <c r="M19" s="27"/>
       <c r="N19" s="27"/>
-      <c r="O19" s="21">
+      <c r="O19" s="20">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>73019190</v>
+        <v>77797196</v>
       </c>
       <c r="P19" s="7"/>
       <c r="Q19" s="5"/>
       <c r="R19" s="5"/>
       <c r="S19" s="5"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="25"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="25"/>
-      <c r="O20" s="25"/>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="24"/>
+      <c r="O20" s="24"/>
       <c r="P20" s="3"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
     </row>
-    <row r="21" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="17"/>
-      <c r="N21" s="17"/>
-      <c r="O21" s="17"/>
-    </row>
-    <row r="22" spans="1:19" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+    </row>
+    <row r="22" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="29"/>
       <c r="C22" s="29"/>
@@ -3557,7 +3563,7 @@
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -3578,7 +3584,7 @@
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -3599,7 +3605,7 @@
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -3620,7 +3626,7 @@
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -3641,7 +3647,7 @@
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -3662,7 +3668,7 @@
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -3683,7 +3689,7 @@
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -3704,7 +3710,7 @@
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -3725,7 +3731,7 @@
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -3746,7 +3752,7 @@
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -3767,7 +3773,7 @@
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -3788,7 +3794,7 @@
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -3809,7 +3815,7 @@
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -3830,7 +3836,7 @@
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -3851,7 +3857,7 @@
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -3872,7 +3878,7 @@
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -3893,7 +3899,7 @@
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -3914,7 +3920,7 @@
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -3935,7 +3941,7 @@
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -3956,7 +3962,7 @@
       <c r="R41" s="1"/>
       <c r="S41" s="1"/>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -3977,7 +3983,7 @@
       <c r="R42" s="1"/>
       <c r="S42" s="1"/>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -3998,7 +4004,7 @@
       <c r="R43" s="1"/>
       <c r="S43" s="1"/>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -4019,7 +4025,7 @@
       <c r="R44" s="1"/>
       <c r="S44" s="1"/>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -4040,7 +4046,7 @@
       <c r="R45" s="1"/>
       <c r="S45" s="1"/>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -4061,7 +4067,7 @@
       <c r="R46" s="1"/>
       <c r="S46" s="1"/>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -4082,7 +4088,7 @@
       <c r="R47" s="1"/>
       <c r="S47" s="1"/>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -4103,7 +4109,7 @@
       <c r="R48" s="1"/>
       <c r="S48" s="1"/>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -4124,7 +4130,7 @@
       <c r="R49" s="1"/>
       <c r="S49" s="1"/>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -4134,9 +4140,7 @@
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
-      <c r="J50" s="30" t="s">
-        <v>29</v>
-      </c>
+      <c r="J50" s="30"/>
       <c r="K50" s="30"/>
       <c r="L50" s="30"/>
       <c r="M50" s="1"/>
@@ -4147,299 +4151,299 @@
       <c r="R50" s="1"/>
       <c r="S50" s="1"/>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A51" s="17"/>
-      <c r="B51" s="17"/>
-      <c r="C51" s="17"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17"/>
-      <c r="F51" s="17"/>
-      <c r="G51" s="17"/>
-      <c r="H51" s="17"/>
-      <c r="I51" s="17"/>
-      <c r="J51" s="17"/>
-      <c r="K51" s="17"/>
-      <c r="L51" s="18"/>
-      <c r="M51" s="17"/>
-      <c r="N51" s="17"/>
-      <c r="O51" s="17"/>
-      <c r="P51" s="17"/>
-      <c r="Q51" s="17"/>
-      <c r="R51" s="17"/>
-      <c r="S51" s="17"/>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A52" s="17"/>
-      <c r="B52" s="17"/>
-      <c r="C52" s="17"/>
-      <c r="D52" s="17"/>
-      <c r="E52" s="17"/>
-      <c r="F52" s="17"/>
-      <c r="G52" s="17"/>
-      <c r="H52" s="17"/>
-      <c r="I52" s="17"/>
-      <c r="J52" s="17"/>
-      <c r="K52" s="17"/>
-      <c r="L52" s="17"/>
-      <c r="M52" s="17"/>
-      <c r="N52" s="17"/>
-      <c r="O52" s="17"/>
-      <c r="P52" s="17"/>
-      <c r="Q52" s="17"/>
-      <c r="R52" s="17"/>
-      <c r="S52" s="17"/>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A53" s="17"/>
-      <c r="B53" s="17"/>
-      <c r="C53" s="17"/>
-      <c r="D53" s="17"/>
-      <c r="E53" s="17"/>
-      <c r="F53" s="17"/>
-      <c r="G53" s="17"/>
-      <c r="H53" s="17"/>
-      <c r="I53" s="17"/>
-      <c r="J53" s="17"/>
-      <c r="K53" s="17"/>
-      <c r="L53" s="17"/>
-      <c r="M53" s="17"/>
-      <c r="N53" s="17"/>
-      <c r="O53" s="17"/>
-      <c r="P53" s="17"/>
-      <c r="Q53" s="17"/>
-      <c r="R53" s="17"/>
-      <c r="S53" s="17"/>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A54" s="17"/>
-      <c r="B54" s="17"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="17"/>
-      <c r="E54" s="17"/>
-      <c r="F54" s="17"/>
-      <c r="G54" s="17"/>
-      <c r="H54" s="17"/>
-      <c r="I54" s="17"/>
-      <c r="J54" s="17"/>
-      <c r="K54" s="17"/>
-      <c r="L54" s="17"/>
-      <c r="M54" s="17"/>
-      <c r="N54" s="17"/>
-      <c r="O54" s="17"/>
-      <c r="P54" s="17"/>
-      <c r="Q54" s="17"/>
-      <c r="R54" s="17"/>
-      <c r="S54" s="17"/>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A55" s="17"/>
-      <c r="B55" s="17"/>
-      <c r="C55" s="17"/>
-      <c r="D55" s="17"/>
-      <c r="E55" s="17"/>
-      <c r="F55" s="17"/>
-      <c r="G55" s="17"/>
-      <c r="H55" s="17"/>
-      <c r="I55" s="17"/>
-      <c r="J55" s="17"/>
-      <c r="K55" s="17"/>
-      <c r="L55" s="17"/>
-      <c r="M55" s="17"/>
-      <c r="N55" s="17"/>
-      <c r="O55" s="17"/>
-      <c r="P55" s="17"/>
-      <c r="Q55" s="17"/>
-      <c r="R55" s="17"/>
-      <c r="S55" s="17"/>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A56" s="17"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="17"/>
-      <c r="E56" s="17"/>
-      <c r="F56" s="17"/>
-      <c r="G56" s="17"/>
-      <c r="H56" s="17"/>
-      <c r="I56" s="17"/>
-      <c r="J56" s="17"/>
-      <c r="K56" s="17"/>
-      <c r="L56" s="17"/>
-      <c r="M56" s="17"/>
-      <c r="N56" s="17"/>
-      <c r="O56" s="17"/>
-      <c r="P56" s="17"/>
-      <c r="Q56" s="17"/>
-      <c r="R56" s="17"/>
-      <c r="S56" s="17"/>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A57" s="17"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="17"/>
-      <c r="D57" s="17"/>
-      <c r="E57" s="17"/>
-      <c r="F57" s="17"/>
-      <c r="G57" s="17"/>
-      <c r="H57" s="17"/>
-      <c r="I57" s="17"/>
-      <c r="J57" s="17"/>
-      <c r="K57" s="17"/>
-      <c r="L57" s="17"/>
-      <c r="M57" s="17"/>
-      <c r="N57" s="17"/>
-      <c r="O57" s="17"/>
-      <c r="P57" s="17"/>
-      <c r="Q57" s="17"/>
-      <c r="R57" s="17"/>
-      <c r="S57" s="17"/>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A58" s="17"/>
-      <c r="B58" s="17"/>
-      <c r="C58" s="17"/>
-      <c r="D58" s="17"/>
-      <c r="E58" s="17"/>
-      <c r="F58" s="17"/>
-      <c r="G58" s="17"/>
-      <c r="H58" s="17"/>
-      <c r="I58" s="17"/>
-      <c r="J58" s="17"/>
-      <c r="K58" s="17"/>
-      <c r="L58" s="17"/>
-      <c r="M58" s="17"/>
-      <c r="N58" s="17"/>
-      <c r="O58" s="17"/>
-      <c r="P58" s="17"/>
-      <c r="Q58" s="17"/>
-      <c r="R58" s="17"/>
-      <c r="S58" s="17"/>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A59" s="17"/>
-      <c r="B59" s="17"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="17"/>
-      <c r="E59" s="17"/>
-      <c r="F59" s="17"/>
-      <c r="G59" s="17"/>
-      <c r="H59" s="17"/>
-      <c r="I59" s="17"/>
-      <c r="J59" s="17"/>
-      <c r="K59" s="17"/>
-      <c r="L59" s="17"/>
-      <c r="M59" s="17"/>
-      <c r="N59" s="17"/>
-      <c r="O59" s="17"/>
-      <c r="P59" s="17"/>
-      <c r="Q59" s="17"/>
-      <c r="R59" s="17"/>
-      <c r="S59" s="17"/>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A60" s="17"/>
-      <c r="B60" s="17"/>
-      <c r="C60" s="17"/>
-      <c r="D60" s="17"/>
-      <c r="E60" s="17"/>
-      <c r="F60" s="17"/>
-      <c r="G60" s="17"/>
-      <c r="H60" s="17"/>
-      <c r="I60" s="17"/>
-      <c r="J60" s="17"/>
-      <c r="K60" s="17"/>
-      <c r="L60" s="17"/>
-      <c r="M60" s="17"/>
-      <c r="N60" s="17"/>
-      <c r="O60" s="17"/>
-      <c r="P60" s="17"/>
-      <c r="Q60" s="17"/>
-      <c r="R60" s="17"/>
-      <c r="S60" s="17"/>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A61" s="17"/>
-      <c r="B61" s="17"/>
-      <c r="C61" s="17"/>
-      <c r="D61" s="17"/>
-      <c r="E61" s="17"/>
-      <c r="F61" s="17"/>
-      <c r="G61" s="17"/>
-      <c r="H61" s="17"/>
-      <c r="I61" s="17"/>
-      <c r="J61" s="17"/>
-      <c r="K61" s="17"/>
-      <c r="L61" s="17"/>
-      <c r="M61" s="17"/>
-      <c r="N61" s="17"/>
-      <c r="O61" s="17"/>
-      <c r="P61" s="17"/>
-      <c r="Q61" s="17"/>
-      <c r="R61" s="17"/>
-      <c r="S61" s="17"/>
-    </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A62" s="17"/>
-      <c r="B62" s="17"/>
-      <c r="C62" s="17"/>
-      <c r="D62" s="17"/>
-      <c r="E62" s="17"/>
-      <c r="F62" s="17"/>
-      <c r="G62" s="17"/>
-      <c r="H62" s="17"/>
-      <c r="I62" s="17"/>
-      <c r="J62" s="17"/>
-      <c r="K62" s="17"/>
-      <c r="L62" s="17"/>
-      <c r="M62" s="17"/>
-      <c r="N62" s="17"/>
-      <c r="O62" s="17"/>
-      <c r="P62" s="17"/>
-      <c r="Q62" s="17"/>
-      <c r="R62" s="17"/>
-      <c r="S62" s="17"/>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A63" s="17"/>
-      <c r="B63" s="17"/>
-      <c r="C63" s="17"/>
-      <c r="D63" s="17"/>
-      <c r="E63" s="17"/>
-      <c r="F63" s="17"/>
-      <c r="G63" s="17"/>
-      <c r="H63" s="17"/>
-      <c r="I63" s="17"/>
-      <c r="J63" s="17"/>
-      <c r="K63" s="17"/>
-      <c r="L63" s="17"/>
-      <c r="M63" s="17"/>
-      <c r="N63" s="17"/>
-      <c r="O63" s="17"/>
-      <c r="P63" s="17"/>
-      <c r="Q63" s="17"/>
-      <c r="R63" s="17"/>
-      <c r="S63" s="17"/>
-    </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A64" s="17"/>
-      <c r="B64" s="17"/>
-      <c r="C64" s="17"/>
-      <c r="D64" s="17"/>
-      <c r="E64" s="17"/>
-      <c r="F64" s="17"/>
-      <c r="G64" s="17"/>
-      <c r="H64" s="17"/>
-      <c r="I64" s="17"/>
-      <c r="J64" s="17"/>
-      <c r="K64" s="17"/>
-      <c r="L64" s="17"/>
-      <c r="M64" s="17"/>
-      <c r="N64" s="17"/>
-      <c r="O64" s="17"/>
-      <c r="P64" s="17"/>
-      <c r="Q64" s="17"/>
-      <c r="R64" s="17"/>
-      <c r="S64" s="17"/>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A51" s="16"/>
+      <c r="B51" s="16"/>
+      <c r="C51" s="16"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="16"/>
+      <c r="H51" s="16"/>
+      <c r="I51" s="16"/>
+      <c r="J51" s="16"/>
+      <c r="K51" s="16"/>
+      <c r="L51" s="17"/>
+      <c r="M51" s="16"/>
+      <c r="N51" s="16"/>
+      <c r="O51" s="16"/>
+      <c r="P51" s="16"/>
+      <c r="Q51" s="16"/>
+      <c r="R51" s="16"/>
+      <c r="S51" s="16"/>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A52" s="16"/>
+      <c r="B52" s="16"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="16"/>
+      <c r="I52" s="16"/>
+      <c r="J52" s="16"/>
+      <c r="K52" s="16"/>
+      <c r="L52" s="16"/>
+      <c r="M52" s="16"/>
+      <c r="N52" s="16"/>
+      <c r="O52" s="16"/>
+      <c r="P52" s="16"/>
+      <c r="Q52" s="16"/>
+      <c r="R52" s="16"/>
+      <c r="S52" s="16"/>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A53" s="16"/>
+      <c r="B53" s="16"/>
+      <c r="C53" s="16"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="16"/>
+      <c r="F53" s="16"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="16"/>
+      <c r="I53" s="16"/>
+      <c r="J53" s="16"/>
+      <c r="K53" s="16"/>
+      <c r="L53" s="16"/>
+      <c r="M53" s="16"/>
+      <c r="N53" s="16"/>
+      <c r="O53" s="16"/>
+      <c r="P53" s="16"/>
+      <c r="Q53" s="16"/>
+      <c r="R53" s="16"/>
+      <c r="S53" s="16"/>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A54" s="16"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="16"/>
+      <c r="E54" s="16"/>
+      <c r="F54" s="16"/>
+      <c r="G54" s="16"/>
+      <c r="H54" s="16"/>
+      <c r="I54" s="16"/>
+      <c r="J54" s="16"/>
+      <c r="K54" s="16"/>
+      <c r="L54" s="16"/>
+      <c r="M54" s="16"/>
+      <c r="N54" s="16"/>
+      <c r="O54" s="16"/>
+      <c r="P54" s="16"/>
+      <c r="Q54" s="16"/>
+      <c r="R54" s="16"/>
+      <c r="S54" s="16"/>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A55" s="16"/>
+      <c r="B55" s="16"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="16"/>
+      <c r="I55" s="16"/>
+      <c r="J55" s="16"/>
+      <c r="K55" s="16"/>
+      <c r="L55" s="16"/>
+      <c r="M55" s="16"/>
+      <c r="N55" s="16"/>
+      <c r="O55" s="16"/>
+      <c r="P55" s="16"/>
+      <c r="Q55" s="16"/>
+      <c r="R55" s="16"/>
+      <c r="S55" s="16"/>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A56" s="16"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="16"/>
+      <c r="I56" s="16"/>
+      <c r="J56" s="16"/>
+      <c r="K56" s="16"/>
+      <c r="L56" s="16"/>
+      <c r="M56" s="16"/>
+      <c r="N56" s="16"/>
+      <c r="O56" s="16"/>
+      <c r="P56" s="16"/>
+      <c r="Q56" s="16"/>
+      <c r="R56" s="16"/>
+      <c r="S56" s="16"/>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A57" s="16"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="16"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="16"/>
+      <c r="F57" s="16"/>
+      <c r="G57" s="16"/>
+      <c r="H57" s="16"/>
+      <c r="I57" s="16"/>
+      <c r="J57" s="16"/>
+      <c r="K57" s="16"/>
+      <c r="L57" s="16"/>
+      <c r="M57" s="16"/>
+      <c r="N57" s="16"/>
+      <c r="O57" s="16"/>
+      <c r="P57" s="16"/>
+      <c r="Q57" s="16"/>
+      <c r="R57" s="16"/>
+      <c r="S57" s="16"/>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A58" s="16"/>
+      <c r="B58" s="16"/>
+      <c r="C58" s="16"/>
+      <c r="D58" s="16"/>
+      <c r="E58" s="16"/>
+      <c r="F58" s="16"/>
+      <c r="G58" s="16"/>
+      <c r="H58" s="16"/>
+      <c r="I58" s="16"/>
+      <c r="J58" s="16"/>
+      <c r="K58" s="16"/>
+      <c r="L58" s="16"/>
+      <c r="M58" s="16"/>
+      <c r="N58" s="16"/>
+      <c r="O58" s="16"/>
+      <c r="P58" s="16"/>
+      <c r="Q58" s="16"/>
+      <c r="R58" s="16"/>
+      <c r="S58" s="16"/>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A59" s="16"/>
+      <c r="B59" s="16"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="16"/>
+      <c r="E59" s="16"/>
+      <c r="F59" s="16"/>
+      <c r="G59" s="16"/>
+      <c r="H59" s="16"/>
+      <c r="I59" s="16"/>
+      <c r="J59" s="16"/>
+      <c r="K59" s="16"/>
+      <c r="L59" s="16"/>
+      <c r="M59" s="16"/>
+      <c r="N59" s="16"/>
+      <c r="O59" s="16"/>
+      <c r="P59" s="16"/>
+      <c r="Q59" s="16"/>
+      <c r="R59" s="16"/>
+      <c r="S59" s="16"/>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A60" s="16"/>
+      <c r="B60" s="16"/>
+      <c r="C60" s="16"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="16"/>
+      <c r="F60" s="16"/>
+      <c r="G60" s="16"/>
+      <c r="H60" s="16"/>
+      <c r="I60" s="16"/>
+      <c r="J60" s="16"/>
+      <c r="K60" s="16"/>
+      <c r="L60" s="16"/>
+      <c r="M60" s="16"/>
+      <c r="N60" s="16"/>
+      <c r="O60" s="16"/>
+      <c r="P60" s="16"/>
+      <c r="Q60" s="16"/>
+      <c r="R60" s="16"/>
+      <c r="S60" s="16"/>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A61" s="16"/>
+      <c r="B61" s="16"/>
+      <c r="C61" s="16"/>
+      <c r="D61" s="16"/>
+      <c r="E61" s="16"/>
+      <c r="F61" s="16"/>
+      <c r="G61" s="16"/>
+      <c r="H61" s="16"/>
+      <c r="I61" s="16"/>
+      <c r="J61" s="16"/>
+      <c r="K61" s="16"/>
+      <c r="L61" s="16"/>
+      <c r="M61" s="16"/>
+      <c r="N61" s="16"/>
+      <c r="O61" s="16"/>
+      <c r="P61" s="16"/>
+      <c r="Q61" s="16"/>
+      <c r="R61" s="16"/>
+      <c r="S61" s="16"/>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A62" s="16"/>
+      <c r="B62" s="16"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="16"/>
+      <c r="G62" s="16"/>
+      <c r="H62" s="16"/>
+      <c r="I62" s="16"/>
+      <c r="J62" s="16"/>
+      <c r="K62" s="16"/>
+      <c r="L62" s="16"/>
+      <c r="M62" s="16"/>
+      <c r="N62" s="16"/>
+      <c r="O62" s="16"/>
+      <c r="P62" s="16"/>
+      <c r="Q62" s="16"/>
+      <c r="R62" s="16"/>
+      <c r="S62" s="16"/>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A63" s="16"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="16"/>
+      <c r="H63" s="16"/>
+      <c r="I63" s="16"/>
+      <c r="J63" s="16"/>
+      <c r="K63" s="16"/>
+      <c r="L63" s="16"/>
+      <c r="M63" s="16"/>
+      <c r="N63" s="16"/>
+      <c r="O63" s="16"/>
+      <c r="P63" s="16"/>
+      <c r="Q63" s="16"/>
+      <c r="R63" s="16"/>
+      <c r="S63" s="16"/>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A64" s="16"/>
+      <c r="B64" s="16"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="16"/>
+      <c r="H64" s="16"/>
+      <c r="I64" s="16"/>
+      <c r="J64" s="16"/>
+      <c r="K64" s="16"/>
+      <c r="L64" s="16"/>
+      <c r="M64" s="16"/>
+      <c r="N64" s="16"/>
+      <c r="O64" s="16"/>
+      <c r="P64" s="16"/>
+      <c r="Q64" s="16"/>
+      <c r="R64" s="16"/>
+      <c r="S64" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Blog Statistics (August 2021)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24204"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24503"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c93c05515dfe04a/GIT Hub/kunal-chowdhury.com/blog-stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="253" documentId="114_{B49989D9-13EE-4EB4-8B18-ED25DB6F8102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75943531-B19F-4C28-BD2D-3CDEC0015002}"/>
+  <xr:revisionPtr revIDLastSave="256" documentId="114_{B49989D9-13EE-4EB4-8B18-ED25DB6F8102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D71B0E6-1B36-4FD2-9B7C-FC33A77BC4C0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1503,7 +1503,7 @@
                   <c:v>26204397</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8984698</c:v>
+                  <c:v>16286690</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2595,7 +2595,7 @@
   <dimension ref="A1:S64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="X34" sqref="X34"/>
+      <selection activeCell="AA22" sqref="AA22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3463,21 +3463,27 @@
       <c r="G18" s="14">
         <v>2440903</v>
       </c>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
+      <c r="H18" s="14">
+        <v>2432014</v>
+      </c>
+      <c r="I18" s="14">
+        <v>2631617</v>
+      </c>
+      <c r="J18" s="14">
+        <v>2238361</v>
+      </c>
       <c r="K18" s="14"/>
       <c r="L18" s="14"/>
       <c r="M18" s="14"/>
       <c r="N18" s="14"/>
       <c r="O18" s="23">
         <f t="shared" si="1"/>
-        <v>8984698</v>
+        <v>16286690</v>
       </c>
       <c r="P18" s="4"/>
       <c r="Q18" s="25">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
-        <v>21563275.200000003</v>
+        <v>24430035</v>
       </c>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
@@ -3499,7 +3505,7 @@
       <c r="N19" s="27"/>
       <c r="O19" s="20">
         <f>SUBTOTAL(109,Table1[Column15])</f>
-        <v>77797196</v>
+        <v>85099188</v>
       </c>
       <c r="P19" s="7"/>
       <c r="Q19" s="5"/>

</xml_diff>

<commit_message>
Site Statistics (March 2022)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -446,7 +446,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="108">
+  <dxfs count="110">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -514,6 +514,650 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFFAA8AA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCCCCD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFDE7E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFDFFFD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF2F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF5F5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8EFF68"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD6FFC8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE8FFE0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEEFFE9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBB1B2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFDE8E8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEEAEA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF1F1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF4F4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF8F8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEFFFE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8BFF64"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8FFA0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2FFD8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE9FFE2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBBDBE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCCFD0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEECEC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEEFF0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA1FF81"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFAEFF92"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD8FFCB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE9FFE1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEAFFE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCBFC0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFDE4E5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFDFFFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEECED"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEEDED"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEEDEE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEFAFA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA7FF8A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFAAFF8D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0FFC0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE7FFDF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFA9799"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCC5C6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFDE7E7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEEFEF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF7F7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF7F8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEFFFD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFAAFF8E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB0FF96"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEDFFE7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFA999B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCC8C9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFDE6E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEEBEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF0F1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF5F6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEFBFB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA3FF84"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0FFC1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD5FFC7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEAFFE2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEFFFE9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF5FFF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFA9C9E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFDD7D8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEEBEC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEEEEE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB1FF97"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCEFFBD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD7FFC9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFA9D9F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCD1D1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF6F6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF94FF70"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC8FFB5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFBB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEDFFE6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEEFFE8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFAA0A2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF4F5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9BFF79"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFBDFFA7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC3FFAE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFAA2A4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCC4C5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFDE1E1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF3F4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF85FF5C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFADFF91"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFFAA9AA"/>
         </patternFill>
       </fill>
@@ -521,357 +1165,42 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFCCDCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFDE9E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFDFFFD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF4F4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF7F7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF002060"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8EFF68"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD6FFC8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE8FFE0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEEFFE9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFBB1B3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEE9EA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEEBEC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF2F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF6F6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEFAFA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEFFFE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF8BFF64"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8FFA0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2FFD8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE9FFE2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFBBDBF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCD0D1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFDFFFC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEEDEE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF1F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA1FF81"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFAEFF92"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD8FFCB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE9FFE1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEAFFE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCC0C1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFDE6E6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEEEEE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEEFEF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEFCFC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA7FF8A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFAAFF8D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD0FFC0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE7FFDF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFA9799"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCC6C7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFDE8E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF0F1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF9F9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEFFFD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFAAFF8E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB0FF96"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD8FFCA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEDFFE7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFA999B"/>
+          <fgColor rgb="FFFDE2E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF3F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6CFF3B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFAEFF93"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB4FF9A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFBABAC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -885,322 +1214,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFDE7E8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEECED"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEFCFD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA3FF84"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD0FFC1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD5FFC7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEFFFE9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF5FFF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFA9D9E"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFDD8D9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEEDED"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEEFF0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB1FF97"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCEFFBD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD7FFC9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFA9D9F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCD2D3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF94FF70"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC8FFB5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCFFBB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFECFFE6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEEFFE8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFAA0A2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF9BFF79"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFBDFFA7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC3FFAE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEBFFE5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFAA2A4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCC5C6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFDE2E3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF5F5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF85FF5C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFADFF91"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFBA9AB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFFDE4E4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF3F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF4F5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF6CFF3B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFAEFF93"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB4FF9A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFBABAD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCCACB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFDE5E6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF0F0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1268,7 +1282,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1342,6 +1356,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1457,7 +1472,7 @@
                   <c:v>29808642</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6739216</c:v>
+                  <c:v>9075444</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1465,17 +1480,17 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="37802343"/>
-        <c:axId val="50036307"/>
+        <c:axId val="64427795"/>
+        <c:axId val="34896245"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="37802343"/>
+        <c:axId val="64427795"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1497,7 +1512,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50036307"/>
+        <c:crossAx val="34896245"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1505,7 +1520,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50036307"/>
+        <c:axId val="34896245"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1520,7 +1535,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1542,7 +1557,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37802343"/>
+        <c:crossAx val="64427795"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1580,9 +1595,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>1699920</xdr:colOff>
+      <xdr:colOff>1699560</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1591,7 +1606,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="1085760" y="10882440"/>
-        <a:ext cx="20261520" cy="8470440"/>
+        <a:ext cx="20261160" cy="8470080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1636,7 +1651,7 @@
   <dimension ref="A1:S65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y56" activeCellId="0" sqref="Y56"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1647,7 +1662,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="1" width="17.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="25.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="25.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="5.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="25.42"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="18" style="1" width="9"/>
@@ -2546,7 +2561,9 @@
       <c r="D19" s="15" t="n">
         <v>2442144</v>
       </c>
-      <c r="E19" s="15"/>
+      <c r="E19" s="15" t="n">
+        <v>2336228</v>
+      </c>
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
@@ -2558,7 +2575,7 @@
       <c r="N19" s="15"/>
       <c r="O19" s="18" t="n">
         <f aca="false">SUM(C19:N19)</f>
-        <v>6739216</v>
+        <v>9075444</v>
       </c>
       <c r="P19" s="13"/>
       <c r="Q19" s="14" t="n">
@@ -2585,7 +2602,7 @@
       <c r="N20" s="19"/>
       <c r="O20" s="20" t="n">
         <f aca="false">SUM(O5:O19)</f>
-        <v>105360356</v>
+        <v>107696584</v>
       </c>
       <c r="P20" s="7"/>
       <c r="Q20" s="4"/>

</xml_diff>

<commit_message>
Blog Statistics (July 2022)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c93c05515dfe04a/GIT Hub/kunal-chowdhury.com/blog-stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="11_91C7ACB7C03E7306CE517BDFACF66E9FD99B01DC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20E028FA-A9DA-44E6-8070-998F5FDCC451}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="11_91C7ACB7C03E7306CE517BDFACF66E9FD99B01DC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0DED57AA-A81B-4E89-855A-1EB04EBA7924}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -314,18 +314,6 @@
   </cellStyleXfs>
   <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -375,6 +363,18 @@
     </xf>
     <xf numFmtId="3" fontId="8" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -722,7 +722,7 @@
                   <c:v>29808642</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>13891142</c:v>
+                  <c:v>19678066</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -901,8 +901,8 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>163286</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>149679</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -917,9 +917,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
+        <a:xfrm flipH="1" flipV="1">
           <a:off x="15865929" y="9824357"/>
-          <a:ext cx="0" cy="3864429"/>
+          <a:ext cx="27214" cy="2530929"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1273,1904 +1273,1908 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O46" sqref="O46"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" style="5" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="5" customWidth="1"/>
-    <col min="3" max="14" width="26.28515625" style="5" customWidth="1"/>
-    <col min="15" max="15" width="32.28515625" style="5" customWidth="1"/>
-    <col min="16" max="16" width="5.42578125" style="5" customWidth="1"/>
-    <col min="17" max="17" width="25.42578125" style="5" customWidth="1"/>
-    <col min="18" max="1024" width="9" style="5"/>
+    <col min="1" max="1" width="5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" style="1" customWidth="1"/>
+    <col min="3" max="14" width="26.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="32.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="5.42578125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="25.42578125" style="1" customWidth="1"/>
+    <col min="18" max="1024" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="O3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="P3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="Q3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="12" customFormat="1" ht="104.45" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="22" t="s">
+    <row r="4" spans="1:19" s="8" customFormat="1" ht="104.45" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="22" t="s">
+      <c r="J4" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="22" t="s">
+      <c r="K4" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="22" t="s">
+      <c r="L4" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="22" t="s">
+      <c r="M4" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="22" t="s">
+      <c r="N4" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="22" t="s">
+      <c r="O4" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
     </row>
     <row r="5" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="6"/>
-      <c r="B5" s="21">
+      <c r="A5" s="2"/>
+      <c r="B5" s="17">
         <v>2008</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="14">
         <v>0</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="14">
         <v>0</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="14">
         <v>0</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="14">
         <v>0</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="14">
         <v>0</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="14">
         <v>0</v>
       </c>
-      <c r="I5" s="18">
+      <c r="I5" s="14">
         <v>0</v>
       </c>
-      <c r="J5" s="18">
+      <c r="J5" s="14">
         <v>0</v>
       </c>
-      <c r="K5" s="18">
+      <c r="K5" s="14">
         <v>0</v>
       </c>
-      <c r="L5" s="18">
+      <c r="L5" s="14">
         <v>105</v>
       </c>
-      <c r="M5" s="18">
+      <c r="M5" s="14">
         <v>112</v>
       </c>
-      <c r="N5" s="18">
+      <c r="N5" s="14">
         <v>109</v>
       </c>
-      <c r="O5" s="23">
+      <c r="O5" s="19">
         <f t="shared" ref="O5:O19" si="0">SUM(C5:N5)</f>
         <v>326</v>
       </c>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="14">
+      <c r="P5" s="9"/>
+      <c r="Q5" s="10">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>326</v>
       </c>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
     </row>
     <row r="6" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="6"/>
-      <c r="B6" s="21">
+      <c r="A6" s="2"/>
+      <c r="B6" s="17">
         <v>2009</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="14">
         <v>210</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="14">
         <v>265</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="14">
         <v>330</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="14">
         <v>459</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="14">
         <v>2711</v>
       </c>
-      <c r="H6" s="18">
+      <c r="H6" s="14">
         <v>4347</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="14">
         <v>7134</v>
       </c>
-      <c r="J6" s="18">
+      <c r="J6" s="14">
         <v>7452</v>
       </c>
-      <c r="K6" s="18">
+      <c r="K6" s="14">
         <v>10193</v>
       </c>
-      <c r="L6" s="18">
+      <c r="L6" s="14">
         <v>11773</v>
       </c>
-      <c r="M6" s="18">
+      <c r="M6" s="14">
         <v>16989</v>
       </c>
-      <c r="N6" s="18">
+      <c r="N6" s="14">
         <v>18516</v>
       </c>
-      <c r="O6" s="23">
+      <c r="O6" s="19">
         <f t="shared" si="0"/>
         <v>80379</v>
       </c>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="14">
+      <c r="P6" s="9"/>
+      <c r="Q6" s="10">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>80379</v>
       </c>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
     </row>
     <row r="7" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="6"/>
-      <c r="B7" s="21">
+      <c r="A7" s="2"/>
+      <c r="B7" s="17">
         <v>2010</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="14">
         <v>16660</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="14">
         <v>23673</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="14">
         <v>32985</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="14">
         <v>35222</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="14">
         <v>39909</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="14">
         <v>42087</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="14">
         <v>54395</v>
       </c>
-      <c r="J7" s="18">
+      <c r="J7" s="14">
         <v>49067</v>
       </c>
-      <c r="K7" s="18">
+      <c r="K7" s="14">
         <v>47658</v>
       </c>
-      <c r="L7" s="18">
+      <c r="L7" s="14">
         <v>38853</v>
       </c>
-      <c r="M7" s="18">
+      <c r="M7" s="14">
         <v>39946</v>
       </c>
-      <c r="N7" s="18">
+      <c r="N7" s="14">
         <v>42658</v>
       </c>
-      <c r="O7" s="23">
+      <c r="O7" s="19">
         <f t="shared" si="0"/>
         <v>463113</v>
       </c>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="14">
+      <c r="P7" s="9"/>
+      <c r="Q7" s="10">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>463113</v>
       </c>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
     </row>
     <row r="8" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="6"/>
-      <c r="B8" s="21">
+      <c r="A8" s="2"/>
+      <c r="B8" s="17">
         <v>2011</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="14">
         <v>45551</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="14">
         <v>69346</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="14">
         <v>47856</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="14">
         <v>64728</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="14">
         <v>73308</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="14">
         <v>82846</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I8" s="14">
         <v>72286</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="14">
         <v>75867</v>
       </c>
-      <c r="K8" s="18">
+      <c r="K8" s="14">
         <v>80961</v>
       </c>
-      <c r="L8" s="18">
+      <c r="L8" s="14">
         <v>62233</v>
       </c>
-      <c r="M8" s="18">
+      <c r="M8" s="14">
         <v>63447</v>
       </c>
-      <c r="N8" s="18">
+      <c r="N8" s="14">
         <v>64581</v>
       </c>
-      <c r="O8" s="23">
+      <c r="O8" s="19">
         <f t="shared" si="0"/>
         <v>803010</v>
       </c>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="14">
+      <c r="P8" s="9"/>
+      <c r="Q8" s="10">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>803010</v>
       </c>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
     </row>
     <row r="9" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="6"/>
-      <c r="B9" s="21">
+      <c r="A9" s="2"/>
+      <c r="B9" s="17">
         <v>2012</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="14">
         <v>76072</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="14">
         <v>77385</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="14">
         <v>70852</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="14">
         <v>72356</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="14">
         <v>78593</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="14">
         <v>70155</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="14">
         <v>72470</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="14">
         <v>70252</v>
       </c>
-      <c r="K9" s="18">
+      <c r="K9" s="14">
         <v>79738</v>
       </c>
-      <c r="L9" s="18">
+      <c r="L9" s="14">
         <v>71284</v>
       </c>
-      <c r="M9" s="18">
+      <c r="M9" s="14">
         <v>76524</v>
       </c>
-      <c r="N9" s="18">
+      <c r="N9" s="14">
         <v>73172</v>
       </c>
-      <c r="O9" s="23">
+      <c r="O9" s="19">
         <f t="shared" si="0"/>
         <v>888853</v>
       </c>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="14">
+      <c r="P9" s="9"/>
+      <c r="Q9" s="10">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>888853</v>
       </c>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
     </row>
     <row r="10" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="6"/>
-      <c r="B10" s="21">
+      <c r="A10" s="2"/>
+      <c r="B10" s="17">
         <v>2013</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="14">
         <v>78648</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="14">
         <v>74894</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="14">
         <v>86029</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="14">
         <v>82489</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="14">
         <v>80316</v>
       </c>
-      <c r="H10" s="18">
+      <c r="H10" s="14">
         <v>78764</v>
       </c>
-      <c r="I10" s="18">
+      <c r="I10" s="14">
         <v>70746</v>
       </c>
-      <c r="J10" s="18">
+      <c r="J10" s="14">
         <v>79324</v>
       </c>
-      <c r="K10" s="18">
+      <c r="K10" s="14">
         <v>79148</v>
       </c>
-      <c r="L10" s="18">
+      <c r="L10" s="14">
         <v>76345</v>
       </c>
-      <c r="M10" s="18">
+      <c r="M10" s="14">
         <v>75329</v>
       </c>
-      <c r="N10" s="18">
+      <c r="N10" s="14">
         <v>73625</v>
       </c>
-      <c r="O10" s="23">
+      <c r="O10" s="19">
         <f t="shared" si="0"/>
         <v>935657</v>
       </c>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="14">
+      <c r="P10" s="9"/>
+      <c r="Q10" s="10">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>935657</v>
       </c>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
     </row>
     <row r="11" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="6"/>
-      <c r="B11" s="21">
+      <c r="A11" s="2"/>
+      <c r="B11" s="17">
         <v>2014</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="14">
         <v>67510</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="14">
         <v>67706</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="14">
         <v>73924</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="14">
         <v>71449</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="14">
         <v>79877</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H11" s="14">
         <v>74705</v>
       </c>
-      <c r="I11" s="18">
+      <c r="I11" s="14">
         <v>79936</v>
       </c>
-      <c r="J11" s="18">
+      <c r="J11" s="14">
         <v>78746</v>
       </c>
-      <c r="K11" s="18">
+      <c r="K11" s="14">
         <v>77891</v>
       </c>
-      <c r="L11" s="18">
+      <c r="L11" s="14">
         <v>77040</v>
       </c>
-      <c r="M11" s="18">
+      <c r="M11" s="14">
         <v>87951</v>
       </c>
-      <c r="N11" s="19">
+      <c r="N11" s="15">
         <v>101904</v>
       </c>
-      <c r="O11" s="23">
+      <c r="O11" s="19">
         <f t="shared" si="0"/>
         <v>938639</v>
       </c>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="14">
+      <c r="P11" s="9"/>
+      <c r="Q11" s="10">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>938639</v>
       </c>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
     </row>
     <row r="12" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="6"/>
-      <c r="B12" s="21">
+      <c r="A12" s="2"/>
+      <c r="B12" s="17">
         <v>2015</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="14">
         <v>90536</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="14">
         <v>80976</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="14">
         <v>95444</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="14">
         <v>71951</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="14">
         <v>67019</v>
       </c>
-      <c r="H12" s="18">
+      <c r="H12" s="14">
         <v>66244</v>
       </c>
-      <c r="I12" s="18">
+      <c r="I12" s="14">
         <v>86294</v>
       </c>
-      <c r="J12" s="19">
+      <c r="J12" s="15">
         <v>128005</v>
       </c>
-      <c r="K12" s="19">
+      <c r="K12" s="15">
         <v>137300</v>
       </c>
-      <c r="L12" s="19">
+      <c r="L12" s="15">
         <v>138705</v>
       </c>
-      <c r="M12" s="19">
+      <c r="M12" s="15">
         <v>125538</v>
       </c>
-      <c r="N12" s="19">
+      <c r="N12" s="15">
         <v>129945</v>
       </c>
-      <c r="O12" s="23">
+      <c r="O12" s="19">
         <f t="shared" si="0"/>
         <v>1217957</v>
       </c>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="14">
+      <c r="P12" s="9"/>
+      <c r="Q12" s="10">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>1217957</v>
       </c>
-      <c r="R12" s="6"/>
-      <c r="S12" s="6"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
     </row>
     <row r="13" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="6"/>
-      <c r="B13" s="21">
+      <c r="A13" s="2"/>
+      <c r="B13" s="17">
         <v>2016</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="15">
         <v>142274</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="15">
         <v>123093</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E13" s="15">
         <v>147266</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F13" s="15">
         <v>152612</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="15">
         <v>134497</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13" s="15">
         <v>132768</v>
       </c>
-      <c r="I13" s="20">
+      <c r="I13" s="16">
         <v>363723</v>
       </c>
-      <c r="J13" s="20">
+      <c r="J13" s="16">
         <v>702130</v>
       </c>
-      <c r="K13" s="20">
+      <c r="K13" s="16">
         <v>608805</v>
       </c>
-      <c r="L13" s="20">
+      <c r="L13" s="16">
         <v>635500</v>
       </c>
-      <c r="M13" s="20">
+      <c r="M13" s="16">
         <v>713080</v>
       </c>
-      <c r="N13" s="20">
+      <c r="N13" s="16">
         <v>674509</v>
       </c>
-      <c r="O13" s="23">
+      <c r="O13" s="19">
         <f t="shared" si="0"/>
         <v>4530257</v>
       </c>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="14">
+      <c r="P13" s="9"/>
+      <c r="Q13" s="10">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>4530257</v>
       </c>
-      <c r="R13" s="6"/>
-      <c r="S13" s="6"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
     </row>
     <row r="14" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="6"/>
-      <c r="B14" s="21">
+      <c r="A14" s="2"/>
+      <c r="B14" s="17">
         <v>2017</v>
       </c>
-      <c r="C14" s="20">
+      <c r="C14" s="16">
         <v>662423</v>
       </c>
-      <c r="D14" s="20">
+      <c r="D14" s="16">
         <v>554842</v>
       </c>
-      <c r="E14" s="20">
+      <c r="E14" s="16">
         <v>657797</v>
       </c>
-      <c r="F14" s="20">
+      <c r="F14" s="16">
         <v>673209</v>
       </c>
-      <c r="G14" s="20">
+      <c r="G14" s="16">
         <v>745540</v>
       </c>
-      <c r="H14" s="20">
+      <c r="H14" s="16">
         <v>660058</v>
       </c>
-      <c r="I14" s="20">
+      <c r="I14" s="16">
         <v>690513</v>
       </c>
-      <c r="J14" s="20">
+      <c r="J14" s="16">
         <v>670496</v>
       </c>
-      <c r="K14" s="20">
+      <c r="K14" s="16">
         <v>577595</v>
       </c>
-      <c r="L14" s="20">
+      <c r="L14" s="16">
         <v>665972</v>
       </c>
-      <c r="M14" s="20">
+      <c r="M14" s="16">
         <v>569447</v>
       </c>
-      <c r="N14" s="20">
+      <c r="N14" s="16">
         <v>565361</v>
       </c>
-      <c r="O14" s="23">
+      <c r="O14" s="19">
         <f t="shared" si="0"/>
         <v>7693253</v>
       </c>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="14">
+      <c r="P14" s="9"/>
+      <c r="Q14" s="10">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>7693253</v>
       </c>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
     </row>
     <row r="15" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="6"/>
-      <c r="B15" s="21">
+      <c r="A15" s="2"/>
+      <c r="B15" s="17">
         <v>2018</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="16">
         <v>628028</v>
       </c>
-      <c r="D15" s="20">
+      <c r="D15" s="16">
         <v>728208</v>
       </c>
-      <c r="E15" s="20">
+      <c r="E15" s="16">
         <v>697376</v>
       </c>
-      <c r="F15" s="20">
+      <c r="F15" s="16">
         <v>707376</v>
       </c>
-      <c r="G15" s="20">
+      <c r="G15" s="16">
         <v>759564</v>
       </c>
-      <c r="H15" s="20">
+      <c r="H15" s="16">
         <v>592381</v>
       </c>
-      <c r="I15" s="20">
+      <c r="I15" s="16">
         <v>545423</v>
       </c>
-      <c r="J15" s="20">
+      <c r="J15" s="16">
         <v>694837</v>
       </c>
-      <c r="K15" s="20">
+      <c r="K15" s="16">
         <v>739656</v>
       </c>
-      <c r="L15" s="20">
+      <c r="L15" s="16">
         <v>763733</v>
       </c>
-      <c r="M15" s="20">
+      <c r="M15" s="16">
         <v>698962</v>
       </c>
-      <c r="N15" s="20">
+      <c r="N15" s="16">
         <v>732173</v>
       </c>
-      <c r="O15" s="23">
+      <c r="O15" s="19">
         <f t="shared" si="0"/>
         <v>8287717</v>
       </c>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="14">
+      <c r="P15" s="9"/>
+      <c r="Q15" s="10">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>8287717</v>
       </c>
-      <c r="R15" s="6"/>
-      <c r="S15" s="6"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
     </row>
     <row r="16" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="6"/>
-      <c r="B16" s="21">
+      <c r="A16" s="2"/>
+      <c r="B16" s="17">
         <v>2019</v>
       </c>
-      <c r="C16" s="20">
+      <c r="C16" s="16">
         <v>816792</v>
       </c>
-      <c r="D16" s="20">
+      <c r="D16" s="16">
         <v>811807</v>
       </c>
-      <c r="E16" s="19">
+      <c r="E16" s="15">
         <v>903678</v>
       </c>
-      <c r="F16" s="19">
+      <c r="F16" s="15">
         <v>1174272</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="15">
         <v>1399881</v>
       </c>
-      <c r="H16" s="19">
+      <c r="H16" s="15">
         <v>1179014</v>
       </c>
-      <c r="I16" s="19">
+      <c r="I16" s="15">
         <v>1380086</v>
       </c>
-      <c r="J16" s="19">
+      <c r="J16" s="15">
         <v>1448886</v>
       </c>
-      <c r="K16" s="19">
+      <c r="K16" s="15">
         <v>1506868</v>
       </c>
-      <c r="L16" s="19">
+      <c r="L16" s="15">
         <v>1761891</v>
       </c>
-      <c r="M16" s="19">
+      <c r="M16" s="15">
         <v>2059856</v>
       </c>
-      <c r="N16" s="19">
+      <c r="N16" s="15">
         <v>2325909</v>
       </c>
-      <c r="O16" s="24">
+      <c r="O16" s="20">
         <f t="shared" si="0"/>
         <v>16768940</v>
       </c>
-      <c r="P16" s="13"/>
-      <c r="Q16" s="14">
+      <c r="P16" s="9"/>
+      <c r="Q16" s="10">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>16768940</v>
       </c>
-      <c r="R16" s="6"/>
-      <c r="S16" s="6"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
     </row>
     <row r="17" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="6"/>
-      <c r="B17" s="21">
+      <c r="A17" s="2"/>
+      <c r="B17" s="17">
         <v>2020</v>
       </c>
-      <c r="C17" s="19">
+      <c r="C17" s="15">
         <v>1694534</v>
       </c>
-      <c r="D17" s="19">
+      <c r="D17" s="15">
         <v>3203938</v>
       </c>
-      <c r="E17" s="19">
+      <c r="E17" s="15">
         <v>3296329</v>
       </c>
-      <c r="F17" s="19">
+      <c r="F17" s="15">
         <v>2694570</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="15">
         <v>2511957</v>
       </c>
-      <c r="H17" s="19">
+      <c r="H17" s="15">
         <v>2264236</v>
       </c>
-      <c r="I17" s="19">
+      <c r="I17" s="15">
         <v>1255353</v>
       </c>
-      <c r="J17" s="19">
+      <c r="J17" s="15">
         <v>1205188</v>
       </c>
-      <c r="K17" s="19">
+      <c r="K17" s="15">
         <v>1622473</v>
       </c>
-      <c r="L17" s="19">
+      <c r="L17" s="15">
         <v>1912285</v>
       </c>
-      <c r="M17" s="19">
+      <c r="M17" s="15">
         <v>2366693</v>
       </c>
-      <c r="N17" s="19">
+      <c r="N17" s="15">
         <v>2176841</v>
       </c>
-      <c r="O17" s="25">
+      <c r="O17" s="21">
         <f t="shared" si="0"/>
         <v>26204397</v>
       </c>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="14">
+      <c r="P17" s="9"/>
+      <c r="Q17" s="10">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>26204397</v>
       </c>
-      <c r="R17" s="6"/>
-      <c r="S17" s="6"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
     </row>
     <row r="18" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="6"/>
-      <c r="B18" s="21">
+      <c r="A18" s="2"/>
+      <c r="B18" s="17">
         <v>2021</v>
       </c>
-      <c r="C18" s="19">
+      <c r="C18" s="15">
         <v>924261</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="15">
         <v>1235225</v>
       </c>
-      <c r="E18" s="19">
+      <c r="E18" s="15">
         <v>2047206</v>
       </c>
-      <c r="F18" s="19">
+      <c r="F18" s="15">
         <v>2337103</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G18" s="15">
         <v>2440903</v>
       </c>
-      <c r="H18" s="19">
+      <c r="H18" s="15">
         <v>2432014</v>
       </c>
-      <c r="I18" s="19">
+      <c r="I18" s="15">
         <v>2631617</v>
       </c>
-      <c r="J18" s="19">
+      <c r="J18" s="15">
         <v>2238361</v>
       </c>
-      <c r="K18" s="19">
+      <c r="K18" s="15">
         <v>3054555</v>
       </c>
-      <c r="L18" s="19">
+      <c r="L18" s="15">
         <v>2855764</v>
       </c>
-      <c r="M18" s="19">
+      <c r="M18" s="15">
         <v>3465933</v>
       </c>
-      <c r="N18" s="19">
+      <c r="N18" s="15">
         <v>4145700</v>
       </c>
-      <c r="O18" s="25">
+      <c r="O18" s="21">
         <f t="shared" si="0"/>
         <v>29808642</v>
       </c>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="14">
+      <c r="P18" s="9"/>
+      <c r="Q18" s="10">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>29808642</v>
       </c>
-      <c r="R18" s="6"/>
-      <c r="S18" s="6"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
     </row>
     <row r="19" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="6"/>
-      <c r="B19" s="21">
+      <c r="A19" s="2"/>
+      <c r="B19" s="17">
         <v>2022</v>
       </c>
-      <c r="C19" s="19">
+      <c r="C19" s="15">
         <v>4297072</v>
       </c>
-      <c r="D19" s="19">
+      <c r="D19" s="15">
         <v>2442144</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E19" s="15">
         <v>2336228</v>
       </c>
-      <c r="F19" s="19">
+      <c r="F19" s="15">
         <v>2718163</v>
       </c>
-      <c r="G19" s="19">
+      <c r="G19" s="15">
         <v>2097535</v>
       </c>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19"/>
-      <c r="O19" s="25">
+      <c r="H19" s="15">
+        <v>2895282</v>
+      </c>
+      <c r="I19" s="15">
+        <v>2891642</v>
+      </c>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="21">
         <f t="shared" si="0"/>
-        <v>13891142</v>
-      </c>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="14" t="e">
+        <v>19678066</v>
+      </c>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="10" t="e">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="R19" s="6"/>
-      <c r="S19" s="6"/>
-    </row>
-    <row r="20" spans="1:19" s="12" customFormat="1" ht="58.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="26">
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+    </row>
+    <row r="20" spans="1:19" s="8" customFormat="1" ht="58.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="22">
         <f>SUM(O5:O19)</f>
-        <v>112512282</v>
-      </c>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="8"/>
-      <c r="S20" s="8"/>
+        <v>118299206</v>
+      </c>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
     </row>
     <row r="21" spans="1:19" ht="26.85" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="6"/>
-      <c r="S21" s="6"/>
-    </row>
-    <row r="22" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
-      <c r="L22" s="16"/>
-      <c r="M22" s="16"/>
-      <c r="N22" s="16"/>
-      <c r="O22" s="16"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+    </row>
+    <row r="22" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
     </row>
     <row r="23" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A23" s="6"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="6"/>
-      <c r="R23" s="6"/>
-      <c r="S23" s="6"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="6"/>
-      <c r="P24" s="6"/>
-      <c r="Q24" s="6"/>
-      <c r="R24" s="6"/>
-      <c r="S24" s="6"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="6"/>
-      <c r="P25" s="6"/>
-      <c r="Q25" s="6"/>
-      <c r="R25" s="6"/>
-      <c r="S25" s="6"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
-      <c r="O26" s="6"/>
-      <c r="P26" s="6"/>
-      <c r="Q26" s="6"/>
-      <c r="R26" s="6"/>
-      <c r="S26" s="6"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
-      <c r="P27" s="6"/>
-      <c r="Q27" s="6"/>
-      <c r="R27" s="6"/>
-      <c r="S27" s="6"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
-      <c r="N28" s="6"/>
-      <c r="O28" s="6"/>
-      <c r="P28" s="6"/>
-      <c r="Q28" s="6"/>
-      <c r="R28" s="6"/>
-      <c r="S28" s="6"/>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
-      <c r="N29" s="6"/>
-      <c r="O29" s="6"/>
-      <c r="P29" s="6"/>
-      <c r="Q29" s="6"/>
-      <c r="R29" s="6"/>
-      <c r="S29" s="6"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
-      <c r="M30" s="6"/>
-      <c r="N30" s="6"/>
-      <c r="O30" s="6"/>
-      <c r="P30" s="6"/>
-      <c r="Q30" s="6"/>
-      <c r="R30" s="6"/>
-      <c r="S30" s="6"/>
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
-      <c r="M31" s="6"/>
-      <c r="N31" s="6"/>
-      <c r="O31" s="6"/>
-      <c r="P31" s="6"/>
-      <c r="Q31" s="6"/>
-      <c r="R31" s="6"/>
-      <c r="S31" s="6"/>
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
+      <c r="S31" s="2"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="6"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6"/>
-      <c r="P32" s="6"/>
-      <c r="Q32" s="6"/>
-      <c r="R32" s="6"/>
-      <c r="S32" s="6"/>
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
+      <c r="S32" s="2"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="6"/>
-      <c r="P33" s="6"/>
-      <c r="Q33" s="6"/>
-      <c r="R33" s="6"/>
-      <c r="S33" s="6"/>
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2"/>
+      <c r="S33" s="2"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
-      <c r="M34" s="6"/>
-      <c r="N34" s="6"/>
-      <c r="O34" s="6"/>
-      <c r="P34" s="6"/>
-      <c r="Q34" s="6"/>
-      <c r="R34" s="6"/>
-      <c r="S34" s="6"/>
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="2"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
-      <c r="M35" s="6"/>
-      <c r="N35" s="6"/>
-      <c r="O35" s="6"/>
-      <c r="P35" s="6"/>
-      <c r="Q35" s="6"/>
-      <c r="R35" s="6"/>
-      <c r="S35" s="6"/>
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2"/>
+      <c r="S35" s="2"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6"/>
-      <c r="M36" s="6"/>
-      <c r="N36" s="6"/>
-      <c r="O36" s="6"/>
-      <c r="P36" s="6"/>
-      <c r="Q36" s="6"/>
-      <c r="R36" s="6"/>
-      <c r="S36" s="6"/>
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
+      <c r="S36" s="2"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
-      <c r="M37" s="6"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="6"/>
-      <c r="P37" s="6"/>
-      <c r="Q37" s="6"/>
-      <c r="R37" s="6"/>
-      <c r="S37" s="6"/>
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2"/>
+      <c r="S37" s="2"/>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="6"/>
-      <c r="M38" s="6"/>
-      <c r="N38" s="6"/>
-      <c r="O38" s="6"/>
-      <c r="P38" s="6"/>
-      <c r="Q38" s="6"/>
-      <c r="R38" s="6"/>
-      <c r="S38" s="6"/>
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="2"/>
+      <c r="S38" s="2"/>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
-      <c r="L39" s="6"/>
-      <c r="M39" s="6"/>
-      <c r="N39" s="6"/>
-      <c r="O39" s="6"/>
-      <c r="P39" s="6"/>
-      <c r="Q39" s="6"/>
-      <c r="R39" s="6"/>
-      <c r="S39" s="6"/>
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="2"/>
+      <c r="S39" s="2"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="6"/>
-      <c r="K40" s="6"/>
-      <c r="L40" s="6"/>
-      <c r="M40" s="6"/>
-      <c r="N40" s="6"/>
-      <c r="O40" s="6"/>
-      <c r="P40" s="6"/>
-      <c r="Q40" s="6"/>
-      <c r="R40" s="6"/>
-      <c r="S40" s="6"/>
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="2"/>
+      <c r="S40" s="2"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="6"/>
-      <c r="K41" s="6"/>
-      <c r="L41" s="6"/>
-      <c r="M41" s="6"/>
-      <c r="N41" s="6"/>
-      <c r="O41" s="6"/>
-      <c r="P41" s="6"/>
-      <c r="Q41" s="6"/>
-      <c r="R41" s="6"/>
-      <c r="S41" s="6"/>
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
+      <c r="R41" s="2"/>
+      <c r="S41" s="2"/>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="6"/>
-      <c r="K42" s="6"/>
-      <c r="L42" s="6"/>
-      <c r="M42" s="6"/>
-      <c r="N42" s="6"/>
-      <c r="O42" s="6"/>
-      <c r="P42" s="6"/>
-      <c r="Q42" s="6"/>
-      <c r="R42" s="6"/>
-      <c r="S42" s="6"/>
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="2"/>
+      <c r="R42" s="2"/>
+      <c r="S42" s="2"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
-      <c r="I43" s="6"/>
-      <c r="J43" s="6"/>
-      <c r="K43" s="6"/>
-      <c r="L43" s="6"/>
-      <c r="M43" s="6"/>
-      <c r="N43" s="6"/>
-      <c r="O43" s="6"/>
-      <c r="P43" s="6"/>
-      <c r="Q43" s="6"/>
-      <c r="R43" s="6"/>
-      <c r="S43" s="6"/>
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
+      <c r="R43" s="2"/>
+      <c r="S43" s="2"/>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
-      <c r="I44" s="6"/>
-      <c r="J44" s="6"/>
-      <c r="K44" s="6"/>
-      <c r="L44" s="6"/>
-      <c r="M44" s="6"/>
-      <c r="N44" s="6"/>
-      <c r="O44" s="6"/>
-      <c r="P44" s="6"/>
-      <c r="Q44" s="6"/>
-      <c r="R44" s="6"/>
-      <c r="S44" s="6"/>
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2"/>
+      <c r="R44" s="2"/>
+      <c r="S44" s="2"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="6"/>
-      <c r="J45" s="6"/>
-      <c r="K45" s="6"/>
-      <c r="L45" s="6"/>
-      <c r="M45" s="6"/>
-      <c r="N45" s="6"/>
-      <c r="O45" s="6"/>
-      <c r="P45" s="6"/>
-      <c r="Q45" s="6"/>
-      <c r="R45" s="6"/>
-      <c r="S45" s="6"/>
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
+      <c r="Q45" s="2"/>
+      <c r="R45" s="2"/>
+      <c r="S45" s="2"/>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
-      <c r="I46" s="6"/>
-      <c r="J46" s="6"/>
-      <c r="K46" s="6"/>
-      <c r="L46" s="6"/>
-      <c r="M46" s="6"/>
-      <c r="N46" s="6"/>
-      <c r="O46" s="6"/>
-      <c r="P46" s="6"/>
-      <c r="Q46" s="6"/>
-      <c r="R46" s="6"/>
-      <c r="S46" s="6"/>
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
+      <c r="Q46" s="2"/>
+      <c r="R46" s="2"/>
+      <c r="S46" s="2"/>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
-      <c r="I47" s="6"/>
-      <c r="J47" s="6"/>
-      <c r="K47" s="6"/>
-      <c r="L47" s="6"/>
-      <c r="M47" s="6"/>
-      <c r="N47" s="6"/>
-      <c r="O47" s="6"/>
-      <c r="P47" s="6"/>
-      <c r="Q47" s="6"/>
-      <c r="R47" s="6"/>
-      <c r="S47" s="6"/>
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
+      <c r="R47" s="2"/>
+      <c r="S47" s="2"/>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="6"/>
-      <c r="J48" s="6"/>
-      <c r="K48" s="6"/>
-      <c r="L48" s="6"/>
-      <c r="M48" s="6"/>
-      <c r="N48" s="6"/>
-      <c r="O48" s="6"/>
-      <c r="P48" s="6"/>
-      <c r="Q48" s="6"/>
-      <c r="R48" s="6"/>
-      <c r="S48" s="6"/>
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
+      <c r="Q48" s="2"/>
+      <c r="R48" s="2"/>
+      <c r="S48" s="2"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
-      <c r="I49" s="6"/>
-      <c r="J49" s="6"/>
-      <c r="K49" s="6"/>
-      <c r="L49" s="6"/>
-      <c r="M49" s="6"/>
-      <c r="N49" s="6"/>
-      <c r="O49" s="6"/>
-      <c r="P49" s="6"/>
-      <c r="Q49" s="6"/>
-      <c r="R49" s="6"/>
-      <c r="S49" s="6"/>
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" s="2"/>
+      <c r="P49" s="2"/>
+      <c r="Q49" s="2"/>
+      <c r="R49" s="2"/>
+      <c r="S49" s="2"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
-      <c r="H50" s="6"/>
-      <c r="I50" s="6"/>
-      <c r="J50" s="6"/>
-      <c r="K50" s="6"/>
-      <c r="L50" s="6"/>
-      <c r="M50" s="6"/>
-      <c r="N50" s="6"/>
-      <c r="O50" s="6"/>
-      <c r="P50" s="6"/>
-      <c r="Q50" s="6"/>
-      <c r="R50" s="6"/>
-      <c r="S50" s="6"/>
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" s="2"/>
+      <c r="P50" s="2"/>
+      <c r="Q50" s="2"/>
+      <c r="R50" s="2"/>
+      <c r="S50" s="2"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A51" s="6"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="6"/>
-      <c r="I51" s="6"/>
-      <c r="J51" s="1"/>
-      <c r="K51" s="1"/>
-      <c r="L51" s="1"/>
-      <c r="M51" s="6"/>
-      <c r="N51" s="6"/>
-      <c r="O51" s="6"/>
-      <c r="P51" s="6"/>
-      <c r="Q51" s="6"/>
-      <c r="R51" s="6"/>
-      <c r="S51" s="6"/>
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="26"/>
+      <c r="K51" s="26"/>
+      <c r="L51" s="26"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+      <c r="O51" s="2"/>
+      <c r="P51" s="2"/>
+      <c r="Q51" s="2"/>
+      <c r="R51" s="2"/>
+      <c r="S51" s="2"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A52" s="16"/>
-      <c r="B52" s="16"/>
-      <c r="C52" s="16"/>
-      <c r="D52" s="16"/>
-      <c r="E52" s="16"/>
-      <c r="F52" s="16"/>
-      <c r="G52" s="16"/>
-      <c r="H52" s="16"/>
-      <c r="I52" s="16"/>
-      <c r="J52" s="16"/>
-      <c r="K52" s="16"/>
-      <c r="L52" s="17"/>
-      <c r="M52" s="16"/>
-      <c r="N52" s="16"/>
-      <c r="O52" s="16"/>
-      <c r="P52" s="16"/>
-      <c r="Q52" s="16"/>
-      <c r="R52" s="16"/>
-      <c r="S52" s="16"/>
+      <c r="A52" s="12"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="12"/>
+      <c r="H52" s="12"/>
+      <c r="I52" s="12"/>
+      <c r="J52" s="12"/>
+      <c r="K52" s="12"/>
+      <c r="L52" s="13"/>
+      <c r="M52" s="12"/>
+      <c r="N52" s="12"/>
+      <c r="O52" s="12"/>
+      <c r="P52" s="12"/>
+      <c r="Q52" s="12"/>
+      <c r="R52" s="12"/>
+      <c r="S52" s="12"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A53" s="16"/>
-      <c r="B53" s="16"/>
-      <c r="C53" s="16"/>
-      <c r="D53" s="16"/>
-      <c r="E53" s="16"/>
-      <c r="F53" s="16"/>
-      <c r="G53" s="16"/>
-      <c r="H53" s="16"/>
-      <c r="I53" s="16"/>
-      <c r="J53" s="16"/>
-      <c r="K53" s="16"/>
-      <c r="L53" s="16"/>
-      <c r="M53" s="16"/>
-      <c r="N53" s="16"/>
-      <c r="O53" s="16"/>
-      <c r="P53" s="16"/>
-      <c r="Q53" s="16"/>
-      <c r="R53" s="16"/>
-      <c r="S53" s="16"/>
+      <c r="A53" s="12"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
+      <c r="H53" s="12"/>
+      <c r="I53" s="12"/>
+      <c r="J53" s="12"/>
+      <c r="K53" s="12"/>
+      <c r="L53" s="12"/>
+      <c r="M53" s="12"/>
+      <c r="N53" s="12"/>
+      <c r="O53" s="12"/>
+      <c r="P53" s="12"/>
+      <c r="Q53" s="12"/>
+      <c r="R53" s="12"/>
+      <c r="S53" s="12"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A54" s="16"/>
-      <c r="B54" s="16"/>
-      <c r="C54" s="16"/>
-      <c r="D54" s="16"/>
-      <c r="E54" s="16"/>
-      <c r="F54" s="16"/>
-      <c r="G54" s="16"/>
-      <c r="H54" s="16"/>
-      <c r="I54" s="16"/>
-      <c r="J54" s="16"/>
-      <c r="K54" s="16"/>
-      <c r="L54" s="16"/>
-      <c r="M54" s="16"/>
-      <c r="N54" s="16"/>
-      <c r="O54" s="16"/>
-      <c r="P54" s="16"/>
-      <c r="Q54" s="16"/>
-      <c r="R54" s="16"/>
-      <c r="S54" s="16"/>
+      <c r="A54" s="12"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+      <c r="H54" s="12"/>
+      <c r="I54" s="12"/>
+      <c r="J54" s="12"/>
+      <c r="K54" s="12"/>
+      <c r="L54" s="12"/>
+      <c r="M54" s="12"/>
+      <c r="N54" s="12"/>
+      <c r="O54" s="12"/>
+      <c r="P54" s="12"/>
+      <c r="Q54" s="12"/>
+      <c r="R54" s="12"/>
+      <c r="S54" s="12"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A55" s="16"/>
-      <c r="B55" s="16"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="16"/>
-      <c r="F55" s="16"/>
-      <c r="G55" s="16"/>
-      <c r="H55" s="16"/>
-      <c r="I55" s="16"/>
-      <c r="J55" s="16"/>
-      <c r="K55" s="16"/>
-      <c r="L55" s="16"/>
-      <c r="M55" s="16"/>
-      <c r="N55" s="16"/>
-      <c r="O55" s="16"/>
-      <c r="P55" s="16"/>
-      <c r="Q55" s="16"/>
-      <c r="R55" s="16"/>
-      <c r="S55" s="16"/>
+      <c r="A55" s="12"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
+      <c r="H55" s="12"/>
+      <c r="I55" s="12"/>
+      <c r="J55" s="12"/>
+      <c r="K55" s="12"/>
+      <c r="L55" s="12"/>
+      <c r="M55" s="12"/>
+      <c r="N55" s="12"/>
+      <c r="O55" s="12"/>
+      <c r="P55" s="12"/>
+      <c r="Q55" s="12"/>
+      <c r="R55" s="12"/>
+      <c r="S55" s="12"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A56" s="16"/>
-      <c r="B56" s="16"/>
-      <c r="C56" s="16"/>
-      <c r="D56" s="16"/>
-      <c r="E56" s="16"/>
-      <c r="F56" s="16"/>
-      <c r="G56" s="16"/>
-      <c r="H56" s="16"/>
-      <c r="I56" s="16"/>
-      <c r="J56" s="16"/>
-      <c r="K56" s="16"/>
-      <c r="L56" s="16"/>
-      <c r="M56" s="16"/>
-      <c r="N56" s="16"/>
-      <c r="O56" s="16"/>
-      <c r="P56" s="16"/>
-      <c r="Q56" s="16"/>
-      <c r="R56" s="16"/>
-      <c r="S56" s="16"/>
+      <c r="A56" s="12"/>
+      <c r="B56" s="12"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
+      <c r="H56" s="12"/>
+      <c r="I56" s="12"/>
+      <c r="J56" s="12"/>
+      <c r="K56" s="12"/>
+      <c r="L56" s="12"/>
+      <c r="M56" s="12"/>
+      <c r="N56" s="12"/>
+      <c r="O56" s="12"/>
+      <c r="P56" s="12"/>
+      <c r="Q56" s="12"/>
+      <c r="R56" s="12"/>
+      <c r="S56" s="12"/>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A57" s="16"/>
-      <c r="B57" s="16"/>
-      <c r="C57" s="16"/>
-      <c r="D57" s="16"/>
-      <c r="E57" s="16"/>
-      <c r="F57" s="16"/>
-      <c r="G57" s="16"/>
-      <c r="H57" s="16"/>
-      <c r="I57" s="16"/>
-      <c r="J57" s="16"/>
-      <c r="K57" s="16"/>
-      <c r="L57" s="16"/>
-      <c r="M57" s="16"/>
-      <c r="N57" s="16"/>
-      <c r="O57" s="16"/>
-      <c r="P57" s="16"/>
-      <c r="Q57" s="16"/>
-      <c r="R57" s="16"/>
-      <c r="S57" s="16"/>
+      <c r="A57" s="12"/>
+      <c r="B57" s="12"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="12"/>
+      <c r="G57" s="12"/>
+      <c r="H57" s="12"/>
+      <c r="I57" s="12"/>
+      <c r="J57" s="12"/>
+      <c r="K57" s="12"/>
+      <c r="L57" s="12"/>
+      <c r="M57" s="12"/>
+      <c r="N57" s="12"/>
+      <c r="O57" s="12"/>
+      <c r="P57" s="12"/>
+      <c r="Q57" s="12"/>
+      <c r="R57" s="12"/>
+      <c r="S57" s="12"/>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A58" s="16"/>
-      <c r="B58" s="16"/>
-      <c r="C58" s="16"/>
-      <c r="D58" s="16"/>
-      <c r="E58" s="16"/>
-      <c r="F58" s="16"/>
-      <c r="G58" s="16"/>
-      <c r="H58" s="16"/>
-      <c r="I58" s="16"/>
-      <c r="J58" s="16"/>
-      <c r="K58" s="16"/>
-      <c r="L58" s="16"/>
-      <c r="M58" s="16"/>
-      <c r="N58" s="16"/>
-      <c r="O58" s="16"/>
-      <c r="P58" s="16"/>
-      <c r="Q58" s="16"/>
-      <c r="R58" s="16"/>
-      <c r="S58" s="16"/>
+      <c r="A58" s="12"/>
+      <c r="B58" s="12"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="12"/>
+      <c r="H58" s="12"/>
+      <c r="I58" s="12"/>
+      <c r="J58" s="12"/>
+      <c r="K58" s="12"/>
+      <c r="L58" s="12"/>
+      <c r="M58" s="12"/>
+      <c r="N58" s="12"/>
+      <c r="O58" s="12"/>
+      <c r="P58" s="12"/>
+      <c r="Q58" s="12"/>
+      <c r="R58" s="12"/>
+      <c r="S58" s="12"/>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A59" s="16"/>
-      <c r="B59" s="16"/>
-      <c r="C59" s="16"/>
-      <c r="D59" s="16"/>
-      <c r="E59" s="16"/>
-      <c r="F59" s="16"/>
-      <c r="G59" s="16"/>
-      <c r="H59" s="16"/>
-      <c r="I59" s="16"/>
-      <c r="J59" s="16"/>
-      <c r="K59" s="16"/>
-      <c r="L59" s="16"/>
-      <c r="M59" s="16"/>
-      <c r="N59" s="16"/>
-      <c r="O59" s="16"/>
-      <c r="P59" s="16"/>
-      <c r="Q59" s="16"/>
-      <c r="R59" s="16"/>
-      <c r="S59" s="16"/>
+      <c r="A59" s="12"/>
+      <c r="B59" s="12"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="12"/>
+      <c r="H59" s="12"/>
+      <c r="I59" s="12"/>
+      <c r="J59" s="12"/>
+      <c r="K59" s="12"/>
+      <c r="L59" s="12"/>
+      <c r="M59" s="12"/>
+      <c r="N59" s="12"/>
+      <c r="O59" s="12"/>
+      <c r="P59" s="12"/>
+      <c r="Q59" s="12"/>
+      <c r="R59" s="12"/>
+      <c r="S59" s="12"/>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A60" s="16"/>
-      <c r="B60" s="16"/>
-      <c r="C60" s="16"/>
-      <c r="D60" s="16"/>
-      <c r="E60" s="16"/>
-      <c r="F60" s="16"/>
-      <c r="G60" s="16"/>
-      <c r="H60" s="16"/>
-      <c r="I60" s="16"/>
-      <c r="J60" s="16"/>
-      <c r="K60" s="16"/>
-      <c r="L60" s="16"/>
-      <c r="M60" s="16"/>
-      <c r="N60" s="16"/>
-      <c r="O60" s="16"/>
-      <c r="P60" s="16"/>
-      <c r="Q60" s="16"/>
-      <c r="R60" s="16"/>
-      <c r="S60" s="16"/>
+      <c r="A60" s="12"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="12"/>
+      <c r="H60" s="12"/>
+      <c r="I60" s="12"/>
+      <c r="J60" s="12"/>
+      <c r="K60" s="12"/>
+      <c r="L60" s="12"/>
+      <c r="M60" s="12"/>
+      <c r="N60" s="12"/>
+      <c r="O60" s="12"/>
+      <c r="P60" s="12"/>
+      <c r="Q60" s="12"/>
+      <c r="R60" s="12"/>
+      <c r="S60" s="12"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A61" s="16"/>
-      <c r="B61" s="16"/>
-      <c r="C61" s="16"/>
-      <c r="D61" s="16"/>
-      <c r="E61" s="16"/>
-      <c r="F61" s="16"/>
-      <c r="G61" s="16"/>
-      <c r="H61" s="16"/>
-      <c r="I61" s="16"/>
-      <c r="J61" s="16"/>
-      <c r="K61" s="16"/>
-      <c r="L61" s="16"/>
-      <c r="M61" s="16"/>
-      <c r="N61" s="16"/>
-      <c r="O61" s="16"/>
-      <c r="P61" s="16"/>
-      <c r="Q61" s="16"/>
-      <c r="R61" s="16"/>
-      <c r="S61" s="16"/>
+      <c r="A61" s="12"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="12"/>
+      <c r="H61" s="12"/>
+      <c r="I61" s="12"/>
+      <c r="J61" s="12"/>
+      <c r="K61" s="12"/>
+      <c r="L61" s="12"/>
+      <c r="M61" s="12"/>
+      <c r="N61" s="12"/>
+      <c r="O61" s="12"/>
+      <c r="P61" s="12"/>
+      <c r="Q61" s="12"/>
+      <c r="R61" s="12"/>
+      <c r="S61" s="12"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A62" s="16"/>
-      <c r="B62" s="16"/>
-      <c r="C62" s="16"/>
-      <c r="D62" s="16"/>
-      <c r="E62" s="16"/>
-      <c r="F62" s="16"/>
-      <c r="G62" s="16"/>
-      <c r="H62" s="16"/>
-      <c r="I62" s="16"/>
-      <c r="J62" s="16"/>
-      <c r="K62" s="16"/>
-      <c r="L62" s="16"/>
-      <c r="M62" s="16"/>
-      <c r="N62" s="16"/>
-      <c r="O62" s="16"/>
-      <c r="P62" s="16"/>
-      <c r="Q62" s="16"/>
-      <c r="R62" s="16"/>
-      <c r="S62" s="16"/>
+      <c r="A62" s="12"/>
+      <c r="B62" s="12"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
+      <c r="G62" s="12"/>
+      <c r="H62" s="12"/>
+      <c r="I62" s="12"/>
+      <c r="J62" s="12"/>
+      <c r="K62" s="12"/>
+      <c r="L62" s="12"/>
+      <c r="M62" s="12"/>
+      <c r="N62" s="12"/>
+      <c r="O62" s="12"/>
+      <c r="P62" s="12"/>
+      <c r="Q62" s="12"/>
+      <c r="R62" s="12"/>
+      <c r="S62" s="12"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A63" s="16"/>
-      <c r="B63" s="16"/>
-      <c r="C63" s="16"/>
-      <c r="D63" s="16"/>
-      <c r="E63" s="16"/>
-      <c r="F63" s="16"/>
-      <c r="G63" s="16"/>
-      <c r="H63" s="16"/>
-      <c r="I63" s="16"/>
-      <c r="J63" s="16"/>
-      <c r="K63" s="16"/>
-      <c r="L63" s="16"/>
-      <c r="M63" s="16"/>
-      <c r="N63" s="16"/>
-      <c r="O63" s="16"/>
-      <c r="P63" s="16"/>
-      <c r="Q63" s="16"/>
-      <c r="R63" s="16"/>
-      <c r="S63" s="16"/>
+      <c r="A63" s="12"/>
+      <c r="B63" s="12"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="12"/>
+      <c r="F63" s="12"/>
+      <c r="G63" s="12"/>
+      <c r="H63" s="12"/>
+      <c r="I63" s="12"/>
+      <c r="J63" s="12"/>
+      <c r="K63" s="12"/>
+      <c r="L63" s="12"/>
+      <c r="M63" s="12"/>
+      <c r="N63" s="12"/>
+      <c r="O63" s="12"/>
+      <c r="P63" s="12"/>
+      <c r="Q63" s="12"/>
+      <c r="R63" s="12"/>
+      <c r="S63" s="12"/>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A64" s="16"/>
-      <c r="B64" s="16"/>
-      <c r="C64" s="16"/>
-      <c r="D64" s="16"/>
-      <c r="E64" s="16"/>
-      <c r="F64" s="16"/>
-      <c r="G64" s="16"/>
-      <c r="H64" s="16"/>
-      <c r="I64" s="16"/>
-      <c r="J64" s="16"/>
-      <c r="K64" s="16"/>
-      <c r="L64" s="16"/>
-      <c r="M64" s="16"/>
-      <c r="N64" s="16"/>
-      <c r="O64" s="16"/>
-      <c r="P64" s="16"/>
-      <c r="Q64" s="16"/>
-      <c r="R64" s="16"/>
-      <c r="S64" s="16"/>
+      <c r="A64" s="12"/>
+      <c r="B64" s="12"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
+      <c r="H64" s="12"/>
+      <c r="I64" s="12"/>
+      <c r="J64" s="12"/>
+      <c r="K64" s="12"/>
+      <c r="L64" s="12"/>
+      <c r="M64" s="12"/>
+      <c r="N64" s="12"/>
+      <c r="O64" s="12"/>
+      <c r="P64" s="12"/>
+      <c r="Q64" s="12"/>
+      <c r="R64" s="12"/>
+      <c r="S64" s="12"/>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A65" s="16"/>
-      <c r="B65" s="16"/>
-      <c r="C65" s="16"/>
-      <c r="D65" s="16"/>
-      <c r="E65" s="16"/>
-      <c r="F65" s="16"/>
-      <c r="G65" s="16"/>
-      <c r="H65" s="16"/>
-      <c r="I65" s="16"/>
-      <c r="J65" s="16"/>
-      <c r="K65" s="16"/>
-      <c r="L65" s="16"/>
-      <c r="M65" s="16"/>
-      <c r="N65" s="16"/>
-      <c r="O65" s="16"/>
-      <c r="P65" s="16"/>
-      <c r="Q65" s="16"/>
-      <c r="R65" s="16"/>
-      <c r="S65" s="16"/>
+      <c r="A65" s="12"/>
+      <c r="B65" s="12"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
+      <c r="G65" s="12"/>
+      <c r="H65" s="12"/>
+      <c r="I65" s="12"/>
+      <c r="J65" s="12"/>
+      <c r="K65" s="12"/>
+      <c r="L65" s="12"/>
+      <c r="M65" s="12"/>
+      <c r="N65" s="12"/>
+      <c r="O65" s="12"/>
+      <c r="P65" s="12"/>
+      <c r="Q65" s="12"/>
+      <c r="R65" s="12"/>
+      <c r="S65" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Blog Statistics (September 2022)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c93c05515dfe04a/GIT Hub/kunal-chowdhury.com/blog-stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="11_91C7ACB7C03E7306CE517BDFACF66E9FD99B01DC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0DED57AA-A81B-4E89-855A-1EB04EBA7924}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="11_91C7ACB7C03E7306CE517BDFACF66E9FD99B01DC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C8A356A-88AD-4C92-9BFA-29E086DFD420}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -312,12 +312,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -329,14 +328,13 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="3" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -367,13 +365,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -722,7 +720,7 @@
                   <c:v>29808642</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>19678066</c:v>
+                  <c:v>26001799</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1271,1910 +1269,1898 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ65"/>
+  <dimension ref="A1:S65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="1" customWidth="1"/>
-    <col min="3" max="14" width="26.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="32.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="5.42578125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="25.42578125" style="1" customWidth="1"/>
-    <col min="18" max="1024" width="9" style="1"/>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="14" width="26.28515625" customWidth="1"/>
+    <col min="15" max="15" width="32.28515625" customWidth="1"/>
+    <col min="16" max="16" width="5.42578125" customWidth="1"/>
+    <col min="17" max="17" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="1"/>
+      <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="N3" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O3" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="8" customFormat="1" ht="104.45" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="18" t="s">
+    <row r="4" spans="1:19" s="7" customFormat="1" ht="104.45" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="18" t="s">
+      <c r="I4" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="J4" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="18" t="s">
+      <c r="K4" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="18" t="s">
+      <c r="L4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="18" t="s">
+      <c r="M4" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="18" t="s">
+      <c r="N4" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="18" t="s">
+      <c r="O4" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
     </row>
     <row r="5" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="17">
+      <c r="A5" s="1"/>
+      <c r="B5" s="15">
         <v>2008</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="12">
         <v>0</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="12">
         <v>0</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="12">
         <v>0</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="12">
         <v>0</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="12">
         <v>0</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="12">
         <v>0</v>
       </c>
-      <c r="I5" s="14">
+      <c r="I5" s="12">
         <v>0</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J5" s="12">
         <v>0</v>
       </c>
-      <c r="K5" s="14">
+      <c r="K5" s="12">
         <v>0</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="12">
         <v>105</v>
       </c>
-      <c r="M5" s="14">
+      <c r="M5" s="12">
         <v>112</v>
       </c>
-      <c r="N5" s="14">
+      <c r="N5" s="12">
         <v>109</v>
       </c>
-      <c r="O5" s="19">
+      <c r="O5" s="17">
         <f t="shared" ref="O5:O19" si="0">SUM(C5:N5)</f>
         <v>326</v>
       </c>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="10">
+      <c r="P5" s="8"/>
+      <c r="Q5" s="9">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>326</v>
       </c>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
     </row>
     <row r="6" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="17">
+      <c r="A6" s="1"/>
+      <c r="B6" s="15">
         <v>2009</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="12">
         <v>210</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="12">
         <v>265</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="12">
         <v>330</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="12">
         <v>459</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="12">
         <v>2711</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="12">
         <v>4347</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="12">
         <v>7134</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="12">
         <v>7452</v>
       </c>
-      <c r="K6" s="14">
+      <c r="K6" s="12">
         <v>10193</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="12">
         <v>11773</v>
       </c>
-      <c r="M6" s="14">
+      <c r="M6" s="12">
         <v>16989</v>
       </c>
-      <c r="N6" s="14">
+      <c r="N6" s="12">
         <v>18516</v>
       </c>
-      <c r="O6" s="19">
+      <c r="O6" s="17">
         <f t="shared" si="0"/>
         <v>80379</v>
       </c>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="10">
+      <c r="P6" s="8"/>
+      <c r="Q6" s="9">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>80379</v>
       </c>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
     </row>
     <row r="7" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="17">
+      <c r="A7" s="1"/>
+      <c r="B7" s="15">
         <v>2010</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="12">
         <v>16660</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="12">
         <v>23673</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="12">
         <v>32985</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="12">
         <v>35222</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="12">
         <v>39909</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="12">
         <v>42087</v>
       </c>
-      <c r="I7" s="14">
+      <c r="I7" s="12">
         <v>54395</v>
       </c>
-      <c r="J7" s="14">
+      <c r="J7" s="12">
         <v>49067</v>
       </c>
-      <c r="K7" s="14">
+      <c r="K7" s="12">
         <v>47658</v>
       </c>
-      <c r="L7" s="14">
+      <c r="L7" s="12">
         <v>38853</v>
       </c>
-      <c r="M7" s="14">
+      <c r="M7" s="12">
         <v>39946</v>
       </c>
-      <c r="N7" s="14">
+      <c r="N7" s="12">
         <v>42658</v>
       </c>
-      <c r="O7" s="19">
+      <c r="O7" s="17">
         <f t="shared" si="0"/>
         <v>463113</v>
       </c>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="10">
+      <c r="P7" s="8"/>
+      <c r="Q7" s="9">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>463113</v>
       </c>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
     </row>
     <row r="8" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="17">
+      <c r="A8" s="1"/>
+      <c r="B8" s="15">
         <v>2011</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="12">
         <v>45551</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="12">
         <v>69346</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="12">
         <v>47856</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="12">
         <v>64728</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="12">
         <v>73308</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="12">
         <v>82846</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8" s="12">
         <v>72286</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="12">
         <v>75867</v>
       </c>
-      <c r="K8" s="14">
+      <c r="K8" s="12">
         <v>80961</v>
       </c>
-      <c r="L8" s="14">
+      <c r="L8" s="12">
         <v>62233</v>
       </c>
-      <c r="M8" s="14">
+      <c r="M8" s="12">
         <v>63447</v>
       </c>
-      <c r="N8" s="14">
+      <c r="N8" s="12">
         <v>64581</v>
       </c>
-      <c r="O8" s="19">
+      <c r="O8" s="17">
         <f t="shared" si="0"/>
         <v>803010</v>
       </c>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="10">
+      <c r="P8" s="8"/>
+      <c r="Q8" s="9">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>803010</v>
       </c>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
     </row>
     <row r="9" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-      <c r="B9" s="17">
+      <c r="A9" s="1"/>
+      <c r="B9" s="15">
         <v>2012</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="12">
         <v>76072</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="12">
         <v>77385</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="12">
         <v>70852</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="12">
         <v>72356</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="12">
         <v>78593</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="12">
         <v>70155</v>
       </c>
-      <c r="I9" s="14">
+      <c r="I9" s="12">
         <v>72470</v>
       </c>
-      <c r="J9" s="14">
+      <c r="J9" s="12">
         <v>70252</v>
       </c>
-      <c r="K9" s="14">
+      <c r="K9" s="12">
         <v>79738</v>
       </c>
-      <c r="L9" s="14">
+      <c r="L9" s="12">
         <v>71284</v>
       </c>
-      <c r="M9" s="14">
+      <c r="M9" s="12">
         <v>76524</v>
       </c>
-      <c r="N9" s="14">
+      <c r="N9" s="12">
         <v>73172</v>
       </c>
-      <c r="O9" s="19">
+      <c r="O9" s="17">
         <f t="shared" si="0"/>
         <v>888853</v>
       </c>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="10">
+      <c r="P9" s="8"/>
+      <c r="Q9" s="9">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>888853</v>
       </c>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
     </row>
     <row r="10" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-      <c r="B10" s="17">
+      <c r="A10" s="1"/>
+      <c r="B10" s="15">
         <v>2013</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="12">
         <v>78648</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="12">
         <v>74894</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="12">
         <v>86029</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="12">
         <v>82489</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="12">
         <v>80316</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="12">
         <v>78764</v>
       </c>
-      <c r="I10" s="14">
+      <c r="I10" s="12">
         <v>70746</v>
       </c>
-      <c r="J10" s="14">
+      <c r="J10" s="12">
         <v>79324</v>
       </c>
-      <c r="K10" s="14">
+      <c r="K10" s="12">
         <v>79148</v>
       </c>
-      <c r="L10" s="14">
+      <c r="L10" s="12">
         <v>76345</v>
       </c>
-      <c r="M10" s="14">
+      <c r="M10" s="12">
         <v>75329</v>
       </c>
-      <c r="N10" s="14">
+      <c r="N10" s="12">
         <v>73625</v>
       </c>
-      <c r="O10" s="19">
+      <c r="O10" s="17">
         <f t="shared" si="0"/>
         <v>935657</v>
       </c>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="10">
+      <c r="P10" s="8"/>
+      <c r="Q10" s="9">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>935657</v>
       </c>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
     </row>
     <row r="11" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-      <c r="B11" s="17">
+      <c r="A11" s="1"/>
+      <c r="B11" s="15">
         <v>2014</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="12">
         <v>67510</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="12">
         <v>67706</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="12">
         <v>73924</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="12">
         <v>71449</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="12">
         <v>79877</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="12">
         <v>74705</v>
       </c>
-      <c r="I11" s="14">
+      <c r="I11" s="12">
         <v>79936</v>
       </c>
-      <c r="J11" s="14">
+      <c r="J11" s="12">
         <v>78746</v>
       </c>
-      <c r="K11" s="14">
+      <c r="K11" s="12">
         <v>77891</v>
       </c>
-      <c r="L11" s="14">
+      <c r="L11" s="12">
         <v>77040</v>
       </c>
-      <c r="M11" s="14">
+      <c r="M11" s="12">
         <v>87951</v>
       </c>
-      <c r="N11" s="15">
+      <c r="N11" s="13">
         <v>101904</v>
       </c>
-      <c r="O11" s="19">
+      <c r="O11" s="17">
         <f t="shared" si="0"/>
         <v>938639</v>
       </c>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="10">
+      <c r="P11" s="8"/>
+      <c r="Q11" s="9">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>938639</v>
       </c>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
     </row>
     <row r="12" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
-      <c r="B12" s="17">
+      <c r="A12" s="1"/>
+      <c r="B12" s="15">
         <v>2015</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="12">
         <v>90536</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="12">
         <v>80976</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="12">
         <v>95444</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="12">
         <v>71951</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="12">
         <v>67019</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="12">
         <v>66244</v>
       </c>
-      <c r="I12" s="14">
+      <c r="I12" s="12">
         <v>86294</v>
       </c>
-      <c r="J12" s="15">
+      <c r="J12" s="13">
         <v>128005</v>
       </c>
-      <c r="K12" s="15">
+      <c r="K12" s="13">
         <v>137300</v>
       </c>
-      <c r="L12" s="15">
+      <c r="L12" s="13">
         <v>138705</v>
       </c>
-      <c r="M12" s="15">
+      <c r="M12" s="13">
         <v>125538</v>
       </c>
-      <c r="N12" s="15">
+      <c r="N12" s="13">
         <v>129945</v>
       </c>
-      <c r="O12" s="19">
+      <c r="O12" s="17">
         <f t="shared" si="0"/>
         <v>1217957</v>
       </c>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="10">
+      <c r="P12" s="8"/>
+      <c r="Q12" s="9">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>1217957</v>
       </c>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
     </row>
     <row r="13" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
-      <c r="B13" s="17">
+      <c r="A13" s="1"/>
+      <c r="B13" s="15">
         <v>2016</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="13">
         <v>142274</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="13">
         <v>123093</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="13">
         <v>147266</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="13">
         <v>152612</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13" s="13">
         <v>134497</v>
       </c>
-      <c r="H13" s="15">
+      <c r="H13" s="13">
         <v>132768</v>
       </c>
-      <c r="I13" s="16">
+      <c r="I13" s="14">
         <v>363723</v>
       </c>
-      <c r="J13" s="16">
+      <c r="J13" s="14">
         <v>702130</v>
       </c>
-      <c r="K13" s="16">
+      <c r="K13" s="14">
         <v>608805</v>
       </c>
-      <c r="L13" s="16">
+      <c r="L13" s="14">
         <v>635500</v>
       </c>
-      <c r="M13" s="16">
+      <c r="M13" s="14">
         <v>713080</v>
       </c>
-      <c r="N13" s="16">
+      <c r="N13" s="14">
         <v>674509</v>
       </c>
-      <c r="O13" s="19">
+      <c r="O13" s="17">
         <f t="shared" si="0"/>
         <v>4530257</v>
       </c>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="10">
+      <c r="P13" s="8"/>
+      <c r="Q13" s="9">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>4530257</v>
       </c>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
     </row>
     <row r="14" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
-      <c r="B14" s="17">
+      <c r="A14" s="1"/>
+      <c r="B14" s="15">
         <v>2017</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="14">
         <v>662423</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="14">
         <v>554842</v>
       </c>
-      <c r="E14" s="16">
+      <c r="E14" s="14">
         <v>657797</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="14">
         <v>673209</v>
       </c>
-      <c r="G14" s="16">
+      <c r="G14" s="14">
         <v>745540</v>
       </c>
-      <c r="H14" s="16">
+      <c r="H14" s="14">
         <v>660058</v>
       </c>
-      <c r="I14" s="16">
+      <c r="I14" s="14">
         <v>690513</v>
       </c>
-      <c r="J14" s="16">
+      <c r="J14" s="14">
         <v>670496</v>
       </c>
-      <c r="K14" s="16">
+      <c r="K14" s="14">
         <v>577595</v>
       </c>
-      <c r="L14" s="16">
+      <c r="L14" s="14">
         <v>665972</v>
       </c>
-      <c r="M14" s="16">
+      <c r="M14" s="14">
         <v>569447</v>
       </c>
-      <c r="N14" s="16">
+      <c r="N14" s="14">
         <v>565361</v>
       </c>
-      <c r="O14" s="19">
+      <c r="O14" s="17">
         <f t="shared" si="0"/>
         <v>7693253</v>
       </c>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="10">
+      <c r="P14" s="8"/>
+      <c r="Q14" s="9">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>7693253</v>
       </c>
-      <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
     </row>
     <row r="15" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
-      <c r="B15" s="17">
+      <c r="A15" s="1"/>
+      <c r="B15" s="15">
         <v>2018</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="14">
         <v>628028</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="14">
         <v>728208</v>
       </c>
-      <c r="E15" s="16">
+      <c r="E15" s="14">
         <v>697376</v>
       </c>
-      <c r="F15" s="16">
+      <c r="F15" s="14">
         <v>707376</v>
       </c>
-      <c r="G15" s="16">
+      <c r="G15" s="14">
         <v>759564</v>
       </c>
-      <c r="H15" s="16">
+      <c r="H15" s="14">
         <v>592381</v>
       </c>
-      <c r="I15" s="16">
+      <c r="I15" s="14">
         <v>545423</v>
       </c>
-      <c r="J15" s="16">
+      <c r="J15" s="14">
         <v>694837</v>
       </c>
-      <c r="K15" s="16">
+      <c r="K15" s="14">
         <v>739656</v>
       </c>
-      <c r="L15" s="16">
+      <c r="L15" s="14">
         <v>763733</v>
       </c>
-      <c r="M15" s="16">
+      <c r="M15" s="14">
         <v>698962</v>
       </c>
-      <c r="N15" s="16">
+      <c r="N15" s="14">
         <v>732173</v>
       </c>
-      <c r="O15" s="19">
+      <c r="O15" s="17">
         <f t="shared" si="0"/>
         <v>8287717</v>
       </c>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="10">
+      <c r="P15" s="8"/>
+      <c r="Q15" s="9">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>8287717</v>
       </c>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
     </row>
     <row r="16" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="2"/>
-      <c r="B16" s="17">
+      <c r="A16" s="1"/>
+      <c r="B16" s="15">
         <v>2019</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="14">
         <v>816792</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="14">
         <v>811807</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="13">
         <v>903678</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="13">
         <v>1174272</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G16" s="13">
         <v>1399881</v>
       </c>
-      <c r="H16" s="15">
+      <c r="H16" s="13">
         <v>1179014</v>
       </c>
-      <c r="I16" s="15">
+      <c r="I16" s="13">
         <v>1380086</v>
       </c>
-      <c r="J16" s="15">
+      <c r="J16" s="13">
         <v>1448886</v>
       </c>
-      <c r="K16" s="15">
+      <c r="K16" s="13">
         <v>1506868</v>
       </c>
-      <c r="L16" s="15">
+      <c r="L16" s="13">
         <v>1761891</v>
       </c>
-      <c r="M16" s="15">
+      <c r="M16" s="13">
         <v>2059856</v>
       </c>
-      <c r="N16" s="15">
+      <c r="N16" s="13">
         <v>2325909</v>
       </c>
-      <c r="O16" s="20">
+      <c r="O16" s="18">
         <f t="shared" si="0"/>
         <v>16768940</v>
       </c>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="10">
+      <c r="P16" s="8"/>
+      <c r="Q16" s="9">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>16768940</v>
       </c>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
     </row>
     <row r="17" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="2"/>
-      <c r="B17" s="17">
+      <c r="A17" s="1"/>
+      <c r="B17" s="15">
         <v>2020</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17" s="13">
         <v>1694534</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="13">
         <v>3203938</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="13">
         <v>3296329</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="13">
         <v>2694570</v>
       </c>
-      <c r="G17" s="15">
+      <c r="G17" s="13">
         <v>2511957</v>
       </c>
-      <c r="H17" s="15">
+      <c r="H17" s="13">
         <v>2264236</v>
       </c>
-      <c r="I17" s="15">
+      <c r="I17" s="13">
         <v>1255353</v>
       </c>
-      <c r="J17" s="15">
+      <c r="J17" s="13">
         <v>1205188</v>
       </c>
-      <c r="K17" s="15">
+      <c r="K17" s="13">
         <v>1622473</v>
       </c>
-      <c r="L17" s="15">
+      <c r="L17" s="13">
         <v>1912285</v>
       </c>
-      <c r="M17" s="15">
+      <c r="M17" s="13">
         <v>2366693</v>
       </c>
-      <c r="N17" s="15">
+      <c r="N17" s="13">
         <v>2176841</v>
       </c>
-      <c r="O17" s="21">
+      <c r="O17" s="19">
         <f t="shared" si="0"/>
         <v>26204397</v>
       </c>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="10">
+      <c r="P17" s="8"/>
+      <c r="Q17" s="9">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>26204397</v>
       </c>
-      <c r="R17" s="2"/>
-      <c r="S17" s="2"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
     </row>
     <row r="18" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="2"/>
-      <c r="B18" s="17">
+      <c r="A18" s="1"/>
+      <c r="B18" s="15">
         <v>2021</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="13">
         <v>924261</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="13">
         <v>1235225</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="13">
         <v>2047206</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="13">
         <v>2337103</v>
       </c>
-      <c r="G18" s="15">
+      <c r="G18" s="13">
         <v>2440903</v>
       </c>
-      <c r="H18" s="15">
+      <c r="H18" s="13">
         <v>2432014</v>
       </c>
-      <c r="I18" s="15">
+      <c r="I18" s="13">
         <v>2631617</v>
       </c>
-      <c r="J18" s="15">
+      <c r="J18" s="13">
         <v>2238361</v>
       </c>
-      <c r="K18" s="15">
+      <c r="K18" s="13">
         <v>3054555</v>
       </c>
-      <c r="L18" s="15">
+      <c r="L18" s="13">
         <v>2855764</v>
       </c>
-      <c r="M18" s="15">
+      <c r="M18" s="13">
         <v>3465933</v>
       </c>
-      <c r="N18" s="15">
+      <c r="N18" s="13">
         <v>4145700</v>
       </c>
-      <c r="O18" s="21">
+      <c r="O18" s="19">
         <f t="shared" si="0"/>
         <v>29808642</v>
       </c>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="10">
+      <c r="P18" s="8"/>
+      <c r="Q18" s="9">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>29808642</v>
       </c>
-      <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
     </row>
     <row r="19" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="2"/>
-      <c r="B19" s="17">
+      <c r="A19" s="1"/>
+      <c r="B19" s="15">
         <v>2022</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="13">
         <v>4297072</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="13">
         <v>2442144</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="13">
         <v>2336228</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F19" s="13">
         <v>2718163</v>
       </c>
-      <c r="G19" s="15">
+      <c r="G19" s="13">
         <v>2097535</v>
       </c>
-      <c r="H19" s="15">
+      <c r="H19" s="13">
         <v>2895282</v>
       </c>
-      <c r="I19" s="15">
+      <c r="I19" s="13">
         <v>2891642</v>
       </c>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="21">
+      <c r="J19" s="13">
+        <v>3141889</v>
+      </c>
+      <c r="K19" s="13">
+        <v>3181844</v>
+      </c>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="19">
         <f t="shared" si="0"/>
-        <v>19678066</v>
-      </c>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="10" t="e">
+        <v>26001799</v>
+      </c>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="9" t="e">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="R19" s="2"/>
-      <c r="S19" s="2"/>
-    </row>
-    <row r="20" spans="1:19" s="8" customFormat="1" ht="58.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="23"/>
-      <c r="O20" s="22">
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+    </row>
+    <row r="20" spans="1:19" s="7" customFormat="1" ht="58.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="20">
         <f>SUM(O5:O19)</f>
-        <v>118299206</v>
-      </c>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
+        <v>124622939</v>
+      </c>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
     </row>
     <row r="21" spans="1:19" ht="26.85" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
-    </row>
-    <row r="22" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
-      <c r="O22" s="12"/>
-    </row>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+    </row>
+    <row r="22" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A23" s="2"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="2"/>
-      <c r="R23" s="2"/>
-      <c r="S23" s="2"/>
+      <c r="A23" s="1"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
-      <c r="Q24" s="2"/>
-      <c r="R24" s="2"/>
-      <c r="S24" s="2"/>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
-      <c r="Q25" s="2"/>
-      <c r="R25" s="2"/>
-      <c r="S25" s="2"/>
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
-      <c r="Q26" s="2"/>
-      <c r="R26" s="2"/>
-      <c r="S26" s="2"/>
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
-      <c r="P27" s="2"/>
-      <c r="Q27" s="2"/>
-      <c r="R27" s="2"/>
-      <c r="S27" s="2"/>
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
-      <c r="O28" s="2"/>
-      <c r="P28" s="2"/>
-      <c r="Q28" s="2"/>
-      <c r="R28" s="2"/>
-      <c r="S28" s="2"/>
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
-      <c r="Q29" s="2"/>
-      <c r="R29" s="2"/>
-      <c r="S29" s="2"/>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
-      <c r="P30" s="2"/>
-      <c r="Q30" s="2"/>
-      <c r="R30" s="2"/>
-      <c r="S30" s="2"/>
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
-      <c r="Q31" s="2"/>
-      <c r="R31" s="2"/>
-      <c r="S31" s="2"/>
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
-      <c r="P32" s="2"/>
-      <c r="Q32" s="2"/>
-      <c r="R32" s="2"/>
-      <c r="S32" s="2"/>
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" s="2"/>
-      <c r="P33" s="2"/>
-      <c r="Q33" s="2"/>
-      <c r="R33" s="2"/>
-      <c r="S33" s="2"/>
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-      <c r="O34" s="2"/>
-      <c r="P34" s="2"/>
-      <c r="Q34" s="2"/>
-      <c r="R34" s="2"/>
-      <c r="S34" s="2"/>
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
-      <c r="O35" s="2"/>
-      <c r="P35" s="2"/>
-      <c r="Q35" s="2"/>
-      <c r="R35" s="2"/>
-      <c r="S35" s="2"/>
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+      <c r="S35" s="1"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
-      <c r="O36" s="2"/>
-      <c r="P36" s="2"/>
-      <c r="Q36" s="2"/>
-      <c r="R36" s="2"/>
-      <c r="S36" s="2"/>
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
+      <c r="S36" s="1"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
-      <c r="O37" s="2"/>
-      <c r="P37" s="2"/>
-      <c r="Q37" s="2"/>
-      <c r="R37" s="2"/>
-      <c r="S37" s="2"/>
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+      <c r="S37" s="1"/>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
-      <c r="O38" s="2"/>
-      <c r="P38" s="2"/>
-      <c r="Q38" s="2"/>
-      <c r="R38" s="2"/>
-      <c r="S38" s="2"/>
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
-      <c r="O39" s="2"/>
-      <c r="P39" s="2"/>
-      <c r="Q39" s="2"/>
-      <c r="R39" s="2"/>
-      <c r="S39" s="2"/>
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
-      <c r="O40" s="2"/>
-      <c r="P40" s="2"/>
-      <c r="Q40" s="2"/>
-      <c r="R40" s="2"/>
-      <c r="S40" s="2"/>
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
+      <c r="R40" s="1"/>
+      <c r="S40" s="1"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
-      <c r="O41" s="2"/>
-      <c r="P41" s="2"/>
-      <c r="Q41" s="2"/>
-      <c r="R41" s="2"/>
-      <c r="S41" s="2"/>
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="1"/>
+      <c r="S41" s="1"/>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
-      <c r="N42" s="2"/>
-      <c r="O42" s="2"/>
-      <c r="P42" s="2"/>
-      <c r="Q42" s="2"/>
-      <c r="R42" s="2"/>
-      <c r="S42" s="2"/>
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="1"/>
+      <c r="R42" s="1"/>
+      <c r="S42" s="1"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
-      <c r="N43" s="2"/>
-      <c r="O43" s="2"/>
-      <c r="P43" s="2"/>
-      <c r="Q43" s="2"/>
-      <c r="R43" s="2"/>
-      <c r="S43" s="2"/>
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="1"/>
+      <c r="P43" s="1"/>
+      <c r="Q43" s="1"/>
+      <c r="R43" s="1"/>
+      <c r="S43" s="1"/>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
-      <c r="L44" s="2"/>
-      <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
-      <c r="O44" s="2"/>
-      <c r="P44" s="2"/>
-      <c r="Q44" s="2"/>
-      <c r="R44" s="2"/>
-      <c r="S44" s="2"/>
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+      <c r="R44" s="1"/>
+      <c r="S44" s="1"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
-      <c r="L45" s="2"/>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
-      <c r="O45" s="2"/>
-      <c r="P45" s="2"/>
-      <c r="Q45" s="2"/>
-      <c r="R45" s="2"/>
-      <c r="S45" s="2"/>
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="1"/>
+      <c r="R45" s="1"/>
+      <c r="S45" s="1"/>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
-      <c r="N46" s="2"/>
-      <c r="O46" s="2"/>
-      <c r="P46" s="2"/>
-      <c r="Q46" s="2"/>
-      <c r="R46" s="2"/>
-      <c r="S46" s="2"/>
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
+      <c r="Q46" s="1"/>
+      <c r="R46" s="1"/>
+      <c r="S46" s="1"/>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-      <c r="K47" s="2"/>
-      <c r="L47" s="2"/>
-      <c r="M47" s="2"/>
-      <c r="N47" s="2"/>
-      <c r="O47" s="2"/>
-      <c r="P47" s="2"/>
-      <c r="Q47" s="2"/>
-      <c r="R47" s="2"/>
-      <c r="S47" s="2"/>
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="1"/>
+      <c r="R47" s="1"/>
+      <c r="S47" s="1"/>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
-      <c r="K48" s="2"/>
-      <c r="L48" s="2"/>
-      <c r="M48" s="2"/>
-      <c r="N48" s="2"/>
-      <c r="O48" s="2"/>
-      <c r="P48" s="2"/>
-      <c r="Q48" s="2"/>
-      <c r="R48" s="2"/>
-      <c r="S48" s="2"/>
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="1"/>
+      <c r="S48" s="1"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
-      <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
-      <c r="O49" s="2"/>
-      <c r="P49" s="2"/>
-      <c r="Q49" s="2"/>
-      <c r="R49" s="2"/>
-      <c r="S49" s="2"/>
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
+      <c r="P49" s="1"/>
+      <c r="Q49" s="1"/>
+      <c r="R49" s="1"/>
+      <c r="S49" s="1"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
-      <c r="K50" s="2"/>
-      <c r="L50" s="2"/>
-      <c r="M50" s="2"/>
-      <c r="N50" s="2"/>
-      <c r="O50" s="2"/>
-      <c r="P50" s="2"/>
-      <c r="Q50" s="2"/>
-      <c r="R50" s="2"/>
-      <c r="S50" s="2"/>
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1"/>
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
+      <c r="Q50" s="1"/>
+      <c r="R50" s="1"/>
+      <c r="S50" s="1"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
-      <c r="J51" s="26"/>
-      <c r="K51" s="26"/>
-      <c r="L51" s="26"/>
-      <c r="M51" s="2"/>
-      <c r="N51" s="2"/>
-      <c r="O51" s="2"/>
-      <c r="P51" s="2"/>
-      <c r="Q51" s="2"/>
-      <c r="R51" s="2"/>
-      <c r="S51" s="2"/>
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="24"/>
+      <c r="K51" s="24"/>
+      <c r="L51" s="24"/>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+      <c r="O51" s="1"/>
+      <c r="P51" s="1"/>
+      <c r="Q51" s="1"/>
+      <c r="R51" s="1"/>
+      <c r="S51" s="1"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A52" s="12"/>
-      <c r="B52" s="12"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
-      <c r="F52" s="12"/>
-      <c r="G52" s="12"/>
-      <c r="H52" s="12"/>
-      <c r="I52" s="12"/>
-      <c r="J52" s="12"/>
-      <c r="K52" s="12"/>
-      <c r="L52" s="13"/>
-      <c r="M52" s="12"/>
-      <c r="N52" s="12"/>
-      <c r="O52" s="12"/>
-      <c r="P52" s="12"/>
-      <c r="Q52" s="12"/>
-      <c r="R52" s="12"/>
-      <c r="S52" s="12"/>
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="11"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="1"/>
+      <c r="P52" s="1"/>
+      <c r="Q52" s="1"/>
+      <c r="R52" s="1"/>
+      <c r="S52" s="1"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A53" s="12"/>
-      <c r="B53" s="12"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="12"/>
-      <c r="G53" s="12"/>
-      <c r="H53" s="12"/>
-      <c r="I53" s="12"/>
-      <c r="J53" s="12"/>
-      <c r="K53" s="12"/>
-      <c r="L53" s="12"/>
-      <c r="M53" s="12"/>
-      <c r="N53" s="12"/>
-      <c r="O53" s="12"/>
-      <c r="P53" s="12"/>
-      <c r="Q53" s="12"/>
-      <c r="R53" s="12"/>
-      <c r="S53" s="12"/>
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+      <c r="O53" s="1"/>
+      <c r="P53" s="1"/>
+      <c r="Q53" s="1"/>
+      <c r="R53" s="1"/>
+      <c r="S53" s="1"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A54" s="12"/>
-      <c r="B54" s="12"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-      <c r="G54" s="12"/>
-      <c r="H54" s="12"/>
-      <c r="I54" s="12"/>
-      <c r="J54" s="12"/>
-      <c r="K54" s="12"/>
-      <c r="L54" s="12"/>
-      <c r="M54" s="12"/>
-      <c r="N54" s="12"/>
-      <c r="O54" s="12"/>
-      <c r="P54" s="12"/>
-      <c r="Q54" s="12"/>
-      <c r="R54" s="12"/>
-      <c r="S54" s="12"/>
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
+      <c r="Q54" s="1"/>
+      <c r="R54" s="1"/>
+      <c r="S54" s="1"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A55" s="12"/>
-      <c r="B55" s="12"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
-      <c r="G55" s="12"/>
-      <c r="H55" s="12"/>
-      <c r="I55" s="12"/>
-      <c r="J55" s="12"/>
-      <c r="K55" s="12"/>
-      <c r="L55" s="12"/>
-      <c r="M55" s="12"/>
-      <c r="N55" s="12"/>
-      <c r="O55" s="12"/>
-      <c r="P55" s="12"/>
-      <c r="Q55" s="12"/>
-      <c r="R55" s="12"/>
-      <c r="S55" s="12"/>
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+      <c r="L55" s="1"/>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+      <c r="O55" s="1"/>
+      <c r="P55" s="1"/>
+      <c r="Q55" s="1"/>
+      <c r="R55" s="1"/>
+      <c r="S55" s="1"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A56" s="12"/>
-      <c r="B56" s="12"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
-      <c r="G56" s="12"/>
-      <c r="H56" s="12"/>
-      <c r="I56" s="12"/>
-      <c r="J56" s="12"/>
-      <c r="K56" s="12"/>
-      <c r="L56" s="12"/>
-      <c r="M56" s="12"/>
-      <c r="N56" s="12"/>
-      <c r="O56" s="12"/>
-      <c r="P56" s="12"/>
-      <c r="Q56" s="12"/>
-      <c r="R56" s="12"/>
-      <c r="S56" s="12"/>
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
+      <c r="P56" s="1"/>
+      <c r="Q56" s="1"/>
+      <c r="R56" s="1"/>
+      <c r="S56" s="1"/>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A57" s="12"/>
-      <c r="B57" s="12"/>
-      <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="12"/>
-      <c r="F57" s="12"/>
-      <c r="G57" s="12"/>
-      <c r="H57" s="12"/>
-      <c r="I57" s="12"/>
-      <c r="J57" s="12"/>
-      <c r="K57" s="12"/>
-      <c r="L57" s="12"/>
-      <c r="M57" s="12"/>
-      <c r="N57" s="12"/>
-      <c r="O57" s="12"/>
-      <c r="P57" s="12"/>
-      <c r="Q57" s="12"/>
-      <c r="R57" s="12"/>
-      <c r="S57" s="12"/>
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="1"/>
+      <c r="P57" s="1"/>
+      <c r="Q57" s="1"/>
+      <c r="R57" s="1"/>
+      <c r="S57" s="1"/>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A58" s="12"/>
-      <c r="B58" s="12"/>
-      <c r="C58" s="12"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="12"/>
-      <c r="F58" s="12"/>
-      <c r="G58" s="12"/>
-      <c r="H58" s="12"/>
-      <c r="I58" s="12"/>
-      <c r="J58" s="12"/>
-      <c r="K58" s="12"/>
-      <c r="L58" s="12"/>
-      <c r="M58" s="12"/>
-      <c r="N58" s="12"/>
-      <c r="O58" s="12"/>
-      <c r="P58" s="12"/>
-      <c r="Q58" s="12"/>
-      <c r="R58" s="12"/>
-      <c r="S58" s="12"/>
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="O58" s="1"/>
+      <c r="P58" s="1"/>
+      <c r="Q58" s="1"/>
+      <c r="R58" s="1"/>
+      <c r="S58" s="1"/>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A59" s="12"/>
-      <c r="B59" s="12"/>
-      <c r="C59" s="12"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12"/>
-      <c r="G59" s="12"/>
-      <c r="H59" s="12"/>
-      <c r="I59" s="12"/>
-      <c r="J59" s="12"/>
-      <c r="K59" s="12"/>
-      <c r="L59" s="12"/>
-      <c r="M59" s="12"/>
-      <c r="N59" s="12"/>
-      <c r="O59" s="12"/>
-      <c r="P59" s="12"/>
-      <c r="Q59" s="12"/>
-      <c r="R59" s="12"/>
-      <c r="S59" s="12"/>
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
+      <c r="O59" s="1"/>
+      <c r="P59" s="1"/>
+      <c r="Q59" s="1"/>
+      <c r="R59" s="1"/>
+      <c r="S59" s="1"/>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A60" s="12"/>
-      <c r="B60" s="12"/>
-      <c r="C60" s="12"/>
-      <c r="D60" s="12"/>
-      <c r="E60" s="12"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="12"/>
-      <c r="H60" s="12"/>
-      <c r="I60" s="12"/>
-      <c r="J60" s="12"/>
-      <c r="K60" s="12"/>
-      <c r="L60" s="12"/>
-      <c r="M60" s="12"/>
-      <c r="N60" s="12"/>
-      <c r="O60" s="12"/>
-      <c r="P60" s="12"/>
-      <c r="Q60" s="12"/>
-      <c r="R60" s="12"/>
-      <c r="S60" s="12"/>
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+      <c r="P60" s="1"/>
+      <c r="Q60" s="1"/>
+      <c r="R60" s="1"/>
+      <c r="S60" s="1"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A61" s="12"/>
-      <c r="B61" s="12"/>
-      <c r="C61" s="12"/>
-      <c r="D61" s="12"/>
-      <c r="E61" s="12"/>
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
-      <c r="H61" s="12"/>
-      <c r="I61" s="12"/>
-      <c r="J61" s="12"/>
-      <c r="K61" s="12"/>
-      <c r="L61" s="12"/>
-      <c r="M61" s="12"/>
-      <c r="N61" s="12"/>
-      <c r="O61" s="12"/>
-      <c r="P61" s="12"/>
-      <c r="Q61" s="12"/>
-      <c r="R61" s="12"/>
-      <c r="S61" s="12"/>
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="1"/>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
+      <c r="O61" s="1"/>
+      <c r="P61" s="1"/>
+      <c r="Q61" s="1"/>
+      <c r="R61" s="1"/>
+      <c r="S61" s="1"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A62" s="12"/>
-      <c r="B62" s="12"/>
-      <c r="C62" s="12"/>
-      <c r="D62" s="12"/>
-      <c r="E62" s="12"/>
-      <c r="F62" s="12"/>
-      <c r="G62" s="12"/>
-      <c r="H62" s="12"/>
-      <c r="I62" s="12"/>
-      <c r="J62" s="12"/>
-      <c r="K62" s="12"/>
-      <c r="L62" s="12"/>
-      <c r="M62" s="12"/>
-      <c r="N62" s="12"/>
-      <c r="O62" s="12"/>
-      <c r="P62" s="12"/>
-      <c r="Q62" s="12"/>
-      <c r="R62" s="12"/>
-      <c r="S62" s="12"/>
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="1"/>
+      <c r="M62" s="1"/>
+      <c r="N62" s="1"/>
+      <c r="O62" s="1"/>
+      <c r="P62" s="1"/>
+      <c r="Q62" s="1"/>
+      <c r="R62" s="1"/>
+      <c r="S62" s="1"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A63" s="12"/>
-      <c r="B63" s="12"/>
-      <c r="C63" s="12"/>
-      <c r="D63" s="12"/>
-      <c r="E63" s="12"/>
-      <c r="F63" s="12"/>
-      <c r="G63" s="12"/>
-      <c r="H63" s="12"/>
-      <c r="I63" s="12"/>
-      <c r="J63" s="12"/>
-      <c r="K63" s="12"/>
-      <c r="L63" s="12"/>
-      <c r="M63" s="12"/>
-      <c r="N63" s="12"/>
-      <c r="O63" s="12"/>
-      <c r="P63" s="12"/>
-      <c r="Q63" s="12"/>
-      <c r="R63" s="12"/>
-      <c r="S63" s="12"/>
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1"/>
+      <c r="M63" s="1"/>
+      <c r="N63" s="1"/>
+      <c r="O63" s="1"/>
+      <c r="P63" s="1"/>
+      <c r="Q63" s="1"/>
+      <c r="R63" s="1"/>
+      <c r="S63" s="1"/>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A64" s="12"/>
-      <c r="B64" s="12"/>
-      <c r="C64" s="12"/>
-      <c r="D64" s="12"/>
-      <c r="E64" s="12"/>
-      <c r="F64" s="12"/>
-      <c r="G64" s="12"/>
-      <c r="H64" s="12"/>
-      <c r="I64" s="12"/>
-      <c r="J64" s="12"/>
-      <c r="K64" s="12"/>
-      <c r="L64" s="12"/>
-      <c r="M64" s="12"/>
-      <c r="N64" s="12"/>
-      <c r="O64" s="12"/>
-      <c r="P64" s="12"/>
-      <c r="Q64" s="12"/>
-      <c r="R64" s="12"/>
-      <c r="S64" s="12"/>
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="1"/>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+      <c r="O64" s="1"/>
+      <c r="P64" s="1"/>
+      <c r="Q64" s="1"/>
+      <c r="R64" s="1"/>
+      <c r="S64" s="1"/>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A65" s="12"/>
-      <c r="B65" s="12"/>
-      <c r="C65" s="12"/>
-      <c r="D65" s="12"/>
-      <c r="E65" s="12"/>
-      <c r="F65" s="12"/>
-      <c r="G65" s="12"/>
-      <c r="H65" s="12"/>
-      <c r="I65" s="12"/>
-      <c r="J65" s="12"/>
-      <c r="K65" s="12"/>
-      <c r="L65" s="12"/>
-      <c r="M65" s="12"/>
-      <c r="N65" s="12"/>
-      <c r="O65" s="12"/>
-      <c r="P65" s="12"/>
-      <c r="Q65" s="12"/>
-      <c r="R65" s="12"/>
-      <c r="S65" s="12"/>
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="1"/>
+      <c r="M65" s="1"/>
+      <c r="N65" s="1"/>
+      <c r="O65" s="1"/>
+      <c r="P65" s="1"/>
+      <c r="Q65" s="1"/>
+      <c r="R65" s="1"/>
+      <c r="S65" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Site Statistics (October 2022)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c93c05515dfe04a/GIT Hub/kunal-chowdhury.com/blog-stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="11_91C7ACB7C03E7306CE517BDFACF66E9FD99B01DC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C8A356A-88AD-4C92-9BFA-29E086DFD420}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="11_91C7ACB7C03E7306CE517BDFACF66E9FD99B01DC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57632288-9E18-4B14-BC4F-7E5759233B21}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4" calcCompleted="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -720,7 +720,7 @@
                   <c:v>29808642</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>26001799</c:v>
+                  <c:v>29092685</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1271,8 +1271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1425,7 +1425,7 @@
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
     </row>
-    <row r="5" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="15">
         <v>2008</v>
@@ -1478,7 +1478,7 @@
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
     </row>
-    <row r="6" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="15">
         <v>2009</v>
@@ -1531,7 +1531,7 @@
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
     </row>
-    <row r="7" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="15">
         <v>2010</v>
@@ -1584,7 +1584,7 @@
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
     </row>
-    <row r="8" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="15">
         <v>2011</v>
@@ -1637,7 +1637,7 @@
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
     </row>
-    <row r="9" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="15">
         <v>2012</v>
@@ -1690,7 +1690,7 @@
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
     </row>
-    <row r="10" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="15">
         <v>2013</v>
@@ -1743,7 +1743,7 @@
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
     </row>
-    <row r="11" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="15">
         <v>2014</v>
@@ -1796,7 +1796,7 @@
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
     </row>
-    <row r="12" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="15">
         <v>2015</v>
@@ -1849,7 +1849,7 @@
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
     </row>
-    <row r="13" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="15">
         <v>2016</v>
@@ -1902,7 +1902,7 @@
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
     </row>
-    <row r="14" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="15">
         <v>2017</v>
@@ -1955,7 +1955,7 @@
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
     </row>
-    <row r="15" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="15">
         <v>2018</v>
@@ -2008,7 +2008,7 @@
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
     </row>
-    <row r="16" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="15">
         <v>2019</v>
@@ -2061,7 +2061,7 @@
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
     </row>
-    <row r="17" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="15">
         <v>2020</v>
@@ -2114,7 +2114,7 @@
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
     </row>
-    <row r="18" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="15">
         <v>2021</v>
@@ -2167,7 +2167,7 @@
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
     </row>
-    <row r="19" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="15">
         <v>2022</v>
@@ -2199,12 +2199,14 @@
       <c r="K19" s="13">
         <v>3181844</v>
       </c>
-      <c r="L19" s="13"/>
+      <c r="L19" s="13">
+        <v>3090886</v>
+      </c>
       <c r="M19" s="13"/>
       <c r="N19" s="13"/>
       <c r="O19" s="19">
         <f t="shared" si="0"/>
-        <v>26001799</v>
+        <v>29092685</v>
       </c>
       <c r="P19" s="8"/>
       <c r="Q19" s="9" t="e">
@@ -2231,7 +2233,7 @@
       <c r="N20" s="21"/>
       <c r="O20" s="20">
         <f>SUM(O5:O19)</f>
-        <v>124622939</v>
+        <v>127713825</v>
       </c>
       <c r="P20" s="5"/>
       <c r="Q20" s="3"/>

</xml_diff>

<commit_message>
Blog Statistics [November 2022]
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c93c05515dfe04a/GIT Hub/kunal-chowdhury.com/blog-stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="11_91C7ACB7C03E7306CE517BDFACF66E9FD99B01DC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57632288-9E18-4B14-BC4F-7E5759233B21}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="11_91C7ACB7C03E7306CE517BDFACF66E9FD99B01DC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFB00C5F-5152-48BC-8E4B-5137F78F8B97}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4" calcCompleted="0"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -720,7 +720,7 @@
                   <c:v>29808642</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>29092685</c:v>
+                  <c:v>32424496</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -945,6 +945,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1271,8 +1275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2202,11 +2206,13 @@
       <c r="L19" s="13">
         <v>3090886</v>
       </c>
-      <c r="M19" s="13"/>
+      <c r="M19" s="13">
+        <v>3331811</v>
+      </c>
       <c r="N19" s="13"/>
       <c r="O19" s="19">
         <f t="shared" si="0"/>
-        <v>29092685</v>
+        <v>32424496</v>
       </c>
       <c r="P19" s="8"/>
       <c r="Q19" s="9" t="e">
@@ -2233,7 +2239,7 @@
       <c r="N20" s="21"/>
       <c r="O20" s="20">
         <f>SUM(O5:O19)</f>
-        <v>127713825</v>
+        <v>131045636</v>
       </c>
       <c r="P20" s="5"/>
       <c r="Q20" s="3"/>

</xml_diff>

<commit_message>
Blog Statistics (December 2022)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c93c05515dfe04a/GIT Hub/kunal-chowdhury.com/blog-stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="11_91C7ACB7C03E7306CE517BDFACF66E9FD99B01DC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFB00C5F-5152-48BC-8E4B-5137F78F8B97}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="11_91C7ACB7C03E7306CE517BDFACF66E9FD99B01DC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{162562B7-89C1-4AE8-9F70-5106F578BE5F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -720,7 +720,7 @@
                   <c:v>29808642</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>32424496</c:v>
+                  <c:v>35470785</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -888,60 +888,6 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>163286</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>149679</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{175D568E-9D4C-E530-0060-57FF456C02F6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="15865929" y="9824357"/>
-          <a:ext cx="27214" cy="2530929"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="76200">
-          <a:prstDash val="lgDash"/>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1275,8 +1221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:N20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2209,10 +2155,12 @@
       <c r="M19" s="13">
         <v>3331811</v>
       </c>
-      <c r="N19" s="13"/>
+      <c r="N19" s="13">
+        <v>3046289</v>
+      </c>
       <c r="O19" s="19">
         <f t="shared" si="0"/>
-        <v>32424496</v>
+        <v>35470785</v>
       </c>
       <c r="P19" s="8"/>
       <c r="Q19" s="9" t="e">
@@ -2239,7 +2187,7 @@
       <c r="N20" s="21"/>
       <c r="O20" s="20">
         <f>SUM(O5:O19)</f>
-        <v>131045636</v>
+        <v>134091925</v>
       </c>
       <c r="P20" s="5"/>
       <c r="Q20" s="3"/>

</xml_diff>

<commit_message>
Blog Statistics [March 2023]
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c93c05515dfe04a/GIT Hub/kunal-chowdhury.com/blog-stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="11_91C7ACB7C03E7306CE517BDFACF66E9FD99B01DC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{162562B7-89C1-4AE8-9F70-5106F578BE5F}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="11_91C7ACB7C03E7306CE517BDFACF66E9FD99B01DC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65024B92-3269-45BA-99DD-F2CE7E6A66C0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -312,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -373,6 +372,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -522,9 +524,9 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$5:$B$19</c:f>
+              <c:f>Sheet1!$B$5:$B$20</c:f>
               <c:strCache>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>2008</c:v>
                 </c:pt>
@@ -569,6 +571,9 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2023</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -619,10 +624,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$19</c:f>
+              <c:f>Sheet1!$B$5:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>2008</c:v>
                 </c:pt>
@@ -667,16 +672,19 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2023</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$5:$O$19</c:f>
+              <c:f>Sheet1!$O$5:$O$20</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>326</c:v>
                 </c:pt>
@@ -721,6 +729,9 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>35470785</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6760294</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -858,13 +869,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>641160</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>27213</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>754771</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>172439</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -890,10 +901,68 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A598D6B-6862-CAAE-519F-E5ABCB42FA48}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="16306800" y="13277850"/>
+          <a:ext cx="0" cy="4781550"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:prstDash val="dashDot"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -1219,23 +1288,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S65"/>
+  <dimension ref="A1:S66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="W18" sqref="W18"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="14" width="26.28515625" customWidth="1"/>
-    <col min="15" max="15" width="32.28515625" customWidth="1"/>
-    <col min="16" max="16" width="5.42578125" customWidth="1"/>
-    <col min="17" max="17" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="14" width="26.33203125" customWidth="1"/>
+    <col min="15" max="15" width="32.33203125" customWidth="1"/>
+    <col min="16" max="16" width="5.44140625" customWidth="1"/>
+    <col min="17" max="17" width="25.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1256,7 +1325,7 @@
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1277,7 +1346,7 @@
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
         <v>0</v>
@@ -1328,7 +1397,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="7" customFormat="1" ht="104.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:19" s="7" customFormat="1" ht="104.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="16" t="s">
@@ -1375,7 +1444,7 @@
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
     </row>
-    <row r="5" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
       <c r="B5" s="15">
         <v>2008</v>
@@ -1428,7 +1497,7 @@
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
     </row>
-    <row r="6" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="B6" s="15">
         <v>2009</v>
@@ -1481,7 +1550,7 @@
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
     </row>
-    <row r="7" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
       <c r="B7" s="15">
         <v>2010</v>
@@ -1534,7 +1603,7 @@
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
     </row>
-    <row r="8" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
       <c r="B8" s="15">
         <v>2011</v>
@@ -1587,7 +1656,7 @@
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
     </row>
-    <row r="9" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
       <c r="B9" s="15">
         <v>2012</v>
@@ -1640,7 +1709,7 @@
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
     </row>
-    <row r="10" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
       <c r="B10" s="15">
         <v>2013</v>
@@ -1693,7 +1762,7 @@
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
     </row>
-    <row r="11" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="1"/>
       <c r="B11" s="15">
         <v>2014</v>
@@ -1746,7 +1815,7 @@
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
     </row>
-    <row r="12" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
       <c r="B12" s="15">
         <v>2015</v>
@@ -1799,7 +1868,7 @@
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
     </row>
-    <row r="13" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
       <c r="B13" s="15">
         <v>2016</v>
@@ -1852,7 +1921,7 @@
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
     </row>
-    <row r="14" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
       <c r="B14" s="15">
         <v>2017</v>
@@ -1905,7 +1974,7 @@
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
     </row>
-    <row r="15" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
       <c r="B15" s="15">
         <v>2018</v>
@@ -1958,7 +2027,7 @@
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
     </row>
-    <row r="16" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="1"/>
       <c r="B16" s="15">
         <v>2019</v>
@@ -2011,7 +2080,7 @@
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
     </row>
-    <row r="17" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
       <c r="B17" s="15">
         <v>2020</v>
@@ -2064,7 +2133,7 @@
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
     </row>
-    <row r="18" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="1"/>
       <c r="B18" s="15">
         <v>2021</v>
@@ -2117,7 +2186,7 @@
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
     </row>
-    <row r="19" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="1"/>
       <c r="B19" s="15">
         <v>2022</v>
@@ -2170,80 +2239,91 @@
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
     </row>
-    <row r="20" spans="1:19" s="7" customFormat="1" ht="58.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="21"/>
-      <c r="O20" s="20">
-        <f>SUM(O5:O19)</f>
-        <v>134091925</v>
-      </c>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
-    </row>
-    <row r="21" spans="1:19" ht="26.85" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="8"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
-    </row>
-    <row r="22" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A23" s="1"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="1"/>
+      <c r="B20" s="15">
+        <v>2023</v>
+      </c>
+      <c r="C20" s="25">
+        <v>2746994</v>
+      </c>
+      <c r="D20" s="25">
+        <v>2114174</v>
+      </c>
+      <c r="E20" s="25">
+        <v>1899126</v>
+      </c>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="25"/>
+      <c r="N20" s="25"/>
+      <c r="O20" s="19">
+        <f>SUM(C20:N20)</f>
+        <v>6760294</v>
+      </c>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+    </row>
+    <row r="21" spans="1:19" s="7" customFormat="1" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="21"/>
+      <c r="O21" s="20">
+        <f>SUM(O5:O20)</f>
+        <v>140852219</v>
+      </c>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+    </row>
+    <row r="22" spans="1:19" ht="26.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+    </row>
+    <row r="23" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:19" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -2257,7 +2337,7 @@
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2278,7 +2358,7 @@
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2299,7 +2379,7 @@
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -2320,7 +2400,7 @@
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -2341,7 +2421,7 @@
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -2362,7 +2442,7 @@
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2383,7 +2463,7 @@
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -2404,7 +2484,7 @@
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -2425,7 +2505,7 @@
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2446,7 +2526,7 @@
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -2467,7 +2547,7 @@
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -2488,7 +2568,7 @@
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -2509,7 +2589,7 @@
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -2530,7 +2610,7 @@
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2551,7 +2631,7 @@
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -2572,7 +2652,7 @@
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2593,7 +2673,7 @@
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -2614,7 +2694,7 @@
       <c r="R41" s="1"/>
       <c r="S41" s="1"/>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -2635,7 +2715,7 @@
       <c r="R42" s="1"/>
       <c r="S42" s="1"/>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -2656,7 +2736,7 @@
       <c r="R43" s="1"/>
       <c r="S43" s="1"/>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -2677,7 +2757,7 @@
       <c r="R44" s="1"/>
       <c r="S44" s="1"/>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -2698,7 +2778,7 @@
       <c r="R45" s="1"/>
       <c r="S45" s="1"/>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -2719,7 +2799,7 @@
       <c r="R46" s="1"/>
       <c r="S46" s="1"/>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -2740,7 +2820,7 @@
       <c r="R47" s="1"/>
       <c r="S47" s="1"/>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -2761,7 +2841,7 @@
       <c r="R48" s="1"/>
       <c r="S48" s="1"/>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -2782,7 +2862,7 @@
       <c r="R49" s="1"/>
       <c r="S49" s="1"/>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -2803,7 +2883,7 @@
       <c r="R50" s="1"/>
       <c r="S50" s="1"/>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -2813,9 +2893,9 @@
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
-      <c r="J51" s="24"/>
-      <c r="K51" s="24"/>
-      <c r="L51" s="24"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
       <c r="O51" s="1"/>
@@ -2824,7 +2904,7 @@
       <c r="R51" s="1"/>
       <c r="S51" s="1"/>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2834,9 +2914,9 @@
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
-      <c r="L52" s="11"/>
+      <c r="J52" s="24"/>
+      <c r="K52" s="24"/>
+      <c r="L52" s="24"/>
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
@@ -2845,7 +2925,7 @@
       <c r="R52" s="1"/>
       <c r="S52" s="1"/>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2857,7 +2937,7 @@
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
+      <c r="L53" s="11"/>
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
@@ -2866,7 +2946,7 @@
       <c r="R53" s="1"/>
       <c r="S53" s="1"/>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -2887,7 +2967,7 @@
       <c r="R54" s="1"/>
       <c r="S54" s="1"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -2908,7 +2988,7 @@
       <c r="R55" s="1"/>
       <c r="S55" s="1"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -2929,7 +3009,7 @@
       <c r="R56" s="1"/>
       <c r="S56" s="1"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -2950,7 +3030,7 @@
       <c r="R57" s="1"/>
       <c r="S57" s="1"/>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2971,7 +3051,7 @@
       <c r="R58" s="1"/>
       <c r="S58" s="1"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2992,7 +3072,7 @@
       <c r="R59" s="1"/>
       <c r="S59" s="1"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -3013,7 +3093,7 @@
       <c r="R60" s="1"/>
       <c r="S60" s="1"/>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -3034,7 +3114,7 @@
       <c r="R61" s="1"/>
       <c r="S61" s="1"/>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -3055,7 +3135,7 @@
       <c r="R62" s="1"/>
       <c r="S62" s="1"/>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -3076,7 +3156,7 @@
       <c r="R63" s="1"/>
       <c r="S63" s="1"/>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -3097,7 +3177,7 @@
       <c r="R64" s="1"/>
       <c r="S64" s="1"/>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -3118,14 +3198,35 @@
       <c r="R65" s="1"/>
       <c r="S65" s="1"/>
     </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="1"/>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
+      <c r="O66" s="1"/>
+      <c r="P66" s="1"/>
+      <c r="Q66" s="1"/>
+      <c r="R66" s="1"/>
+      <c r="S66" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B20:N20"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="J51:L51"/>
+    <mergeCell ref="B21:N21"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="J52:L52"/>
   </mergeCells>
-  <conditionalFormatting sqref="C5:N19">
+  <conditionalFormatting sqref="C5:N20">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Site Statistics (June 2023)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c93c05515dfe04a/GIT Hub/kunal-chowdhury.com/blog-stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="11_91C7ACB7C03E7306CE517BDFACF66E9FD99B01DC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65024B92-3269-45BA-99DD-F2CE7E6A66C0}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="11_91C7ACB7C03E7306CE517BDFACF66E9FD99B01DC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1A782DE-F971-47A3-9855-87D412C199D1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -140,7 +140,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -178,39 +178,42 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="22"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="22"/>
-      <color rgb="FF002060"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="22"/>
+      <b/>
+      <sz val="30"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <b/>
-      <sz val="22"/>
+      <sz val="24"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
-      <sz val="22"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="24"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -311,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -331,39 +334,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -373,7 +345,46 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -731,7 +742,7 @@
                   <c:v>35470785</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6760294</c:v>
+                  <c:v>12564075</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -963,6 +974,10 @@
 </file>
 
 <file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person1.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -1290,21 +1305,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="14" width="26.33203125" customWidth="1"/>
-    <col min="15" max="15" width="32.33203125" customWidth="1"/>
-    <col min="16" max="16" width="5.44140625" customWidth="1"/>
-    <col min="17" max="17" width="25.44140625" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="14" width="26.28515625" customWidth="1"/>
+    <col min="15" max="15" width="32.28515625" customWidth="1"/>
+    <col min="16" max="16" width="5.42578125" customWidth="1"/>
+    <col min="17" max="17" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1325,7 +1340,7 @@
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1346,7 +1361,7 @@
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
         <v>0</v>
@@ -1397,46 +1412,46 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="7" customFormat="1" ht="104.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:19" s="7" customFormat="1" ht="104.45" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="J4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="16" t="s">
+      <c r="K4" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="16" t="s">
+      <c r="L4" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="16" t="s">
+      <c r="M4" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="16" t="s">
+      <c r="N4" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="16" t="s">
+      <c r="O4" s="14" t="s">
         <v>28</v>
       </c>
       <c r="P4" s="5"/>
@@ -1444,802 +1459,802 @@
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
     </row>
-    <row r="5" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="1"/>
       <c r="B5" s="15">
         <v>2008</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="16">
         <v>0</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="16">
         <v>0</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="16">
         <v>0</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="16">
         <v>0</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="16">
         <v>0</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="16">
         <v>0</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="16">
         <v>0</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="16">
         <v>0</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="16">
         <v>0</v>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="16">
         <v>105</v>
       </c>
-      <c r="M5" s="12">
+      <c r="M5" s="16">
         <v>112</v>
       </c>
-      <c r="N5" s="12">
+      <c r="N5" s="16">
         <v>109</v>
       </c>
       <c r="O5" s="17">
         <f t="shared" ref="O5:O19" si="0">SUM(C5:N5)</f>
         <v>326</v>
       </c>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="9">
+      <c r="P5" s="18"/>
+      <c r="Q5" s="19">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>326</v>
       </c>
-      <c r="R5" s="1"/>
+      <c r="R5" s="20"/>
       <c r="S5" s="1"/>
     </row>
-    <row r="6" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="1"/>
       <c r="B6" s="15">
         <v>2009</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="16">
         <v>210</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="16">
         <v>265</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="16">
         <v>330</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="16">
         <v>459</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="16">
         <v>2711</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="16">
         <v>4347</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="16">
         <v>7134</v>
       </c>
-      <c r="J6" s="12">
+      <c r="J6" s="16">
         <v>7452</v>
       </c>
-      <c r="K6" s="12">
+      <c r="K6" s="16">
         <v>10193</v>
       </c>
-      <c r="L6" s="12">
+      <c r="L6" s="16">
         <v>11773</v>
       </c>
-      <c r="M6" s="12">
+      <c r="M6" s="16">
         <v>16989</v>
       </c>
-      <c r="N6" s="12">
+      <c r="N6" s="16">
         <v>18516</v>
       </c>
       <c r="O6" s="17">
         <f t="shared" si="0"/>
         <v>80379</v>
       </c>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="9">
+      <c r="P6" s="18"/>
+      <c r="Q6" s="19">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>80379</v>
       </c>
-      <c r="R6" s="1"/>
+      <c r="R6" s="20"/>
       <c r="S6" s="1"/>
     </row>
-    <row r="7" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="1"/>
       <c r="B7" s="15">
         <v>2010</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="16">
         <v>16660</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="16">
         <v>23673</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="16">
         <v>32985</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="16">
         <v>35222</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="16">
         <v>39909</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="16">
         <v>42087</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="16">
         <v>54395</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="16">
         <v>49067</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="16">
         <v>47658</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="16">
         <v>38853</v>
       </c>
-      <c r="M7" s="12">
+      <c r="M7" s="16">
         <v>39946</v>
       </c>
-      <c r="N7" s="12">
+      <c r="N7" s="16">
         <v>42658</v>
       </c>
       <c r="O7" s="17">
         <f t="shared" si="0"/>
         <v>463113</v>
       </c>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="9">
+      <c r="P7" s="18"/>
+      <c r="Q7" s="19">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>463113</v>
       </c>
-      <c r="R7" s="1"/>
+      <c r="R7" s="20"/>
       <c r="S7" s="1"/>
     </row>
-    <row r="8" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A8" s="1"/>
       <c r="B8" s="15">
         <v>2011</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="16">
         <v>45551</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="16">
         <v>69346</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="16">
         <v>47856</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="16">
         <v>64728</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="16">
         <v>73308</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="16">
         <v>82846</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="16">
         <v>72286</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J8" s="16">
         <v>75867</v>
       </c>
-      <c r="K8" s="12">
+      <c r="K8" s="16">
         <v>80961</v>
       </c>
-      <c r="L8" s="12">
+      <c r="L8" s="16">
         <v>62233</v>
       </c>
-      <c r="M8" s="12">
+      <c r="M8" s="16">
         <v>63447</v>
       </c>
-      <c r="N8" s="12">
+      <c r="N8" s="16">
         <v>64581</v>
       </c>
       <c r="O8" s="17">
         <f t="shared" si="0"/>
         <v>803010</v>
       </c>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="9">
+      <c r="P8" s="18"/>
+      <c r="Q8" s="19">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>803010</v>
       </c>
-      <c r="R8" s="1"/>
+      <c r="R8" s="20"/>
       <c r="S8" s="1"/>
     </row>
-    <row r="9" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="1"/>
       <c r="B9" s="15">
         <v>2012</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="16">
         <v>76072</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="16">
         <v>77385</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="16">
         <v>70852</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="16">
         <v>72356</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="16">
         <v>78593</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="16">
         <v>70155</v>
       </c>
-      <c r="I9" s="12">
+      <c r="I9" s="16">
         <v>72470</v>
       </c>
-      <c r="J9" s="12">
+      <c r="J9" s="16">
         <v>70252</v>
       </c>
-      <c r="K9" s="12">
+      <c r="K9" s="16">
         <v>79738</v>
       </c>
-      <c r="L9" s="12">
+      <c r="L9" s="16">
         <v>71284</v>
       </c>
-      <c r="M9" s="12">
+      <c r="M9" s="16">
         <v>76524</v>
       </c>
-      <c r="N9" s="12">
+      <c r="N9" s="16">
         <v>73172</v>
       </c>
       <c r="O9" s="17">
         <f t="shared" si="0"/>
         <v>888853</v>
       </c>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="9">
+      <c r="P9" s="18"/>
+      <c r="Q9" s="19">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>888853</v>
       </c>
-      <c r="R9" s="1"/>
+      <c r="R9" s="20"/>
       <c r="S9" s="1"/>
     </row>
-    <row r="10" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="1"/>
       <c r="B10" s="15">
         <v>2013</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="16">
         <v>78648</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="16">
         <v>74894</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="16">
         <v>86029</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="16">
         <v>82489</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="16">
         <v>80316</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="16">
         <v>78764</v>
       </c>
-      <c r="I10" s="12">
+      <c r="I10" s="16">
         <v>70746</v>
       </c>
-      <c r="J10" s="12">
+      <c r="J10" s="16">
         <v>79324</v>
       </c>
-      <c r="K10" s="12">
+      <c r="K10" s="16">
         <v>79148</v>
       </c>
-      <c r="L10" s="12">
+      <c r="L10" s="16">
         <v>76345</v>
       </c>
-      <c r="M10" s="12">
+      <c r="M10" s="16">
         <v>75329</v>
       </c>
-      <c r="N10" s="12">
+      <c r="N10" s="16">
         <v>73625</v>
       </c>
       <c r="O10" s="17">
         <f t="shared" si="0"/>
         <v>935657</v>
       </c>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="9">
+      <c r="P10" s="18"/>
+      <c r="Q10" s="19">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>935657</v>
       </c>
-      <c r="R10" s="1"/>
+      <c r="R10" s="20"/>
       <c r="S10" s="1"/>
     </row>
-    <row r="11" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A11" s="1"/>
       <c r="B11" s="15">
         <v>2014</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="16">
         <v>67510</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="16">
         <v>67706</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="16">
         <v>73924</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="16">
         <v>71449</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="16">
         <v>79877</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="16">
         <v>74705</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="16">
         <v>79936</v>
       </c>
-      <c r="J11" s="12">
+      <c r="J11" s="16">
         <v>78746</v>
       </c>
-      <c r="K11" s="12">
+      <c r="K11" s="16">
         <v>77891</v>
       </c>
-      <c r="L11" s="12">
+      <c r="L11" s="16">
         <v>77040</v>
       </c>
-      <c r="M11" s="12">
+      <c r="M11" s="16">
         <v>87951</v>
       </c>
-      <c r="N11" s="13">
+      <c r="N11" s="21">
         <v>101904</v>
       </c>
       <c r="O11" s="17">
         <f t="shared" si="0"/>
         <v>938639</v>
       </c>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="9">
+      <c r="P11" s="18"/>
+      <c r="Q11" s="19">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>938639</v>
       </c>
-      <c r="R11" s="1"/>
+      <c r="R11" s="20"/>
       <c r="S11" s="1"/>
     </row>
-    <row r="12" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A12" s="1"/>
       <c r="B12" s="15">
         <v>2015</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="16">
         <v>90536</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="16">
         <v>80976</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="16">
         <v>95444</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="16">
         <v>71951</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="16">
         <v>67019</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="16">
         <v>66244</v>
       </c>
-      <c r="I12" s="12">
+      <c r="I12" s="16">
         <v>86294</v>
       </c>
-      <c r="J12" s="13">
+      <c r="J12" s="21">
         <v>128005</v>
       </c>
-      <c r="K12" s="13">
+      <c r="K12" s="21">
         <v>137300</v>
       </c>
-      <c r="L12" s="13">
+      <c r="L12" s="21">
         <v>138705</v>
       </c>
-      <c r="M12" s="13">
+      <c r="M12" s="21">
         <v>125538</v>
       </c>
-      <c r="N12" s="13">
+      <c r="N12" s="21">
         <v>129945</v>
       </c>
       <c r="O12" s="17">
         <f t="shared" si="0"/>
         <v>1217957</v>
       </c>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="9">
+      <c r="P12" s="18"/>
+      <c r="Q12" s="19">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>1217957</v>
       </c>
-      <c r="R12" s="1"/>
+      <c r="R12" s="20"/>
       <c r="S12" s="1"/>
     </row>
-    <row r="13" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A13" s="1"/>
       <c r="B13" s="15">
         <v>2016</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="21">
         <v>142274</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="21">
         <v>123093</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="21">
         <v>147266</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="21">
         <v>152612</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="21">
         <v>134497</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="21">
         <v>132768</v>
       </c>
-      <c r="I13" s="14">
+      <c r="I13" s="22">
         <v>363723</v>
       </c>
-      <c r="J13" s="14">
+      <c r="J13" s="22">
         <v>702130</v>
       </c>
-      <c r="K13" s="14">
+      <c r="K13" s="22">
         <v>608805</v>
       </c>
-      <c r="L13" s="14">
+      <c r="L13" s="22">
         <v>635500</v>
       </c>
-      <c r="M13" s="14">
+      <c r="M13" s="22">
         <v>713080</v>
       </c>
-      <c r="N13" s="14">
+      <c r="N13" s="22">
         <v>674509</v>
       </c>
       <c r="O13" s="17">
         <f t="shared" si="0"/>
         <v>4530257</v>
       </c>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="9">
+      <c r="P13" s="18"/>
+      <c r="Q13" s="19">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>4530257</v>
       </c>
-      <c r="R13" s="1"/>
+      <c r="R13" s="20"/>
       <c r="S13" s="1"/>
     </row>
-    <row r="14" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" s="1"/>
       <c r="B14" s="15">
         <v>2017</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="22">
         <v>662423</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="22">
         <v>554842</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="22">
         <v>657797</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="22">
         <v>673209</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G14" s="22">
         <v>745540</v>
       </c>
-      <c r="H14" s="14">
+      <c r="H14" s="22">
         <v>660058</v>
       </c>
-      <c r="I14" s="14">
+      <c r="I14" s="22">
         <v>690513</v>
       </c>
-      <c r="J14" s="14">
+      <c r="J14" s="22">
         <v>670496</v>
       </c>
-      <c r="K14" s="14">
+      <c r="K14" s="22">
         <v>577595</v>
       </c>
-      <c r="L14" s="14">
+      <c r="L14" s="22">
         <v>665972</v>
       </c>
-      <c r="M14" s="14">
+      <c r="M14" s="22">
         <v>569447</v>
       </c>
-      <c r="N14" s="14">
+      <c r="N14" s="22">
         <v>565361</v>
       </c>
       <c r="O14" s="17">
         <f t="shared" si="0"/>
         <v>7693253</v>
       </c>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="9">
+      <c r="P14" s="18"/>
+      <c r="Q14" s="19">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>7693253</v>
       </c>
-      <c r="R14" s="1"/>
+      <c r="R14" s="20"/>
       <c r="S14" s="1"/>
     </row>
-    <row r="15" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A15" s="1"/>
       <c r="B15" s="15">
         <v>2018</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="22">
         <v>628028</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="22">
         <v>728208</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="22">
         <v>697376</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="22">
         <v>707376</v>
       </c>
-      <c r="G15" s="14">
+      <c r="G15" s="22">
         <v>759564</v>
       </c>
-      <c r="H15" s="14">
+      <c r="H15" s="22">
         <v>592381</v>
       </c>
-      <c r="I15" s="14">
+      <c r="I15" s="22">
         <v>545423</v>
       </c>
-      <c r="J15" s="14">
+      <c r="J15" s="22">
         <v>694837</v>
       </c>
-      <c r="K15" s="14">
+      <c r="K15" s="22">
         <v>739656</v>
       </c>
-      <c r="L15" s="14">
+      <c r="L15" s="22">
         <v>763733</v>
       </c>
-      <c r="M15" s="14">
+      <c r="M15" s="22">
         <v>698962</v>
       </c>
-      <c r="N15" s="14">
+      <c r="N15" s="22">
         <v>732173</v>
       </c>
       <c r="O15" s="17">
         <f t="shared" si="0"/>
         <v>8287717</v>
       </c>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="9">
+      <c r="P15" s="18"/>
+      <c r="Q15" s="19">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>8287717</v>
       </c>
-      <c r="R15" s="1"/>
+      <c r="R15" s="20"/>
       <c r="S15" s="1"/>
     </row>
-    <row r="16" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A16" s="1"/>
       <c r="B16" s="15">
         <v>2019</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C16" s="22">
         <v>816792</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16" s="22">
         <v>811807</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="21">
         <v>903678</v>
       </c>
-      <c r="F16" s="13">
+      <c r="F16" s="21">
         <v>1174272</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G16" s="21">
         <v>1399881</v>
       </c>
-      <c r="H16" s="13">
+      <c r="H16" s="21">
         <v>1179014</v>
       </c>
-      <c r="I16" s="13">
+      <c r="I16" s="21">
         <v>1380086</v>
       </c>
-      <c r="J16" s="13">
+      <c r="J16" s="21">
         <v>1448886</v>
       </c>
-      <c r="K16" s="13">
+      <c r="K16" s="21">
         <v>1506868</v>
       </c>
-      <c r="L16" s="13">
+      <c r="L16" s="21">
         <v>1761891</v>
       </c>
-      <c r="M16" s="13">
+      <c r="M16" s="21">
         <v>2059856</v>
       </c>
-      <c r="N16" s="13">
+      <c r="N16" s="21">
         <v>2325909</v>
       </c>
-      <c r="O16" s="18">
+      <c r="O16" s="23">
         <f t="shared" si="0"/>
         <v>16768940</v>
       </c>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="9">
+      <c r="P16" s="18"/>
+      <c r="Q16" s="19">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>16768940</v>
       </c>
-      <c r="R16" s="1"/>
+      <c r="R16" s="20"/>
       <c r="S16" s="1"/>
     </row>
-    <row r="17" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A17" s="1"/>
       <c r="B17" s="15">
         <v>2020</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17" s="21">
         <v>1694534</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="21">
         <v>3203938</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="21">
         <v>3296329</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="21">
         <v>2694570</v>
       </c>
-      <c r="G17" s="13">
+      <c r="G17" s="21">
         <v>2511957</v>
       </c>
-      <c r="H17" s="13">
+      <c r="H17" s="21">
         <v>2264236</v>
       </c>
-      <c r="I17" s="13">
+      <c r="I17" s="21">
         <v>1255353</v>
       </c>
-      <c r="J17" s="13">
+      <c r="J17" s="21">
         <v>1205188</v>
       </c>
-      <c r="K17" s="13">
+      <c r="K17" s="21">
         <v>1622473</v>
       </c>
-      <c r="L17" s="13">
+      <c r="L17" s="21">
         <v>1912285</v>
       </c>
-      <c r="M17" s="13">
+      <c r="M17" s="21">
         <v>2366693</v>
       </c>
-      <c r="N17" s="13">
+      <c r="N17" s="21">
         <v>2176841</v>
       </c>
-      <c r="O17" s="19">
+      <c r="O17" s="24">
         <f t="shared" si="0"/>
         <v>26204397</v>
       </c>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="9">
+      <c r="P17" s="18"/>
+      <c r="Q17" s="19">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>26204397</v>
       </c>
-      <c r="R17" s="1"/>
+      <c r="R17" s="20"/>
       <c r="S17" s="1"/>
     </row>
-    <row r="18" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A18" s="1"/>
       <c r="B18" s="15">
         <v>2021</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="21">
         <v>924261</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="21">
         <v>1235225</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="21">
         <v>2047206</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="21">
         <v>2337103</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="21">
         <v>2440903</v>
       </c>
-      <c r="H18" s="13">
+      <c r="H18" s="21">
         <v>2432014</v>
       </c>
-      <c r="I18" s="13">
+      <c r="I18" s="21">
         <v>2631617</v>
       </c>
-      <c r="J18" s="13">
+      <c r="J18" s="21">
         <v>2238361</v>
       </c>
-      <c r="K18" s="13">
+      <c r="K18" s="21">
         <v>3054555</v>
       </c>
-      <c r="L18" s="13">
+      <c r="L18" s="21">
         <v>2855764</v>
       </c>
-      <c r="M18" s="13">
+      <c r="M18" s="21">
         <v>3465933</v>
       </c>
-      <c r="N18" s="13">
+      <c r="N18" s="21">
         <v>4145700</v>
       </c>
-      <c r="O18" s="19">
+      <c r="O18" s="24">
         <f t="shared" si="0"/>
         <v>29808642</v>
       </c>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="9">
+      <c r="P18" s="18"/>
+      <c r="Q18" s="19">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>29808642</v>
       </c>
-      <c r="R18" s="1"/>
+      <c r="R18" s="20"/>
       <c r="S18" s="1"/>
     </row>
-    <row r="19" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A19" s="1"/>
       <c r="B19" s="15">
         <v>2022</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C19" s="21">
         <v>4297072</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D19" s="21">
         <v>2442144</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="21">
         <v>2336228</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F19" s="21">
         <v>2718163</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G19" s="21">
         <v>2097535</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H19" s="21">
         <v>2895282</v>
       </c>
-      <c r="I19" s="13">
+      <c r="I19" s="21">
         <v>2891642</v>
       </c>
-      <c r="J19" s="13">
+      <c r="J19" s="21">
         <v>3141889</v>
       </c>
-      <c r="K19" s="13">
+      <c r="K19" s="21">
         <v>3181844</v>
       </c>
-      <c r="L19" s="13">
+      <c r="L19" s="21">
         <v>3090886</v>
       </c>
-      <c r="M19" s="13">
+      <c r="M19" s="21">
         <v>3331811</v>
       </c>
-      <c r="N19" s="13">
+      <c r="N19" s="21">
         <v>3046289</v>
       </c>
-      <c r="O19" s="19">
+      <c r="O19" s="24">
         <f t="shared" si="0"/>
         <v>35470785</v>
       </c>
-      <c r="P19" s="8"/>
-      <c r="Q19" s="9" t="e">
+      <c r="P19" s="18"/>
+      <c r="Q19" s="19" t="e">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="R19" s="1"/>
+      <c r="R19" s="20"/>
       <c r="S19" s="1"/>
     </row>
-    <row r="20" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A20" s="1"/>
       <c r="B20" s="15">
         <v>2023</v>
@@ -2253,77 +2268,83 @@
       <c r="E20" s="25">
         <v>1899126</v>
       </c>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
+      <c r="F20" s="25">
+        <v>1806635</v>
+      </c>
+      <c r="G20" s="25">
+        <v>1707937</v>
+      </c>
+      <c r="H20" s="25">
+        <v>2289209</v>
+      </c>
       <c r="I20" s="25"/>
       <c r="J20" s="25"/>
       <c r="K20" s="25"/>
       <c r="L20" s="25"/>
       <c r="M20" s="25"/>
       <c r="N20" s="25"/>
-      <c r="O20" s="19">
+      <c r="O20" s="24">
         <f>SUM(C20:N20)</f>
-        <v>6760294</v>
-      </c>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="1"/>
+        <v>12564075</v>
+      </c>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="19"/>
+      <c r="R20" s="20"/>
       <c r="S20" s="1"/>
     </row>
-    <row r="21" spans="1:19" s="7" customFormat="1" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" s="7" customFormat="1" ht="58.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="21"/>
-      <c r="O21" s="20">
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="27">
         <f>SUM(O5:O20)</f>
-        <v>140852219</v>
-      </c>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
+        <v>146656000</v>
+      </c>
+      <c r="P21" s="28"/>
+      <c r="Q21" s="29"/>
+      <c r="R21" s="29"/>
       <c r="S21" s="3"/>
     </row>
-    <row r="22" spans="1:19" ht="26.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
+    <row r="22" spans="1:19" ht="26.85" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
       <c r="P22" s="8"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
     </row>
-    <row r="23" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:19" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -2337,7 +2358,7 @@
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2358,7 +2379,7 @@
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2379,7 +2400,7 @@
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -2400,7 +2421,7 @@
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -2421,7 +2442,7 @@
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -2442,7 +2463,7 @@
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2463,7 +2484,7 @@
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -2484,7 +2505,7 @@
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -2505,7 +2526,7 @@
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2526,7 +2547,7 @@
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -2547,7 +2568,7 @@
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -2568,7 +2589,7 @@
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -2589,7 +2610,7 @@
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -2610,7 +2631,7 @@
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2631,7 +2652,7 @@
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -2652,7 +2673,7 @@
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2673,7 +2694,7 @@
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -2694,7 +2715,7 @@
       <c r="R41" s="1"/>
       <c r="S41" s="1"/>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -2715,7 +2736,7 @@
       <c r="R42" s="1"/>
       <c r="S42" s="1"/>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -2736,7 +2757,7 @@
       <c r="R43" s="1"/>
       <c r="S43" s="1"/>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -2757,7 +2778,7 @@
       <c r="R44" s="1"/>
       <c r="S44" s="1"/>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -2778,7 +2799,7 @@
       <c r="R45" s="1"/>
       <c r="S45" s="1"/>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -2799,7 +2820,7 @@
       <c r="R46" s="1"/>
       <c r="S46" s="1"/>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -2820,7 +2841,7 @@
       <c r="R47" s="1"/>
       <c r="S47" s="1"/>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -2841,7 +2862,7 @@
       <c r="R48" s="1"/>
       <c r="S48" s="1"/>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -2862,7 +2883,7 @@
       <c r="R49" s="1"/>
       <c r="S49" s="1"/>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -2883,7 +2904,7 @@
       <c r="R50" s="1"/>
       <c r="S50" s="1"/>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -2904,7 +2925,7 @@
       <c r="R51" s="1"/>
       <c r="S51" s="1"/>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2914,9 +2935,9 @@
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
-      <c r="J52" s="24"/>
-      <c r="K52" s="24"/>
-      <c r="L52" s="24"/>
+      <c r="J52" s="13"/>
+      <c r="K52" s="13"/>
+      <c r="L52" s="13"/>
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
@@ -2925,7 +2946,7 @@
       <c r="R52" s="1"/>
       <c r="S52" s="1"/>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2937,7 +2958,7 @@
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
-      <c r="L53" s="11"/>
+      <c r="L53" s="10"/>
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
@@ -2946,7 +2967,7 @@
       <c r="R53" s="1"/>
       <c r="S53" s="1"/>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -2967,7 +2988,7 @@
       <c r="R54" s="1"/>
       <c r="S54" s="1"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -2988,7 +3009,7 @@
       <c r="R55" s="1"/>
       <c r="S55" s="1"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -3009,7 +3030,7 @@
       <c r="R56" s="1"/>
       <c r="S56" s="1"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -3030,7 +3051,7 @@
       <c r="R57" s="1"/>
       <c r="S57" s="1"/>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -3051,7 +3072,7 @@
       <c r="R58" s="1"/>
       <c r="S58" s="1"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -3072,7 +3093,7 @@
       <c r="R59" s="1"/>
       <c r="S59" s="1"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -3093,7 +3114,7 @@
       <c r="R60" s="1"/>
       <c r="S60" s="1"/>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -3114,7 +3135,7 @@
       <c r="R61" s="1"/>
       <c r="S61" s="1"/>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -3135,7 +3156,7 @@
       <c r="R62" s="1"/>
       <c r="S62" s="1"/>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -3156,7 +3177,7 @@
       <c r="R63" s="1"/>
       <c r="S63" s="1"/>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -3177,7 +3198,7 @@
       <c r="R64" s="1"/>
       <c r="S64" s="1"/>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -3198,7 +3219,7 @@
       <c r="R65" s="1"/>
       <c r="S65" s="1"/>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>

</xml_diff>

<commit_message>
Blog Statistics (August 2023)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c93c05515dfe04a/GIT Hub/kunal-chowdhury.com/blog-stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="11_91C7ACB7C03E7306CE517BDFACF66E9FD99B01DC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1A782DE-F971-47A3-9855-87D412C199D1}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="11_91C7ACB7C03E7306CE517BDFACF66E9FD99B01DC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{201EE36A-992F-448A-A4CB-360A9163B7EB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -336,15 +336,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -375,9 +366,6 @@
     <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="6" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -386,6 +374,18 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -742,7 +742,7 @@
                   <c:v>35470785</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>12564075</c:v>
+                  <c:v>16801879</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1002,7 +1002,7 @@
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Column152"/>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Column16"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1305,8 +1305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="Y8" sqref="Y8"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="W20" sqref="W20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1415,43 +1415,43 @@
     <row r="4" spans="1:19" s="7" customFormat="1" ht="104.45" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="K4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="14" t="s">
+      <c r="L4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="14" t="s">
+      <c r="M4" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="14" t="s">
+      <c r="N4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="14" t="s">
+      <c r="O4" s="11" t="s">
         <v>28</v>
       </c>
       <c r="P4" s="5"/>
@@ -1461,835 +1461,839 @@
     </row>
     <row r="5" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="1"/>
-      <c r="B5" s="15">
+      <c r="B5" s="12">
         <v>2008</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="13">
         <v>0</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="13">
         <v>0</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="13">
         <v>0</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="13">
         <v>0</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="13">
         <v>0</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H5" s="13">
         <v>0</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="13">
         <v>0</v>
       </c>
-      <c r="J5" s="16">
+      <c r="J5" s="13">
         <v>0</v>
       </c>
-      <c r="K5" s="16">
+      <c r="K5" s="13">
         <v>0</v>
       </c>
-      <c r="L5" s="16">
+      <c r="L5" s="13">
         <v>105</v>
       </c>
-      <c r="M5" s="16">
+      <c r="M5" s="13">
         <v>112</v>
       </c>
-      <c r="N5" s="16">
+      <c r="N5" s="13">
         <v>109</v>
       </c>
-      <c r="O5" s="17">
+      <c r="O5" s="14">
         <f t="shared" ref="O5:O19" si="0">SUM(C5:N5)</f>
         <v>326</v>
       </c>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="19">
+      <c r="P5" s="15"/>
+      <c r="Q5" s="16">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>326</v>
       </c>
-      <c r="R5" s="20"/>
+      <c r="R5" s="17"/>
       <c r="S5" s="1"/>
     </row>
     <row r="6" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="1"/>
-      <c r="B6" s="15">
+      <c r="B6" s="12">
         <v>2009</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="13">
         <v>210</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="13">
         <v>265</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="13">
         <v>330</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="13">
         <v>459</v>
       </c>
-      <c r="G6" s="16">
+      <c r="G6" s="13">
         <v>2711</v>
       </c>
-      <c r="H6" s="16">
+      <c r="H6" s="13">
         <v>4347</v>
       </c>
-      <c r="I6" s="16">
+      <c r="I6" s="13">
         <v>7134</v>
       </c>
-      <c r="J6" s="16">
+      <c r="J6" s="13">
         <v>7452</v>
       </c>
-      <c r="K6" s="16">
+      <c r="K6" s="13">
         <v>10193</v>
       </c>
-      <c r="L6" s="16">
+      <c r="L6" s="13">
         <v>11773</v>
       </c>
-      <c r="M6" s="16">
+      <c r="M6" s="13">
         <v>16989</v>
       </c>
-      <c r="N6" s="16">
+      <c r="N6" s="13">
         <v>18516</v>
       </c>
-      <c r="O6" s="17">
+      <c r="O6" s="14">
         <f t="shared" si="0"/>
         <v>80379</v>
       </c>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="19">
+      <c r="P6" s="15"/>
+      <c r="Q6" s="16">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>80379</v>
       </c>
-      <c r="R6" s="20"/>
+      <c r="R6" s="17"/>
       <c r="S6" s="1"/>
     </row>
     <row r="7" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="1"/>
-      <c r="B7" s="15">
+      <c r="B7" s="12">
         <v>2010</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="13">
         <v>16660</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="13">
         <v>23673</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="13">
         <v>32985</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="13">
         <v>35222</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="13">
         <v>39909</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7" s="13">
         <v>42087</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I7" s="13">
         <v>54395</v>
       </c>
-      <c r="J7" s="16">
+      <c r="J7" s="13">
         <v>49067</v>
       </c>
-      <c r="K7" s="16">
+      <c r="K7" s="13">
         <v>47658</v>
       </c>
-      <c r="L7" s="16">
+      <c r="L7" s="13">
         <v>38853</v>
       </c>
-      <c r="M7" s="16">
+      <c r="M7" s="13">
         <v>39946</v>
       </c>
-      <c r="N7" s="16">
+      <c r="N7" s="13">
         <v>42658</v>
       </c>
-      <c r="O7" s="17">
+      <c r="O7" s="14">
         <f t="shared" si="0"/>
         <v>463113</v>
       </c>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="19">
+      <c r="P7" s="15"/>
+      <c r="Q7" s="16">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>463113</v>
       </c>
-      <c r="R7" s="20"/>
+      <c r="R7" s="17"/>
       <c r="S7" s="1"/>
     </row>
     <row r="8" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A8" s="1"/>
-      <c r="B8" s="15">
+      <c r="B8" s="12">
         <v>2011</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="13">
         <v>45551</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="13">
         <v>69346</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="13">
         <v>47856</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="13">
         <v>64728</v>
       </c>
-      <c r="G8" s="16">
+      <c r="G8" s="13">
         <v>73308</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H8" s="13">
         <v>82846</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="13">
         <v>72286</v>
       </c>
-      <c r="J8" s="16">
+      <c r="J8" s="13">
         <v>75867</v>
       </c>
-      <c r="K8" s="16">
+      <c r="K8" s="13">
         <v>80961</v>
       </c>
-      <c r="L8" s="16">
+      <c r="L8" s="13">
         <v>62233</v>
       </c>
-      <c r="M8" s="16">
+      <c r="M8" s="13">
         <v>63447</v>
       </c>
-      <c r="N8" s="16">
+      <c r="N8" s="13">
         <v>64581</v>
       </c>
-      <c r="O8" s="17">
+      <c r="O8" s="14">
         <f t="shared" si="0"/>
         <v>803010</v>
       </c>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="19">
+      <c r="P8" s="15"/>
+      <c r="Q8" s="16">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>803010</v>
       </c>
-      <c r="R8" s="20"/>
+      <c r="R8" s="17"/>
       <c r="S8" s="1"/>
     </row>
     <row r="9" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="1"/>
-      <c r="B9" s="15">
+      <c r="B9" s="12">
         <v>2012</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="13">
         <v>76072</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="13">
         <v>77385</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="13">
         <v>70852</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="13">
         <v>72356</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="13">
         <v>78593</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="13">
         <v>70155</v>
       </c>
-      <c r="I9" s="16">
+      <c r="I9" s="13">
         <v>72470</v>
       </c>
-      <c r="J9" s="16">
+      <c r="J9" s="13">
         <v>70252</v>
       </c>
-      <c r="K9" s="16">
+      <c r="K9" s="13">
         <v>79738</v>
       </c>
-      <c r="L9" s="16">
+      <c r="L9" s="13">
         <v>71284</v>
       </c>
-      <c r="M9" s="16">
+      <c r="M9" s="13">
         <v>76524</v>
       </c>
-      <c r="N9" s="16">
+      <c r="N9" s="13">
         <v>73172</v>
       </c>
-      <c r="O9" s="17">
+      <c r="O9" s="14">
         <f t="shared" si="0"/>
         <v>888853</v>
       </c>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="19">
+      <c r="P9" s="15"/>
+      <c r="Q9" s="16">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>888853</v>
       </c>
-      <c r="R9" s="20"/>
+      <c r="R9" s="17"/>
       <c r="S9" s="1"/>
     </row>
     <row r="10" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="1"/>
-      <c r="B10" s="15">
+      <c r="B10" s="12">
         <v>2013</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="13">
         <v>78648</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="13">
         <v>74894</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="13">
         <v>86029</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="13">
         <v>82489</v>
       </c>
-      <c r="G10" s="16">
+      <c r="G10" s="13">
         <v>80316</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10" s="13">
         <v>78764</v>
       </c>
-      <c r="I10" s="16">
+      <c r="I10" s="13">
         <v>70746</v>
       </c>
-      <c r="J10" s="16">
+      <c r="J10" s="13">
         <v>79324</v>
       </c>
-      <c r="K10" s="16">
+      <c r="K10" s="13">
         <v>79148</v>
       </c>
-      <c r="L10" s="16">
+      <c r="L10" s="13">
         <v>76345</v>
       </c>
-      <c r="M10" s="16">
+      <c r="M10" s="13">
         <v>75329</v>
       </c>
-      <c r="N10" s="16">
+      <c r="N10" s="13">
         <v>73625</v>
       </c>
-      <c r="O10" s="17">
+      <c r="O10" s="14">
         <f t="shared" si="0"/>
         <v>935657</v>
       </c>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="19">
+      <c r="P10" s="15"/>
+      <c r="Q10" s="16">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>935657</v>
       </c>
-      <c r="R10" s="20"/>
+      <c r="R10" s="17"/>
       <c r="S10" s="1"/>
     </row>
     <row r="11" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A11" s="1"/>
-      <c r="B11" s="15">
+      <c r="B11" s="12">
         <v>2014</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="13">
         <v>67510</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="13">
         <v>67706</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="13">
         <v>73924</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="13">
         <v>71449</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G11" s="13">
         <v>79877</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="13">
         <v>74705</v>
       </c>
-      <c r="I11" s="16">
+      <c r="I11" s="13">
         <v>79936</v>
       </c>
-      <c r="J11" s="16">
+      <c r="J11" s="13">
         <v>78746</v>
       </c>
-      <c r="K11" s="16">
+      <c r="K11" s="13">
         <v>77891</v>
       </c>
-      <c r="L11" s="16">
+      <c r="L11" s="13">
         <v>77040</v>
       </c>
-      <c r="M11" s="16">
+      <c r="M11" s="13">
         <v>87951</v>
       </c>
-      <c r="N11" s="21">
+      <c r="N11" s="18">
         <v>101904</v>
       </c>
-      <c r="O11" s="17">
+      <c r="O11" s="14">
         <f t="shared" si="0"/>
         <v>938639</v>
       </c>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="19">
+      <c r="P11" s="15"/>
+      <c r="Q11" s="16">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>938639</v>
       </c>
-      <c r="R11" s="20"/>
+      <c r="R11" s="17"/>
       <c r="S11" s="1"/>
     </row>
     <row r="12" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A12" s="1"/>
-      <c r="B12" s="15">
+      <c r="B12" s="12">
         <v>2015</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="13">
         <v>90536</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="13">
         <v>80976</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12" s="13">
         <v>95444</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F12" s="13">
         <v>71951</v>
       </c>
-      <c r="G12" s="16">
+      <c r="G12" s="13">
         <v>67019</v>
       </c>
-      <c r="H12" s="16">
+      <c r="H12" s="13">
         <v>66244</v>
       </c>
-      <c r="I12" s="16">
+      <c r="I12" s="13">
         <v>86294</v>
       </c>
-      <c r="J12" s="21">
+      <c r="J12" s="18">
         <v>128005</v>
       </c>
-      <c r="K12" s="21">
+      <c r="K12" s="18">
         <v>137300</v>
       </c>
-      <c r="L12" s="21">
+      <c r="L12" s="18">
         <v>138705</v>
       </c>
-      <c r="M12" s="21">
+      <c r="M12" s="18">
         <v>125538</v>
       </c>
-      <c r="N12" s="21">
+      <c r="N12" s="18">
         <v>129945</v>
       </c>
-      <c r="O12" s="17">
+      <c r="O12" s="14">
         <f t="shared" si="0"/>
         <v>1217957</v>
       </c>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="19">
+      <c r="P12" s="15"/>
+      <c r="Q12" s="16">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>1217957</v>
       </c>
-      <c r="R12" s="20"/>
+      <c r="R12" s="17"/>
       <c r="S12" s="1"/>
     </row>
     <row r="13" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A13" s="1"/>
-      <c r="B13" s="15">
+      <c r="B13" s="12">
         <v>2016</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C13" s="18">
         <v>142274</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D13" s="18">
         <v>123093</v>
       </c>
-      <c r="E13" s="21">
+      <c r="E13" s="18">
         <v>147266</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="18">
         <v>152612</v>
       </c>
-      <c r="G13" s="21">
+      <c r="G13" s="18">
         <v>134497</v>
       </c>
-      <c r="H13" s="21">
+      <c r="H13" s="18">
         <v>132768</v>
       </c>
-      <c r="I13" s="22">
+      <c r="I13" s="19">
         <v>363723</v>
       </c>
-      <c r="J13" s="22">
+      <c r="J13" s="19">
         <v>702130</v>
       </c>
-      <c r="K13" s="22">
+      <c r="K13" s="19">
         <v>608805</v>
       </c>
-      <c r="L13" s="22">
+      <c r="L13" s="19">
         <v>635500</v>
       </c>
-      <c r="M13" s="22">
+      <c r="M13" s="19">
         <v>713080</v>
       </c>
-      <c r="N13" s="22">
+      <c r="N13" s="19">
         <v>674509</v>
       </c>
-      <c r="O13" s="17">
+      <c r="O13" s="14">
         <f t="shared" si="0"/>
         <v>4530257</v>
       </c>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="19">
+      <c r="P13" s="15"/>
+      <c r="Q13" s="16">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>4530257</v>
       </c>
-      <c r="R13" s="20"/>
+      <c r="R13" s="17"/>
       <c r="S13" s="1"/>
     </row>
     <row r="14" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" s="1"/>
-      <c r="B14" s="15">
+      <c r="B14" s="12">
         <v>2017</v>
       </c>
-      <c r="C14" s="22">
+      <c r="C14" s="19">
         <v>662423</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="19">
         <v>554842</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E14" s="19">
         <v>657797</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="19">
         <v>673209</v>
       </c>
-      <c r="G14" s="22">
+      <c r="G14" s="19">
         <v>745540</v>
       </c>
-      <c r="H14" s="22">
+      <c r="H14" s="19">
         <v>660058</v>
       </c>
-      <c r="I14" s="22">
+      <c r="I14" s="19">
         <v>690513</v>
       </c>
-      <c r="J14" s="22">
+      <c r="J14" s="19">
         <v>670496</v>
       </c>
-      <c r="K14" s="22">
+      <c r="K14" s="19">
         <v>577595</v>
       </c>
-      <c r="L14" s="22">
+      <c r="L14" s="19">
         <v>665972</v>
       </c>
-      <c r="M14" s="22">
+      <c r="M14" s="19">
         <v>569447</v>
       </c>
-      <c r="N14" s="22">
+      <c r="N14" s="19">
         <v>565361</v>
       </c>
-      <c r="O14" s="17">
+      <c r="O14" s="14">
         <f t="shared" si="0"/>
         <v>7693253</v>
       </c>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="19">
+      <c r="P14" s="15"/>
+      <c r="Q14" s="16">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>7693253</v>
       </c>
-      <c r="R14" s="20"/>
+      <c r="R14" s="17"/>
       <c r="S14" s="1"/>
     </row>
     <row r="15" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A15" s="1"/>
-      <c r="B15" s="15">
+      <c r="B15" s="12">
         <v>2018</v>
       </c>
-      <c r="C15" s="22">
+      <c r="C15" s="19">
         <v>628028</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="19">
         <v>728208</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E15" s="19">
         <v>697376</v>
       </c>
-      <c r="F15" s="22">
+      <c r="F15" s="19">
         <v>707376</v>
       </c>
-      <c r="G15" s="22">
+      <c r="G15" s="19">
         <v>759564</v>
       </c>
-      <c r="H15" s="22">
+      <c r="H15" s="19">
         <v>592381</v>
       </c>
-      <c r="I15" s="22">
+      <c r="I15" s="19">
         <v>545423</v>
       </c>
-      <c r="J15" s="22">
+      <c r="J15" s="19">
         <v>694837</v>
       </c>
-      <c r="K15" s="22">
+      <c r="K15" s="19">
         <v>739656</v>
       </c>
-      <c r="L15" s="22">
+      <c r="L15" s="19">
         <v>763733</v>
       </c>
-      <c r="M15" s="22">
+      <c r="M15" s="19">
         <v>698962</v>
       </c>
-      <c r="N15" s="22">
+      <c r="N15" s="19">
         <v>732173</v>
       </c>
-      <c r="O15" s="17">
+      <c r="O15" s="14">
         <f t="shared" si="0"/>
         <v>8287717</v>
       </c>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="19">
+      <c r="P15" s="15"/>
+      <c r="Q15" s="16">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>8287717</v>
       </c>
-      <c r="R15" s="20"/>
+      <c r="R15" s="17"/>
       <c r="S15" s="1"/>
     </row>
     <row r="16" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A16" s="1"/>
-      <c r="B16" s="15">
+      <c r="B16" s="12">
         <v>2019</v>
       </c>
-      <c r="C16" s="22">
+      <c r="C16" s="19">
         <v>816792</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="19">
         <v>811807</v>
       </c>
-      <c r="E16" s="21">
+      <c r="E16" s="18">
         <v>903678</v>
       </c>
-      <c r="F16" s="21">
+      <c r="F16" s="18">
         <v>1174272</v>
       </c>
-      <c r="G16" s="21">
+      <c r="G16" s="18">
         <v>1399881</v>
       </c>
-      <c r="H16" s="21">
+      <c r="H16" s="18">
         <v>1179014</v>
       </c>
-      <c r="I16" s="21">
+      <c r="I16" s="18">
         <v>1380086</v>
       </c>
-      <c r="J16" s="21">
+      <c r="J16" s="18">
         <v>1448886</v>
       </c>
-      <c r="K16" s="21">
+      <c r="K16" s="18">
         <v>1506868</v>
       </c>
-      <c r="L16" s="21">
+      <c r="L16" s="18">
         <v>1761891</v>
       </c>
-      <c r="M16" s="21">
+      <c r="M16" s="18">
         <v>2059856</v>
       </c>
-      <c r="N16" s="21">
+      <c r="N16" s="18">
         <v>2325909</v>
       </c>
-      <c r="O16" s="23">
+      <c r="O16" s="20">
         <f t="shared" si="0"/>
         <v>16768940</v>
       </c>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="19">
+      <c r="P16" s="15"/>
+      <c r="Q16" s="16">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>16768940</v>
       </c>
-      <c r="R16" s="20"/>
+      <c r="R16" s="17"/>
       <c r="S16" s="1"/>
     </row>
     <row r="17" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A17" s="1"/>
-      <c r="B17" s="15">
+      <c r="B17" s="12">
         <v>2020</v>
       </c>
-      <c r="C17" s="21">
+      <c r="C17" s="18">
         <v>1694534</v>
       </c>
-      <c r="D17" s="21">
+      <c r="D17" s="18">
         <v>3203938</v>
       </c>
-      <c r="E17" s="21">
+      <c r="E17" s="18">
         <v>3296329</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17" s="18">
         <v>2694570</v>
       </c>
-      <c r="G17" s="21">
+      <c r="G17" s="18">
         <v>2511957</v>
       </c>
-      <c r="H17" s="21">
+      <c r="H17" s="18">
         <v>2264236</v>
       </c>
-      <c r="I17" s="21">
+      <c r="I17" s="18">
         <v>1255353</v>
       </c>
-      <c r="J17" s="21">
+      <c r="J17" s="18">
         <v>1205188</v>
       </c>
-      <c r="K17" s="21">
+      <c r="K17" s="18">
         <v>1622473</v>
       </c>
-      <c r="L17" s="21">
+      <c r="L17" s="18">
         <v>1912285</v>
       </c>
-      <c r="M17" s="21">
+      <c r="M17" s="18">
         <v>2366693</v>
       </c>
-      <c r="N17" s="21">
+      <c r="N17" s="18">
         <v>2176841</v>
       </c>
-      <c r="O17" s="24">
+      <c r="O17" s="21">
         <f t="shared" si="0"/>
         <v>26204397</v>
       </c>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="19">
+      <c r="P17" s="15"/>
+      <c r="Q17" s="16">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>26204397</v>
       </c>
-      <c r="R17" s="20"/>
+      <c r="R17" s="17"/>
       <c r="S17" s="1"/>
     </row>
     <row r="18" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A18" s="1"/>
-      <c r="B18" s="15">
+      <c r="B18" s="12">
         <v>2021</v>
       </c>
-      <c r="C18" s="21">
+      <c r="C18" s="18">
         <v>924261</v>
       </c>
-      <c r="D18" s="21">
+      <c r="D18" s="18">
         <v>1235225</v>
       </c>
-      <c r="E18" s="21">
+      <c r="E18" s="18">
         <v>2047206</v>
       </c>
-      <c r="F18" s="21">
+      <c r="F18" s="18">
         <v>2337103</v>
       </c>
-      <c r="G18" s="21">
+      <c r="G18" s="18">
         <v>2440903</v>
       </c>
-      <c r="H18" s="21">
+      <c r="H18" s="18">
         <v>2432014</v>
       </c>
-      <c r="I18" s="21">
+      <c r="I18" s="18">
         <v>2631617</v>
       </c>
-      <c r="J18" s="21">
+      <c r="J18" s="18">
         <v>2238361</v>
       </c>
-      <c r="K18" s="21">
+      <c r="K18" s="18">
         <v>3054555</v>
       </c>
-      <c r="L18" s="21">
+      <c r="L18" s="18">
         <v>2855764</v>
       </c>
-      <c r="M18" s="21">
+      <c r="M18" s="18">
         <v>3465933</v>
       </c>
-      <c r="N18" s="21">
+      <c r="N18" s="18">
         <v>4145700</v>
       </c>
-      <c r="O18" s="24">
+      <c r="O18" s="21">
         <f t="shared" si="0"/>
         <v>29808642</v>
       </c>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="19">
+      <c r="P18" s="15"/>
+      <c r="Q18" s="16">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>29808642</v>
       </c>
-      <c r="R18" s="20"/>
+      <c r="R18" s="17"/>
       <c r="S18" s="1"/>
     </row>
     <row r="19" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A19" s="1"/>
-      <c r="B19" s="15">
+      <c r="B19" s="12">
         <v>2022</v>
       </c>
-      <c r="C19" s="21">
+      <c r="C19" s="18">
         <v>4297072</v>
       </c>
-      <c r="D19" s="21">
+      <c r="D19" s="18">
         <v>2442144</v>
       </c>
-      <c r="E19" s="21">
+      <c r="E19" s="18">
         <v>2336228</v>
       </c>
-      <c r="F19" s="21">
+      <c r="F19" s="18">
         <v>2718163</v>
       </c>
-      <c r="G19" s="21">
+      <c r="G19" s="18">
         <v>2097535</v>
       </c>
-      <c r="H19" s="21">
+      <c r="H19" s="18">
         <v>2895282</v>
       </c>
-      <c r="I19" s="21">
+      <c r="I19" s="18">
         <v>2891642</v>
       </c>
-      <c r="J19" s="21">
+      <c r="J19" s="18">
         <v>3141889</v>
       </c>
-      <c r="K19" s="21">
+      <c r="K19" s="18">
         <v>3181844</v>
       </c>
-      <c r="L19" s="21">
+      <c r="L19" s="18">
         <v>3090886</v>
       </c>
-      <c r="M19" s="21">
+      <c r="M19" s="18">
         <v>3331811</v>
       </c>
-      <c r="N19" s="21">
+      <c r="N19" s="18">
         <v>3046289</v>
       </c>
-      <c r="O19" s="24">
+      <c r="O19" s="21">
         <f t="shared" si="0"/>
         <v>35470785</v>
       </c>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="19" t="e">
+      <c r="P19" s="15"/>
+      <c r="Q19" s="16" t="e">
         <f>SUM((Table1[[#This Row],[Column15]]/COUNT(Table1[[#This Row],[Column2]:[Column13]]))*12)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="R19" s="20"/>
+      <c r="R19" s="17"/>
       <c r="S19" s="1"/>
     </row>
     <row r="20" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A20" s="1"/>
-      <c r="B20" s="15">
+      <c r="B20" s="12">
         <v>2023</v>
       </c>
-      <c r="C20" s="25">
+      <c r="C20" s="22">
         <v>2746994</v>
       </c>
-      <c r="D20" s="25">
+      <c r="D20" s="22">
         <v>2114174</v>
       </c>
-      <c r="E20" s="25">
+      <c r="E20" s="22">
         <v>1899126</v>
       </c>
-      <c r="F20" s="25">
+      <c r="F20" s="22">
         <v>1806635</v>
       </c>
-      <c r="G20" s="25">
+      <c r="G20" s="22">
         <v>1707937</v>
       </c>
-      <c r="H20" s="25">
+      <c r="H20" s="22">
         <v>2289209</v>
       </c>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="25"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="25"/>
-      <c r="O20" s="24">
+      <c r="I20" s="22">
+        <v>2206719</v>
+      </c>
+      <c r="J20" s="22">
+        <v>2031085</v>
+      </c>
+      <c r="K20" s="22"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="21">
         <f>SUM(C20:N20)</f>
-        <v>12564075</v>
-      </c>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="19"/>
-      <c r="R20" s="20"/>
+        <v>16801879</v>
+      </c>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="17"/>
       <c r="S20" s="1"/>
     </row>
     <row r="21" spans="1:19" s="7" customFormat="1" ht="58.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2307,13 +2311,13 @@
       <c r="L21" s="26"/>
       <c r="M21" s="26"/>
       <c r="N21" s="26"/>
-      <c r="O21" s="27">
+      <c r="O21" s="23">
         <f>SUM(O5:O20)</f>
-        <v>146656000</v>
-      </c>
-      <c r="P21" s="28"/>
-      <c r="Q21" s="29"/>
-      <c r="R21" s="29"/>
+        <v>150893804</v>
+      </c>
+      <c r="P21" s="24"/>
+      <c r="Q21" s="25"/>
+      <c r="R21" s="25"/>
       <c r="S21" s="3"/>
     </row>
     <row r="22" spans="1:19" ht="26.85" customHeight="1" x14ac:dyDescent="0.35">
@@ -2339,12 +2343,12 @@
     <row r="23" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -2935,9 +2939,9 @@
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
-      <c r="J52" s="13"/>
-      <c r="K52" s="13"/>
-      <c r="L52" s="13"/>
+      <c r="J52" s="29"/>
+      <c r="K52" s="29"/>
+      <c r="L52" s="29"/>
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>

</xml_diff>

<commit_message>
Blog Statistics (October 2023)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c93c05515dfe04a/GIT Hub/kunal-chowdhury.com/blog-stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="11_91C7ACB7C03E7306CE517BDFACF66E9FD99B01DC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{201EE36A-992F-448A-A4CB-360A9163B7EB}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="11_91C7ACB7C03E7306CE517BDFACF66E9FD99B01DC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CC9587F-B4B0-4C84-A968-21ABB22B8167}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -742,7 +742,7 @@
                   <c:v>35470785</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16801879</c:v>
+                  <c:v>22067841</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -978,6 +978,14 @@
 </file>
 
 <file path=xl/persons/person1.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person2.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person3.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -1305,8 +1313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="W20" sqref="W20"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2283,13 +2291,17 @@
       <c r="J20" s="22">
         <v>2031085</v>
       </c>
-      <c r="K20" s="22"/>
-      <c r="L20" s="22"/>
+      <c r="K20" s="22">
+        <v>2804382</v>
+      </c>
+      <c r="L20" s="22">
+        <v>2461580</v>
+      </c>
       <c r="M20" s="22"/>
       <c r="N20" s="22"/>
       <c r="O20" s="21">
         <f>SUM(C20:N20)</f>
-        <v>16801879</v>
+        <v>22067841</v>
       </c>
       <c r="P20" s="15"/>
       <c r="Q20" s="16"/>
@@ -2313,7 +2325,7 @@
       <c r="N21" s="26"/>
       <c r="O21" s="23">
         <f>SUM(O5:O20)</f>
-        <v>150893804</v>
+        <v>156159766</v>
       </c>
       <c r="P21" s="24"/>
       <c r="Q21" s="25"/>

</xml_diff>

<commit_message>
Blog Statistics (November 2023)
</commit_message>
<xml_diff>
--- a/blog-stats/Blog Hits - Report.xlsx
+++ b/blog-stats/Blog Hits - Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c93c05515dfe04a/GIT Hub/kunal-chowdhury.com/blog-stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="11_91C7ACB7C03E7306CE517BDFACF66E9FD99B01DC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CC9587F-B4B0-4C84-A968-21ABB22B8167}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="11_91C7ACB7C03E7306CE517BDFACF66E9FD99B01DC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4636A8D8-9AF8-4451-8D1B-85257F5CB29C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -742,7 +742,7 @@
                   <c:v>35470785</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>22067841</c:v>
+                  <c:v>24225630</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -986,6 +986,10 @@
 </file>
 
 <file path=xl/persons/person3.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person4.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -1313,8 +1317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="V8" sqref="V8"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2297,11 +2301,13 @@
       <c r="L20" s="22">
         <v>2461580</v>
       </c>
-      <c r="M20" s="22"/>
+      <c r="M20" s="22">
+        <v>2157789</v>
+      </c>
       <c r="N20" s="22"/>
       <c r="O20" s="21">
         <f>SUM(C20:N20)</f>
-        <v>22067841</v>
+        <v>24225630</v>
       </c>
       <c r="P20" s="15"/>
       <c r="Q20" s="16"/>
@@ -2325,7 +2331,7 @@
       <c r="N21" s="26"/>
       <c r="O21" s="23">
         <f>SUM(O5:O20)</f>
-        <v>156159766</v>
+        <v>158317555</v>
       </c>
       <c r="P21" s="24"/>
       <c r="Q21" s="25"/>

</xml_diff>